<commit_message>
Fixed some errors when using BERTopic and finished script for generating pilot data
</commit_message>
<xml_diff>
--- a/data/top_docs/ctm/thetas_sample_top_docs.xlsx
+++ b/data/top_docs/ctm/thetas_sample_top_docs.xlsx
@@ -476,32 +476,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>credits composition allmusic listing charts piano drums beats liner label recording download ballad songwriter vocals albums musicians accompanying remix singer mixing singing adapted lyrically tempo formats lyrical pop lyrics acoustic billboard charted musically promotion performing mixed instrumentation background grammy videos promotional reception vocal personnel promote rolling_stone releases artist digital influences usher debuted sounds backing hip footage songwriting compilation guitars chart youtube listings handled popmatters bonus concert musician keyboards reviewer studio studios catchy percussion nme remixes airplay hop mexican vocalist guitarist band recordings thirty peaked tracks jazz sing collaboration rap electronic recorded bass hear highlight radio hot sings listeners dvd stan</t>
+          <t>['credits', 'composition', 'allmusic', 'listing', 'charts', 'piano', 'drums', 'beats', 'liner', 'label', 'recording', 'download', 'ballad', 'songwriter', 'vocals']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The Family Jewels ( Marina and the Diamonds album ) = The Family Jewels is the debut studio album recorded by Welsh singer Marina Diamandis , professionally known as Marina and the Diamonds . It was released on 15 February 2010 by 679 Recordings and Atlantic Records . Diamandis collaborated with several producers including Pascal Gabriel , Liam Howe , Greg Kurstin , Richard " Biff " Stannard , and Starsmith during its recording . She identifies the lyrical themes as " the seduction of commercialism , modern social values , family and female sexuality . " Contemporary music critics gave The Family Jewels fairly positive reviews , with the vocal delivery dividing opinions . The record debuted at number five on the UK Albums Chart with first-week sales of 27,618 copies . The album was eventually certified Gold by the British Phonographic Industry and has sold 195,358 units in the United Kingdom . The Family Jewels performed moderately on international record charts ; it peaked at number 1</t>
+          <t>Tomoyo After : It 's a Wonderful Life = Tomoyo After : It 's a Wonderful Life ( 智代アフター ～ It 's a Wonderful Life ～ , Tomoyo Afutā ~ It 's a Wonderful Life ~ ) is a Japanese adult visual novel developed by Key released on November 25 , 2005 for Windows PCs . The game is a spin-off of Key 's earlier all ages game Clannad . Key later released versions of Tomoyo After without the erotic content , and the game was ported to the PlayStation 2 , PlayStation Portable , Xbox 360 and PlayStation 3 under the title Tomoyo After : It 's a Wonderful Life CS Edition ; CS stands for " consumer software " . The story follows the lives of Tomoya Okazaki , a young man who recently graduated from high school , and his close friend Tomoyo Sakagami as they start to see more of each other in a romantic relationship . The gameplay in Tomoyo After follows a branching plot line which offers pre-determined scenarios with courses of interaction , and focuses on the appeal of the title character Tomoyo . Being a sp</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Marilyn Monroe ( Nicki Minaj song ) = " Marilyn Monroe " is a song by Trinidadian born recording artist Nicki Minaj . The song was written by Minaj , Daniel James , Leah Haywood , Ross Golan and J.R. Rotem , while production was handled by J.R. Rotem and Dreamlab . Musically , " Marilyn Monroe " is an introspective mid-tempo ballad that contains an upbeat piano , synth beats , and features influences of bubblegum pop . Lyrically , the song alludes to oneself questioning the status of their relationship . The song makes frequent references to pop icon Marilyn Monroe , with many of her quotes woven into the song . " Marilyn Monroe " was generally well received by music critics , with some noting its crossover potential , while others felt like the song was too similar to other artists . The song has received comparisons to the 2011 singles " Disaster " by JoJo and " Stuttering " by Fefe Dobson , as well as Minaj 's own 2010 single " Your Love " from her debut album Pink Friday . The albu</t>
+          <t>Basarab I of Wallachia = Basarab I ( Romanian pronunciation : [ basaˈrab ] ) , also known as Basarab the Founder ( Romanian : Basarab Întemeietorul ) , was a voivode , and later the first independent ruler of Wallachia who lived in the first half of the 14th century . Many details of his life are uncertain . Although his name is of Turkic origin , 14th-century sources unanimously state that he was a Vlach . Basarab came into power before 1324 , but the circumstances of his ascension are unknown . According to two popular theories , he succeeded either his father , Thocomerius , or the legendary founder of Wallachia , Radu Negru . A royal charter issued on 26 July 1324 is the first document to reference Basarab . According to the charter , he was subject to Charles I of Hungary as the voivode of Wallachia . Basarab became " disloyal to the Holy Crown of Hungary " in 1325 . He seized the Banate of Severin and raided the southern regions of the Kingdom of Hungary . Basarab supported Micha</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Down Town = for the Greek magazine see Down Town ( magazine ) " Down Town " was the a 1987 release by The Justified Ancients of Mu Mu ( better known as The KLF ) . The song is gospel music driven by house music rhythms , incorporating a sample of Petula Clark 's 1964 single " Downtown " . = = Origins = = In 1987 , Bill Drummond and Jimmy Cauty formed The Justified Ancients of Mu Mu ( The JAMs ) , and busily released provocatively sample-heavy electronic music with beatbox rhythms and Drummond 's socially aware raps . Their debut single " All You Need Is Love " and album 1987 ( What the Fuck Is Going On ? ) were both investigated by the Mechanical Copyright Protection Society , who ordered The JAMs to recall and destroy all unsold copies of 1987 . A new single , " Whitney Joins The JAMs " , followed , along with a satirically edited version of the album , 1987 ( The JAMs 45 Edits ) , and the debut release from spinoff project Disco 2000 , " I Gotta CD " . By the time of the release of "</t>
+          <t>Long Way to Go ( Gwen Stefani and André 3000 song ) = " Long Way to Go " is a song by American singer-songwriter Gwen Stefani with American rapper André 3000 . The song appears as the closing track on Stefani 's debut studio album , Love . Angel . Music . Baby . ( 2004 ) . It was released on November 23 , 2004 , along with the rest of Love . Angel . Music . Baby. by Interscope Records . The track was written by both Stefani and 3000 , while 3000 was the sole producer of the track . Although the song was scrapped from 3000 's critically acclaimed OutKast studio album , The Love Below ( 2003 ) , Stefani and 3000 finalized a reworked version of the song to be included on Stefani 's album . The song prominently features a sample from Martin Luther King , Jr . ' s " I Have a Dream " speech in its closing outro . King is not credited for contributed lyrics to the song . Musically , " Long Way to Go " is influenced by electronic music and alternative hip hop , with partial influence from both</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The Manchester Rambler = " The Manchester Rambler " , also known as " I 'm a Rambler " and " The Rambler 's Song " , is a song written by the English folk singer Ewan MacColl . It was inspired by his participation in the Kinder trespass , a protest by the urban Young Communist League of Manchester , and was the work that began MacColl 's career as a singer-songwriter . Since the 1950s , the song has become a standard among folk musicians , as it was for MacColl himself . It has been covered many times , including by The Dubliners and The Houghton Weavers . It has been sung both in clubs and in the open air on a variety of occasions , including at Kinder Downfall in 2009 when Kinder was designated as a National Nature Reserve . = = Context = = The Kinder mass trespass was a deliberate act of civil disobedience ( the law of trespass having already been repealed ) by men of the Young Communist League of Manchester , and others from Sheffield . The protest was intended to secure free acces</t>
+          <t>Strange Overtones = " Strange Overtones " is a song recorded by David Byrne and Brian Eno , written by the duo with Leo Abrahams . It was released on August 4 , 2008 by means of free download as the lead single from Byrne 's and Eno 's second collaborative studio album Everything That Happens Will Happen Today ( 2008 ) . " Strange Overtones " is an uptempo electronic gospel song , and its lyrics explore the themes of humanity overcoming technology that are central to the album . " Strange Overtones " was well received by critics , and was downloaded 40,000 times in its first three days of release . = = Recording and release = = While discussing the 2006 remix of My Life in the Bush of Ghosts at a dinner party , Eno suggested finishing some songs that he had written but that did not have lyrics . Byrne visited Eno 's studio to listen to the demos and the two decided to collaborate to finish writing the songs . They continued working on the tracks in New York City and London , with regul</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>HMS Duke of Edinburgh = HMS Duke of Edinburgh was the lead ship of the Duke of Edinburgh-class armoured cruisers built for the Royal Navy in the mid-1900s . She was stationed in the Mediterranean when the First World War began and participated in the pursuit of the German battlecruiser SMS Goeben and light cruiser SMS Breslau . After the German ships reached Ottoman waters , the ship was sent to the Red Sea in mid-August to protect troop convoys arriving from India . Duke of Edinburgh was transferred to the Grand Fleet in December 1914 and participated in the Battle of Jutland in May 1916 . She was not damaged during the battle and was the only ship of her squadron to survive . She was eventually transferred to the Atlantic Ocean in August 1917 for convoy escort duties . The ship was sold for scrap in 1920 . = = Description = = Duke of Edinburgh displaced 12,590 long tons ( 12,790 t ) as built and 13,965 long tons ( 14,189 t ) fully loaded . The ship had an overall length of 505 feet 6</t>
+          <t>Harold Washington Cultural Center = Harold Washington Cultural Center is a performance facility located in the Grand Boulevard community area of Chicago in Cook County , Illinois , United States . It was named after Chicago 's first African-American Mayor Harold Washington and opened August 17 , 2004 ten years after initial groundbreaking . In addition to the 1000 seat Com-Ed Theatre , the center offers a Digital Media Resource Center . Former Chicago City Council Alderman Dorothy Tillman and singer Lou Rawls take credit for championing the center , which cost $ 19.5 million . It was originally to be named the Lou Rawls Cultural Center , but Alderman Tillman changed the name without telling Rawls . Although it is considered part of the Bronzeville neighborhood it is not part of the Chicago Landmark Black Metropolis-Bronzeville District that is in the Douglas community area . The limestone building , which is located on the same site as a former historic black theatre , has become the s</t>
         </is>
       </c>
     </row>
@@ -511,32 +511,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>film release released million story scene scenes script effects production opening plot filming original director sequel action movie weekend blu character bond highest batman score dvd photography cast based reviews films shot box grossing stars visual gave trailer screenplay disney version rotten_tomatoes marvel characters studio said office like rating set filmmakers sequels toy gross theaters wanted making footage burton idea animation critics worldwide animated direct theatrical cinematic shots grossed james_bond stated development horror sequence critical create principal cameron best special north_america halloween screening reception written escapes kills woody filmed villain animators cgi budget sequences movies role features place kill takes</t>
+          <t>['film', 'release', 'released', 'million', 'story', 'scene', 'scenes', 'script', 'effects', 'production', 'opening', 'plot', 'filming', 'original', 'director']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pacific Rim ( film ) = Pacific Rim is a 2013 American science fiction monster film directed by Guillermo del Toro , and starring Charlie Hunnam , Idris Elba , Rinko Kikuchi , Charlie Day , Robert Kazinsky , Max Martini , and Ron Perlman . The screenplay is by Travis Beacham and del Toro , with a story by Beacham . The film is set in the future , when Earth is at war with the Kaiju , colossal monsters which have emerged from an interdimensional portal on the bottom of the Pacific Ocean . To combat the monsters , humanity unites to create the Jaegers , gigantic humanoid mechas each controlled by at least two pilots , whose minds are joined by a neural bridge . Focusing on the war 's later days , the story follows Raleigh Becket , a washed-up Jaeger pilot called out of retirement and teamed with rookie pilot Mako Mori as part of a last-ditch effort to defeat the Kaiju . Principal photography began on November 14 , 2011 in Toronto and lasted through April 2012 . The film was produced by Le</t>
+          <t xml:space="preserve">St Mary 's Church , Acton = St Mary 's Church is an active Anglican parish church located in Monk 's Lane , Acton , a village to the west of Nantwich , Cheshire , England . Since 1967 it has been designated a Grade I listed building . A church has been present on this site since before the time of the Domesday Survey . The tower is the oldest in Cheshire , although it had to be largely rebuilt after it fell in 1757 . One unusual feature of the interior of the church is that the old stone seating around its sides has been retained . In the south aisle are some ancient carved stones dating back to the Norman era . The architectural historian Alec Clifton-Taylor includes the church in his list of ' best ' English parish churches . In the churchyard is a tall 17th-century sundial . The church is an active Anglican parish church in the diocese of Chester , the archdeaconry of Macclesfield and the deanery of Nantwich . Its benefice is united with those of St David , Wettenhall , St Oswald , </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Husayn ibn Hamdan = Husayn ibn Hamdan ibn Hamdun ibn al-Harith al-Taghlibi was an early member of the Hamdanid family , who distinguished himself as a general for the Abbasid Caliphate and played a major role in the Hamdanids ' rise to power among the Arab tribes in the Jazira . Husayn entered caliphal service in 895 , and through his co-operation with the caliphal government , he established himself and his family as the leader of the Arabs and Kurds of the Jazira , leading his troops to successful campaigns against the Qarmatians , Dulafids and Tulunids over the next few years . As one of the most distinguished generals of the Abbasid Caliphate , he rose in power and influence until 908 , when he was one of the leading conspirators in the abortive coup against Caliph al-Muqtadir . Although the coup failed and Husayn was forced to flee the capital , he soon secured a pardon and served as governor in Jibal , where he again distinguished himself in military operations in south-central I</t>
+          <t>Captain America : The Winter Soldier = Captain America : The Winter Soldier is a 2014 American superhero film featuring the Marvel Comics character Captain America , produced by Marvel Studios and distributed by Walt Disney Studios Motion Pictures . It is the sequel to 2011 's Captain America : The First Avenger and the ninth film in the Marvel Cinematic Universe ( MCU ) . The film was directed by Anthony and Joe Russo , with a screenplay by Christopher Markus &amp; Stephen McFeely , who had also written The First Avenger . It stars Chris Evans as Captain America , leading an ensemble cast that includes Scarlett Johansson , Sebastian Stan , Anthony Mackie , Cobie Smulders , Frank Grillo , Emily VanCamp , Hayley Atwell , Robert Redford and Samuel L. Jackson . In Captain America : The Winter Soldier , Captain America , Black Widow , and Falcon join forces to uncover a conspiracy within S.H.I.E.L.D. while facing a mysterious assassin known as the Winter Soldier . A major influence in The Wint</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Italian battleship Andrea Doria = Andrea Doria was the lead ship of her class of battleships built by the Regia Marina ( Royal Navy ) . The class included only one sister ship , Caio Duilio . Andrea Doria was named after the 16th century Genoese admiral of the same name . Laid down in March 1912 , the battleship was launched a year later in March 1913 , and completed in March 1916 . She was armed with a main battery of thirteen 305 mm ( 12.0 in ) guns and had a top speed of 21 kn ( 39 km / h ; 24 mph ) . Andrea Doria saw no major action in World War I , and served extensively in Mediterranean in the 1920s and 1930s . She was involved in the suppression of rebels in Fiume and the Corfu incident in the 1920s . Starting in 1937 , Andrea Doria underwent an extensive modernization , which lasted until 1940 . She saw relatively little action during World War II ; she was tasked with escorting convoys to Libya throughout 1941 and into 1942 , during which she engaged in the inconclusive First </t>
+          <t>Southampton Castle = Southampton Castle was located in the town of Southampton in Hampshire , England . Constructed after the Norman conquest of England , it was located in the north-west corner of the town overlooking the River Test , initially as a wooden motte and bailey design . By the late 12th century the royal castle had been largely converted to stone , playing an important part in the wine trade conducted through the Southampton docks . By the end of the 13th century the castle was in decline , but the threat of French raids in the 1370s led Richard II to undertake extensive rebuilding . The result was a powerfully defended castle , one of the first in England to be equipped with cannon . The castle declined again in the 16th century and was sold off to property speculators in 1618 . After being used for various purposes , including the construction of a Gothic mansion in the early 19th century , the site was flattened and largely redeveloped . Only a few elements of the castl</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Yeah 3x = " Yeah 3x " ( pronounced " Yeah three times " or " Yeah Yeah Yeah " ) is a song by American recording artist Chris Brown , released as the lead single from his fourth studio album F.A.M.E. on October 25 , 2010 . It was written by Brown , DJ Frank E , Kevin McCall , Amber Streeter and Calvin Harris , and was produced by DJ Frank E. Brown recorded the song for his pop audience as he had been doing a lot of mixtapes and urban records . " Yeah 3x " is an uptempo dance-pop , Europop , and electro house song ; it uses a video game-type beat and features a thick bassline and big synth chords . The song uses elements of Harris ' 2009 single " I 'm Not Alone " . Critical reception towards the song was positive , with critics praising its production and lyrics . Other critics noted its similarities to Brown 's 2008 single " Forever " . " Yeah 3x " attained top-ten positions in Australia , Austria , Belgium ( Flanders ) , Denmark , Germany , Hungary , Ireland , Netherlands , New Zealand</t>
+          <t>Cardcaptor Sakura = Cardcaptor Sakura ( カードキャプターさくら , Kādokyaputā Sakura ) , abbreviated as CCS and also known as Cardcaptors , is a Japanese shōjo manga series written and illustrated by the manga group Clamp . The manga was originally serialized in Nakayoshi from May 1996 to June 2000 , and published in 12 tankōbon volumes by Kodansha from November 1996 to July 2000 . The story focuses on Sakura Kinomoto , an elementary school student who discovers that she possesses magical powers after accidentally freeing a set of magical cards from the book they had been sealed in for years . She is then tasked with retrieving those cards in order to avoid an unknown catastrophe from befalling the world . A sequel by Clamp focusing on Sakura in junior high school began serialization in Nakayoshi with the July 2016 issue . The series was adapted into a 70-episode anime TV series by Madhouse that aired on Japan 's satellite television channel NHK BS2 from April 1998 to March 2000 . Additional media</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Lawrence Berry Washington = Lawrence Berry Washington ( November 26 , 1811 – September 21 , 1856 ) was an American lawyer , military officer , author , Forty-niner , Border Ruffian , and a member of the Washington family . Washington was born on his family 's Cedar Lawn plantation near Charles Town , Virginia ( present-day West Virginia ) and was the eldest of 13 children . He practiced law , then served as a second lieutenant in the Virginia Volunteers during the Mexican – American War . During his service in the war , Washington reportedly wore the sword of his great-granduncle George Washington . Following the Mexican – American War , Washington traveled to California in 1849 as a Forty-niner in the California Gold Rush and authored the novel , A Tale to be Told Some Fifty Years Hence . Washington then relocated east to Missouri in the 1850s , where he remained for a few years and fought as a Border Ruffian during the Bleeding Kansas confrontations over slavery along the border betw</t>
+          <t>Tintin in America = Tintin in America ( French : Tintin en Amérique ) is the third volume of The Adventures of Tintin , the comics series by Belgian cartoonist Hergé . Commissioned by the conservative Belgian newspaper Le Vingtième Siècle for its children 's supplement Le Petit Vingtième , it was serialised weekly from September 1931 to October 1932 before being published in a collected volume by Éditions du Petit Vingtième in 1932 . The story tells of young Belgian reporter Tintin and his dog Snowy who travel to the United States , where Tintin reports on organised crime in Chicago . Pursuing a gangster across the country , he encounters a tribe of Blackfoot Native Americans before defeating the Chicago crime syndicate . Following the publication of Tintin in the Congo , Hergé conducted research for a story set in the United States , desiring to reflect his concerns regarding the treatment of Native communities by the U.S. government . Bolstered by a publicity stunt , Tintin in Americ</t>
         </is>
       </c>
     </row>
@@ -546,32 +546,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>career hit games season league baseball major_league_baseball signed home played manager professional minor earned hits pitcher mlb leagues base giants roster strikeouts average pitched runs spent playing hitter starts spring era pitching basketball cubs inning team catcher national_league traded record starting rookie draft double named year run dodgers baseman batted contract disabled bats batters reds percentage hitting postseason pitchers rbi new_york_yankees seasons plate sophomore pirates prospect pitch rbis bases drafted pitches braves hitters walks ninth signing pennant finished player assists major boston_red_sox american_league chicago_cubs throwing philadelphia_phillies outfielder fastball handed batting fielder fielding shortstop texas_rangers freshman detroit_tigers tied san_francisco_giants list cincinnati_reds</t>
+          <t>['career', 'hit', 'games', 'season', 'league', 'baseball', 'major_league_baseball', 'signed', 'home', 'played', 'manager', 'professional', 'minor', 'earned', 'hits']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sexy ( Glee ) = " Sexy " is the fifteenth episode of the second season of the American musical comedy-drama television series Glee , and the thirty-seventh episode overall . It was written by Brad Falchuk , directed by Ryan Murphy , and first aired on the Fox network on March 8 , 2011 . The episode mainly revolves around the topics of sex and adolescent sexuality . In it , Holly Holliday ( Gwyneth Paltrow ) returns to McKinley High School as a substitute teacher in a class devoted to sex education . Glee club director Will Schuester ( Matthew Morrison ) begins to develop feelings for Holly , and guidance counselor and celibacy club advisor Emma Pillsbury ( Jayma Mays ) is less than pleased with Holly 's lessons . Santana ( Naya Rivera ) expresses her love for Brittany ( Heather Morris ) , and Burt Hummel ( Mike O 'Malley ) has a talk with his son Kurt ( Chris Colfer ) about sex . " Sexy " received generally positive reviews . Many critics praised Paltrow 's performance , preferring it </t>
+          <t xml:space="preserve">2010 Auto Club 500 = The 2010 Auto Club 500 was a NASCAR Sprint Cup Series race held on February 21 , 2010 at Auto Club Speedway in Fontana , California . Contested over 250 laps , it was the second race of the 2010 Sprint Cup Series season . The race was won by Jimmie Johnson for Hendrick Motorsports . Kevin Harvick finished second and Jeff Burton clinched third . Polesitter driver Jamie McMurray maintained his lead into the first corner , but outsider Juan Pablo Montoya took the lead before the first lap was over . Afterward , Johnson became the leader , and would eventually lead to the race high of 101 laps . During the final pit stops , Johnson was on pit lane as the caution flag came out . Burton , who led the race during Johnson 's pit stop , did not pass Johnson to put him a lap down . Therefore , Johnson retained the first position upon the completion of pit stops . On the final lap , Harvick was gaining on Johnson , but Johnson maintained his position to win his first race of </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Architecture of Denmark = The architecture of Denmark has its origins in the Viking period , richly revealed by archaeological finds . It became firmly established in the Middle Ages when first Romanesque , then Gothic churches and cathedrals sprang up throughout the country . It was during this period that , in a country with little access to stone , brick became the construction material of choice , not just for churches but also for fortifications and castles . Under the influence of Frederick II and Christian IV , both of whom had been inspired by the castles of France , Dutch and Flemish designers were brought to Denmark , initially to improve the country 's fortifications , but increasingly to build magnificent royal castles and palaces in the Renaissance style . In parallel , the half-timbered style became popular for ordinary dwellings in towns and villages across the country . Late in his reign , Christian IV also became an early proponent of Baroque which was to continue for </t>
+          <t xml:space="preserve">María del Luján Telpuk = Lorena Telpuk , formerly María del Luján Telpuk , ( sometimes María de Luján Telpuk ) or the Suitcase Girl ( c . 1981 ) is a former airport police officer at Aeroparque Jorge Newbery in Buenos Aires , Argentina , who noticed a suitcase with US $ 800,000 as it went through an X-ray machine in August 2007 . In December 2007 , the money became a very public part of an international election suitcase scandal , known as Maletinazo . When the suitcase scandal became public , she became an international celebrity and appeared on the cover of several magazines , including those of the February 2008 issue of the Argentine edition of Playboy magazine and the March 2008 issue of the Venezuelan edition of Playboy magazine . In 2008 , according to foreign language sources , she changed her name from María del Luján Telpuk to Lorena Telpuk ; she posed for additional adult modeling photographs ; and continued her pursuit of stardom . She also testified in court regarding her </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dear Doctor = " Dear Doctor " is the thirteenth episode of the first season of the American science fiction television series Star Trek : Enterprise and originally aired on January 23 , 2002 , on UPN . The episode was written by Maria and Andre Jacquemetton , and was directed by James A. Contner . Set in the 22nd century , the series follows the adventures of the first Starfleet starship Enterprise , registration NX-01 . In this episode , Doctor Phlox ( John Billingsley ) faces a serious dilemma as a dying race begs for help from the crew of the Enterprise . The culture consists of two related races , but only the more genetically advanced race has been stricken by a planet-wide plague . UPN requested that the ending of the episode be changed , something that Billingsley did not like . However , he and other members of the cast and crew approved of the final episode . Due to the subject matter and the ending , it is seen as a controversial episode by fans . Although " Dear Doctor " rec</t>
+          <t>M-57 ( Michigan highway ) = M-57 is an east – west state trunkline highway in the US state of Michigan . The 105.377-mile ( 169.588 km ) highway connects US Highway 131 ( US 131 ) near Rockford on the west end to M-15 near Otisville in the Lower Peninsula . In between , the mostly rural highway passes through farmland and connects several highways and smaller towns together . Three of these highways are freeways : US 131 , US 127 and Interstate 75 ( I-75 ) . Along the way , between 3,700 and 22,300 vehicles use the highway daily . The current highway that bears the M-57 moniker is the second to do so . The first is now M-75 in the Northern Lower Peninsula . This second highway was designated in the 1930s along a different , but parallel , routing . The first major changes shifted that routing southward to the current corridor in stages . Through additional extensions and truncations , the modern routing was formed by the 1970s . = = Route description = = M-57 is a rural , two-lane high</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Shelley Chaplin = Shelley Chaplin ( born 4 September 1984 ) is an Australian 3.5-point player wheelchair basketball player . She participated in the 2004 Summer Paralympics in Athens , where she won a silver medal ; in the 2008 Summer Paralympics in Beijing , where she won a bronze medal , and the 2012 Summer Paralympics in London , where she won a second silver medal , a win she dedicated to her lifelong friend Shannon . Chaplin began playing wheelchair basketball in 1999 , after initially contemplating developing her archery skills , and made her debut in the Women 's National Wheelchair Basketball League ( WNWBL ) in 2000 . She was part of the WNWBL championship Dandenong Rangers sides in 2011 and 2012 . She was first selected for the Australia women 's national wheelchair basketball team , known as the Gliders , in 2001 , and first represented Australia in 2002 , winning a bronze medal as part of the team at the 2002 World Wheelchair Basketball Championship . She played for the Uni</t>
+          <t>2008 Philadelphia Phillies season = The Philadelphia Phillies ' 2008 season was the 126th in the history of the franchise . The team finished with a regular season record of 92 – 70 , first in the National League East . In the post-season , the Phillies won the World Series ; this was the first major sports championship for Philadelphia since the 76ers swept the 1983 NBA Finals . During the season , they were managed by Charlie Manuel . The Phillies opened the season by posting their first winning April since 2003 . They also scored 60 runs over 5 games in late May in a sweep over the Colorado Rockies and accrued a 14 – 4 record over 18 games entering the month of June . The Phillies ' performance declined in late June , but they improved after the All-Star break , going 9 – 6 immediately following the midseason hiatus . Closer Brad Lidge earned eight saves in those games , and did not blow a save throughout the season and the postseason . Philadelphia traded sweeps with the Los Angele</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Allen Craig = Allen Thomas Craig ( born July 18 , 1984 ) is an American professional baseball first baseman and outfielder in the Boston Red Sox organization . He has played in Major League Baseball ( MLB ) for the St. Louis Cardinals and Boston Red Sox . The Cardinals drafted him from the University of California , Berkeley , in 2006 , and he made his Major League debut with the Cardinals in 2010 . Besides the outfield and first base , he has appeared at every position except pitcher , catcher and shortstop . Each season in the minor leagues from 2007 – 09 , Craig finished with a batting average of over .300 with at least 20 home runs . A .306 career hitter in MLB through 2013 , he increased his production with runners in scoring position ( RISP ) . In 2012 , he posted a .400 batting average with RISP . The next season , he raised that figure to .454 , the third-highest average of all time . Craig has appeared in two World Series and in both made history . In the 2011 World Series , h</t>
+          <t>Hell-O ( Glee ) = " Hell-O " is the fourteenth episode of the American television series Glee . The episode premiered on the Fox network on April 13 , 2010 . It was written by series creator Ian Brennan and directed by Brad Falchuk . In " Hell-O " , cheer-leading coach Sue Sylvester ( Jane Lynch ) attempts to sabotage the relationship between glee club members Finn Hudson ( Cory Monteith ) and Rachel Berry ( Lea Michele ) . Glee club director Will Schuester ( Matthew Morrison ) attempts to begin a relationship with school guidance counsellor Emma Pillsbury ( Jayma Mays ) , but several obstacles come between them , including the coach of rival glee club Vocal Adrenaline . " Hell-O " introduces special guest stars Idina Menzel as Shelby Corcoran , the coach of Vocal Adrenaline , and Jonathan Groff as Jesse St. James , the group 's lead singer . Glee fans had previously lobbied for Menzel to be cast as Rachel 's biological mother . The episode features cover versions of six songs , five o</t>
         </is>
       </c>
     </row>
@@ -581,32 +581,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>work life wrote writing published book written women works history world writer woman early books years known literary thought according children man people author novel poetry death art god human ideas society stories write poems literature historical story family age described writers modern century later church born writings study mother poem father science believed like social school culture poet view spiritual use religious tradition contemporary christian friend novels theory taught characters believe studies idea considered academic prize criticism old form account cult belief comics argued cultural professor great views political chess nature publication readers called publishing sexual teaching influenced philosophical</t>
+          <t>['work', 'life', 'wrote', 'writing', 'published', 'book', 'written', 'women', 'works', 'history', 'world', 'writer', 'woman', 'early', 'books']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sera Monastery = Sera Monastery ( Tibetan : སེ ་ ར ་ དགོན ་ པ , Wylie : se ra dgon pa " Wild Roses Monastery " ; Chinese : 色拉寺 ; pinyin : Sèlā Sì ) is one of the " great three " Gelug university monasteries of Tibet , located 1.25 miles ( 2.01 km ) north of Lhasa and about 5 kilometres ( 3.1 mi ) north of the Jokhang . The other two are Ganden Monastery and Drepung Monastery . The origin of its name is attributed to a fact that the site where the monastery was built was surrounded by wild roses in bloom . The original Sera Monastery is responsible for some 19 hermitages , including four nunneries , which are all located in the foot hills north of Lhasa . The Sera Monastery , as a complex of structures with the Great Assembly Hall and three colleges , was founded in 1419 by Jamchen Chojey of Sakya Yeshe of Zel Gungtang ( 1355 – 1435 ) , a disciple of Je Tsongkhapa . During the 1959 revolt in Lhasa , Sera monastery suffered severe damage , with its colleges destroyed and hundreds of monk</t>
+          <t>Fark = Fark is a community website created by Drew Curtis that allows members to comment on a daily batch of news articles and other items from various websites . The site receives many story submissions per day and approximately 100 of them are publicly displayed on the site , spread out over the main page and tabs ( Entertainment , Sports , Geek , Politics and Business ) . Founder Drew Curtis says the stories are selected without intentional political bias , but that he tries to run both far-left and far-right articles . Links are submitted by Fark members ( collectively referred to as " Farkers " ) , which admins can approve ( " greenlight " ) for posting on either the main page or one of the subsidiary tab pages . All links ( excluding those of sponsors ) , whether approved or not , have associated threads where users can comment on the link . Greenlit links can generate upwards of 300,000 page views in one month for the recipient . This can generate such an enormous amount of traf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Architecture of Madagascar = The architecture of Madagascar is unique in Africa , bearing strong resemblance to the construction norms and methods of Southern Borneo from which the earliest inhabitants of Madagascar are believed to have immigrated . Throughout Madagascar and the Kalimantan region of Borneo , most traditional houses follow a rectangular rather than round form , and feature a steeply sloped , peaked roof supported by a central pillar . Differences in the predominant traditional construction materials used serve as the basis for much of the diversity in Malagasy architecture . Locally available plant materials were the earliest materials used and remain the most common among traditional communities . In intermediary zones between the central highlands and humid coastal areas , hybrid variations have developed that use cob and sticks . Wood construction , once common across the island , declined as a growing human population destroyed greater swaths of virgin rainforest fo</t>
+          <t>Seneca Falls Convention = The Seneca Falls Convention was the first women 's rights convention . It advertised itself as " a convention to discuss the social , civil , and religious condition and rights of woman " . Held in Seneca Falls , New York , it spanned two days over July 19 – 20 , 1848 . Attracting widespread attention , it was soon followed by other women 's rights conventions , including one in Rochester , New York , two weeks later . In 1850 the first in a series of annual National Women 's Rights Conventions met in Worcester , Massachusetts . Female Quakers local to the area organized the meeting along with Elizabeth Cady Stanton , who was not a Quaker . They planned the event during a visit to the area by Philadelphia-based Lucretia Mott . Mott , a Quaker , was famous for her oratorical ability , which was rare during an era in which women were often not allowed to speak in public . The meeting comprised six sessions including a lecture on law , a humorous presentation , a</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The Lion King = The Lion King is a 1994 American animated epic musical film produced by Walt Disney Feature Animation and released by Walt Disney Pictures . It is the 32nd animated feature in the Walt Disney Animated Classics series . The story takes place in a kingdom of lions in Africa , and was influenced by William Shakespeare 's Hamlet . The film was produced during a period known as the Disney Renaissance . The Lion King was directed by Roger Allers and Rob Minkoff , produced by Don Hahn , and has a screenplay credited to Irene Mecchi , Jonathan Roberts and Linda Woolverton . Its original songs were written by composer Elton John and lyricist Tim Rice , and original scores were written by Hans Zimmer . The film features an ensemble voice cast that includes Matthew Broderick , James Earl Jones , Jeremy Irons , Jonathan Taylor Thomas , Moira Kelly , Nathan Lane , Ernie Sabella , Rowan Atkinson , Robert Guillaume , Madge Sinclair , Whoopi Goldberg , Cheech Marin , and Jim Cummings .</t>
+          <t>Maryland Route 322 = Maryland Route 322 ( MD 322 ) is a state highway in the U.S. state of Maryland . Known as Easton Parkway , the highway runs 5.12 miles ( 8.24 km ) on the west side of Easton between two junctions with U.S. Route 50 ( US 50 ) . MD 322 serves as a bypass of downtown Easton for traffic between US 50 and highways to western Talbot County , including MD 33 toward Saint Michaels and MD 333 toward Oxford . Easton Parkway was constructed in the mid to late 1960s . The state highway was originally designated as part of MD 33 ; MD 322 became the sole designation on the bypass in 1978 . = = Route description = = MD 322 begins at a directional intersection with US 50 ( Ocean Gateway ) south of Easton ; there is no direct access from southbound MD 322 to westbound US 50 . MD 322 heads north as a four-lane divided highway to MD 565 ( Washington Street ) . Beyond this intersection , the state highway reduces to two lanes , curves to the northwest , and crosses Paper Mill Pond . M</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jeriome Robertson = Jeriome Paul Robertson ( March 30 , 1977 – May 29 , 2010 ) was an American left-handed baseball pitcher who played three seasons in Major League Baseball for the Houston Astros and Cleveland Indians . In 51 pitching appearances ( 32 starts ) , Robertson posted a win – loss record of 16 – 12 with a 5.71 earned run average and 111 strikeouts in 184 ⅓ innings of work . Robertson attended Exeter High School before being drafted by the Astros in 1995 . He spent the next seven years moving up the minor league system before making his debut in September 2002 . His most productive year was 2003 , where he won 15 games and finished seventh in Rookie of the Year voting . He was traded to the Indians the following year , where he played in eight games before being demoted to the minor leagues . Robertson spent the next few years playing in various Minor League and independent baseball organizations , including the Mexican League , Chinese Professional Baseball League , Puerto </t>
+          <t>Diving cylinder = A diving cylinder , scuba tank or diving tank is a gas cylinder used to store and transport the high pressure breathing gas required by a scuba set . It may also be used for surface-supplied diving or as decompression gas or an emergency gas supply for surface supplied diving or scuba . Cylinders provide gas to the diver through the demand valve of a diving regulator or the breathing loop of a diving rebreather . Diving cylinders are usually manufactured from aluminium or steel alloys , and are normally fitted with one of two common types of cylinder valve for filling and connection to the regulator . Other accessories such as manifolds , cylinder bands , protective nets and boots and carrying handles may be provided . Various configurations of harness may be used to carry the cylinder or cylinders while diving , depending on the application . Cylinders used for scuba typically have an internal volume ( known as water capacity ) of between 3 and 18 litres ( 0.11 and 0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Louis Braille = Louis Braille ( / ˈbreɪl / , listen ; French : [ lwi bʁaj ( ə ) ] ; 4 January 1809 – 6 January 1852 ) was a French educator and inventor of a system of reading and writing for use by the blind or visually impaired . His system remains known worldwide simply as braille . Blinded in both eyes as a result of an early childhood accident , Braille mastered his disability while still a boy . He excelled in his education and received scholarship to France 's Royal Institute for Blind Youth . While still a student there , he began developing a system of tactile code that could allow blind people to read and write quickly and efficiently . Inspired by the military cryptography of Charles Barbier , Braille constructed a new method built specifically for the needs of the blind . He presented his work to his peers for the first time in 1824 . In adulthood , Braille served as a professor at the Institute and enjoyed an avocation as a musician , but he largely spent the remainder of </t>
+          <t>Next ( Desperate Housewives ) = " Next " is the second season premiere episode of the American comedy-drama series Desperate Housewives , and the 24th episode overall . It was originally broadcast in the United States on September 25 , 2005 , on ABC . It was written by Jenna Bans and Kevin Murphy and was directed by Larry Shaw . In the episode , Susan ( Teri Hatcher ) recovers from having been held hostage while Gabrielle ( Eva Longoria ) attempts to salvage her marriage to her incarcerated husband , Carlos ( Ricardo Antonio Chavira ) . Meanwhile , Bree ( Marcia Cross ) deals with her mother-in-law following her husband 's death and Lynette ( Felicity Huffman ) goes back to work . The episode also introduces the mystery storyline revolving around Betty Applewhite ( Alfre Woodard ) and her family . According to Nielsen ratings , " Next " was watched by 28.4 million viewers , making it the most watched season premiere on ABC in nine years . The episode also ranks as the second-most watch</t>
         </is>
       </c>
     </row>
@@ -616,32 +616,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>tons beam deck consisted guns laid horsepower armor hull boilers displaced steam mounted armament battery knots armored protected stern inch belt commissioned aft scrap torpedo carried waterline ironclad muzzle ship tubes amidships italian shipyard assigned propulsion indicated thick nautical enlisted broken stricken millimeter conning armed trials turrets shaft launched flagship gun twin propeller fired pounder ironclads cruiser caliber submerged load bow driving engines sisters quick powered casemates armour coal forward supplied maximum turbines outbreak draft rounds mounts plates wrought superstructure inches broadside expansion loading iron russian reduced battleship provided secondary hotchkiss class maneuvers fore transverse ammunition backed austro barbettes calibre</t>
+          <t>['tons', 'beam', 'deck', 'consisted', 'guns', 'laid', 'horsepower', 'armor', 'hull', 'boilers', 'displaced', 'steam', 'mounted', 'armament', 'battery']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fur-bearing trout = The fur-bearing trout ( or furry trout ) is a fictional creature purportedly found in North America and Iceland . According to tales , the trout has created a thick coat of fur to maintain its body heat . Tales of furry fish date to the 17th-century and later the " shaggy trout " of Iceland . The earliest known American publication dates from a 1929 Montana Wildlife magazine article by J.H. Hicken . A taxidermy furry trout produced by Ross C. Jobe is a specimen at the Royal Museum of Scotland ; it is a trout with white rabbit fur " ingeniously " attached . There are no real examples of any fur-bearing trout species , but two examples of hair-like growths on fish are known . The " cotton mold " , Saprolegnia , can infect fish , which can result in the appearance of fish covered in the white " fur " . A real fish , Mirapinna esau , also known as the " Hairy Fish " , has hair-like outgrowths and wings . = = Commonalities = = Fur-bearing trout are fictional creatures th</t>
+          <t>Tropical Storm Julio ( 2008 ) = Tropical Storm Julio was a tropical storm that made landfall on the southern tip of Baja California Sur in August 2008 . The tenth named storm of the 2008 Pacific hurricane season , it developed from a tropical wave on August 23 off the coast of Mexico . It moved parallel to the coast , reaching peak winds of 50 mph ( 85 km / h ) before moving ashore and weakening . On August 26 it dissipated in the Gulf of California . Julio was the third tropical cyclone to make landfall in the Pacific Ocean basin during the season , after Tropical Storm Alma , which struck Nicaragua in May , and Tropical Depression Five-E , which moved ashore along southwestern Mexico in July . The storm brought locally heavy rainfall to southern Baja California , killing one person and leaving several towns isolated . Moisture from Julio reached Arizona , producing thunderstorms , including one which damaged ten small planes in Chandler . = = Meteorological history = = On August 20 ,</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Aaron Loup = Aaron Christopher Loup ( born December 19 , 1987 ) is an American professional baseball relief pitcher for the Toronto Blue Jays of Major League Baseball . He stands 6 feet 0 inches ( 183 cm ) and weighs 210 pounds ( 95 kg ) . Born in Raceland , Louisiana , Loup played baseball at Hahnville High School and Tulane University , where he led his teams to several state playoff appearances and recorded a five-hit shutout . He was drafted by the Blue Jays out of Tulane in the ninth round of the 2009 draft . After playing for three years with minor-league affiliates for the Toronto Blue Jays and even being chosen for the 2012 Eastern League All-Star Game , Loup was called up to the Blue Jays as a replacement for Luis Pérez and retired all six batters he faced . He was later voted the 2012 Toronto Blue Jays Rookie of the Year by the Toronto chapter of the Baseball Writers Association of America ( BBWAA ) . Loup pitched 11 ⁄ 3 innings on Opening Day in 2013 , and would go on to win</t>
+          <t>Mark Steel 's in Town = Mark Steel 's in Town is a stand-up comedy show on BBC Radio 4 , co-written and performed by Mark Steel . The series , that was first broadcast on 18 March 2009 , is recorded in various small towns in the United Kingdom . Each episode is tailored to the town it is recorded in and the show is performed in front of a local audience . The first series of six episodes was recorded in five towns in England ( Skipton , Boston , Lewes , Walsall and the Isle of Portland ) and one in Wales ( Merthyr Tydfil ) . The second series , also of six episodes and first broadcast on 7 April 2010 , was performed in four towns in England ( Dartford , Wilmslow , Penzance and Gateshead ) and two in Scotland ( Dumfries and Kirkwall ) . The third series of six episodes , broadcast between December 2011 and January 2012 , visited four towns in England ( Berwick-upon-Tweed , Basingstoke , Wigan and Bungay ) , one in Wales ( Holyhead ) and one on the Isle of Man ( Douglas ) . A special epi</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tropical Storm Bret ( 2011 ) = Tropical Storm Bret was the second named storm of the 2011 Atlantic hurricane season . Bret formed along the southwestern periphery of a weather front north of the Bahamas on July 17 . At first , the storm moved little and gradually strengthened in response to favorable upper-level conditions , reaching peak sustained winds of 70 mph ( 110 km / h ) . Steering currents in the area subsequently became better established , and Bret turned toward the northeast only to encounter a substantial increase in vertical wind shear . Despite the shear , the storm maintained a well-defined wind circulation for several days , with intermittent bursts of thunderstorms near its center . By July 22 , Bret had been devoid of strong thunderstorm activity for several hours , prompting the National Hurricane Center to discontinue public advisories when it was located about 375 miles ( 605 km ) north of Bermuda . Since Bret remained over the open Atlantic for most of its existe</t>
+          <t>Fursuit = Fursuits are animal costumes . Fursuits can be worn for personal enjoyment , work or charity . The term " fursuit " is believed to have been coined in 1993 by Robert King and is usually used to describe custom-made animal costumes owned and worn by cosplayers or members of the furry fandom . Unlike mascot suits , which are usually affiliated with a team or organization , fursuits represent a stand-alone character . Fursuiters may adopt another personality while in costume for the purpose of performance . Fursuits are typically sold online by commission or auction , but can also be sold at conventions . = = Creation and construction = = Most fursuits are created by specialized online businesses if they are not self-made . Workmanship quality varies widely depending on the cost of the suit and skill of the maker . A fursuit may cost more than a thousand dollars . Many suits include special padding or undersuits to give the character its desired shape ( this is especially presen</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Borodino-class battlecruiser = The Borodino-class battlecruisers ( Russian : Линейные крейсера типа « Измаил » ) were a group of four battlecruisers ordered by the Imperial Russian Navy before World War I. Also referred to as the Izmail class , they were laid down in December 1912 at Saint Petersburg for service with the Baltic Fleet . Construction of the ships was delayed as many domestic factories were overloaded with orders and some components had to be ordered from abroad . The start of World War I slowed their construction still further as the imported components were often not delivered and domestic production was diverted into areas more immediately useful for the war effort . Three of the four ships were launched in 1915 and the fourth in 1916 . Work on the gun turrets lagged , and it became evident that Russian industry would not be able to complete the ships during the war . The Russian Revolution of 1917 put a stop to their construction , which was never resumed . Although s</t>
+          <t>K-179 ( Kansas highway ) = K-179 is an 11.588-mile-long ( 18.649 km ) state highway in Harper County , Kansas . It runs from Oklahoma State Highway 132 ( SH-132 ) the Oklahoma state line north to the city of Anthony , where it ends at K-44 . The route was designated around 1956 , and is not part of the National Highway System . = = Route description = = Just north of Manchester , Oklahoma , K-179 begins running west along the Oklahoma state line as a continuation of SH-132 . The route then turns due north and continues through flat farm fields . A series of curves take the highway slightly to the northeast before it enters the city of Anthony , where it becomes known as Jennings Avenue . Just more than 0.5 miles ( 0.80 km ) north of the Anthony city limits , K-179 meets its northern terminus at an intersection with K-44 , also known as Main Street . K-179 is maintained by the Kansas Department of Transportation ( KDOT ) . Every year , KDOT measures traffic on each of its state highways</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">SMS Gazelle = SMS Gazelle was the lead ship of the ten-vessel light cruiser Gazelle class , built by the Imperial German Navy . She was built by the Germaniawerft shipyard in Kiel , laid down in 1897 , launched in March 1898 , and commissioned into the High Seas Fleet in June 1901 . Armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and two 45 cm ( 18 in ) torpedo tubes , Gazelle was capable of a top speed of 19.5 knots ( 36.1 km / h ; 22.4 mph ) . Initially assigned to overseas service , Gazelle participated in the Venezuelan crisis of 1902 – 03 . She returned to German waters in 1904 , and served with the fleet until 1914 . She was employed as a coastal defense ship after the outbreak of World War I in August 1914 . She served in this role until the night of 25 – 26 January 1916 , when she struck a mine off Cape Arkona . The Navy deemed Gazelle not worth repairing and reduced her to a mine storage hulk , a role she retained through the end of the war . In August 1920 , she was </t>
+          <t>HMS Agincourt ( 1865 ) = HMS Agincourt was a Minotaur-class armoured frigate built for the Royal Navy during the 1860s . She spent most of her career as the flagship of the Channel Fleet 's second-in-command . During the Russo-Turkish War of 1877 – 78 , she was one of the ironclads sent to Constantinople to forestall a Russian occupation of the Ottoman capital . Agincourt participated in Queen Victoria 's Golden Jubilee Fleet Review in 1887 . The ship was placed in reserve two years later and served as a training ship from 1893 to 1909 . That year she was converted into a coal hulk and renamed as C.109. Agincourt served at Sheerness until sold for scrap in 1960 . = = Design and description = = The three Minotaur-class armoured frigates were essentially enlarged versions of the ironclad HMS Achilles with heavier armament , armour , and more powerful engines . They retained the broadside ironclad layout of their predecessor , but their sides were fully armoured to protect the 50 guns the</t>
         </is>
       </c>
     </row>
@@ -651,32 +651,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>different called given form example point elements real use possible formula sequence particular result simple similar method function known physical results defined terms non problem theory important equivalent functions instance shown uses related constant space set value applications linear types zero complex basic field values light figure energy mechanical matrix systems plane standard properties corresponding case triangle gives mathematical direction methods group equation numbers code allows element definition continuous independent structure type frequency fact useful means map components analysis sense finite dimensional ways normal change equal infinite information certain order filter rules surface electrical ratio image step mechanics quantum cell</t>
+          <t>['different', 'called', 'given', 'form', 'example', 'point', 'elements', 'real', 'use', 'possible', 'formula', 'sequence', 'particular', 'result', 'simple']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Take It Off ( Kesha song ) = " Take It Off " is a song by American recording artist and songwriter Kesha , from her debut album , Animal . It was written by Kesha Sebert , Lukasz Gottwald and Claude Kelly and it was produced by Dr. Luke with vocal editing done by Emily Wright . It was released as the fourth and final single from the album on July 13 , 2010 . " Take It Off " ' s initial writing consisted of Kesha attending a drag show and becoming turned on by drag queens taking their clothing off . The song is an upbeat song that uses heavy amounts of auto tune and utilizes an electro infused beat . Due to strong digital sales from the release of Animal , the song charted in the United States , the United Kingdom and Canada before being announced as a single . After being released as a single the song reached the top ten in Canada , Australia and the United States . With the song reaching the top-ten in the United States , Kesha became only the eleventh artist in history to amass four </t>
+          <t>Hurricane Otto ( 2010 ) = Hurricane Otto produced days of torrential rain over much of the northeastern Caribbean in October 2010 . Otto originated as a subtropical cyclone lingering north of Puerto Rico on October 6 , and transitioned into a tropical storm the next day , the fifteenth of the 2010 hurricane season . Accelerating toward the northeast , Otto strengthened into a Category 1 hurricane on the Saffir – Simpson scale on October 8 , attaining peak winds of 85 mph ( 140 km / h ) . The storm began weakening due to incompatible surroundings and became extratropical west of the Azores on October 10 . Otto was the first Atlantic tropical cyclone on record to transition from a subtropical storm since Tropical Storm Laura in 2008 . Drifting near the northeastern Caribbean for several days , Otto and its precursor disturbance brought prolonged rainfall to the Leeward Islands , the Virgin Islands , and Puerto Rico , triggering widespread flooding and numerous mudslides . Damage from the</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Benjamin Hardin Helm = Benjamin Hardin Helm ( June 2 , 1831 – September 21 , 1863 ) was a Kentucky politician , attorney , Confederate brigadier general , and a brother-in-law of Abraham Lincoln . He was also the son of Kentucky Governor John L. Helm . Helm was born in Bardstown , Kentucky . He attended the Kentucky Military Institute and the West Point Military Academy and then went to study law at the University of Louisville and Harvard University . He served as a state legislator and the state 's attorney in Kentucky . He also served as the assistant inspector-general for the Kentucky state guard . Helm was offered the position of Union Army paymaster by his brother-in-law , President Abraham Lincoln , a position which he declined . Helm felt it was an honor to serve in the Confederate States Army , where he was initially a colonel and later promoted to brigadier general . Helm commanded the 1st Kentucky Brigade more commonly known as The Orphan Brigade . He died on the battlefield</t>
+          <t>Imperial War Museum = Imperial War Museums ( IWM ) is a British national museum organisation with branches at five locations in England , three of which are in London . Founded as the Imperial War Museum in 1917 , the museum was intended to record the civil and military war effort and sacrifice of Britain and its Empire during the First World War . The museum 's remit has since expanded to include all conflicts in which British or Commonwealth forces have been involved since 1914 . As of 2012 , the museum aims ' to provide for , and to encourage , the study and understanding of the history of modern war and " wartime experience " ' . Originally housed in the Crystal Palace at Sydenham Hill , the museum opened to the public in 1920 . In 1924 the museum moved to space in the Imperial Institute in South Kensington , and finally in 1936 the museum acquired a permanent home which was previously the Bethlem Royal Hospital in Southwark . The outbreak of the Second World War saw the museum exp</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Group 12 element = Group 12 , by modern IUPAC numbering , is a group of chemical elements in the periodic table . It includes zinc ( Zn ) , cadmium ( Cd ) and mercury ( Hg ) . The further inclusion of copernicium ( Cn ) in group 12 is supported by recent experiments on individual copernicium atoms . Group 12 is also known as the volatile metals , although this can also more generally refer to any metal ( which need not be in group 12 ) that has high volatility , such as polonium or flerovium . Formerly this group was named IIB ( pronounced as " group two B " , as the " II " is a Roman numeral ) by CAS and old IUPAC system . The three group 12 elements that occur naturally are zinc , cadmium and mercury . They are all widely used in electric and electronic applications , as well as in various alloys . The first two members of the group share similar properties as they are solid metals under standard conditions . Mercury is the only metal that is a liquid at room temperature . While zinc</t>
+          <t>Penrose tiling = A Penrose tiling is an example of non-periodic tiling generated by an aperiodic set of prototiles . Penrose tilings are named after mathematician and physicist Roger Penrose , who investigated these sets in the 1970s . The aperiodicity of prototiles implies that a shifted copy of a tiling will never match the original . A Penrose tiling may be constructed so as to exhibit both reflection symmetry and fivefold rotational symmetry , as in the diagram at the right . A Penrose tiling has many remarkable properties , most notably : It is non-periodic , which means that it lacks any translational symmetry . It is self-similar , so the same patterns occur at larger and larger scales . Thus , the tiling can be obtained through " inflation " ( or " deflation " ) and any finite patch from the tiling occurs infinitely many times . It is a quasicrystal : implemented as a physical structure a Penrose tiling will produce Bragg diffraction and its diffractogram reveals both the fivef</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Primary line constants = The primary line constants are parameters that describe the characteristics of conductive transmission lines , such as pairs of copper wires , in terms of the physical electrical properties of the line . The primary line constants are only relevant to such lines and are to be contrasted with the secondary line constants , which can be derived from them , and are more generally applicable . The secondary line constants can be used , for instance , to compare the characteristics of a waveguide to a copper line , whereas the primary constants have no meaning for a waveguide . The constants are conductor resistance and inductance , and insulator capacitance and conductance , which are by convention given the symbols R , L , C , and G respectively . The constants are enumerated in terms of per unit length . The circuit representation of these elements requires a distributed element model and consequently calculus must be used to analyse the circuit . The secondary c</t>
+          <t>Alvin M. Weinberg = Alvin Martin Weinberg ( April 20 , 1915 – October 18 , 2006 ) was an American nuclear physicist who was the administrator at Oak Ridge National Laboratory ( ORNL ) during and after the Manhattan Project . He came to Oak Ridge , Tennessee , in 1945 and remained there until his death in 2006 . He was the first to use the term " Faustian bargain " to describe nuclear energy . A graduate of the University of Chicago , which awarded him his doctorate in mathematical biophysics in 1939 , Weinberg joined the Manhattan Project 's Metallurgical Laboratory in September 1941 . The following year he became part of Eugene Wigner 's Theoretical Group , whose task was to design the nuclear reactors that would convert uranium into plutonium . Weinberg replaced Wigner as Director of Research at ORNL in 1948 , and became director of the laboratory in 1955 . Under his direction it worked on the Aircraft Nuclear Propulsion program , and pioneered many innovative reactor designs , inclu</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Princess Theatre ( Edmonton ) = The Princess Theatre is a two-screen art-house cinema located at 10337 Whyte Avenue in Edmonton ’ s historic Old Strathcona neighbourhood . The building was designed by prominent Edmonton architects Wilson and Herrald , a firm responsible for the design of many other Edmonton heritage sites . It became Edmonton 's oldest surviving theatre after the demolition of the Gem Theatre in 2006 . The building currently houses the main 400-seat theatre as well as the 100-seat Princess II , located in the basement . It was originally known as the McKernan Block , after John W. McKernan , the building 's original financier , owner , and manager . McKernan was already a recognized theatre operator having previously run two other south side theatres before the Princess : the south side Gem and the South Side Bijou . Only the Princess was to survive the collapse of Strathcona ’ s building boom in 1913 . The building and the theatre within has changed ownership several </t>
+          <t>Brachytherapy = Brachytherapy is a form of radiotherapy where a sealed radiation source is placed inside or next to the area requiring treatment . Brachytherapy is commonly used as an effective treatment for cervical , prostate , breast , and skin cancer and can also be used to treat tumours in many other body sites . Treatment results have demonstrated that the cancer cure rates of brachytherapy are either comparable to surgery and EBRT or are improved when used in combination with these techniques . Brachytherapy can be used alone or in combination with other therapies such as surgery , external beam radiotherapy ( EBRT ) and chemotherapy . Brachytherapy contrasts with unsealed source radiotherapy in which a therapeutic radionuclide ( radioisotope ) is injected into the body to chemically localize to the tissue requiring destruction . It also contrasts to EBRT , in which high-energy x-rays ( or occasionally gamma-rays from a radioisotope like cobalt-60 ) are directed at the tumour fr</t>
         </is>
       </c>
     </row>
@@ -686,32 +686,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>war american later wrote years began men time british land united_states known general early received including southern day returned state military lincoln new_york near governor family continued led march sent north south town command small president took hamilton major came gave battle new left large died massachusetts july arnold texas fort remained troops washington arrived called soldiers went slavery expedition included ordered settlers colonial end man city government named officers year house slaves new_england death miles days jefferson june navy life white congress virginia army return grant spanish area boston great confederate people slave commander following attack little served moved</t>
+          <t>['war', 'american', 'later', 'wrote', 'years', 'began', 'men', 'time', 'british', 'land', 'united_states', 'known', 'general', 'early', 'received']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>History of Singapore = The written history of Singapore dates back to the third century . Later , the Kingdom of Singapura rose in importance during the 14th century under the rule of Sultan Iskandar Shah and Singapore became an important port . Until it was invaded by the Majapahit in 1398 . It then came under the Malacca Sultanate and then the Portuguese , then rapidly becoming a major port city . During World War II , Singapore was conquered and occupied by the Japanese Empire from 1942 to 1945 . When the war ended , Singapore reverted to British control , with increasing levels of self-government being granted , culminating in Singapore 's merger with the Federation of Malaya to form Malaysia in 1963 . But social unrest and disputes between Singapore 's ruling People 's Action Party and Malaysia 's Alliance Party resulted in Singapore 's separation from Malaysia . Singapore became an independent republic on August 9 , 1965 . Facing severe unemployment and a housing crisis , Singapo</t>
+          <t>Battle of Carillon = The Battle of Carillon , also known as the 1758 Battle of Ticonderoga , was fought on July 8 , 1758 , during the French and Indian War ( which was part of the global Seven Years ' War ) . It was fought near Fort Carillon ( now known as Fort Ticonderoga ) on the shore of Lake Champlain in the frontier area between the British colony of New York and the French colony of New France . In the battle , which took place primarily on a rise about three-quarters of a mile ( one km ) from the fort itself , a French army of about 3,600 men under General Louis-Joseph de Montcalm and the Chevalier de Levis decisively defeated an overwhelmingly numerically superior force of British troops under General James Abercrombie , which frontally assaulted an entrenched French position without using field artillery , a lack that left the British and its allies vulnerable and allowed the French to win a decisive victory . The battle was the bloodiest of the war , with over 3,000 casualtie</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Jiloca ( river ) = The Jiloca ( Spanish pronunciation : [ xiˈloka ] ) is a river in Aragón , Spain , a tributary of the river Jalón , and part of the watershed of the Ebro basin . The course of the river runs through the provinces of Teruel and Zaragoza . It has a length of 126 kilometres ( 78 mi ) and an average flow rate of 2.1 cubic metres per second ( 74 cu ft / s ) , although this varies between the seasons . The river flows in a generally north easterly direction from its source near Monreal del Campo . The valley was an historic route between the Meseta Central and the Mediterranean coast . Roman bridges remain in many pueblos and remains of watermills can be seen . The water is generally of good quality and supports a range of wildlife . Cleaning works by the regional government have been criticised by environmental organisations who claim that the ecology has been damaged . The watershed covers an area of 2,957 square kilometres ( 1,142 sq mi ) . = = Course = = The source is d</t>
+          <t>Eduard von Capelle = Admiral Eduard von Capelle ( 10 October 1855 – 23 February 1931 ) was a German Imperial Navy officer from Celle . He served in the navy from 1872 until his retirement in October , 1918 . During his career , Capelle served in the Reichsmarineamt ( Imperial Navy Office ) , where he was primarily responsible for writing the Fleet Laws that funded the expansion of the High Seas Fleet . By the time he retired , Capelle had risen to the rank of admiral , and had served at the post of state secretary for the Reichsmarineamt . From this post , he oversaw the German naval war during the latter three years of World War I. Capelle retired to Wiesbaden , where he died on 23 February 1931 . = = Early career = = Eduard Capelle was born on 10 October 1855 , in Celle , in what was then the Kingdom of Hanover . His father , Eduard ( 1832 – 1897 ) , was a factory owner , and his mother was Emilie Kraus ( 1831 – 1903 ) ; the younger Eduard had a brother , Hans ( 1864 – 1948 ) , a phy</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Humphrey Atherton = Major-General Humphrey Atherton , ( ca.1608 – September 16 , 1661 ) an early settler of Dorchester , Massachusetts , held the highest military rank in colonial New England . He first appeared in the records of Dorchester on March 18 , 1637 and made freeman May 2 , 1638 . He became a representative in the General Court in 1638 and 1639 – 41 . In 1653 , he was Speaker of the House , representing Springfield , Massachusetts . He was chosen assistant governor , a member of the lower house of the General Court who also served as magistrate in the judiciary of colonial government , in 1654 , and remained as such until his death . " He was a member of the Ancient and Honorable Artillery Company of Massachusetts and held the ranks of lieutenant and captain for several years before rising to the rank of major-general . He also organized the first militia in Massachusetts . It is unclear where and when Atherton was born . It is presumed he came from Lancashire , England . He </t>
+          <t>Thomas Brassey = Thomas Brassey ( 7 November 1805 – 8 December 1870 ) was an English civil engineering contractor and manufacturer of building materials who was responsible for building much of the world 's railways in the 19th century . By 1847 , he had built about one-third of the railways in Britain , and by time of his death in 1870 he had built one in every twenty miles of railway in the world . This included three-quarters of the lines in France , major lines in many other European countries and in Canada , Australia , South America and India . He also built the structures associated with those railways , including docks , bridges , viaducts , stations , tunnels and drainage works . As well as railway engineering , Brassey was active in the development of steamships , mines , locomotive factories , marine telegraphy , and water supply and sewage systems . He built part of the London sewerage system , still in operation today , and was a major shareholder in Brunel 's The Great Ea</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Purr by Katy Perry = Purr by Katy Perry is a fragrance created by American singer Katy Perry and Gigantic Parfums . Katy 's love for cats and kittens influenced both her decision to create the perfume and its design , although further inspiration for the bottle 's design came from other perfume products worldwide . Purr features a variety of scents , including citrus fruits . Released in November 2010 , it is available in a purple cat-shaped bottle . Purr is available in 1.7 and 3.4 fluid ounce bottles , with a retail price in the US of $ 35.00 to $ 45.00 for the smaller size and $ 65.00 for the larger . = = Conception = = Katy Perry chose to release her own signature fragrance , Purr , to add a personal touch and compete with other celebrities ' perfumes ; she cited Beyoncé and Kim Kardashian as examples . Having teamed up with Gigantic Parfums , she was actively involved in the development of her fragrance . She mentioned in an interview that she created the product because she loves</t>
+          <t>Frederick Russell Burnham = Frederick Russell Burnham DSO ( May 11 , 1861 – September 1 , 1947 ) was an American scout and world-traveling adventurer . He is known for his service to the British South Africa Company and to the British Army in colonial Africa , and for teaching woodcraft to Robert Baden-Powell in Rhodesia . He helped inspire the founding of the international Scouting Movement . Burnham was born on a Lakota Sioux Indian reservation in Minnesota where he learned the ways of American Indians as a boy . By the age of 14 , he was supporting himself in California , while also learning scouting from some of the last of the cowboys and frontiersmen of the American Southwest . Burnham had little formal education , never finishing high school . After moving to the Arizona Territory in the early 1880s , he was drawn into the Pleasant Valley War , a feud between families of ranchers and sheepherders . He escaped and later worked as a civilian tracker for the United States Army in t</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Agneepath ( 2012 film ) = Agneepath ( English : The Path of Fire ) is a 2012 Indian action drama film produced by Hiroo Yash Johar and Karan Johar under the banner of Dharma Productions . It is a retelling of the 1990 film of the same name and was directed by Johar 's former assistant Karan Malhotra . The screenplay was written by Malhotra along with Ila Dutta Bedi . Johar pays tribute to his father , Yash Johar , the producer of the original , through the film . The music of the film was composed by Ajay-Atul , with lyrics written by Amitabh Bhattacharya . Though publicised as a remake , the film borrows only the basic plot of the original , while making the characters and incidents completely different . The film 's title was taken from a poem of the same name by Harivansh Rai Bachchan , which forms a thematic link through the film , both literally and metaphorically . Hrithik Roshan plays the lead role of Vijay Deenanath Chauhan and Sanjay Dutt plays the role of the antagonist Kanch</t>
+          <t xml:space="preserve">A. P. J. Abdul Kalam = Avul Pakir Jainulabdeen " A. P. J. " Abdul Kalam ( / ˈæbdʊl kəˈlɑːm / ; 15 October 1931 – 27 July 2015 ) was the 11th President of India from 2002 to 2007 . A career scientist turned politician , Kalam was born and raised in Rameswaram , Tamil Nadu , and studied physics and aerospace engineering . He spent the next four decades as a scientist and science administrator , mainly at the Defence Research and Development Organisation ( DRDO ) and Indian Space Research Organisation ( ISRO ) and was intimately involved in India 's civilian space program and military missile development efforts . He thus came to be known as the Missile Man of India for his work on the development of ballistic missile and launch vehicle technology . He also played a pivotal organizational , technical , and political role in India 's Pokhran-II nuclear tests in 1998 , the first since the original nuclear test by India in 1974 . Kalam was elected as the 11th President of India in 2002 with </t>
         </is>
       </c>
     </row>
@@ -721,32 +721,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>game released games player music version original series release story characters players main character japan based development soundtrack tracks hero theme playing japanese published new guitar plot enix playstation gaming created video gameplay versions features included called scenario anime sold localization received previous songs mode composed final_fantasy playable persona tales developed battle square_enix famitsu praised titled manga multiplayer content dragon online best world use rpg developers include arranged ign xbox create downloadable ending console portable different abilities arrangements controller nintendo volumes soundtracks hearts fantasy gamespot items wii protagonist featured difficulty ps2 similar multiple mortal cutscenes fan key containing additional reviewers</t>
+          <t>['game', 'released', 'games', 'player', 'music', 'version', 'original', 'series', 'release', 'story', 'characters', 'players', 'main', 'character', 'japan']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Phillips Exeter Academy Library = The Phillips Exeter Academy Library in Exeter , New Hampshire , U.S. , with 160,000 volumes on nine levels and a shelf capacity of 250,000 volumes , is the largest secondary school library in the world . It is part of the Phillips Exeter Academy , an independent boarding school . When it became clear in the 1950s that the library had outgrown its existing building , the school initially hired an architect who proposed a traditional design for the new building . Deciding instead to construct a library with a contemporary design , the school gave the commission to Louis Kahn in 1965 . In 1997 the library received the Twenty-five Year Award from the American Institute of Architects , an award that recognizes architecture of enduring significance that is given to no more than one building per year . Kahn structured the library in three concentric square rings . The outer ring , which is built of load-bearing brick , includes all four exterior walls and the</t>
+          <t xml:space="preserve">Adventure Time ( season 4 ) = The fourth season of the American animated television series Adventure Time , created by Pendleton Ward , originally aired on Cartoon Network in the United States . The series is based on a short produced for Frederator 's Nicktoons Network animation incubator series Random ! Cartoons . The season debuted on April 2 , 2012 , and the season finale was aired on October 22 , 2012 . The season follows the adventures of Finn , a human boy , and his best friend and adoptive brother Jake , a dog with magical powers to change shape and grow and shrink at will . Finn and Jake live in the post-apocalyptic Land of Ooo . Along the way , they interact with the other main characters of the show : Princess Bubblegum , The Ice King , and Marceline the Vampire Queen . The first episode of the season , " Hot to the Touch " was watched by 2.655 million viewers ; this marked a slight decrease in viewers watching Cartoon Network when compared to the previous season 's debut . </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Tayutama : Kiss on my Deity = Tayutama : Kiss on my Deity ( タユタマ -Kiss on my Deity- ) is a Japanese visual novel developed by Lump of Sugar . It was first released as an adult game for Windows PCs on July 11 , 2008 in both limited and regular editions , and was later followed by an Xbox 360 version . Tayutama is Lump of Sugar 's third title after their previous titles Nursery Rhyme and Itsuka , Todoku , Ano Sora ni . The story centers on the male protagonist Yuri Mito , a high school student who is the son of a family that presides over the local Shinto shrine . As Yuri performs a ritual to transfer a relic that hosts a fictional , supernatural race called Tayutai , he and his friends accidentally summon a goddess , who incarnates as a young girl . The gameplay in Tayutama mainly consists of reading a text-based , branching plot line with multiple endings , and offers pre-determined scenarios and courses of interaction based on the player 's decisions . The game received two awards fro</t>
+          <t>Bachata Number 1 's , Vol . 3 = Bachata # 1 's , Vol . 3 is a compilation album released by Machete Music on March 30 , 2010 . The album includes tracks recorded by several artists from the bachata genre , such as Aventura , Héctor Acosta , Xtreme , Ivy Queen , Grupo Rush , Andy Andy , Carlos &amp; Alejandra , and Marcy Place . It also features select bachata versions of songs by reggaetón and Latin pop artists including R.K.M &amp; Ken-Y , Alejandro Fernández , Luis Fonsi , and Cristian Castro . Upon release , the album peaked at number forty-one on the Billboard Latin Albums chart and number four on the Billboard Tropical Albums chart . It became the twentieth best-selling Tropical Album of 2010 . Several songs included on the album were released as singles from their respective parent albums including the opening " El Perdedor " by Aventura , " No Me Doy Por Vencido " by Luis Fonsi , and " Dime " by Ivy Queen . The fourth volume in the Bachata # 1 's series was released in 2011 . = = Backgr</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ultima Underworld II : Labyrinth of Worlds = Ultima Underworld II : Labyrinth of Worlds is a 1993 first-person role-playing video game developed by Looking Glass Technologies and published by Origin Systems . As the sequel to Ultima Underworld : The Stygian Abyss , the game is set in the Ultima fantasy universe . Players assume the role of the Avatar — the protagonist of the Ultima series — and adventure through multiple dimensions while seeking to prevent the evil Guardian from achieving world domination . Progression is largely nonlinear and the game allows for emergent gameplay . Ultima Underworld II began production in April 1992 , shortly after the completion of Ultima Underworld ; and it was developed in nine months . The team sought to improve upon the foundation laid by the game 's predecessor , particularly by increasing the size and interactivity of the game world . The team reused and improved the first game 's engine . Development was impeded by insufficient staffing and ex</t>
+          <t>Knife Edge Two Piece 1962 – 65 = Knife Edge Two Piece 1962 – 65 is an abstract bronze sculpture by Henry Moore . It is one of Moore 's earliest sculptures in two pieces , a mode that he started to adopt in 1959 . Its form was inspired by the shape of a bone fragment . Moore created the sculpture from an edition of 10 working models in 1962 ; these working models are now in public collections . Moore created four full-size casts between 1962-1965 , with one retained by him . The three casts are on public display on College Green in Westminster , London , Queen Elizabeth Park in Vancouver , and the garden at Kykuit , the house of the Rockefeller family in Tarrytown , New York . Moore 's own cast is on display at his former studio and estate , ' Hoglands ' in Perry Green , Hertfordshire in southern England . A similar work , Mirror Knife Edge 1977 ( or Knife Edge Mirror Two Piece ) , is displayed at the entrance to I. M. Pei 's east wing of the National Gallery of Art in Washington , D.C.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Man Enters the Cosmos = Man Enters the Cosmos is a cast bronze sculpture by Henry Moore located on the Lake Michigan lakefront outside the Adler Planetarium in the Museum Campus area of downtown Chicago in Cook County , Illinois , United States . The planetarium , which is both a National Historic Landmark and listed on the National Register of Historic Places , is located in the Near South Side community area of Chicago . Moore 's sculpture is a functional bowstring equatorial sundial created in 1980 measuring approximately 13 feet ( 4.0 m ) . The sundial was formerly located slightly further south at the steps of the main entry plaza to the Planetarium , but it now sits directly on the lakefront . The work is a later copy of a composition first created in the 1960s for the offices of The Times newspaper at Printing House Square in London , and according to the Henry Moore Foundation is titled Sundial 1965-66 . = = Details = = The sundial has two plaques on its base . The one on the l</t>
+          <t>Samuel Turell Armstrong = Samuel Turell Armstrong ( April 29 , 1784 – March 26 , 1850 ) was a U.S. political figure . Born in 1784 in Dorchester , Massachusetts , he was a printer and bookseller in Boston , specializing in religious materials . Among his works were an early stereotype edition of Scott 's Family Bible , which was very popular , and The Panoplist , a religious magazine devoted to missionary interests . Armstrong began to withdraw from the printing business in 1825 , and focused instead on politics . He was active in Boston politics during the 1820s , twice winning a seat in the Massachusetts General Court ( state legislature ) . In 1833 he was elected Lieutenant Governor of Massachusetts as a Whig , and served three consecutive annual terms . For most of the last term he was Acting Governor after Governor John Davis resigned to take a seat in the United States Senate . He lost a bid to be elected governor in his own right in 1836 , but was elected Mayor of Boston , a pos</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Angry Birds ( video game ) = Angry Birds is a puzzle video game developed by Finnish computer game developer Rovio Mobile that started the Angry Birds franchise . Inspired primarily by a sketch of stylized wingless birds , the game was first released for iOS and Maemo in December 2009 . Since that time , over 12 million copies of the game have been purchased from the iOS App Store , which has prompted the company to design versions for other touchscreen-based smartphones , most notably those using the Android , Symbian , Windows Phone and BlackBerry 10 operating systems . The series has since expanded to include titles for dedicated video game consoles and for PCs . A sequel named Angry Birds 2 was released on July 30 , 2015,In the game , players use a slingshot to launch birds at pigs stationed in or around various structures with the goal of destroying all the pigs on the playing field . As players advance through the game new types of birds become available , some with special abili</t>
+          <t>Tomorrow 's Modern Boxes = Tomorrow 's Modern Boxes is the second solo album by Thom Yorke of the English alternative rock band Radiohead , released on 26 September 2014 . It was produced by Radiohead producer Nigel Godrich , with artwork by Radiohead artist Stanley Donwood . The album blends Yorke 's vocals and piano playing with electronic beats and textures . Yorke first released Tomorrow 's Modern Boxes independently via a paid-for BitTorrent bundle . He and Godrich expressed their wish to find " an effective way of handing some control of internet commerce back to people who are creating the work " . The album was downloaded over a million times within six days of release , and became the most-downloaded legal torrent of 2014 ; by February 2015 , it had been downloaded over 4.5 million times . A vinyl edition was also sold from the official site , and in August 2015 a CD edition was released in Japan by Hostess Entertainment . On 26 December 2014 , Yorke released Tomorrow 's Moder</t>
         </is>
       </c>
     </row>
@@ -756,32 +756,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>tropical storm cyclone area cyclones near level wind low formed depression miles winds water west sea activity ice high southwest northwest system storms south volcano peak typhoon coast mph disturbance shear trough surface cold southeast eruption weather feet form circulation temperature day moved upper days formation caused hurricane convection ocean northeast rainfall flows land august developed monsoon volcanic mountain east lava ridge significant air turned subtropical warm atmosphere moving intensity westward july basin dissipated pressure cloud center region weakened lower september severe snow clouds southern strong temperatures active pacific areas zone extratropical large island organized metres mid waters eastern lake</t>
+          <t>['tropical', 'storm', 'cyclone', 'area', 'cyclones', 'near', 'level', 'wind', 'low', 'formed', 'depression', 'miles', 'winds', 'water', 'west']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Matagorda Bay = Matagorda Bay ( / ˈmætəˈɡɔərdə / ) is a large Gulf of Mexico estuary bay on the Texas coast , lying in Calhoun and Matagorda counties and located approximately 80 miles ( 130 km ) northeast of Corpus Christi , 143 miles ( 230 km ) east-southeast of San Antonio , 108 miles ( 174 km ) south-southwest of Houston , and 167 miles ( 269 km ) south-southeast of Austin . It is separated from the Gulf of Mexico by Matagorda Peninsula and serves as the mouth of numerous streams , most notably the Lavaca and Colorado Rivers . The major Texas seaport of Port Lavaca is located on the system 's northwestern extension of Lavaca Bay . The city of Palacios is found on northeastern extension of Tres Palacios Bay , and Port O 'Connor is located on the southwestern tip of the main bay 's shore . The ghost town of Indianola , which was a major port before it was destroyed by two hurricanes in the late 19th Century , is also found on the bay . The bay 's shore , especially near the Colorado </t>
+          <t xml:space="preserve">1987 Gulf Coast tropical storm = The 1987 Gulf Coast tropical storm caused flooding along the Gulf Coast of the United States . The second tropical cyclone and first tropical storm of the 1987 Atlantic hurricane season , it originated from a tropical wave in the Gulf of Mexico , southeast of Texas , on August 9 . Initially a tropical depression , the cyclone moved north-northwestward and slightly intensified into a tropical storm later that day . By August 10 , it made landfall between Galveston and Beaumont . The system weakened after moving inland and turned towards the east and later southeast . Briefly reemerging over the Gulf on August 15 , the depression moved onshore a second time in Florida , before dissipating over eastern Georgia on August 17 . Due to the relatively weak nature of the system , it caused relatively little damage . However , the system dropped heavy rainfall , peaking at 21.05 inches ( 535 mm ) in southern Mississippi . This resulted in flooding , which forced </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1973 Atlantic hurricane season = The 1973 Atlantic hurricane season was the first season to use the Saffir – Simpson hurricane scale , a scale developed in 1971 by Herbert Saffir and Robert Simpson to rate the intensity of tropical cyclones . The season produced 24 tropical and subtropical cyclones , of which only 8 reached storm intensity , 4 became hurricanes , and only 1 reached major hurricane status . Although more active than the 1972 season , 1973 brought few storms of note . Nearly half of the season 's storms affected land , one of which resulted in severe damage . The season officially began on June 1 , 1973 , and lasted until November 30 , 1973 . These dates conventionally delimit the period of each year when most tropical cyclones form in the Atlantic basin . However , the first system formed on April 18 , more than a month before the official start . Three more depressions formed before June 1 ; however , none attained storm intensity . The first named storm of the year wa</t>
+          <t xml:space="preserve">Till I Die ( Chris Brown song ) = " Till I Die " is a song by American recording artist Chris Brown , featuring American rappers Big Sean and Wiz Khalifa . It was written by Brown , Sean Anderson , Cameron Thomaz , Marcella Araica and Nathaniel " Danja " Hills , while the production was handled by Danja . " Till I Die " was released digitally on April 13 , 2012 , as the third single from Brown 's fifth studio album , Fortune ( 2012 ) . It was sent to rhythmic contemporary radio in the United States on May 1 , 2012 . " Till I Die " is an uptempo hip hop and R &amp; B song that displays elements of electro music and features military drumbeats , R &amp; B synths and " arcade-game blips " . The song contains lyrics about women , smoking weed , partying in the club and living the good life . " Till I Die " garnered positive reviews from music critics , who praised the production and the trio 's verses . Although it was released worldwide , the song only charted in the United States . It peaked at </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Hurricane Hernan ( 2002 ) = Hurricane Hernan was the second of three Category 5 hurricanes during the 2002 Pacific hurricane season . The twelfth tropical cyclone , tenth named storm and sixth hurricane of the season , Hernan originated from a tropical wave that formed in the Atlantic Ocean and crossed to the Pacific Ocean . The wave spawned a low pressure system which organized into a tropical depression on August 30 , a tropical storm on August 31 and a hurricane later that day . Hernan rapidly intensified and reached peak intensity as a Category 5 storm on the Saffir-Simpson Hurricane Scale . Proceeding northwest , it maintained this strength for eight hours , but on September 2 it entered cooler waters and began to weaken . By September 6 it had degenerated into a remnant area of low pressure . Hernan was the second most intense hurricane of the season , and it maintained Category 5 status for the second-longest time of the season , behind Hurricane Kenna . Although Hernan remained</t>
+          <t>Inside No. 9 = Inside No. 9 is a British dark comedy anthology television programme written by Reece Shearsmith and Steve Pemberton and produced by the BBC . The first series was broadcast between 5 February and 12 March 2014 on BBC Two , and a second series aired from 26 March to 29 April 2015 . Each half-hour episode is a self-contained story with new characters and a new setting , and all star at least one ( usually both ) of Pemberton and Shearsmith . Aside from the writers , each episode has a new cast , allowing Inside No. 9 to attract a number of well-known actors . The stories are linked only by the fact that each takes place at a number 9 , whether this is a suburban house , a gothic mansion or a barn . Pemberton and Shearsmith took inspiration for Inside No. 9 from an episode of Psychoville , a previous project , which was filmed in a single room . This episode was , in turn , inspired by Alfred Hitchcock 's Rope . Inside No. 9 was also a reaction to Psychoville , which featu</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Millennium Stadium = The Millennium Stadium ( Welsh : Stadiwm y Mileniwm ) , currently named the Principality Stadium ( Welsh : Stadiwm Principality ) for sponsorship purposes , is the national stadium of Wales , located in Cardiff . It is the home of the Wales national rugby union team and has also staged games of the Wales national football team . Initially built to host the 1999 Rugby World Cup , it has gone on to host many other large-scale events , such as the Tsunami Relief concert , the Super Special Stage of Wales Rally Great Britain , the Speedway Grand Prix of Great Britain and various music concerts . It also hosted six FA Cup finals and several other high profile football fixtures whilst Wembley Stadium was being redeveloped . The stadium is owned by Millennium Stadium plc , a subsidiary company of the Welsh Rugby Union ( WRU ) . The stadium was designed by a team led by architects Bligh Lobb Sports Architecture . WS Atkins were the structural engineers , and the building c</t>
+          <t>Lysurus mokusin = Lysurus mokusin , commonly known as the lantern stinkhorn , the small lizard 's claw , or the ribbed lizard claw , is a saprobic species of fungus in the family Phallaceae . The fruit body consists of a reddish , cylindrical fluted stipe that is capped with several " arms " . The arms can approach or even close in on each other to form a spire . The gleba — an olive-green slimy spore mass — is carried on the outer surface of the arms . The fruit body , which has an odor comparable to " fresh dog feces " , " rotting flesh " , or " sewage " when mature , is edible in its immature " egg " stage . The fungus is native to Asia , and is also found in Australia , Europe and North America , where it is probably an introduced species . It has been used medicinally in China as an ulcer remedy . = = History , taxonomy , and phylogeny = = The species was first described by the Catholic Priest and missionary Pierre-Martial Cibot in the publication Novi Commentarii Academiae Scient</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Tropical Storm Debby ( 1994 ) = Tropical Storm Debby was a weak but costly tropical cyclone that affected the Lesser Antilles in September 1994 . It was the fourth named tropical storm of the 1994 Atlantic hurricane season ; it developed on September 9 east of Barbados . Debby made landfall on Saint Lucia early on September 10 , producing heavy rainfall and tropical storm-force wind gusts . The rains caused flooding and landslides , damaging about half of the island 's banana plantations . Several villages were isolated after roads and bridges were damaged . Damage totaled about $ 103 million ( 1994 USD ) . On nearby Dominica , Debby damaged crops and fisheries . While Debby was crossing Saint Lucia , its strongest thunderstorms were located north and east of the center due to wind shear . A station in Martinique reported hurricane-force winds , and about 20,000 people on the island lost power . After entering the eastern Caribbean Sea , Debby attained peak winds of 70 mph ( 110 km / h</t>
+          <t>Calakmul = Calakmul ( / ˌkɑːlɑːkˈmuːl / ; also Kalakmul and other less frequent variants ) is a Maya archaeological site in the Mexican state of Campeche , deep in the jungles of the greater Petén Basin region . It is 35 kilometres ( 22 mi ) from the Guatemalan border . Calakmul was one of the largest and most powerful ancient cities ever uncovered in the Maya lowlands . Calakmul was a major Maya power within the northern Petén Basin region of the Yucatán Peninsula of southern Mexico . Calakmul administered a large domain marked by the extensive distribution of their emblem glyph of the snake head sign , to be read " Kaan " . Calakmul was the seat of what has been dubbed the Kingdom of the Snake or Snake Kingdom . This Snake Kingdom reigned during most of the Classic period . Calakmul itself is estimated to have had a population of 50,000 people and had governance , at times , over places as far away as 150 kilometers . There are 6,750 ancient structures identified at Calakmul ; the la</t>
         </is>
       </c>
     </row>
@@ -791,32 +791,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>court act public law state rights case government right cases united_states courts decision singapore person held review legal states constitutional required appeal provisions subject article constitution section purpose judges non order free federal justice executive laws process jurisdiction requires members amendment powers apply shall human persons action provision clause information criminal question means judgment common freedom property specifically authority people certain statute purposes argued supreme_court necessary interest judicial applicable report effect provides bill opinion prevent judge limited exercise provided protection view congress power citizens scope passed legislation considered acts provide ensure issued judiciary decisions enacted personal involving actions parliament adopted</t>
+          <t>['court', 'act', 'public', 'law', 'state', 'rights', 'case', 'government', 'right', 'cases', 'united_states', 'courts', 'decision', 'singapore', 'person']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bacon : A Love Story = Bacon : A Love Story , A Salty Survey of Everybody 's Favorite Meat is a 2009 non-fiction book about bacon.Written by American writer Heather Lauer . Lauer started the blog Bacon Unwrapped and a social networking site about bacon in 2005 , after the idea came to her while she was out drinking with her two brothers ; her online success inspired her to write the book , which describes curing and cooking bacon , gives over 20 bacon recipes , and analyzes the impact of bacon on popular culture . The text is interspersed with facts about bacon and bacon-related quips from comedian Jim Gaffigan . The book had a generally positive reception ; The Sacramento Bee called it " entertaining and informational " . The Toronto Star and The Sacramento Bee recommended it as a Father 's Day gift . The Portsmouth Herald and The Arizona Republic highlighted the book on lists of summer reading recommendations . Publishers Weekly wrote that bacon lovers would enjoy the book , but othe</t>
+          <t>Mary Dyer = Mary Dyer , born Marie Barrett ( c . 1611 – 1 June 1660 ) , was an English and colonial American Puritan turned Quaker who was hanged in Boston , Massachusetts Bay Colony , for repeatedly defying a Puritan law banning Quakers from the colony . She is one of the four executed Quakers known as the Boston martyrs . While the place of her birth is not known , she was married in London in 1633 to the milliner William Dyer . Mary and William were Puritans who were interested in reforming the Anglican Church from within , without separating from it . As the English king increased pressure on the Puritans , they left England by the thousands to go to New England in the early 1630s . Mary and William arrived in Boston by 1635 , joining the Boston Church in December of that year . Like most members of Boston 's church , they soon became involved in the Antinomian Controversy , a theological crisis lasting from 1636 to 1638 . Mary and William were strong advocates of Anne Hutchinson a</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>K-104 ( Kansas highway ) = K-104 is a state highway in Saline County , Kansas . The route travels 2.3 miles ( 3.7 km ) from a junction with K-4 to a junction with Interstate 135 / U.S. Route 81 ( I-135 / US-81 ) at I-135 exit 86 . It has an annual average daily traffic of between 1000 and 1300 and is paved with composite pavement . The highway is not a part of the National Highway System . The route was established around 1967 , and has not been changed since . = = Route description = = The route begins in the south at a junction with K-4 near I-135 / US-81 . It closely parallels I-135 / US-81 through about 2 miles ( 3.2 km ) of rural farmland before abruptly turning west at Smolan Road just west of Mentor . After traveling west approximately 0.3 miles ( 0.48 km ) the route ends at an interchange with I-135 / US-81 . The route has a total distance of 2.3 miles ( 3.7 km ) , all of it in Saline County . The highway has an annual average daily traffic ( the total volume of vehicle traffic</t>
+          <t>Second Generation ( advertisement ) = " Second Generation " is a 2006 television advertisement introducing Nike 's Air Jordan XXI brand of basketball shoes . The ad depicts signature moves from Michael Jordan 's NBA career , recreated in the present day by twelve young basketball players around the world . Included are moments from the 1989 , 1991 , 1992 , and 1998 NBA playoffs and the iconic 1992 slam dunk . The ad was produced by Smuggler and directed by Brian Beletic for the advertising agency Wieden + Kennedy . Casting began in November 2005 , filming took place in January 2006 , and the ad debuted on television that February . Advertising publications gave favorable reviews to " Second Generation " , although it did not win major awards . The ad is also listed as " 2nd Generation " ; its tagline is " Let your game speak " . = = Production = = The ad was conceived by the agency Wieden + Kennedy . Copywriters Derek Barnes and Paul Renner were in a shopping mall when they noticed man</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Washington State Route 100 = State Route 100 ( SR 100 ) is a 4.68-mile-long ( 7.53 km ) state highway in the U.S. state of Washington , serving Cape Disappointment State Park in Pacific County . The highway travels counterclockwise from U.S. Route 101 ( US 101 ) in Ilwaco south to Cape Disappointment and north to an intersection with itself in Ilwaco . SR 100 , part of the Lewis and Clark Trail Scenic Byway , serves as a loop route and has a spur route that serves the state park and a Coast Guard station . SR 100 was established in 1991 on the existing North Head Road , which was a paved county road by the late 1950s . The highway was washed away during a 1994 winter storm and had its spur route shortened in 2006 . = = Route description = = SR 100 begins at an intersection with US 101 in Ilwaco as the highway turns north onto 1st Avenue towards Seaview . The highway , part of the Lewis and Clark Trail Scenic Byway , travels west on Spruce Street through an intersection with the clockwi</t>
+          <t>Closing Time ( album ) = Closing Time is the debut studio album by the American singer-songwriter Tom Waits , released in March 1973 on Asylum Records . Produced and arranged by former Lovin ' Spoonful member Jerry Yester , Closing Time was the first of seven of Waits ' major releases through Asylum . The album is noted for being predominantly folk influenced although Waits intended for Closing Time to be " a jazz , piano-led album . " Upon release , the album was mildly successful in the United States , although it did not chart and received little attention from music press in the United Kingdom and elsewhere internationally . Critical reaction to Closing Time was positive . The album 's only single — " Ol ' ' 55 " — attracted attention due to a cover version by Waits ' better-known label mates The Eagles . Other songs from the album were covered by artists ranging from Tim Buckley to Bette Midler . The album has been certified Gold in the United Kingdom and has gained a contemporary</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Wilhelm Steinitz = Wilhelm ( later William ) Steinitz ( May 17 , 1836 – August 12 , 1900 ) was an Austrian and later American chess Master player , and the first undisputed world chess champion from 1886 to 1894 . He was also a highly influential writer and chess theoretician . When discussing chess history from the 1850s onwards , commentators have debated whether Steinitz could be effectively considered the champion from an earlier time , perhaps as early as 1866 . Steinitz lost his title to Emanuel Lasker in 1894 , and also lost a rematch in 1896 – 97 . Statistical rating systems give Steinitz a rather low ranking among world champions , mainly because he took several long breaks from competitive play . However , an analysis based on one of these rating systems shows that he was one of the most dominant players in the history of the game . Steinitz was unbeaten in match play for 32 years , from 1862 to 1894 . Although Steinitz became " world number one " by winning in the all-out at</t>
+          <t>Russian language in Israel = The Russian language in Israel is spoken natively by a large proportion of the population , reaching about 20 percent of the total population by 1989 , mostly by immigrants who came from the former Soviet Union in the early 1990s and later years . It is a major foreign language in the country and is used in many aspects of life . Russian is by far the most used non-official native language in Israel . The government and businesses often provide information in Russian , and it is semi-official in some areas with high concentration of Russian Jewish immigrants . The Russian-speaking population of Israel is the world 's third-largest population of Russian native-speakers living outside the former Soviet Union territories after Germany and the United States , and the highest as a proportion of the population . As of 2013 , 1,231,003 residents of the Post-Soviet states have immigrated to Israel . = = History = = The first large scale immigration of Russian-speak</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barzillai J. Chambers = Barzillai Jefferson Chambers ( December 5 , 1817 – September 16 , 1895 ) was an American surveyor , lawyer , and politician of the Gilded Age . Born in Kentucky , he moved to Texas to join that state 's war for independence against Mexico . Chambers stayed in Texas after its independence and annexation by the United States , earning a living as a surveyor and farmer in Johnson County . In the American Civil War , he served briefly in the Confederate army , then returned to his farming and business interests , becoming part-owner of a bank in his hometown of Cleburne . In the 1870s , Chambers became concerned with farming and monetary issues in politics , eventually joining the nascent Greenback Party in 1877 . He ran unsuccessfully for Vice President on the Greenback ticket with presidential nominee James B. Weaver of Iowa in 1880 . The Greenback nominees finished in a distant third place , receiving only 3.3 % of the popular vote and no electoral votes . After </t>
+          <t>Our Father ( Dexter ) = " Our Father " is the third season premiere and twenty-fifth overall episode of the American television drama series Dexter , which first aired on September 28 , 2008 on Showtime in the United States . The episode was written by Clyde Phillips and directed by Keith Gordon . In the episode , which takes place several months after the second season finale , Dexter Morgan ( Michael C. Hall ) mistakenly kills an innocent man but forms a friendship with the man 's brother , well-known assistant district attorney Miguel Prado ( Jimmy Smits ) . Dexter 's sister Debra ( Jennifer Carpenter ) , meanwhile , has turned over a new leaf in her life and is determined to become a detective . To carry the remainder of the third season , Dexter 's writers introduced Miguel as a new character so that his relationship with Dexter could serve as a " central arc " . In order to allow them to explore Dexter 's psychological and emotional reactions , the writers revealed Dexter 's girl</t>
         </is>
       </c>
     </row>
@@ -826,32 +826,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>bridge miles area road construction river route line traffic dam water station feet tunnel built valley project park opened canal south railway motorway bridges mile section completed land creek near north street city toll service proposed located watershed access flood link plans lake lanes downstream roads coal constructed channel rail drainage london west navigation acres lane flows stations east upstream lock mouth crossing site town km2 passengers connect cubic tributaries tributary junction wildlife tunnels connecting areas services routes transit western reaches trout trains reservoir cost extension railroad tolls trail interchange border locks basin transport plan corridor rest passenger operated lower</t>
+          <t>['bridge', 'miles', 'area', 'road', 'construction', 'river', 'route', 'line', 'traffic', 'dam', 'water', 'station', 'feet', 'tunnel', 'built']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Huletts Landing , New York = Huletts Landing is a hamlet in the town of Dresden in northern Washington County , New York , United States . A lakeside community on the eastern shore of Lake George in the Adirondack Mountains , Huletts Landing is located entirely within the Adirondack Park . There is only one roadway access to the hamlet , County Route 6 and its suffixed routes , which head north-south . Huletts Landing is geographically located at 43 ° 38 ′ 21 ″ N 73 ° 30 ′ 25 ″ W and has approximately two centuries of written history . The hamlet derives its name from the Hulett family , which resided in the area for several generations after Revolutionary War soldier David Hulett moved near the lakeside and began farming . In 1874 his descendant Philander Hulett built a boat landing , a general store , and a post office . This opened the scenic corner of the lake to steamship traffic and tourism . This suffered a major setback in 1915 when the hamlet 's largest hotel burned to its fou</t>
+          <t>California State Route 14 = State Route 14 ( SR 14 ) is a north – south state highway in the U.S. state of California , largely in the Mojave Desert . The southern portion of the highway is signed as the Antelope Valley Freeway . The route connects Interstate 5 , or Golden State Freeway , on the border of the city of Santa Clarita to the north and the Los Angeles neighborhoods of Granada Hills and Sylmar to the south , with U.S. Route 395 near Inyokern . Legislatively , the route extends south of I-5 to State Route 1 in the Pacific Palisades area of Los Angeles , however the portion south of the junction with I-5 has not been constructed . The southern part of the constructed route is a busy commuter freeway serving and connecting the cities of Santa Clarita , Palmdale , and Lancaster with the rest of the Greater Los Angeles area . The northern portion , from Vincent ( south of Palmdale ) to Route 395 , is legislatively named the Aerospace Highway , as the highway serves Edwards Air Fo</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Bedminster railway station = Bedminster railway station is on the Bristol to Exeter Line and serves the districts of Bedminster and Windmill Hill in Bristol , England . It is 0.9 miles ( 1.4 km ) to the west of Bristol Temple Meads , and 119 miles ( 192 km ) from London Paddington . Its three letter station code is BMT . It was opened in 1871 by the Bristol and Exeter Railway , was resited slightly further to the west in 1884 and was rebuilt in 1932 . The station , which has three through-lines and two island platforms , but minimal facilities , is managed by Great Western Railway , the seventh company to be responsible for the station , and the third franchise since privatisation in 1997 . They provide all train services at the station , mainly an hourly service between Bristol Parkway and Weston-super-Mare . There is local support for the line to be electrified , as an extension of the planned electrification of the London to Bristol route , and the level of service will be increased</t>
+          <t>Myrmecia ( ant ) = Myrmecia is a genus of ants first established by Danish zoologist Johan Christian Fabricius in 1804 . The genus is a member of the subfamily Myrmeciinae of the family Formicidae . Myrmecia is a large genus of ants , comprising at least 93 species that are found throughout Australia and its coastal islands , while a single species is only known from New Caledonia . One species has been introduced out of its natural distribution and was found in New Zealand in 1940 , but the ant was last seen in 1981 . These ants are commonly known as " bulldog ants " or " jack jumper " ants , and are also associated with many other common names . They are characterised by their extreme aggressiveness , ferocity , and painful stings . Some species are known for the jumping behaviour they exhibit when agitated . Species of this genus are also characterised by their elongated mandibles and large compound eyes that provide excellent vision . They vary in colour and size , ranging from 8 t</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Grantham Canal = The Grantham Canal is a canal that runs for 33 miles ( 53 km ) from Grantham , falling through 18 locks to West Bridgford where it joins the River Trent . It was built primarily to allow for the transportation of coal to Grantham . It opened in 1797 , and its profitability steadily increased until 1841 . It was then sold to a railway company , after which it declined , and was finally closed in 1936 . Because it was used as a water supply for agriculture , most of the channel remained in water , although bridges were lowered . Since the 1970s , the Grantham Canal Society have been working towards its restoration , and two stretches are navigable to small vessels . Full restoration will require a new route where the canal joins the Trent , as road building has effectively severed the original route . = = History = = The concept of a canal from the River Trent to Grantham was first raised on 27 August 1791 , as a way of supplying the district with cheaper coal . The inte</t>
+          <t>Langit Makin Mendung = " Langit Makin Mendung " ( " The Sky is Increasingly Cloudy " ) is a controversial Indonesian short story . Published in Sastra magazine under the pen name Kipandjikusmin in August 1968 , it tells the story of Muhammad descending to Earth with the angel Gabriel to investigate the decreasing number of Muslims entering heaven , only to find that Muslims in Indonesia have begun fornicating , drinking alcohol , waging war on Muslims , and otherwise going against the tenets of Islam because of nasakom , a government policy during Sukarno 's administration that combined nationalism , religion , and communism . Unable to do anything to stop the rampant sinning , Muhammad and Gabriel watch the political maneuvering , crime , and famine in Jakarta in the form of eagles . Upon publication , " Langit Makin Mendung " drew heavy criticism for its depictions of Allah , Muhammad , and Gabriel . Sastra was banned in North Sumatra , and the magazine 's offices in Jakarta were att</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Washington State Route 516 = State Route 516 ( SR 516 ) is a 16.49-mile-long ( 26.54 km ) state highway in the U.S. state of Washington , serving communities in southern King County . The highway travels east as the Kent-Des Moines Road and the Kent-Kangley Road from a concurrency with SR 509 in Des Moines through Kent and Covington to an intersection with SR 169 in Maple Valley . SR 516 , designated as part of the National Highway System within Kent , intersects three major freeways in the area : Interstate 5 ( I-5 ) in western Kent , SR 167 in downtown Kent , and SR 18 in Covington . The roadway , built in the 1890s , was codified in 1937 as Secondary State Highway 1K ( SSH 1K ) from Des Moines to Kent and SSH 5A from Kent to Maple Valley . The two highways were combined during the 1964 highway renumbering to form SR 516 on its current route . = = Route description = = SR 516 begins in Des Moines at Marine View Drive as SR 509 turns north towards Burien near the East Passage of Puget</t>
+          <t xml:space="preserve">Effects of Hurricane Dennis in Georgia = The effects of Hurricane Dennis in Georgia included two deaths and $ 24 million ( 2005 USD ) in damage . On June 29 , 2005 , a tropical wave emerged off the west coast of Africa . Gradually , the system organized on July 2 and formed a broad low pressure area . The system continued to organize , and it became a tropical depression on July 4 . Tracking westward , it became a tropical storm on July 5 and a hurricane on July 7 . Dennis rapidly intensified to attain Category 4 status on the Saffir-Simpson Hurricane Scale before making landfall on Cuba . The storm weakened to Category 1 status before re-emerging in the Gulf of Mexico and intensifying . Dennis made landfall on the Florida Panhandle on July 10 , then tracked over southeast Alabama . Dennis had moderate effects in the state , primarily from flooding . One rainband in particular stalled in southwest portions of the state and produced 4 – 8 inches ( 100 – 200 mm ) of rain , with isolated </t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>BR Standard Class 7 = The BR Standard Class 7 , otherwise known as the Britannia Class , is a class of 4-6-2 Pacific steam locomotive designed by Robert Riddles for use by British Railways for mixed traffic duties . Fifty-five were constructed between 1951 and 1954 . The design was a result of the 1948 locomotive exchanges undertaken in advance of further locomotive classes being constructed . Three batches were constructed at Crewe Works , before the publication of the 1955 Modernisation Plan . The Britannia Class was based on several previous LMS locomotive designs , and also significantly influenced by the Bulleid SR Pacifics , notably in the boiler and rear truck design , incorporating the best practices in locomotive technology as regards labour-saving and lowering maintenance costs ; various weight-saving measures also increased the route availability of a Pacific-type locomotive on the British Railways network . The Britannias received a positive reception from their crews , wit</t>
+          <t>Penrose tiling = A Penrose tiling is an example of non-periodic tiling generated by an aperiodic set of prototiles . Penrose tilings are named after mathematician and physicist Roger Penrose , who investigated these sets in the 1970s . The aperiodicity of prototiles implies that a shifted copy of a tiling will never match the original . A Penrose tiling may be constructed so as to exhibit both reflection symmetry and fivefold rotational symmetry , as in the diagram at the right . A Penrose tiling has many remarkable properties , most notably : It is non-periodic , which means that it lacks any translational symmetry . It is self-similar , so the same patterns occur at larger and larger scales . Thus , the tiling can be obtained through " inflation " ( or " deflation " ) and any finite patch from the tiling occurs infinitely many times . It is a quasicrystal : implemented as a physical structure a Penrose tiling will produce Bragg diffraction and its diffractogram reveals both the fivef</t>
         </is>
       </c>
     </row>
@@ -861,32 +861,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>century known breed horses horse found popular island today breeds including period dog large early include small breeding food region modern islands europe wine population dogs established area especially bred use traditional seen tea quality plants leaves considered common european plant northern imported arabian brought years fried important native birds stud variety red scotland produce grown 19th areas cuisine generally present particularly southern species different meat park britain culture history chinese produced black old vegetables called english tradition stallion chicken 20th regions breeders earliest tree scottish usually water wild local spread cooked norse registered late herd coat created land ancient</t>
+          <t>['century', 'known', 'breed', 'horses', 'horse', 'found', 'popular', 'island', 'today', 'breeds', 'including', 'period', 'dog', 'large', 'early']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Waterspout = A waterspout is an intense columnar vortex ( usually appearing as a funnel-shaped cloud ) that occurs over a body of water . They are connected to a towering cumuliform cloud or a cumulonimbus cloud . In the common form , it is a non-supercell tornado over water . While it is often weaker than most of its land counterparts , stronger versions spawned by mesocyclones do occur . Most waterspouts do not suck up water ; they are small and weak rotating columns of air over water . While waterspouts form mostly in the tropics and subtropical areas , other areas also report waterspouts , including Europe , New Zealand , the Great Lakes and Antarctica . Although rare , waterspouts have been observed in connection with lake-effect snow precipitation bands . Waterspouts have a five-part life cycle : formation of a dark spot on the water surface , spiral pattern on the water surface , formation of a spray ring , development of the visible condensation funnel , and ultimately decay . </t>
+          <t>Utah State Route 68 = State Route 68 ( SR-68 ) is a state highway in the U.S. state of Utah . It is a major thoroughfare throughout the Wasatch Front as it runs north – south for 70.832 miles ( 113.993 km ) , linking US-6 near Elberta to US-89 in Woods Cross . The route intersects several major freeways and highways in the Salt Lake City metropolitan area including I-215 , I-80 , and I-15 . The route is more commonly referred to as Redwood Road , after the street it is routed along throughout Salt Lake County . The highway is also routed for a short distance along 500 South and 200 West in Bountiful and Camp Williams Road in Utah County . The route is a surface street for its entire length . SR-68 became a state highway in 1931 , at which time the route ran from then – US-40 ( North Temple Street ) in Salt Lake City to present-day US-89 in Lehi . In 1933 , the route was extended north to US-89 at Beck 's Hot Springs . SR-68 was routed onto Redwood Road in 1943 , taking over what had be</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ain 't = Ain 't is a contraction for am not , is not , are not , has not , and have not in the common English language vernacular . In some dialects ain 't is also used as a contraction of do not , does not , and did not . The development of ain 't for the various forms of to be not , to have not , and to do not occurred independently , at different times . The usage of ain 't for the forms of to be not was established by the mid-18th century , and for the forms of to have not by the early 19th century . The usage of ain 't is a perennial subject of controversy in English . Ain 't is commonly used by many speakers in oral or informal settings , especially in certain regions and dialects . Its usage is often highly stigmatized , and it may be used as a marker of low socio-economic or regional status or education level . Its use is generally considered non-standard by dictionaries and style guides except when used for rhetorical effect , and it is rarely found in formal written works . =</t>
+          <t>Hungry Bay Nature Reserve = Hungry Bay Nature Reserve is a nature reserve on the east coast of Bermuda . It was established in 1986 . It is considered the best example of coastal mangrove swamp on the island . It includes the Hungry Bay area and the largest mangrove coastal swamp in Bermuda . It is protected by a Tree preservation order ( T.P.O. ) and designated as an official Nature Reserve within the Parks system of Bermuda . The Hungry Bay Mangrove Swamp Reserve , a wetland site , is one of the seven Ramsar Sites in Bermuda . This designation recognises its international importance as a northerly mangrove swamp , as a habitat for its native crustaceans and as an important destination for migratory birds . Most of the reserve consists of mangrove swamp , while in the southern part there is a small area of saltmarsh . Much damage was done to the site by a storm in 2003 and residents have expressed concern about possible environmental damage resulting from pollution from the village of</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ben Thompson ( actor ) = Ben Thompson ( born 1 June 1992 ) is an English actor best known for his role as Ryan Connor in the British soap opera Coronation Street . Brought up in Radcliffe , Greater Manchester , Thompson made his screen debut when he appeared in the 2002 film Re-Inventing Eddie . Shortly before turning 13 , he appeared in the 2004 CBBC children 's comedy programme Stupid ! . Thompson rose to further prominence when he was cast as teenager Ryan Connor in Coronation Street in 2006 . As part of the longstanding series , he has been involved in storylines that have dealt with varying topics , including family life , death and coming of age . In addition to his career as an actor , Thompson is also an amateur musician . He is a member of the Rusholme Ruffians , an indie group who are largely influenced by established Manchester bands . = = Youth and early career = = Ben Thompson was brought up in Radcliffe , a town within the Metropolitan Borough of Bury , in Greater Manches</t>
+          <t xml:space="preserve">Skin Trade ( film ) = Skin Trade is a 2014 action thriller film directed by Ekachai Uekrongtham , and starring Dolph Lundgren , Tony Jaa , Michael Jai White , and Ron Perlman . Lundgren wrote the film with Gabriel Dowrick and Steven Elder , while John Hyams performed uncredited script revisions . The film centers around New Jersey police detective Nick Cassidy , as he travels to Asia intent on killing the man who murdered his family , mobster Viktor Dragovic . He is also set on destroying Dragovic 's human trafficking network . Development started in 2007 after Lundgren read a news report about a group of girls being smuggled into the United States from Mexico . The girls were left in a vehicle along the border , and trapped inside , they all died of heat stroke and suffocation . Skin Trade had a $ 9 million production budget , and was shot over 50 days in Canada and Thailand . It was the first film to be shot in English by an organization based in Asia ( outside of Hong Kong ) for an </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Centennial Light = The Centennial Light is the world 's longest-lasting light bulb , burning since 1901 . It is at 4550 East Avenue , Livermore , California , and maintained by the Livermore-Pleasanton Fire Department . Due to its longevity , the bulb has been noted by The Guinness Book of World Records , Ripley 's Believe It or Not ! , and General Electric . It is often cited as evidence for the existence of planned obsolescence in later-produced light bulbs . = = History = = The Centennial Light was originally a 30-watt or 60-watt bulb but now is very dim , emitting about the same light as a 4-watt nightlight . The hand-blown , carbon-filament common light bulb was manufactured in Shelby , Ohio , by the Shelby Electric Company in the late 1890s ; many just like it still exist and can be found functioning . According to Zylpha Bernal Beck , the bulb was donated to the Fire Department by her father , Dennis Bernal , in 1901 . Bernal owned the Livermore Power and Water Company and donat</t>
+          <t>Martin Bormann = Martin Bormann ( 17 June 1900 – 2 May 1945 ) was a prominent official in Nazi Germany as head of the Parteikanzlei ( Nazi Party Chancellery ) . He gained immense power within the Third Reich by using his position as Adolf Hitler 's private secretary to control the flow of information and access to Hitler . Bormann joined a paramilitary Freikorps organisation in 1922 while working as manager of a large estate . He served nearly a year in prison as an accomplice to his friend Rudolf Höss ( later commandant of Auschwitz concentration camp ) in the murder of Walther Kadow . Bormann joined the Nazi Party in 1927 and the Schutzstaffel ( SS ) in 1937 . He initially worked in the party 's insurance service , and transferred in July 1933 to the office of Deputy Führer Rudolf Hess , where he served as chief of staff . Bormann used his position to create an extensive bureaucracy and involve himself as much as possible in the decision making . He gained acceptance into Hitler 's i</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>SM UB-10 = SM UB-10 was a German Type UB I submarine or U-boat in the German Imperial Navy ( German : Kaiserliche Marine ) during World War I. UB-10 was ordered in October 1914 and was laid down at the AG Weser shipyard in Bremen in November . UB-10 was a little under 28 metres ( 92 ft ) in length and displaced between 127 and 141 t ( 125 and 139 long tons ) , depending on whether surfaced or submerged . She carried two torpedoes for her two bow torpedo tubes and was also armed with a deck-mounted machine gun . UB-10 was broken into sections and shipped by rail to Antwerp for reassembly . She was launched in February 1915 and commissioned as SM UB-10 in March . The U-boat was the first of her class to commence operations when she entered service on 27 March 1915 . UB-10 was the first boat assigned to the Flanders Flotilla , the unit in which she spent her entire career . Her first two commanders were Otto Steinbrinck and Reinhold Saltzwedel , fifth and eleventh , respectively , among t</t>
+          <t>Black Brunswickers = The Brunswicker Ducal Corps , in German : Herzoglich Braunschweigisches Korps , commonly known as the Black Brunswickers in English and the Schwarze Schar ( " Black Troop " , also translated as " Black Horde " or " Black Host " ) or Schwarze Legion ( " Black Legion " ) in German were a military unit in the Napoleonic Wars . The corps was raised from volunteers by German-born Frederick William , Duke of Brunswick-Wolfenbüttel ( 1771 – 1815 ) . The Duke was a harsh opponent of Napoleon Bonaparte 's occupation of his native Germany . Formed in 1809 when war broke out between the First French Empire and the Austrian Empire , the corps initially comprised a mixed force , around 2,300 strong , of infantry , cavalry and later supporting artillery . Most units of the corps wore black uniforms , leading to the " black " nicknames of the unit , though some light units ( such as sharpshooters and uhlans ) wore green uniforms . The Brunswickers wore a silvered skull badge on t</t>
         </is>
       </c>
     </row>
@@ -896,32 +896,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>september storm mph august hurricane october day damage near early developed later tropical began caused winds system west reported strong people days continued produced moved heavy july late june east reached destroyed brought depression november damaged quickly hours north million shortly florida category peaked status south occurred passed peak turned homes formed northeast deaths resulted estimated initially curved landfall flooding coast rainfall northwestward issued northeastward reaching briefly slightly located area strengthened southern names moving fatalities eastern utc overall struck wave lesser low sustained minimal bermuda southeast maximum island central africa atlantic curving antilles caribbean_sea northwest weakened offshore remnants hurricanes mbar</t>
+          <t>['september', 'storm', 'mph', 'august', 'hurricane', 'october', 'day', 'damage', 'near', 'early', 'developed', 'later', 'tropical', 'began', 'caused']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Psychedelic music = Psychedelic music ( sometimes psychedelia ) covers a range of popular music styles and genres influenced by the 1960s psychedelic culture , a subculture of people who used psychedelic drugs such as LSD , psilocybin mushrooms , mescaline and DMT to experience visual and auditory hallucinations , synesthesia and altered states of consciousness . Psychedelic music attempted to replicate the hallucinogenic experience of using these drugs or enhance the experience of using them . Psychedelic music emerged during the mid-1960s among folk rock and blues rock bands in the United States and Britain . Psychedelic bands often drew on non-Western sources such as the ragas , drones and sitars of Indian music and they used electric instruments and electronic effects – notably the lead electric guitar played with heavy distortion – and new , unorthodox recording techniques , such as playing tapes backwards or panning the music from one side to the other . Psychedelic influences sp</t>
+          <t>1970 Canada hurricane = The 1970 Canada hurricane was an unnamed tropical cyclone that brought impact to Bermuda and Newfoundland . The fourth hurricane and ninth tropical storm of the annual hurricane season , this system developed northeast of the Bahamas as a subtropical depression on October 12 . While tracking northeastward , the system intensified , becoming a subtropical storm on the following day . The subtropical storm transitioned into a tropical cyclone on October 16 , and strengthened into a hurricane about twelve hours later . The hurricane later bypassed Bermuda , before further intensifying into a Category 2 hurricane on the Saffir – Simpson hurricane wind scale . Thereafter , the hurricane accelerated rapidly northeastward , and made landfall on the Avalon Peninsula of Newfoundland as a Category 1 hurricane . It transitioned into an extratropical cyclone early on October 17 . The system produced tropical storm force winds on Bermuda , which caused the suspension of scho</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">1956 Atlantic hurricane season = The 1956 Atlantic hurricane season featured a low number of tropical cyclones , although every tropical storm and hurricane affected land . There were twelve tropical storms , a third of which became hurricanes . One of the hurricanes strengthened to the equivalent of a major hurricane , which is a Category 3 or greater on the Saffir-Simpson scale . The strongest hurricane of the season was Betsy , which was also the most damaging storm of the season : it destroyed 15,000 houses and left $ 40 million in damage in Puerto Rico . Betsy was also the deadliest of the season , having killed 18 people in the French West Indies , two from a shipwreck in the Caribbean Sea , and 16 in Puerto Rico . Tropical Storm Dora struck Mexico in September and killed 27 people . The season officially started on June 15 , although an unnamed storm developed about a week prior over the western North Atlantic Ocean . A later storm that formed over the Gulf of Mexico on June 12 </t>
+          <t xml:space="preserve">Battle of Salamis = The Battle of Salamis ( / ˈsæləmɪs / ; Ancient Greek : Ναυμαχία τῆς Σαλαμῖνος , Naumachia tēs Salaminos ) was a naval battle fought between an alliance of Greek city-states under Themistocles and the Persian Empire under King Xerxes in 480 BC which resulted in a decisive victory for the outnumbered Greeks . The battle was fought in the straits between the mainland and Salamis , an island in the Saronic Gulf near Athens , and marked the high-point of the second Persian invasion of Greece . To block the Persian advance , a small force of Greeks blocked the pass of Thermopylae , while an Athenian-dominated Allied navy engaged the Persian fleet in the nearby straits of Artemisium . In the resulting Battle of Thermopylae , the rearguard of the Greek force was annihilated , whilst in the Battle of Artemisium the Greeks had heavy losses and retreated after the loss at Thermopylae . This allowed the Persians to conquer Boeotia and Attica . The Allies prepared to defend the </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>The Aenar = " The Aenar " is the fourteenth episode of the fourth season of the American science fiction television series Star Trek : Enterprise , and originally aired on February 11 , 2005 . It was written by André Bormanis from a story by Manny Coto , and was directed by Mike Vejar . " The Aenar " was the third installment of a three-part story which concluded the events of episodes " Babel One " and " United " . Set in the 22nd century , the series follows the adventures of the first Starfleet starship Enterprise . In this episode , Captain Jonathan Archer ( Scott Bakula ) and Commander Shran ( Jeffrey Combs ) travel to Andoria , a moon , seeking the help of the Aenar — an offshoot race of the Andorians — one of whom has been taken by the Romulans to pilot a drone vessel ( first seen in the previous episode ) . The episode showed the home world of the Andorians for the first time , with the sets for the planet 's ice tunnels being created on a sound stage . Alexandra Lydon and Alic</t>
+          <t>Hurricane Hernan ( 2002 ) = Hurricane Hernan was the second of three Category 5 hurricanes during the 2002 Pacific hurricane season . The twelfth tropical cyclone , tenth named storm and sixth hurricane of the season , Hernan originated from a tropical wave that formed in the Atlantic Ocean and crossed to the Pacific Ocean . The wave spawned a low pressure system which organized into a tropical depression on August 30 , a tropical storm on August 31 and a hurricane later that day . Hernan rapidly intensified and reached peak intensity as a Category 5 storm on the Saffir-Simpson Hurricane Scale . Proceeding northwest , it maintained this strength for eight hours , but on September 2 it entered cooler waters and began to weaken . By September 6 it had degenerated into a remnant area of low pressure . Hernan was the second most intense hurricane of the season , and it maintained Category 5 status for the second-longest time of the season , behind Hurricane Kenna . Although Hernan remained</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1942 Matagorda hurricane = The 1942 Matagorda hurricane was the most intense and costliest tropical cyclone of the 1942 Atlantic hurricane season . The second tropical storm and hurricane , as well as the first major hurricane of the year , it originated from a tropical wave near the island of St. Lucia on August 21 . Moving generally westward across the Caribbean Sea , the storm remained weak for much of its early existence . However , it gradually intensified , and reach hurricane strength south of Jamaica on August 25 before coming ashore the Yucatán Peninsula late on August 27 . Once in the Gulf of Mexico , the hurricane quickly strengthened , and attained its peak intensity on August 29 as a Category 3 hurricane with winds of 115 mph ( 185 km / h ) . However , nearing the Texas Gulf Coast , the storm waned in intensity , and was only a Category 1 hurricane by the time it made a final landfall near Matagorda , Texas on August 30 . Continuing inland , the hurricane weakened , and di</t>
+          <t>1903 Atlantic hurricane season = The 1903 Atlantic hurricane season featured seven hurricanes , the most in a season since 1893 . The first tropical cyclone was initially observed in the western Atlantic Ocean near Puerto Rico on July 21 . The tenth and final system transitioned into an extratropical cyclone well northwest of the Azores on November 25 . These dates fall within the period with the most tropical cyclone activity in the Atlantic . Six of the ten tropical cyclones existed simultaneously . Of the season 's ten tropical storms , seven of those strengthened into a hurricane . One of the seven hurricanes deepened further into a major hurricane , which are tropical cyclones that reach at least Category 3 on the modern day Saffir – Simpson hurricane wind scale . The second , third , and fourth systems left the most significant impacts during this season . The second storm , which struck Jamaica in August , devastated Martinique , Jamaica , and the Cayman Islands . At least 149 d</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Tewkesbury Medieval Festival = The Tewkesbury Medieval Festival is a medieval fair held over the second weekend of every July near the town of Tewkesbury , United Kingdom . Its main feature is the re-enactment of the Battle of Tewkesbury , which was fought in 1471 . Located on parts of the ground where the original battle was fought , the festival also features a medieval camp , in which traders ply their wares and visitors are entertained by musicians and acrobats . The largest medieval fair in the United Kingdom , the Tewkesbury Medieval Festival was listed in Footprint England as one of the " ten most bizarre festivals " in the country . = = Background = = The Tewkesbury Medieval Festival started in 1984 as a simple fair with 10 stalls , a beer tent , and a small-scale re-enactment of the Battle of Tewkesbury , which was originally fought in 1471 near the town of Tewkesbury , United Kingdom . The festival became a regular celebration held over the second weekend of every July on par</t>
+          <t xml:space="preserve">1989 Atlantic hurricane season = The 1989 Atlantic hurricane season featured the costliest tropical cyclone in the Atlantic basin at the time , Hurricane Hugo . The season officially began on June 1 , and ended on November 30 . It was a near average season with 11 named storms . The first storm , Tropical Depression One , developed on June 15 , and dissipated two days later without effects on land . Later that month , Tropical Storm Allison caused severe flooding , especially in Texas and Louisiana . Tropical Storm Barry , Tropical Depressions Six , Nine , and Thirteen , and Hurricanes Erin and Felix caused negligible impact . Hurricane Gabrielle and Tropical Storm Iris caused light effects on land , with the former resulting in nine fatalities from rip currents offshore the East Coast of the United States and Atlantic Canada , while the latter produced minor flooding in the United States Virgin Islands . The most notable storm of the season was Hurricane Hugo , a Category 5 hurricane </t>
         </is>
       </c>
     </row>
@@ -931,32 +931,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>said told death police murder family life found asked relationship killed later mother character man killing hospital father child house away help shot kill leave storyline prison arrested trial old find guilty left money sentenced taken bond case wife woman died people stated shooting body revealed years evidence having crime knew authorities sister months sentence investigation charges going days friend friends convicted discovered mercedes incident come soap children tells think believed inmates murders daughter room victim wanted described court home scene testified heard went charged prisoners tried arrest judge officers investigators execution affair saying suicide officer involved escape report sarah</t>
+          <t>['said', 'told', 'death', 'police', 'murder', 'family', 'life', 'found', 'asked', 'relationship', 'killed', 'later', 'mother', 'character', 'man']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gheorghe Tătărescu = For the artist , see Gheorghe Tattarescu . Gheorghe I. Tătărescu ( also known as Guță Tătărescu , with a slightly antiquated pet form of his given name ; 2 November 1886 – 28 March 1957 ) was a Romanian politician who served twice as Prime Minister of Romania ( 1934 – 1937 ; 1939 – 1940 ) , three times as Minister of Foreign Affairs ( interim in 1934 and 1938 ; appointed to the office in 1945-1947 ) , and once as Minister of War ( 1934 ) . Representing the " young liberals " faction inside the National Liberal Party ( PNL ) , Tătărescu began his political career as a collaborator of Ion G. Duca , becoming noted for his anti-Communism and , in time , for his conflicts with the PNL 's leader Dinu Brătianu and the Foreign Minister Nicolae Titulescu . During his first time in office , he moved closer to King Carol II , leading an ambivalent policy toward the fascist Iron Guard and ultimately becoming instrumental in establishing the authoritarian and corporatist regime</t>
+          <t>Marguerite LeHand = Marguerite Alice " Missy " LeHand ( September 13 , 1898 – July 31 , 1944 ) was private secretary to U.S. President Franklin D. Roosevelt ( FDR ) for 21 years . According to Roosevelt biographer Doris Kearns Goodwin , during FDR 's presidency , LeHand became " the most celebrated private secretary in the country " . Born into a poor Irish-American family in New York , LeHand attended secretarial school , took a series of clerical jobs , and eventually began to work for the Democratic Party 's New York office . There she came to the attention of FDR 's wife Eleanor during his 1920 vice presidential candidacy and was hired as FDR 's personal secretary . After FDR was partially paralyzed by polio , LeHand became his daily companion , to the extent of adopting his favorite hobbies , games , and drinks . She remained his secretary when he became Governor of New York in 1929 and when he became president in 1933 , serving until a 1941 stroke left her unable to speak . She m</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Psycho ( 1960 film ) = Psycho is a 1960 American psychological horror thriller directed and produced by Alfred Hitchcock , and written by Joseph Stefano , starring Anthony Perkins , Janet Leigh , John Gavin , Vera Miles and Martin Balsam , and was based on the 1959 novel of the same name by Robert Bloch . The film centers on the encounter between a secretary , Marion Crane ( Leigh ) , who ends up at a secluded motel after stealing money from her employer , and the motel 's disturbed owner-manager , Norman Bates ( Perkins ) , and its aftermath . When originally made , the film was seen as a departure from Hitchcock 's previous film North by Northwest , having been filmed on a low budget , with a television crew and in black and white . Psycho initially received mixed reviews , but outstanding box office returns prompted reconsideration which led to overwhelming critical acclaim and four Academy Award nominations , including Best Supporting Actress for Leigh and Best Director for Hitchco</t>
+          <t>Momchil = Momchil ( Bulgarian : Момчил , Greek : Μομ [ ι ] τζίλος or Μομιτζίλας ; c . 1305 – 7 July 1345 ) was a 14th-century Bulgarian brigand and local ruler . Initially a member of a bandit gang in the borderlands of Bulgaria , Byzantium and Serbia , Momchil was recruited by the Byzantines as a mercenary . Through his opportunistic involvement in the Byzantine civil war of 1341 – 1347 , where he played the various sides against each other , he became ruler of a large area in the Rhodopes and western Thrace . Momchil achieved initial successes against Turks and Byzantines alike , setting Turkish ships on fire and almost managing to kill one of his main opponents at the time , John VI Kantakouzenos . Despite this , he was defeated and killed by a joint Byzantine – Turkish army in 1345 . Due to his opposition to the Turks , he is remembered in popular South Slavic legend as a fighter against the Turkish invasion of the Balkans . = = Brigandage and role in the Byzantine civil war = = Co</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>French cruiser Sully = The French cruiser Sully was an armored cruiser of the Gloire class that was built for the French Navy in the early 1900s . She was named in honor of Maximilien de Béthune , Duke of Sully , trusted minister of King Henry IV . The ship struck a rock in Hạ Long Bay , French Indochina in 1905 , only eight months after she was completed , and was a total loss . = = Design and description = = The Gloire-class ships were designed as enlarged and improved versions of the Gueydon-class armored cruisers by Emile Bertin . Her crew numbered 612 officers and men . The ship measured 139.8 meters ( 458 ft 8 in ) overall , with a beam of 20.2 meters ( 66 ft 3 in ) . Sully had a draft of 7.7 meters ( 25 ft 3 in ) and displaced 10,014 metric tons ( 9,856 long tons ) . Sully had three propeller shafts , each powered by one vertical triple-expansion steam engine , which were rated at a total of 20,500 indicated horsepower ( 15,300 kW ) . Twenty-four Belleville water-tube boilers pr</t>
+          <t>Joe Aiello = Giuseppe " Joe " Aiello ( 1891 – October 23 , 1930 ) was a Chicago bootlegger and organized crime leader during the Prohibition era . The leader of his own Sicilian Mafia family , he was best known for his long and bloody feud with Chicago Outfit boss Al Capone . Aiello masterminded several unsuccessful attempts to assassinate Capone , and fought against his former business partner Antonio Lombardo , a Capone ally , for control of the Chicago branch of the Unione Siciliana benevolent society . Aiello and his ally Bugs Moran are believed to have arranged the murder of Lombardo , which directly led Capone to organize the St. Valentine 's Day Massacre in retaliation . Despite being forced to flee Chicago multiple times throughout the gang war , Aiello eventually took control of the Unione Siciliana in 1929 , and ranked seventh among the Chicago Crime Commission 's list of top " public enemies " . Aiello was killed after Capone gunmen ambushed him as he exited a Chicago apartm</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Jereboam O. Beauchamp = Jereboam Orville Beauchamp ( / dʒɛrəˈboʊ.əm ˈɔːrvɪl ˈbiːtʃəm / ; September 6 , 1802 – July 7 , 1826 ) was an American lawyer who murdered the Kentucky legislator Solomon P. Sharp ; the crime is known as the Beauchamp – Sharp Tragedy . In 1821 , Sharp had been accused in Bowling Green , Kentucky by Anna Cooke of fathering her illegitimate child ; it was stillborn . [ a ] Sharp denied paternity , and public opinion favored him . In 1824 , Beauchamp married Cooke , who was sixteen years older than he . She asked him to kill Sharp to defend her honor . When Sharp campaigned in 1825 for a seat in the Kentucky House of Representatives , opponents revived the story of his alleged illegitimate child by Cooke . They distributed campaign literature claiming the child was mulatto . Enraged , Beauchamp renewed his intention to avenge his wife 's honor . In the early morning of November 7 , 1825 , he tricked Sharp to open the door at his home in Frankfort , and fatally stabb</t>
+          <t>Oskar Gröning = Oskar Gröning ( sometimes transliterated as Oscar Groening in English ; born 10 June 1921 ) is a German former SS junior squad leader who was stationed at Auschwitz concentration camp . His responsibilities included counting and sorting the money taken from prisoners , and he was in charge of the personal property prisoners had arrived with . On a few occasions he witnessed the procedures of mass-killing in the camp . After being transferred from Auschwitz to a combat unit in October 1944 , Gröning was captured by the British on 10 June 1945 when his unit surrendered . He was eventually transferred to Britain as a prisoner of war and worked as a forced labourer . Upon his return to Germany he led a normal life , reluctant to talk about his time in Auschwitz . However , more than 40 years later , he decided to make his activities at Auschwitz public after learning about Holocaust denial . He has since openly criticised those who deny the events that he witnessed , and th</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Adam Mitchell ( Doctor Who ) = Adam Mitchell is a fictional character in the British science fiction television series Doctor Who , played by Bruno Langley . Adam is introduced in the first series of the programme 's revival as the second television companion of the Ninth Doctor ( Christopher Eccleston ) . However unlike the Ninth Doctor 's primary companion , Rose Tyler ( Billie Piper ) , who provided an effective human contrast to the Doctor 's centuries-old alien , Adam was created to provide an example of an inept time traveller . The character is introduced as a boy genius from the year 2012 who attracts the attention of the Doctor 's traveling companion Rose after she and the Doctor meet him in his place of work . Despite Rose 's willingness to accept Adam as a fellow traveller , the Doctor is skeptical . After Adam attempts to use information from the future for his own gain he throws Adam out of his time machine , the TARDIS . This was the first example of the Doctor forcing a </t>
+          <t>The Living Daylights = The Living Daylights ( 1987 ) is the fifteenth entry in the James Bond film series and the first to star Timothy Dalton as the fictional MI6 agent James Bond . The film 's title is taken from Ian Fleming 's short story , " The Living Daylights " . It was the last film to use the title of an Ian Fleming story until the 2006 instalment Casino Royale . The film was produced by Albert R. Broccoli , his stepson , Michael G. Wilson and his daughter , Barbara Broccoli . The Living Daylights was generally well received by most critics and was also a financial success , grossing $ 191.2 million worldwide . = = Plot = = James Bond is assigned to aid the defection of a KGB officer , General Georgi Koskov , covering his escape from a concert hall in Bratislava , Czechoslovakia during intermission . During the mission , Bond notices that the KGB sniper assigned to prevent Koskov 's escape is a female cellist from the orchestra . Disobeying his orders to kill the sniper , he i</t>
         </is>
       </c>
     </row>
@@ -966,32 +966,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>city million school company building stadium students center schools year sports largest located community years including library sold public education business area campus hosted financial market founded new local university host include college festival population facilities arena student development billion events established olympic residents companies chicago street museum program firm neighborhoods businesses downtown opened industry united_states expanded arts private facility annual retail buildings housing football expansion mayor venues programs theatre includes offices acquired neighborhood institutions households designed jobs census products commercial home board investment organization members professional art location median families funds fraternity management collection owned national fund culture historic</t>
+          <t>['city', 'million', 'school', 'company', 'building', 'stadium', 'students', 'center', 'schools', 'year', 'sports', 'largest', 'located', 'community', 'years']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wizards of the Coast = Wizards of the Coast ( often referred to as WotC / wɑːt.siː / or simply Wizards ) is an American publisher of games , primarily based on fantasy and science fiction themes , and formerly an operator of retail stores for games . Originally a basement-run role-playing game publisher , the company popularized the collectible card game genre with Magic : The Gathering in the mid-1990s , acquired the popular Dungeons &amp; Dragons role-playing game by purchasing the failing company TSR , and experienced tremendous success by publishing the licensed Pokémon Trading Card Game . The company 's corporate headquarters are located in Renton , Washington in the United States of America . Today , Wizards of the Coast publishes role-playing games , board games , and collectible card games . They have received numerous awards , including several Origins Awards . The company has been a subsidiary of Hasbro since 1999 . All Wizards of the Coast stores were closed in 2004 . = = Histor</t>
+          <t>Malloch Building = The Malloch Building is a private residential apartment building on Telegraph Hill in San Francisco designed in the Streamline Moderne style and built in 1937 . The building , one of the best examples of its type in San Francisco , is also known as Malloch Apartments , Malloch Apartment Building , and simply by its address : 1360 Montgomery Street . Some have called it the " Ocean-Liner House " , though other Moderne buildings have also been known by that nickname . Designed by Irvin Goldstine for father / son architects John " Jack " S. Malloch and John Rolph Malloch , the building was used as a filming location in 1947 's Dark Passage , a noir work starring Humphrey Bogart and Lauren Bacall . = = Design and construction = = The building was intended as a home for Jack Malloch and his son , John Rolph Malloch . Both men were partners in a father / son architectural firm based in San Francisco , and both wanted to live on Telegraph Hill with a view of the San Francis</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1990 – 91 South Pacific cyclone season = The 1990 – 91 South Pacific cyclone season was one of the least active cyclone seasons , with only three tropical cyclones occurring within the South Pacific basin which is to the east of 160 ° E. The season officially ran from November 1 , 1990 , to April 30 , 1991 with the first disturbance of the season forming on November 23 and the last disturbance dissipating on May 19 . This is the period of the year when most tropical cyclones form within the South Pacific Ocean . During the season there was no deaths recorded from any of the tropical cyclones while they were within the basin . However six people were killed by Cyclone Joy , when it made landfall on Australia . As a result of the impacts caused by Joy and Sina , the names were retired from the tropical cyclone naming lists . During the season , tropical cyclones were monitored by the Tropical Cyclone Warning Centers ( TCWC ) in Nadi , Fiji , and in Wellington , New Zealand . Whilst tropi</t>
+          <t>Hospice care in the United States = Hospice care in the United States is a type and philosophy of end-of-life care which focuses on the palliation of a terminally ill patient 's symptoms . These symptoms can be physical , emotional , spiritual or social in nature . The concept of hospice as a place to treat the incurably ill has been evolving since the 11th century and came into the United States in the 1970s in response to the work of Cicely Saunders in the United Kingdom . Since its first establishment , the industry has rapidly expanded . In the United States , it is distinguished by more extensive volunteerism and a greater emphasis on the patient 's psychological needs in coming to terms with dying . With practices largely defined by the Medicare system , a social insurance program in the United States , and other health insurance providers , hospice care is made available in the United States to patients of any age with any terminal prognosis who are medically certified to have l</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Constitution Center ( Washington , D.C. ) = Constitution Center ( formerly known as the David Nassif Building ) is an office building located at 400 7th Street SW in Washington , D.C. It is 140 feet ( 43 m ) high and has 10 floors . Covering an entire city block , it is the largest privately owned office building in the District of Columbia . Current tenants include the Federal Housing Finance Agency and the Office of the Comptroller of the Currency . As of February 2014 , Constitution Center was worth $ 725.8 million , making it the most valuable , taxable property in the city . = = Original structure = = In the 1950s , the U.S. Congress , then the governing institution of the District of Columbia , undertook the Southwest D.C. urban renewal project , the first in the capital district and one of the earliest such programs in the nation . In 1946 , Congress passed the District of Columbia Redevelopment Act , which established the District of Columbia Redevelopment Land Agency ( RLA ) a</t>
+          <t>John Olver = John Walter Olver ( born September 3 , 1936 ) is an American politician who was the U.S. Representative for Massachusetts 's 1st congressional district from 1991 to 2013 . Raised on a farm in Pennsylvania , Olver graduated from college at the age of 18 and went on to earn a Ph.D. in chemistry from the Massachusetts Institute of Technology , and later taught chemistry at the University of Massachusetts Amherst for eight years . He served in both chambers of the Massachusetts General Court , being elected to the Massachusetts House of Representatives in 1968 , and the Massachusetts Senate in 1972 . He ran in a 1991 special election to succeed 17-term Congressman Silvio O. Conte , who died in office . He was the first Democrat to ever represent the 1st congressional district . Olver announced that he would not seek re-election in 2012 , and retired at the end of his eleventh term in Congress after his district was dismantled in redistricting . = = Early life , education , and</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Design management = Design management is a business discipline that uses project management , design , strategy , and supply chain techniques to control a creative process , support a culture of creativity , and build a structure and organization for design . The objective of design management is to develop and maintain a business environment in which an organization can achieve its strategic and mission goals through design , and by establishing and managing an efficient and effective system . Design management is a comprehensive activity at all levels of business ( operational to strategic ) , from the discovery phase to the execution phase . " Simply put , design management is the business side of design . Design management encompasses the ongoing processes , business decisions , and strategies that enable innovation and create effectively-designed products , services , communications , environments , and brands that enhance our quality of life and provide organizational success . "</t>
+          <t>Samuel J. Briskin = Samuel J. Briskin ( February 8 , 1896 – November 14 , 1968 ) was one of the foremost producers of Hollywood 's Golden Age , who was the head of production during his career of 3 of the " Big 8 " major film studios of its Golden Age : Columbia ( twice ) , Paramount , and RKO . In the late 1950s he would also serve briefly on the board of directors of another major , MGM . During World War II Briskin served in the Army 's Signal Corps as a film producer , attaining the rank of Lieutenant Colonel . After the war he co-founded Liberty Films with Frank Capra , who were later joined by William Wyler and George Stevens . The studio only produced two films , but both are now considered classics : It 's a Wonderful Life and State of the Union . All three of his brothers were also film producers , as well as one of his sons , and his sister was married to the eventual Chairman of Columbia , where Briskin spent the last decade of his life as a vice-president and head of produc</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Steve Beshear = Steven Lynn " Steve " Beshear ( born September 21 , 1944 ) is an American attorney and Democratic Party politician who was the 61st Governor of Kentucky from 2007 to 2015 . He served in the Kentucky House of Representatives from 1974 to 1979 , was the state 's Attorney General from 1980 to 1983 , and was the 49th Lieutenant Governor from 1983 to 1987 . After graduating from the University of Kentucky College of Law in 1968 , Beshear briefly practiced law in New York before returning to Kentucky and being elected to the state legislature , where he gained a reputation as a consumer advocate . He parlayed that reputation into a term as attorney general , serving under Governor John Y. Brown , Jr . As attorney general , Beshear issued an opinion that copies of the Ten Commandments would have to be removed from the walls of the state 's classrooms in the wake of the U.S. Supreme Court 's decision in Stone v. Graham . He also clashed with first lady Phyllis George Brown when</t>
+          <t>Robert C. Michelson = Robert C. Michelson ( born 1951 ) is an American engineer and academic widely known for inventing the entomopter , a biologically inspired flapping-winged aerial robot , and for having established the International Aerial Robotics Competition . He has received degrees in electrical engineering from the Virginia Polytechnic Institute and the Georgia Institute of Technology . Michelson 's professional career began at the U.S. Naval Research Laboratory where he worked on radar-based ocean surveillance systems . He later became a member of the research faculty at the Georgia Institute of Technology . At the Georgia Tech Research Institute ( GTRI ) he was involved in full-time research , directing over 30 major research programs . He is the author of three U.S. patents and over 90 journal papers , book chapters and reports . Michelson also developed classes in avionics and taught in the School of Aerospace Engineering at the Georgia Institute of Technology until his re</t>
         </is>
       </c>
     </row>
@@ -1001,32 +1001,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>film role appeared award acting director roles success actor performance directed comedy drama actors films cast movie festival starred television received box awards played actress career play production starring musical reviews theatre alongside debut critical stage best filmography tamil supporting cinema critics stars romantic thriller screen hollywood telugu script performances successful broadway adaptation feature nominations filming life worked mother playing nominated wrote opposite portrayed ballet acclaim screenplay critic acclaimed born met critically commercial theatrical remake picture productions screened indian los_angeles directorial married personal work lynch bollywood producer woman cannes actresses portrayal bafta academy_award movies miss comedian dance voice earned grossed</t>
+          <t>['film', 'role', 'appeared', 'award', 'acting', 'director', 'roles', 'success', 'actor', 'performance', 'directed', 'comedy', 'drama', 'actors', 'films']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Død Kalm = " Død Kalm " is the nineteenth episode of the second season of the American science fiction television series The X-Files . It premiered on the Fox network on March 10 , 1995 . The story was written by Howard Gordon , the teleplay was written by Gordon and Alex Gansa , and the episode was directed by Rob Bowman . The episode is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . " Død Kalm " earned a Nielsen household rating of 10.7 , being watched by 10.2 million households in its initial broadcast . The episode received mostly mixed-to-positive reviews . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . In the episode , Mulder and Scully are called in when a boatload of survivors from a U.S. Navy destroyer escort are found . What particularly catches Agent Mulder 's attention is that all of these sailors appear to have aged many </t>
+          <t>Kajol = Kajol Devgan ( née Mukherjee ) ( born 5 August 1974 ) , known mononymously as Kajol , is an Indian film actress who predominantly works in Hindi cinema . Born into the Mukherjee-Samarth family , she is the daughter of actress Tanuja and late filmmaker Shomu Mukherjee . Through her Bollywood career , Kajol has established herself as one of the most popular actresses in India . She is the recipient of numerous accolades , including six Filmfare Awards , among twelve nominations , and along with her late aunt Nutan , holds the record for most Best Actress wins at Filmfare , with five . In 2011 , the Government of India awarded her with the Padma Shri , the fourth highest civilian honour of the country . Kajol made her acting debut with the unsuccessful romantic drama Bekhudi ( 1992 ) , while still in school . She quit her studies to pursue acting , and had her first commercial successes with the thriller Baazigar ( 1993 ) . She subsequently rose to prominence by playing the lead f</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lactarius vietus = Lactarius vietus ( commonly known as the grey milkcap ) is a species of fungus in the family Russulaceae , first described by Elias Magnus Fries . It produces moderately sized and brittle mushrooms , which grow on the forest floor or on rotting wood . The flattened-convex cap can vary in shape , sometimes forming the shape of a wide funnel . It is typically grey , but the colour varies . The species has crowded , light-coloured gills , which produce white milk . The spore print is typically whitish , but also varies considerably . The mushrooms typically have a strong , acrid taste and have been described as inedible , but other authors have described them as consumable after boiling . L. vietus feeds by forming an ectomycorrhizal relationship with surrounding trees , and it favours birch . It grows in autumn months and is fairly common in Europe , North America and eastern Asia . = = Taxonomy = = Lactarius vietus was first described by Elias Magnus Fries in 1821 as </t>
+          <t>Gerty Cori = Gerty Theresa Cori ( née Radnitz ; August 15 , 1896 – October 26 , 1957 ) was a Czech-American biochemist who became the third woman — and first American woman — to win a Nobel Prize in science , and the first woman to be awarded the Nobel Prize in Physiology or Medicine . Cori was born in Prague ( then in the Austro-Hungarian Empire , now the Czech Republic ) . Gerty was not a nickname , but rather she was named after an Austrian warship . Growing up at a time when women were marginalized in science and allowed few educational opportunities , she gained admittance to medical school , where she met her future husband Carl Ferdinand Cori ; upon their graduation in 1920 , they married . Because of deteriorating conditions in Europe , the couple emigrated to the United States in 1922 . Gerty Cori continued her early interest in medical research , collaborating in the laboratory with Carl . She published research findings coauthored with her husband , as well as publishing sin</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Christine Hakim = Herlina Christine Natalia Hakim ( born 25 December 1956 ) , also known by the popular name Christine Hakim , is an Indonesian actress , film producer , and activist . Born to a devout Muslim family of a mixed-race background in Jambi , she grew up in Yogyakarta , aspiring to be an architect or psychologist . This changed after she was discovered by Teguh Karya for his 1973 movie Cinta Pertama , a role which garnered her a Citra Award for Best Actress and convinced her to follow a career in acting . Since then , she has starred in numerous films , including 1977 's Badai Pasti Berlalu and 1988 's Tjoet Nja ' Dhien ; she also had a minor role in the 2010 Hollywood movie Eat Pray Love . As of 2011 , she has won six Citra Awards , received a lifetime achievement award from the Cinemanila International Film Festival , and served as a member of the jury at the Cannes Film Festival Hakim began branching out from acting in 1998 , beginning with roles as producer of Daun di At</t>
+          <t>Amanda Seyfried = Amanda Michelle Seyfried ( / ˈsaɪfrɛd / SY-fred ; born December 3 , 1985 ) is an American actress , model , and singer . She began her career as a model when she was 11 , then her acting career at 15 began an acting career with recurring parts on the soap operas As the World Turns and All My Children . In 2004 , Seyfried made her film debut in the teen comedy Mean Girls . Her subsequent supporting roles were in independent films , such as the drama Nine Lives ( 2005 ) and the crime drama Alpha Dog ( 2006 ) , she also had a recurring role in the UPN drama show Veronica Mars ( 2004 – 06 ) . Between 2006 and 2011 , she starred on the HBO drama series Big Love and appeared in the 2008 musical feature film Mamma Mia ! . Her other appearances include leading roles in the black comedy horror film Jennifer 's Body ( 2009 ) , as a call girl in the erotic thriller Chloe ( 2009 ) , the romantic drama-war film Dear John ( 2010 ) , and the romantic drama Letters to Juliet ( 2010 )</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Carl Tanzler = Carl Tanzler , or sometimes Count Carl von Cosel ( February 8 , 1877 – July 3 , 1952 ) , was a German-born radiologic technologist at the United States Marine Hospital in Key West , Florida who developed a morbid obsession for a young Cuban-American tuberculosis patient , Elena Milagro " Helen " de Hoyos ( July 31 , 1909 – October 25 , 1931 ) , that carried on well after the disease had caused her death . In 1933 , almost two years after her death , Tanzler removed Hoyos 's body from its tomb , and lived with the corpse at his home for seven years until its discovery by Hoyos 's relatives and authorities in 1940 . = = Name = = Tanzler went by many names ; he was listed as Georg Karl Tänzler on his German marriage certificate . He was listed as Carl Tanzler von Cosel on his United States citizenship papers , and he was listed as Carl Tanzler on his Florida death certificate . Some of his hospital records were signed Count Carl Tanzler von Cosel . = = Early life = = He was</t>
+          <t>Paul Thomas Anderson = Paul Thomas Anderson ( born June 26 , 1970 ) also known as P.T. Anderson , is an American film director , screenwriter and producer . Interested in film-making at a young age , Anderson was encouraged by his father Ernie Anderson ( a disc jockey , and television and radio announcer / voiceover artist ) to become a filmmaker . In 1993 , he wrote and directed a short film titled Cigarettes &amp; Coffee on a budget of $ 20,000 . After he attended the Sundance Institute , Anderson had a deal with Rysher Entertainment to direct his first feature film , a neo-noir crime thriller titled Hard Eight , in 1996 . Anderson received critical and commercial success for his film Boogie Nights ( 1997 ) , set during the Golden Age of Porn in the 1970s and 1980s . His third feature , Magnolia ( 1999 ) , received wide acclaim despite struggling at the box office . In 2002 , the romantic comedy-drama Punch-Drunk Love , Anderson 's fourth feature , was released to generally favorable rev</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Nate Parker = Nate Parker ( born November 18 , 1979 ) is an American actor , director , producer , writer and musical performer who has appeared in Beyond the Lights , Red Tails , The Secret Life of Bees , The Great Debaters , Arbitrage , Non-Stop , Felon and Pride . He was an All-American wrestler at both Great Bridge High School and the University of Oklahoma . Parker has been active in charitable work , donating his time both as a volunteer wrestling coach and a political activist . = = Background = = Parker was born in Norfolk , Virginia , to Carolyn , a 17-year-old mother at the time . His mother never married his biological father , but did wed the man who gave Parker his last name . Parker has four younger sisters . According to a DNA analysis , some of his ancestry is from the Tikar people of modern-day Cameroon . During Parker 's time in middle school , his mother fell in love with Walter Whitfield , who was stationed in Bath , Maine , in the United States Air Force . Although</t>
+          <t xml:space="preserve">The Little Mermaid ( 1989 film ) = The Little Mermaid is a 1989 American animated musical fantasy film produced by Walt Disney Feature Animation and released by Walt Disney Pictures . Based on the Danish fairy tale of the same name by Hans Christian Andersen , The Little Mermaid tells the story of a beautiful mermaid princess who dreams of becoming human . Written , directed , and produced by Ron Clements and John Musker , with music by Alan Menken and Howard Ashman ( who also served as a co-producer ) , the film features the voices of Jodi Benson , Christopher Daniel Barnes , Pat Carroll , Samuel E. Wright , Jason Marin , Kenneth Mars , Buddy Hackett , and René Auberjonois . The 28th Disney animated feature film , The Little Mermaid was released to theaters on November 17 , 1989 to largely positive reviews , garnering $ 84 million at the domestic box office during its initial release , and $ 211 million in total lifetime gross worldwide . After the success of the 1988 Disney / Amblin </t>
         </is>
       </c>
     </row>
@@ -1036,32 +1036,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>cambridge oxford boat competition silver summer competed referred medal seconds olympics compete athletes champions heat race championships crews finishing honour reigning thames rowing olympic races blues medals cox lengths contest paralympics beijing sport stroke bronze surrey universities coached athlete opponents excluding rowed university_of_cambridge fixture participants contained toss gold umpire isis university_of_oxford rower competing annually represented rivalry pounds junior coaches umpired wheelchair competitors participating participate middlesex handing favour swimming clear overall paralympic qualified boxing sports event hammersmith_bridge mile_post contested preliminary river_thames flag worldwide athletics ahead delegation course winner strokes polo participation favourites freestyle rowers disability reserve swimmer events consecutive qualification relay</t>
+          <t>['cambridge', 'oxford', 'boat', 'competition', 'silver', 'summer', 'competed', 'referred', 'medal', 'seconds', 'olympics', 'compete', 'athletes', 'champions', 'heat']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Far Away Places ( Mad Men ) = " Far Away Places " is the sixth episode of the fifth season of the American television drama series Mad Men and the 58th episode of the series overall . It was written by series creator and executive producer Matthew Weiner and writer Semi Chellas , and directed by Scott Hornbacher . It originally aired on AMC in the United States on April 22 , 2012 . The episode takes place almost entirely over a single day , telling three stories in a non-linear narrative . Peggy becomes alienated after separate fights with her boyfriend Abe and a client . Roger and Jane take LSD with a group of intellectuals , altering how they see the world and allowing them to speak honestly about their marriage . Don and Megan leave the office and take an impromptu road trip to Plattsburgh , New York , which doesn 't turn out as planned after Megan becomes aggrieved with how Don treats her . " Far Away Places " was watched by 2.6 million viewers and achieved 0.9 million viewers in t</t>
+          <t>Rich Girl ( Gwen Stefani song ) = " Rich Girl " is a song by American singer and songwriter Gwen Stefani from her debut solo studio album , Love . Angel . Music . Baby . ( 2004 ) . Produced by Dr. Dre , the track features American rapper Eve , and is a remake of Louchie Lou &amp; Michie One 's 1993 song of the same name , which is in turn an adaptation of the Fiddler on the Roof song " If I Were a Rich Man " . Stefani says the song discusses her dreams of fame and riches from the perspective of " when she was just an Orange County girl " . The last song to be included on the album , " Rich Girl " was released as the album 's second single in late 2004 to mixed reviews from music critics . It was a commercial success , reaching the top 10 on most of the charts it entered . In the United States , " Rich Girl " was certified gold , and it received a nomination for Best Rap / Sung Collaboration at the 47th Grammy Awards . = = Writing and development = = Stefani and Eve had previously collabora</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>The Boat Race 1978 = The 124th Boat Race between crews from the University of Oxford and the University of Cambridge took place on the River Thames on 25 March 1978 . Umpired by former Cambridge rower James Crowden , Oxford won in a time of 18 minutes and 58 seconds . The race was complicated by bad weather , and when faced with choppy water , a strong headwind and horizontal , driving rain , the Cambridge boat , which lacked splashboards , took on water and sank . It was the fifth time a boat had sunk during the event . In the reserve race , Cambridge 's Goldie beat Oxford 's Isis by one-and-a-quarter lengths . Cambridge won the 33rd Women 's Boat Race . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford and the University of Cambridge . First held in 1829 , the competition is a 4.2-mile ( 6.8 km ) race along the River Thames in southwest London . The rivalry is a major point of honour between the two universities and is followed thr</t>
+          <t>The Boat Race 1866 = The 23rd Boat Race took place on the River Thames on 24 March 1866 . The Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge . Oxford won by three lengths in a time of 25 minutes and 35 seconds , one of the slowest times in the history of the event . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Oxford went into the race as reigning champions , having defeated Cambridge by four lengths in the previous year 's race . Oxford led overall with twelve wins to Cambridge 's ten . In late 1865 , the Cambridge University Boat Club president Robert Kinglake wrote to Oxford in order to draw up</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Leilani Kai = Patty Seymour ( born January 23 , 1960 ) is a semi-retired professional wrestler , better known by her ring name Leilani Kai . She began training with The Fabulous Moolah right after finishing high school . In the 1980s , as part of the World Wrestling Federation ( WWF ) ' s Rock ' n ' Wrestling Connection , a storyline that combined wrestling and music , Kai defeated Wendi Richter to become the WWF Women 's Champion . Kai , however , lost the title at the inaugural WrestleMania event . She was later paired with Judy Martin , in a tag team that would become known as The Glamour Girls . The team held the WWF Women 's Tag Team Championship twice ( managed by " The Mouth of the South " Jimmy Hart ) and the LPWA Tag Team Championship once . In her later career , Kai returned briefly to the WWF in 1994 , challenging for the Women 's Championship at WrestleMania X. She also wrestled for World Championship Wrestling under the name Patty Stonegrinder and held the NWA World Women </t>
+          <t>2001 American Memorial = The 2001 American Memorial was a Championship Auto Racing Teams ( CART ) motor race held on September 15 , 2001 , at the EuroSpeedway Lausitz in Klettwitz , Germany . It was the 16th round of the 2001 CART season and the first race in the series to be held in Europe . Originally known as the German 500 , the race 's name was changed by CART in the aftermath of the September 11 attacks . Kenny Bräck won the race for Team Rahal ; his teammate Max Papis finished in second place , and Patrick Carpentier was third . The season points leader entering the race , Gil de Ferran , was awarded the pole position when qualifying was cancelled after a practice session was rained out . Bräck took the lead early in the race , and built a seven-second advantage before going off course while trying to lap another car . Carpentier took his place after the lap 64 incident , and held the lead until Tony Kanaan passed him on lap 95 . After passing Carpentier for second , Alex Zanard</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Navy SEALS ( video game ) = Navy SEALS is a shoot ' em up platform video game developed and published by Ocean Software . It was first released in the United Kingdom for the Amstrad CPC , Amstrad GX4000 and Commodore 64 in 1990 . It was later re-released in the rest of Europe for the ZX Spectrum , Atari ST and Amiga home computers in the following year . It was then ported to the Game Boy on 1 September 1991 in the United States . The game is based on the film of the same name and follows the protagonist , Lieutenant Dale Hawkins , progressing through five side-scrolling levels . The game was developed by Ocean Software , in which they were renowned for creating video games related to their respective films . Navy SEALS focuses on Hawkins recovering caches of Stinger missiles from Arab soldiers in the Middle East . The game received positive reviews upon release , with critics mainly praising the graphics , presentation and challenging gameplay . However , criticism was directed at the</t>
+          <t xml:space="preserve">Laurentia Tan = Laurentia Tan Yen Yi BBM PBM ( / lɒˈrɛnʃə / lo-REN-shə ; Chinese : 陈雁仪 ; pinyin : Chén Yànyí , pronounced [ tʂə ̌ n jɛ ̂ n í ] ) ( born 24 April 1979 ) , is a United Kingdom-based Singaporean Para-equestrian competitor . Tan developed cerebral palsy and profound deafness after birth , and moved to the United Kingdom with her parents at the age of three . She took up horse riding at age of five years as a form of physiotherapy . She subsequently completed her A-levels at the Mary Hare Grammar School , a residential special school for the deaf , and graduated with an honours degree from Oxford Brookes University in hospitality management and tourism . In March 2007 , the Riding for the Disabled Association Singapore ( RDA ) invited Tan to join the Singapore team for the World Para Dressage Championships at Hartpury College in Hartpury , Gloucester , in England in July that year . At this event , her first international competition , she did well enough to qualify for the </t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Aruba at the 2008 Summer Olympics = Aruba competed at the 2008 Summer Olympics in Beijing , China . Their participation marked their sixth Olympic appearance , and included the smallest number of athletes that had ever represented Aruba in its history . Two Arubans competed in the Olympic games : Jan Roodzant participated as a swimmer , and Fiderd Vis participated in judo . The Aruban delegation arrived in Beijing between August 1 and August 4 , including the athletes , coaches , and various officials from both the IOC and the Aruban Olympic Committee ( Comité Olimpico Arubano , COA ) , Aruba 's local Olympic committee . Fiderd Vis came to Beijing on special invitation from the IOC , which had observed his progress while he trained in Brazil . Vis was the flagbearer in the opening ceremony , while Roodzant was so in the closing ceremony . Both athletes were eliminated in the preliminary rounds on August 12 , 2008 ; consequently , Aruba did not earn any medals . = = Background = = Aruba</t>
+          <t>Alekseyev I-212 = The Alekseyev I-212 was a twin-engined , jet fighter designed in the USSR in 1947 at OKB-21 ( OKB - experimental design bureau ) . It was a two-seat variant of the I-21 ( Istrebitel ' - Fighter ) designed in response to a requirement for a very long-range fighter issued by the Voenno-Vozdushnye Sily ( VVS ) , ( Soviet Air Forces ) , in 1946 . Intended as an escort fighter , it was also designed for use as a night fighter and reconnaissance aircraft . Sources are unclear whether a prototype was built , but it is known that the aircraft never flew . = = Development = = After working as Lavochkin 's right-hand man during World War II , Semyon Alekseyev was appointed as Chief Designer of OKB-21 at Gor 'kiy in 1946 . The Council of the People 's Commissars directed Alekseyev , among others , to develop jet fighters using more powerful engines than the captured German examples and Soviet-built copies . The OKB was tasked to design a single-seat jet fighter that could meet t</t>
         </is>
       </c>
     </row>
@@ -1071,32 +1071,32 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>album music songs rock recorded recording band beatles lyrics musicians george_harrison sound harrison song bands track release live things guitar version vocals apple musical 1970s psychedelic included cover written record like material studio group drums backing solo folk metal reissue love single released compositions guitarist genre sessions describes morrison 1960s john_lennon acoustic tour slide recordings bass playing composition musician writes inspired albums piano style author progressive paul_mccartney producer guitars played rolling_stone riff success bob_dylan audience wrote drummer writing particularly biographer popular let blues krishna rhythm jazz lord biographers early emi described sleeve living overdubbed remastered rolling_stones glam late mojo issued</t>
+          <t>['album', 'music', 'songs', 'rock', 'recorded', 'recording', 'band', 'beatles', 'lyrics', 'musicians', 'george_harrison', 'sound', 'harrison', 'song', 'bands']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>The Voice Within = " The Voice Within " is a song recorded by American singer Christina Aguilera for her fourth studio album , Stripped ( 2002 ) . The song was written by Aguilera and Glen Ballard , with production handled by Ballard . It is a piano-driven ballad that talks about trusting oneself and one 's instincts . " The Voice Within " was released as the fifth and final single from Stripped on October 27 , 2003 by RCA Records . Upon its release , " The Voice Within " received mainly positive reviews from music critics , who called it an inspirational ballad and praised Aguilera 's strong vocals on the track . Some likened the song to works by Celine Dion and Mariah Carey . Commercially , " The Voice Within " achieved moderate success on charts worldwide , peaking within the top ten of charts in several countries including Australia , Ireland , Switzerland and the United Kingdom , and it reached number 33 on the US Billboard Hot 100 . An accompanying music video for " The Voice Wit</t>
+          <t>My Sweet Lord = " My Sweet Lord " is a song by English musician and former Beatle George Harrison that was released in November 1970 on his triple album All Things Must Pass . Also issued as a single , Harrison 's first as a solo artist , " My Sweet Lord " topped charts worldwide and was the biggest-selling single of 1971 in the UK . In America and Britain , the song was the first number 1 single by an ex-Beatle . Harrison originally gave the song to his fellow Apple Records artist Billy Preston to record ; this version , which Harrison co-produced , appeared on Preston 's Encouraging Words album in September 1970 . Harrison wrote " My Sweet Lord " in praise of the Hindu god Krishna , while at the same time intending the lyrics to serve as a call to abandon religious sectarianism through his deliberate blending of the Hebrew word hallelujah with chants of " Hare Krishna " and Vedic prayer . The recording features producer Phil Spector 's Wall of Sound treatment and heralded the arrival</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>More popular than Jesus = " More popular than Jesus " ( or " Bigger than Jesus " ) was a controversial remark made by the Beatles ' John Lennon in 1966 . Lennon said that Christianity was in decline and that the Beatles had become more popular than Jesus Christ . The comment drew no controversy when originally published in the United Kingdom , but angry reactions flared up in Christian communities when it was republished in the United States five months later . Lennon had originally made the remark in March 1966 during an interview with Maureen Cleave for the London Evening Standard , which drew no public reaction . When Datebook , a US teen magazine , quoted Lennon 's comments in August , five months later , extensive protests broke out in the Southern United States . Some radio stations stopped playing Beatles songs , their records were publicly burned , press conferences were cancelled , and threats were made . The controversy coincided with the group 's US tour in August 1966 , and</t>
+          <t xml:space="preserve">Christian metal = Christian metal , also known as white metal or heavenly metal , is a form of heavy metal music usually defined by its message using song lyrics as well as the dedication of the band members to Christianity . Christian metal is typically performed by professed Christians sometimes principally for Christians who listen to heavy metal music and often produced and distributed through various Christian networks . Christian metal bands exist in all the subgenres of heavy metal music , and the only common link among most Christian metal bands are the lyrics . The Christian themes are often melded with the subjects of the genre the band is rooted in , regularly providing a Christian take on the subject matter . It has been argued that the marginal yet transnational Christian metal subculture provides its core members an alternative religious expression and Christian identity , and that the music serves the purpose of offering a positive message through lyrical content . This </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Roof ( Back in Time ) = " The Roof " is a song by American singer-songwriter Mariah Carey , taken from her sixth studio album , Butterfly ( 1997 ) . It was released as the third single from the album in Europe , on March 20 , 1998 by Columbia Records . Similar to the treatments of " Butterfly " and " Breakdown " , " The Roof " received a limited worldwide release due to Carey 's conflict at the time with Sony . The song was written and produced by Carey and Trackmasters , and is built around a sample from " Shook Ones part II " by Mobb Deep . The song 's lyrics recount an intimate roof-top encounter between lovers , and how the memory affects the protagonist . The extended remix features a rap verse by Mobb Deep ; both versions were well received by contemporary music critics . In the music video , Carey is seen in a limousine recounting an encounter she shared on a rainy night . Additionally , past scenes of the event are shown , with Carey caressing her lover at a roof-top party </t>
+          <t xml:space="preserve">Mass in B minor structure = The Mass in B minor is Johann Sebastian Bach 's only setting of the complete Latin text of the Ordinarium missae ( short : mass ) . Towards the end of his life , mainly in 1748 and 1749 , he finished composing new sections and compiling it into a complex , unified structure . Bach structured the work in four parts : No. 1 Missa No. 2 Symbolum Nicenum No. 3 Sanctus No. 4 Osanna , Benedictus , Agnus Dei et Dona nobis pacem The four sections of the manuscript are numbered , and Bach 's usual closing formula ( S.D.G = Soli Deo Gloria ) is found at the end of the Dona nobis pacem . Some parts of the mass were used in Latin even in Lutheran Leipzig , and Bach had composed them : five settings of the Missa , containing Kyrie and Gloria , and several additional settings of Kyrie and Sanctus . To achieve the Missa tota , a setting of the complete text of the mass , he combined his most elaborate Missa , the Missa in B minor , written in 1733 for the court in Dresden </t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Burger King legal issues = The legal issues of Burger King include several legal disputes and lawsuits , as both plaintiff and defendant , of the international fast food restaurant chain Burger King ( BK ) , in the years since its founding in 1954 . Situations involving these many legal topics have affected almost every aspect of the company 's operations . Depending on the ownership and executive staff at the time of these incidents , the company 's responses to these challenges have ranged from a conciliatory dialog with its critics and litigants to a more aggressive opposition with questionable tactics and negative consequences . The company 's response to these various issues has drawn praise , scorn , and accusations of political appeasement from different parties over the years . Controversies and disputes have arisen from a diverse source of group such as People for the Ethical Treatment of Animals ( PETA ) over the welfare of animals , governmental and social agencies over heal</t>
+          <t>Leucopaxillus giganteus = Leucopaxillus giganteus , commonly known as the giant leucopax ( formerly as the giant clitocybe ) or the giant funnel , is a saprobic species of fungus in the Tricholomataceae family . As its common names imply , the fruit body , or mushroom , can become quite large — the cap reaches diameters of up to 40 cm ( 16 in ) . It has a white or pale cream cap , and is funnel-shaped when mature , with the gills running down the length of the stem . Considered by some to be a choice edible when young , this species has a cosmopolitan distribution , and is typically found growing in groups or rings in grassy pastures , roadside hedges , or woodland clearings . Leucopaxillus giganteus contains a number of bioactive compounds , one of which has displayed antibiotic and anti-tumor properties in laboratory tests . = = Taxonomy = = The species was first described as Agaricus giganteus by English naturalist James Sowerby in 1809 , who illustrated it in his book Coloured Figu</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Flu Shot ( 30 Rock ) = " Flu Shot " is the eighth episode of the third season of the American television comedy series 30 Rock . It was written by Jon Pollack , and directed by series producer Don Scardino . The episode originally aired on the National Broadcasting Company ( NBC ) in the United States on January 15 , 2009 . Guest stars in this episode include George Bartenieff , Scott Bryce , Salma Hayek , and Chris Parnell . In the episode , Liz Lemon ( Tina Fey ) campaigns for her staff 's right to get flu shots from Dr. Leo Spaceman ( Parnell ) , but Jack Donaghy ( Alec Baldwin ) will not allow it due to a limited supply . Meanwhile , Jack tries to think of creative ways to spend time with his girlfriend , Elisa ( Hayek ) , as she works seven days a week . At the same time , Jenna Maroney ( Jane Krakowski ) and Tracy Jordan ( Tracy Morgan ) try to do something nice for the crew . " Flu Shot " received a mixed response from television critics , with Robert Canning of IGN concluding t</t>
+          <t>Music of the Final Fantasy series = Final Fantasy is a media franchise created by Hironobu Sakaguchi and owned by Square Enix that includes video games , motion pictures , and other merchandise . The series began in 1987 as an eponymous role-playing video game developed by Square , spawning a video game series that became the central focus of the franchise . The music of the Final Fantasy series refers to the soundtracks of the Final Fantasy series of video games , as well as the surrounding medley of soundtrack , arranged , and compilation albums . The series ' music ranges from very light background music to emotionally intense interweavings of character and situation leitmotifs . The franchise includes a main series of numbered games as well as several spin-off series such as Crystal Chronicles and the Final Fantasy Tactics series . The primary composer of music for the main series was Nobuo Uematsu , who single-handedly composed the soundtracks for the first nine games , as well as</t>
         </is>
       </c>
     </row>
@@ -1106,32 +1106,32 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>song video number like performance tour music madonna performed best songs stage beyoncé week gaga single dance shows chart called wrote spears live audience said dancers singer million felt described noted tickets gave love sold way received included performances billboard hot version musical choreography critics concert fans glee album praised featured release pop released commented debuted according wearing saying list girl added night black kurt sang copies choreographed track wanted costumes onstage dancing britney dress scene interlude awards spectacle cyrus scenes look broadway total weeks cover end lady_gaga singing artist videos lyrics dates napoleon rachel set people mtv different covered</t>
+          <t>['song', 'video', 'number', 'like', 'performance', 'tour', 'music', 'madonna', 'performed', 'best', 'songs', 'stage', 'beyoncé', 'week', 'gaga']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Little owl = The little owl ( Athene noctua ) is a bird that inhabits much of the temperate and warmer parts of Europe , Asia east to Korea , and north Africa . It was introduced into Britain at the end of the nineteenth century and into the South Island of New Zealand in the early twentieth century . This owl is a member of the typical or true owl family , Strigidae , which contains most species of owl , the other grouping being the barn owls , Tytonidae . It is a small , cryptically coloured , mainly nocturnal species and is found in a range of habitats including farmland , woodland fringes , steppes and semi-deserts . It feeds on insects , earthworms , other invertebrates and small vertebrates . Males hold territories which they defend against intruders . This owl is a cavity nester and a clutch of about four eggs is laid in spring . The female does the incubation and the male brings food to the nest , first for the female and later for the newly hatched young . As the chicks grow ,</t>
+          <t>Back from Vacation = " Back from Vacation " is the twelfth episode of the third season of the American comedy television series The Office , and the show 's 40th episode overall . It first aired on January 4 , 2007 , on NBC , and was the first episode to air after the December holiday hiatus . " Back from Vacation " was the first script written by Justin Spitzer for the series . Julian Farino served as the episode director . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania , branch of the fictional Dunder Mifflin Paper Company . In this episode , Michael Scott ( Steve Carell ) returns from his vacation in Jamaica and has a luau in the warehouse to celebrate . It is revealed that he went to Jamaica with Jan Levinson ( Melora Hardin ) when a racy photograph of him and Jan is circulated . Meanwhile , Karen Filippelli ( Rashida Jones ) and Jim Halpert ( John Krasinski ) have an argument over Karen 's living situation , leading to Pam Beesly ( Jenna F</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Just the Way You Are ( Bruno Mars song ) = " Just the Way You Are " is the debut solo single recorded by American singer-songwriter Bruno Mars . It is the lead single from his debut studio album , Doo-Wops &amp; Hooligans ( 2010 ) . The song was written by The Smeezingtons , Khalil Walton and Needlz and produced by The Smeezingtons , and Needlz . It was released in the United States to Contemporary hit radio on August 10 , 2010 . The track was added to BBC Radio 1 A Playlist in the United Kingdom , and was released in the United Kingdom on September 19 , 2010 as " Just the Way You Are ( Amazing ) " . The debut single received positive reviews from critics , who considered it a stand-out track on Doo-Wops &amp; Hooligans and praised The Smeezington 's production . It won a Grammy Award for Best Male Pop Vocal Performance at the 2011 ceremony . The song peaked at number one on the US Billboard Hot 100 and Mainstream Top 40 charts and charted in the top five in other countries . It was certified </t>
+          <t>Anticipating = " Anticipating " is a song recorded by American singer Britney Spears for her self-titled third studio album , Britney ( 2001 ) . It was written by Spears alongside the song 's producers Brian Kierulf and Josh Schwartz . The song was released on June 24 , 2002 , by Jive Records , as the fourth single from the album in France . Lyrically , the disco song is about friendship and camaradie between women . It was met with critical praise , with reviewers complimenting its empowering lyrics and comparing it to 1980s compositions of Madonna , Rick Astley and Janet Jackson 's " All for You " . " Anticipating " achieved minor commercial success , peaking at number 38 on the French Singles Chart . The song was promoted with a performance in the Dream Within a Dream Tour ( 2001 – 2002 ) , where Spears wore a patched denim skirt and danced in front of giant crayon drawings . An accompanying music video , directed by Marty Callner , consisted of the performance from Live from Las Ve</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Gimme More = " Gimme More " is a song recorded by American singer Britney Spears for her fifth studio album , Blackout ( 2007 ) . It was released on September 18 , 2007 by Jive Records as the lead single from the album . The song was written by Nate " Danja " Hills , James " Jim Beanz " Washington , Keri Hilson and Marcella Araica , while production was handled by Jack Black and vocal production was handled by Washington and Hilson . " Gimme More " was recorded in 2006 during Spears 's second pregnancy , and was one of the first solo productions by Danja . The song opens with an intro in which Spears says the phrase " It 's Britney , bitch " . Musically , " Gimme More " is an uptempo dance-pop song with breathy vocals and influences from other genres , such as electro music . The track closes with a speak-sing outro by Danja . " Gimme More " received positive reviews from critics , praising the music and Spears 's breathy vocals . The song peaked at number three on the U.S. Billboard H</t>
+          <t>Boyfriend ( Justin Bieber song ) = " Boyfriend " is a song by Canadian recording artist Justin Bieber , taken from his third studio album Believe ( 2012 ) . Bieber explained that the track would surprise people in different ways , since it is a musical departure from his previous material . A snippet of " Boyfriend " was previewed on The Ellen DeGeneres Show on March 1 , 2012 , Bieber 's 18th birthday . The song was announced as a single on the same day , and was released on March 26 , 2012 . The cover art was revealed on March 19 , 2012 . Musically , " Boyfriend " is a R &amp; B influenced song that features pop beats reminiscent of American record producer Pharrell Williams and boy band ' N Sync . The instrumentation is kept in a lower sound to highlight Bieber 's vocals . However , critics dismissed the lyrics as immature and silly . " Boyfriend " was a commercial success , debuting at number two on the Billboard Hot 100 after selling a total of 521,000 digital units of the single . The</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>She Ain 't You = " She Ain 't You " is a song by American recording artist Chris Brown . The mid-tempo R &amp; B , pop-flavored ballad was written by Brown , Jean Baptiste , Ryan Buendia , Kevin McCall and Jason Boyd , and was produced by Free School . It was sent to urban contemporary radio in the United States on March 28 , 2011 , as the fourth US single from Brown 's fourth studio album , F.A.M.E. ( 2011 ) . Musically , " She Ain 't You " samples the remixed version of SWV 's " Right Here " ( 1993 ) , which in turn samples Michael Jackson 's " Human Nature " ( 1983 ) . The song 's lyrics are about Brown falling in and out of love . " She Ain 't You " received mixed to positive reviews from music critics . " She Ain 't You " reached number five on the US Hot R &amp; B / Hip-Hop Songs chart , number 17 on the US Pop Songs chart , and number 27 on the US Billboard Hot 100 chart . Although it was only officially released in the US , the song also charted in Australia , Canada , New Zealand , Sl</t>
+          <t>Washington State Route 538 = State Route 538 ( SR 538 , alternatively named College Way ) is a 3.62-mile ( 5.83 km ) long state highway located within the northern area of Mount Vernon city limits and the urban growth boundary , located in Skagit County , a subdivision of the U.S. state of Washington . The highway , which has existed as a county road since 1911 , travels from Interstate 5 ( I-5 ) in the west , passing former U.S. Route 99 ( US 99 ) , now Riverside Drive , and Skagit Valley College 's main Mount Vernon campus before terminating at a roundabout with SR 9 . Before being designated Secondary State Highway 1G ( SSH 1G ) in 1937 , the current roadway that is now SR 538 was a county road through farmland for 26 years . SSH 1G traveled between Primary State Highway 1 ( PSH 1 ) , also known as US 99 , and SSH 1A until 1964 , when the current designation of SR 538 was created . US 99 was bypassed by I-5 after 1966 and became Riverside Drive . The roundabout at SR 9 was construct</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Veronica Mars = Veronica Mars is an American teen noir mystery drama television series created by screenwriter Rob Thomas . The series is set in the fictional town of Neptune , California , and stars Kristen Bell as the eponymous character . The series premiered on September 22 , 2004 , during television network UPN 's final two years , and ended on May 22 , 2007 , after a season on UPN 's successor , The CW , airing for three seasons total . Veronica Mars was produced by Warner Bros. Television , Silver Pictures Television , Stu Segall Productions , and Rob Thomas Productions . Joel Silver and Rob Thomas were executive producers for the entire run of the series , while Diane Ruggiero was promoted in the third season . Veronica Mars is a student who progresses from high school to college while moonlighting as a private investigator under the tutelage of her detective father . In each episode , Veronica solves a different stand-alone case while working to solve a more complex mystery . </t>
+          <t>Europa Point Lighthouse = The Europa Point Lighthouse , also referred to as the Trinity Lighthouse at Europa Point and the Victoria Tower or La Farola in Llanito , is a lighthouse at Europa Point , on the southeastern tip of the British Overseas Territory of Gibraltar , on the southern end of the Iberian Peninsula , at the entrance to the Mediterranean Sea . Europa Lighthouse was inaugurated on 1 August 1841 in a brief ceremony witnessed by about 10,000 people . The first upgrade of the lighthouse occurred in 1864 , when the single-wick lamp was replaced with a Chance Brothers four-wick burner , with further changes in 1875 and in 1894 when the amount of light emitted was increased . A three incandescent mantle burner was added in 1905 . Following further modernisation in the 20th century , the lighthouse was fully automated in 1994 . Europa Point Lighthouse is operated by Trinity House . The cylindrical tower is painted white , with a wide red horizontal band in the middle . The light</t>
         </is>
       </c>
     </row>
@@ -1141,32 +1141,32 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>class built main guns line castle new service use long locomotives london speed intended locomotive fire continued range gun designed high war increased ships end originally construction additional carried lines tons maximum railways railway turrets large extended station designs inch turret work design provided aircraft tower instead control steam defences remained decided initially forward mounted power passenger armour armament gauge services bailey artillery fitted castles trains replaced standard short fortification heavy light original south reduced existing required towers rounds ran running improved century mph opened converted belt allow period battlecruisers engines taken proved delivered better gatehouse platform early boiler need</t>
+          <t>['class', 'built', 'main', 'guns', 'line', 'castle', 'new', 'service', 'use', 'long', 'locomotives', 'london', 'speed', 'intended', 'locomotive']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>HMS Renown ( 1895 ) = HMS Renown was a second-class predreadnought battleship built for the Royal Navy in the early 1890s . Intended to command cruiser squadrons operating on foreign stations , the ship served as the flagship of the North America and West Indies Station and the Mediterranean Fleet early in her career . Becoming obsolete as cruiser speeds increased , Renown became a royal yacht and had all of her secondary armament removed to make her more suitable for such duties . She became a stoker 's training ship in 1909 and was listed for disposal in 1913 . The ship was sold for scrap in early 1914 . = = Design and description = = Production of a new 12-inch gun was behind schedule and the three battleships planned for the 1892 Naval Programme that were intended to use the new gun had to be delayed . In their stead , an improved Centurion-class battleship design was chosen to keep the workers at Pembroke Dockyard fully employed . No formal requirement for a second-class battleshi</t>
+          <t>Siege of Lal Masjid = The Siege of Lal Masjid ( Urdu : لال مسجد محاصرہ , code-named Operation Sunrise ) was a confrontation in July 2007 between Islamic fundamentalist militants and the Government of Pakistan , led by President Pervez Musharraf and Prime Minister Shaukat Aziz . The focal points of the operation were the Lal Masjid ( " Red Mosque " ) and the Jamia Hafsa madrasah complex in Islamabad , Pakistan . Since January 2006 , Lal Masjid and the adjacent Jamia Hafsa madrasah had been operated by Islamic militants led by two brothers , Maulana Abdul Aziz and Abdul Rashid Ghazi . This organisation advocated the imposition of Sharia ( Islamic religious law ) in Pakistan and openly called for the overthrow of the Pakistani government . Lal Masjid was in constant conflict with authorities in Islamabad for 18 months prior to the military operation . They engaged in violent demonstrations , destruction of property , kidnapping , arson and armed clashes with the authorities . After Lal Ma</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>North Circular Road = The North Circular Road ( officially the A406 and sometimes known as simply the North Circular ) is a 25.7-mile-long ( 41.4 km ) ring road around Central London in England . It runs from Chiswick in the west to Woolwich in the east , and connects the various suburbs in the area , including Ealing , Willesden , Wembley , Southgate , Tottenham , Woodford and Barking . Together with its counterpart , the South Circular Road , it forms a ring road through the Outer London suburbs . This ring road does not make a complete circuit of the city , being C-shaped rather than a complete loop as the crossing of the River Thames in the east is made on the Woolwich Ferry . The road was originally designed to connect local industrial communities together in addition to bypassing London , and was constructed in the 1920s and ' 30s . It received significant upgrades after the Second World War , and was at one point planned to be upgraded to motorway as part of the controversial an</t>
+          <t>SECR N1 class = The SECR N1 class was a type of 3-cylinder 2-6-0 ( ' mogul ' ) steam locomotive designed by Richard Maunsell for mixed traffic duties , initially on the South Eastern and Chatham Railway ( SECR ) , and later operated for the Southern Railway ( SR ) . The N1 was a development of the basic principles established by the Great Western Railway 's ( GWR ) Chief Mechanical Engineer ( CME ) George Jackson Churchward and by Maunsell 's previous N class design . The N1 prototype was the result of modifications made to N class No. 822 during construction in 1922 . The locomotive became operational in 1923 and used parts interchangeable with other Maunsell locomotive classes . The prototype N1 was the only member of the class constructed before the SECR became part of the Southern Railway at the Grouping in 1923 , and featured a variant of the Gresley conjugated valve gear designed by Harold Holcroft . The class set the precedent for the Southern Railway 's subsequent 3-cylinder de</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Avro Vulcan = The Avro Vulcan ( later Hawker Siddeley Vulcan from July 1963 ) is a jet-powered tailless delta wing high-altitude strategic bomber , which was operated by the Royal Air Force ( RAF ) from 1956 until 1984 . Aircraft manufacturer A.V. Roe and Company ( Avro ) designed the Vulcan in response to Specification B.35 / 46 . Of the three V bombers produced , the Vulcan was considered the most technically advanced and hence the riskiest option . Several scale aircraft , designated Avro 707 , were produced to test and refine the delta wing design principles . The Vulcan B.1 was first delivered to the RAF in 1956 ; deliveries of the improved Vulcan B.2 started in 1960 . The B.2 featured more powerful engines , a larger wing , an improved electrical system and electronic countermeasures ( ECM ) ; many were modified to accept the Blue Steel missile . As a part of the V-force , the Vulcan was the backbone of the United Kingdom ’ s airborne nuclear deterrent during much of the Cold War</t>
+          <t>Cine City , Withington = Cine City was a cinema in Withington , Manchester , England located at 494 Wilmslow Road , Withington , Manchester , M20 3BG . It opened in 1912 as The Scala , and was the third cinema to open in Britain . During the 1930s , cinemas became increasingly popular ; The Scala was one of 109 cinemas in Manchester at its peak . The road outside was hit by a small bomb during the Second World War , but the cinema ( which was showing several films at the time ) survived with only minor damage . After the war , television led to a decline in cinema attendances , and by 1965 , only 40 cinemas remained in Manchester . Cine City closed in July 2001 , making it the third-longest running cinema in England . By 2005 the building was in a bad state of repair , and was threatened with demolition . Although heritage groups won a stay of execution , the cinema was demolished in spring 2008 . A replacement building is planned for the site . = = History = = The cinema opened in 191</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Spencer ( surname ) = Spencer ( also Spence , Spender , Spens , and Spenser ) is a surname . The origin can be traced directly to Robert d 'Abbetot , who is listed as Robert le Dispenser , a tenant-in-chief of several counties , in the Domesday Book of 1086 . Robert was possibly one of the Norman knights who fought alongside ( or accompanied ) William the Conqueror in the defeat of Harold II , King of England at the Battle of Hastings in 1066 . There is little doubt that both Robert and his brother Urse came to England at about the time of the Battle of Hastings . They were both beneficiaries of William over the years , and were given titles and substantial land and property — suggesting repayment for some earlier deeds . It is likely that Robert 's first acknowledgment was his official appointment as Royal " Dispencier " sometimes expressed more grandly as " Royal Steward " , " King 's Steward " or " Lord Steward " . As dispenser of provisions to the King and his household Robert was </t>
+          <t>Lion-class battlecruiser = The Lion class were a class of battlecruisers built for the British Royal Navy before World War I. Nicknamed the " Splendid Cats " , the ships were a significant improvement over their predecessors of the Indefatigable class in terms of speed , armament and armour . The Lion-class battlecruisers were 2 knots ( 3.7 km / h ; 2.3 mph ) faster , exchanged the 12-inch ( 305 mm ) guns of the older ships for 13.5-inch ( 343 mm ) guns , and had a waterline armour belt 9 inches ( 229 mm ) thick versus the 6 inches ( 152 mm ) of the Indefatigables . These improvements were in response to the German Moltke class , the first German battlecruisers , which were larger and more powerful than the first British battlecruisers of the Invincible class . Lion served as the flagship of the Grand Fleet 's battlecruisers throughout World War I , except when she was being refitted or under repair . She sank the German light cruiser Cöln during the Battle of Heligoland Bight and serv</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Naroda Patiya massacre = The Naroda Patiya massacre took place on 28 February 2002 at Naroda , in Ahmedabad , India , during the 2002 Gujarat riots . 97 Muslims were killed by a mob of approximately 5,000 people , organised by the Bajrang Dal , a militant wing of the Vishva Hindu Parishad , and supported by the Bharatiya Janata Party which was in power in the Gujarat State Government . The massacre at Naroda occurred during the bandh ( strike protest ) called by Vishwa Hindu Parishad ; a day after the Godhra train burning . During the post-Godhra rioting , which lasted over 10 hours , during which the mob looted , stabbed , sexually assaulted , gang-raped and burnt people individually and in groups . After the conflict , a curfew was imposed in the state and army troops were called in to contain further violence . The communal violence at Naroda was deemed " the largest single case of mass murder " during the 2002 Gujarat riots ; it accounted for the greatest number of deaths during a </t>
+          <t xml:space="preserve">Kronshtadt-class battlecruiser = The Kronshtadt-class battlecruisers , with the Soviet designation as Project 69 heavy cruisers , ( Russian : Тяжёлые крейсера проекта 69 ) , were ordered for the Soviet Navy in the late 1930s . Two ships were started but none were completed due to World War II . These ships had a complex and prolonged design process which was hampered by constantly changing requirements and the Great Purge in 1937 . They were laid down in 1939 , with an estimated completion date in 1944 , but Stalin 's naval construction program proved to be more than the shipbuilding and armaments industries could handle . Prototypes of the armament and machinery had not even been completed by 22 June 1941 , almost two years after the start of construction . This is why the Soviets bought twelve surplus 38-centimeter ( 15.0 in ) SK C / 34 guns , and their twin turrets , similar to those used in the Bismarck-class battleships , from Germany in 1940 . The ships were partially redesigned </t>
         </is>
       </c>
     </row>
@@ -1176,32 +1176,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>cap fruit color shaped spores bodies fungus stem mushroom spore taxonomy yellow diameter collected gill somewhat commonly hyphae bearing description typically colored epithet grow grows north_america slightly flesh smooth thin orange pale distinguished gills genus covered mushrooms scattered forests specific closely basidia taste whitish roughly measuring characteristics reddish margin attached caps growing dry connections wide brownish distinct clamp distributed odor mycologist similar distinctive specimens mature stipe microscopic translucent occasionally edible measure fine spored hollow hyaline cystidia tissue fungi habitat brown lacks ellipsoid layer yellowish produces broadly attachment narrow distribution maturity walled differences print cheilocystidia cuticle cylindrical cells pink rounded apex</t>
+          <t>['cap', 'fruit', 'color', 'shaped', 'spores', 'bodies', 'fungus', 'stem', 'mushroom', 'spore', 'taxonomy', 'yellow', 'diameter', 'collected', 'gill']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Hygrophorus eburneus = Hygrophorus eburneus , commonly known as the ivory waxy cap or the cowboy 's handkerchief , is a species of edible mushroom in the waxgill family of fungi . It is widespread in Europe and North America , and has also been collected in northern Africa . The fruit bodies are medium-sized , pure white , and when wet are covered in a layer of slime thick enough to make the mushroom difficult to pick up . The gills are broadly attached to the stem or running down it ; as the family name suggests , they feel waxy when rubbed between the fingers . Like all Hygrophorus species , the fungus is mycorrhizal — a symbiotic association whereby the underground fungal mycelia penetrate and exchange nutrients with tree roots . They are common in a variety of forest types , where they grow on the ground in thickets or grassy areas . Hygrophorus eburneus is the type species of the genus Hygrophorus . A number of biologically active chemicals have been purified from the fruit bodies</t>
+          <t>Reborn doll = A reborn doll is a manufactured skin doll that has been transformed to resemble a human infant with as much realism as possible . The process of creating a reborn doll is referred to as reborning and the doll artists are referred to as reborners . Reborn dolls are also known as Bodo dolls or unliving dolls . The hobby of creating reborn baby dolls began around 1939 when doll enthusiasts wanted more realistic dolls . Since then , an industry surrounding reborn dolls has emerged . Reborn dolls are primarily purchased on the internet but are available at fairs . Depending on craftsmanship , they range in price from hundreds to thousands of dollars . The International Reborn Doll Artists ( IRDA ) group was created to educate artists in the art form of reborn doll making . Any artist can join the association , however certain ethical guidelines must be upheld by members . Reborning involves numerous time consuming steps . The most basic form of the process involves taking a vi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Cyathus stercoreus = Cyathus stercoreus , commonly known as the dung-loving bird 's nest , is a species of fungus in the genus Cyathus , family Nidulariaceae . Like other species in the Nidulariaceae , the fruiting bodies of C. stercoreus resemble tiny bird 's nests filled with eggs . The fruiting bodies are referred to as splash cups , because they are designed to use the force of falling drops of water to dislodge and disperse their spores . The species has a worldwide distribution , and prefers growing on dung , or soil containing dung ; the specific epithet is derived from the Latin word stercorarius , meaning " of dung " . = = Description = = The fruiting bodies , or perida , are funnel- or barrel-shaped , 6 – 15 mm tall , 4 – 8 mm wide at the mouth , sometimes short-stalked , golden brown to blackish brown in age . The outside wall of the peridium , the ectoperidium , is covered with tufts of fungal hyphae that resembles shaggy , untidy hair . However , in older specimens this ou</t>
+          <t xml:space="preserve">Hydnellum ferrugineum = Hydnellum ferrugineum , commonly known as the mealy tooth or the reddish-brown corky spine fungus , is a species of tooth fungus in the family Bankeraceae . A widely distributed species , it is found in north Africa , Asia , Europe , and North America . The fungus fruits on the ground singly or in clusters in conifer forest , usually in poor ( low nutrient ) or sandy soil . Fruit bodies are somewhat top-shaped , measuring 3 – 10 cm ( 1 – 4 in ) in diameter . Their velvety surfaces , initially white to pink , sometimes exude drops of red liquid . The lower surface of the fruit body features white to reddish-brown spines up to 6 mm long . Mature fruit bodies become dark reddish brown in color , and are then difficult to distinguish from other similar Hydnellum species . H. ferrugineum forms a mat of mycelia in the humus and upper soil where it grows . The presence of the fungus changes the characteristics of the soil , making it more podzolized . = = Taxonomy = = </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Mycena adscendens = Mycena adscendens , commonly known as the frosty bonnet , is a species of fungus in the family Mycenaceae . The fungus produces small white fruit bodies ( mushrooms ) with caps up to 7.5 mm ( 0.3 in ) in diameter that appear to be dusted with sugar-like granules . Caps are supported by thin , hollow stems up to 20 mm ( 0.8 in ) long , which are set on a disc-like base . It is distributed in the United States , where it has been found from Washington to California , Europe , and Turkey . The fruit bodies grow on fallen twigs and other woody debris on the forest floor , including fallen hazel nuts . The variety carpophila is known from Japan . There are several small white Mycena species that are similar in appearance to M. adscendens , some of which can be reliably distinguished only by examining microscopic characteristics . = = Taxonomy = = The species , originally named Agaricus adscendens by Wilhelm Gottfried Lasch in 1829 , was first collected in the Province of</t>
+          <t>Pulveroboletus ravenelii = Pulveroboletus ravenelii , commonly known as Ravenel 's bolete or the powdery sulfur bolete , is a species of bolete fungus in the family Boletaceae . Described as new to science in 1853 , the widely distributed species is known from Asia , Australia , North America , Central America , and South America . Mycorrhizal with oak , the fungus fruits on the ground singly , scattered , or in groups in woods . Fruit bodies ( mushrooms ) have convex to flat , yellowish to brownish-red caps up to 10 cm ( 4 in ) in diameter . On the cap underside , the pore surface is bright yellow before turning dingy yellow to grayish brown with age ; it stains greenish blue then grayish brown after injury . A cottony and powdery partial veil remains as a ring on the stipe . The mushrooms are edible , and have been used in traditional Chinese medicine and for mushroom dyeing . = = Taxonomy = = The species was first described as Boletus ravenelii by Miles Joseph Berkeley and Moses Ash</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Vanilla Chocolat = " Vanilla Chocolat " is a song recorded by Romanian singer Alexandra Stan for her second studio album , Unlocked ( 2014 ) . It features guest vocals provided by Romanian rapper Connect-R. The track was made available for digital download on 24 December 2014 as the album 's fourth single . " Vanilla Chocolat " was written by Stan , Connect-R , Sava Constantin , Alexandru Cotoi and Mika Moupondo , while production was handled by Cotoi . A selfie music video for the song was directed by Stan and The Architect , and debuted on Stan 's YouTube channel on 18 December 2014 . After its release , musical critics praised " Vanilla Chocolat " for Connect-R 's " catchy rap " and French bits , while others pointed out the " easy-to-sing " , but at the same time " nonsense " lyrics of the track . The song was performed during Stan 's " Unlocked Tour " ( 2014 ) , and together with " Cherry Pop " at the Romanian show , Vocea României . = = Background and recording = = " Vanilla Choc</t>
+          <t>Fort Senneville = Fort Senneville is one of the outlying forts of Montreal , Quebec , Canada , built by the Canadiens of New France near the Sainte-Anne rapids in 1671 . The property was part of a fief ceded to Dugué de Boisbriant in 1672 by the Sulpicians . A large stone windmill , which doubled as a watch tower , was built on a hill by late 1686 and featuring machicolation and other castle-like features . The fort was burned down by Iroquois in 1691 , with only the mill itself left standing . Governor-General Frontenac ordered the construction of a second , more imposing fort in 1692 . It was rebuilt in 1702-1703 to protect the nearby fur trading post . With extensive cannons and swiveling wall guns , it was the " most substantial castle-like fort " near Montreal . It was eventually destroyed in 1776 by Benedict Arnold , under American military control , but the ruins have been maintained since then . In 2003 , it was classified as a historic site . = = Background = = Thanks to the t</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Eurasian wryneck = The Eurasian wryneck ( Jynx torquilla ) is a species of wryneck in the woodpecker family . This species mainly breeds in temperate regions of Europe and Asia . Most populations are migratory , wintering in tropical Africa and in southern Asia from Iran to the Indian Subcontinent , but some are resident in northwestern Africa . It is a bird of open countryside , woodland and orchards . Eurasian wrynecks measure about 16.5 cm ( 6.5 in ) in length and have bills shorter and less dagger-like than those of other woodpeckers . Their upperparts are barred and mottled in shades of pale brown with rufous and blackish bars and wider black streaks . Their underparts are cream speckled and spotted with brown . Their chief prey is ants and other insects , which they find in decaying wood or on the ground . The eggs are white as is the case with many birds that nest in holes and a clutch of seven to ten eggs is laid during May and June . These birds get their English name from the</t>
+          <t>Hugh Bradner = Hugh Bradner ( November 5 , 1915 – May 5 , 2008 ) was an American physicist at the University of California who is credited with inventing the neoprene wetsuit , which helped to revolutionize scuba diving . A graduate of Ohio 's Miami University , he received his doctorate from California Institute of Technology in Pasadena , California , in 1941 . He worked at the US Naval Ordnance Laboratory during World War II , where he researched naval mines . In 1943 , he was recruited by Robert Oppenheimer to join the Manhattan Project at the Los Alamos Laboratory . There , he worked with scientists including Luis Alvarez , John von Neumann and George Kistiakowsky on the development of the high explosives and exploding-bridgewire detonators required by atomic bombs . After the war , Bradner took a position studying high-energy physics at the University of California , Berkeley , under Luis Alvarez . Bradner investigated the problems encountered by frogmen staying in cold water for</t>
         </is>
       </c>
     </row>
@@ -1211,32 +1211,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>episode mulder plot find scully nielsen doctor files scene david_duchovny finds x-files filmed dana_scully enterprise gillian_anderson alien fox olivia filming agents fox_mulder previously fbi broadcast script paranormal man mythology fringe households agent planet watched chris_carter carter archer smoking viewers linked effects believe rating noting walter duchovny arrives kill frank_spotnitz zack_handlen episodes reception discover lars_pearson skinner trek monster star reviews thought bbc generation voyager cinefantastique tardis wanting robert_shearman producers special ratings stars rated lone paula_vitaris walter_skinner skeptical centers creature kim_manners television tucker amy story scenes aliens gunmen investigate starfleet aired unconnected finale believes mitch_pileggi tells household watching creator mixed reyes killing</t>
+          <t>['episode', 'mulder', 'plot', 'find', 'scully', 'nielsen', 'doctor', 'files', 'scene', 'david_duchovny', 'finds', 'x-files', 'filmed', 'dana_scully', 'enterprise']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Mercedes McQueen = Mercedes Maria Theresa Immaculata McQueen ( previously Owen , Fisher and Browning ) is a fictional character from the British Channel 4 soap opera Hollyoaks , played by Jennifer Metcalfe . She debuted on-screen during the episode airing on 19 June 2006 as the first character to be introduced to the series by series producer , Bryan Kirkwood . In 2008 Metcalfe feared that the character was to be axed but was later reassured by the series producer that she would not be . Metcalfe later stated her intention to stay with the series . Mercedes is part of the McQueen family and is the longest serving McQueen on the series . On 26 August 2014 , it was revealed that Metcalfe had decided to quit the soap . In November 2014 , Mercedes was presumably stabbed to death , with her body discarded . However , Metcalfe returned to screens on 17 February 2015 in a surprise , unannounced twist which saw Mercedes revealed as alive and well , living in Nice , France . It was announced th</t>
+          <t>Galapagos shark = The Galapagos shark ( Carcharhinus galapagensis ) is a species of requiem shark , in the family Carcharhinidae , found worldwide . This species favors clear reef environments around oceanic islands , where it is often the most abundant shark species . A large species that often reaches 3.0 m ( 9.8 ft ) , the Galapagos reef shark has a typical fusiform " reef shark " shape and is very difficult to distinguish from the dusky shark ( C. obscurus ) and the grey reef shark ( C. amblyrhynchos ) . An identifying character of this species is its tall first dorsal fin , which has a slightly rounded tip and originates over the rear tips of the pectoral fins . Galapagos sharks are active predators often encountered in large groups . They feed mainly on bottom-dwelling bony fishes and cephalopods ; larger individuals have a much more varied diet , consuming other sharks , marine iguanas , sea lions , and even garbage . As in other requiem sharks , reproduction is viviparous , wit</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">District Railway = The Metropolitan District Railway ( commonly known as the District Railway ) was a passenger railway that served London from 1868 to 1933 . Established in 1864 to complete the inner circle , an underground railway in London , the first part of the line opened using gas-lit wooden carriages hauled by steam locomotives . The Metropolitan Railway operated all services until the District introduced its own trains in 1871 . The railway was soon extended westwards through Earl 's Court to Fulham , Richmond , Ealing and Hounslow . After completing the inner circle and reaching Whitechapel in 1884 , it was extended to Upminster in Essex in 1902 . To finance electrification at the beginning of the 20th century , American financier Charles Yerkes took it over and made it part of his Underground Electric Railways Company of London ( UERL ) group . Electric propulsion was introduced in 1905 , and by the end of the year electric multiple units operated all of the services . On 1 </t>
+          <t xml:space="preserve">Liverpool Scottish = The Liverpool Scottish , known diminutively as " the Scottish " , is a unit of the British Army , part of the Army Reserve ( formerly the Territorial Army ) , raised in 1900 as an infantry battalion of the King 's ( Liverpool Regiment ) . The Liverpool Scottish became affiliated to the Queen 's Own Cameron Highlanders in the 1920s and formally transferred to the regiment in 1937 with its identity preserved . Reflecting the Territorial Army 's decline in size since the late 1940s , the battalion was reduced to a company in 1967 , then to a platoon of " A " ( King 's ) Company , King 's and Cheshire Regiment in 1999 . In 2006 , the company was incorporated into the 4th Battalion , Duke of Lancaster 's Regiment ( King 's , Lancashire and Border ) . Service in the First World War was extensive and the Liverpool Scottish was one of the first territorial battalions to arrive on the Western Front when it deployed in November 1914 . Approximately 1,000 of more than 10,000 </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Window of Opportunity ( Stargate SG-1 ) = " Window of Opportunity " is the sixth episode from season 4 of the science fiction television series Stargate SG-1 , and first aired on the American subscription channel Showtime on August 4 , 2000 . The episode is based on a time loop scenario , with SG-1 team members Colonel O 'Neill and Teal 'c repeatedly reliving the same ten hours after a mission on a planet . Since the rest of their team and all personnel at Stargate Command are unaware of the happenings and do not remember the time resets , O 'Neill and Teal 'c are forced to find a solution on their own . Penned by Joseph Mallozzi and Paul Mullie , " Window of Opportunity " was the writing duo 's second script , and their first episode to air . Mallozzi and Mullie later became executive producers of both Stargate SG-1 and Stargate Atlantis . The episode 's unique story style caused an unexpected shortage of footage during filming , which director Peter DeLuise compensated for by shootin</t>
+          <t>Quatermass and the Pit ( film ) = Quatermass and the Pit ( US title : Five Million Years to Earth ) is a 1967 British science fiction horror film . Made by Hammer Film Productions it is a sequel to the earlier Hammer films The Quatermass Xperiment and Quatermass 2 . Like its predecessors it is based on a BBC Television serial – Quatermass and the Pit – written by Nigel Kneale . It was directed by Roy Ward Baker and stars Andrew Keir in the title role as Professor Bernard Quatermass , replacing Brian Donlevy who played the role in the two earlier films . James Donald , Barbara Shelley and Julian Glover appear in co-starring roles . The plot , which is largely faithful to the original television production , centres on the discovery of a mysterious object buried at the site of an extension to the London Underground . Also uncovered nearby are the remains of early human ancestors more than five million years old . Realising that the object is in fact an ancient Martian spacecraft , Quater</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Refugio oil spill = The Refugio oil spill on May 19 , 2015 deposited 142,800 U.S. gallons ( 3,400 barrels ) of crude oil onto one of the most biologically diverse coastlines of the west coast . The corroded pipeline blamed for the spill has been closed indefinitely , resulting in financial impacts to the county estimated as high as $ 74 million if it and a related pipeline remain out of service for three years . The cost of the cleanup was estimated by the company to be $ 96 million with overall expenses including expected legal claims and potential settlements to be around $ 257 million . The oil spill , located immediately north of Refugio State Beach in Santa Barbara County , California , originated in a 2 feet ( 61 cm ) diameter underground pipeline named Line 901 owned by Plains All American Pipeline . Crude oil produced by offshore platforms was transported from onshore receiving plants to another pipeline that transported the oil inland for processing . The oil pipeline operator</t>
+          <t>The Proclamation of Dušan 's Law Codex = The Proclamation of Dušan 's Law Codex ( Serbian : Proglašenje Dušanovog zakonika ) is the name given to each of seven versions of a composition painted by Paja Jovanović which depict Dušan the Mighty introducing Serbia 's earliest surviving law codex to his subjects in Skopje in 1349 . The Royal Serbian Government commissioned the first version for 30,000 dinars in 1899 , intending for it to be displayed at the following year 's Exposition Universelle ( world 's fair ) in Paris . When originally commissioned , the painting was intended to depict Dušan 's 1346 coronation as Emperor of Serbia . After consulting with the politician and historian Stojan Novaković , Jovanović decided against painting a scene from Dušan 's coronation , and opted to depict the proclamation of his law codex instead . Thus , the painting has often erroneously been described as depicting the coronation . Jovanović paid a great deal of attention to historical detail in pr</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Son of a Gun ( Homicide : Life on the Street ) = " Son of a Gun " is the third episode of the first season of the American police drama television series Homicide : Life on the Street . It originally aired on NBC in the United States on February 10 , 1993 . The teleplay was written by James Yoshimura based on a story by executive producer Tom Fontana , and the episode was directed by Nick Gomez . In the episode , recurring character Officer Thormann ( Lee Tergesen ) is shot while on duty , and his close friend Crosetti takes the investigation personally . " Son of a Gun " was originally supposed to be the fourth episode of the first season , but was broadcast third when the episode " Night of the Dead Living " was moved to the end of the season . The shooting of a police officer , as well as other aspects of the script , were directly inspired by real-life events chronicled in David Simon 's non-fiction book , Homicide : A Year on the Killing Streets . The episode included guest appear</t>
+          <t xml:space="preserve">Spooks ( series 3 ) = The third series of the British spy drama television series Spooks ( known as MI-5 in the United States ) began broadcasting on 11 October 2004 on BBC One , before ending on 13 December 2004 . It consists of ten episodes which continue to follow the actions of Section B , a counter-terrorism division of the British Security Services ( MI5 ) . It also sees the departure of three principal characters : Tom Quinn ( Matthew Macfadyen ) is decommissioned in the second episode , Zoe Reynolds ( Keeley Hawes ) is exiled to Chile in the sixth episode , and Danny Hunter ( David Oyelowo ) is killed in the series finale . In addition to Macfadyen , Hawes and Oyelowo , Peter Firth , Rupert Penry-Jones , Nicola Walker , Hugh Simon , Shauna Macdonald and Rory MacGregor are listed as the main cast . Though the producers knew that Macfayden would leave the series , they did not know when he would do so , and so the first two episodes were initially written without him . In either </t>
         </is>
       </c>
     </row>
@@ -1246,32 +1246,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>son king died brother death daughter father reign royal kings younger succeeded sons kingdom probably bishop brothers married claim according marriage appears granted wife mentioned lands emperor duke sources edward empire historians successor fortress hungary prince possibly ruler refused conflict account crown powerful stephen fled historian byzantine siege hungarian secure peace castle confirmed likely john invaded chronicle rome sent hands heir seized managed pope cousin surviving ill invasion eldest alexander buried authority crowned uncle records chronicler throne grandfather earl constantinople archbishop ruled nephew bishops william alliance imperial accepted tried papal iii rebellion succession ireland exile mac constantine certainly dublin persuaded</t>
+          <t>['son', 'king', 'died', 'brother', 'death', 'daughter', 'father', 'reign', 'royal', 'kings', 'younger', 'succeeded', 'sons', 'kingdom', 'probably']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Siege of Lal Masjid = The Siege of Lal Masjid ( Urdu : لال مسجد محاصرہ , code-named Operation Sunrise ) was a confrontation in July 2007 between Islamic fundamentalist militants and the Government of Pakistan , led by President Pervez Musharraf and Prime Minister Shaukat Aziz . The focal points of the operation were the Lal Masjid ( " Red Mosque " ) and the Jamia Hafsa madrasah complex in Islamabad , Pakistan . Since January 2006 , Lal Masjid and the adjacent Jamia Hafsa madrasah had been operated by Islamic militants led by two brothers , Maulana Abdul Aziz and Abdul Rashid Ghazi . This organisation advocated the imposition of Sharia ( Islamic religious law ) in Pakistan and openly called for the overthrow of the Pakistani government . Lal Masjid was in constant conflict with authorities in Islamabad for 18 months prior to the military operation . They engaged in violent demonstrations , destruction of property , kidnapping , arson and armed clashes with the authorities . After Lal Ma</t>
+          <t>PHP = PHP is a server-side scripting language designed for web development but also used as a general-purpose programming language . Originally created by Rasmus Lerdorf in 1994 , the PHP reference implementation is now produced by The PHP Group . PHP originally stood for Personal Home Page , but it now stands for the recursive backronym PHP : Hypertext Preprocessor . PHP code may be embedded into HTML code , or it can be used in combination with various web template systems , web content management systems and web frameworks . PHP code is usually processed by a PHP interpreter implemented as a module in the web server or as a Common Gateway Interface ( CGI ) executable . The web server combines the results of the interpreted and executed PHP code , which may be any type of data , including images , with the generated web page . PHP code may also be executed with a command-line interface ( CLI ) and can be used to implement standalone graphical applications . The standard PHP interpret</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Edge of the Ocean = " Edge of the Ocean " is a song recorded by American indie rock band Ivy . It was released as the third single from their third studio album , Long Distance ( 2000 ) . The single was made available as a CD single , 10 " , and 12 " single in the United States on July 10 , 2001 , before being reissued internationally on May 27 , 2002 . " Edge of the Ocean " was released alongside Ivy 's other single , " Disappointed " , on the same day . The track was written by Dominique Durand , Adam Schlesinger and Andy Chase , while production was handled by the latter two . The track received general acclaim from music critics who highlighted it as a " standout " track . Stylistically different from Ivy 's previous material , " Edge of the Ocean " is an indie pop and trip hop song with " romantic " lyrics . The song was featured on the soundtracks for several films , including Angel Eyes and Shallow Hal . The single was subsequently considered their signature song , including by </t>
+          <t>Armenian Monastic Ensembles of Iran = The Armenian Monastic Ensembles of Iran , located in the West Azerbaijan and East Azerbaijan provinces in Iran , is an ensemble of three Armenian churches that were established during the period between the 7th and 14th centuries A.D. The edifices — the St. Thaddeus Monastery , the Saint Stepanos Monastery , and the Chapel of Dzordzor — have undergone many renovations . These sites were inscribed as cultural heritages in the 32nd session of the World Heritage Committee on 8 July 2008 under the UNESCO ’ s World Heritage List . The three churches lie in a total area of 129 hectares ( 320 acres ) and were inscribed under UNESCO criteria ( ii ) , ( iii ) , and ( vi ) for their outstanding value in showcasing Armenian architectural and decorative traditions , for being a major centre for diffusion of Armenian culture in the region , and for being a place of pilgrimage of the apostle St. Thaddeus , a key figure in Armenian religious traditions . They rep</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Isa ibn Muhanna = Sharaf ad-Din Isa ibn Muhanna at-Ta 'i , better known as Isa ibn Muhanna ( d . 1284 / 85 ) , was an emir ( commander / prince ) of the Al Fadl , a Bedouin dynasty that dominated the Syrian Desert and steppe during the 13th – 15th centuries . He was appointed amir al-ʿarab ( commander of the Bedouin ) by the Mamluks after their conquest of Syria in 1260 . Isa 's father served the same post under the Ayyubids . His assignment gave him command over the nomadic Arab tribes of Syria and obliged him to provide auxiliary troops in times of war and guard the desert frontier from the Mongol Ilkhanate in Iraq . As part of his emirate , he was granted Salamiyah and Sarmin . He participated in numerous campaigns against the Ilkhanate during Sultan Baybars ' reign ( 1260 – 1277 ) . In 1379 / 80 , Isa defected from Baybars ' successor , Qalawun , and joined the rebellion of the Mamluk viceroy of Syria , Sunqur al-Ashqar . However , Isa dissuaded Sunqur from joining the Ilkhanids ' </t>
+          <t>Vic Fontaine = Vic Fontaine is a fictional character who appeared in the sixth season onwards of the American science fiction television series Star Trek : Deep Space Nine . Portrayed by James Darren , he is a holographic representation of a 1960s-era Las Vegas Rat Pack-style singer and entertainer , as part of a program run in the holosuites at Quark 's bar . The character was developed from an idea by executive producer Ira Steven Behr , who had sought to introduce a character of that type during the fourth season to be played by Frank Sinatra , Jr . ; however , after Sinatra turned down the role , it was considered during the following season to be played by Steve Lawrence , but once again it was not used . Darren landed the role after Behr met him at a memorabilia show in North Hollywood and had him invited to audition . The character made his first appearance in the episode " His Way " , and returned later in the sixth season in " Tears of the Prophets " and throughout the seventh</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reid Blackburn = Reid Turner Blackburn ( August 11 , 1952 – May 18 , 1980 ) was a photographer killed in the 1980 volcanic eruption of Mount St. Helens . A photojournalist covering the eruption for a local newspaper — the Vancouver , Washington Columbian — as well as National Geographic magazine and the United States Geological Survey , he was caught at Coldwater Camp in the blast . Blackburn 's car and body were found four days after the eruption . His camera , buried under the debris of the eruption , was found roughly one week later . After his death , Reid was praised by his coworkers and friends alike . They spoke of his talent and enthusiasm , as well as his sometimes " acerbic " sense of humor . His wife , Fay , concluded that he had died doing what he loved . = = Life = = Blackburn was born in 1952 , the son of an engineer who possessed " a fixation on figuring out the way things worked " . He loved the idea of photography , once equating it to " painting with light " . He was </t>
+          <t>Brereton Jones = Brereton Chandler Jones ( born June 27 , 1939 ) is an American politician and horse breeder from Kentucky . From 1987 to 1991 , he served as the 50th Lieutenant Governor of Kentucky and from 1991 to 1995 , he was the state 's 58th governor . He now chairs the Kentucky Equine Education Project ( KEEP ) , a lobbying organization for the Kentucky horse industry . Born in Ohio and raised in West Virginia , Jones became the youngest-ever member of the West Virginia House of Delegates in 1964 . Two years later , he was chosen as the Republican floor leader in the House . In 1968 , he decided to leave politics and focus on his real estate business . He married Elizabeth " Libby " Lloyd in 1970 and in 1972 , the family moved to historic Airdrie Farm , Libby 's family estate in Woodford County , Kentucky . There , Jones founded Airdrie Stud , now an internationally recognized Thoroughbred farm . Although he remained mostly out of politics , Jones changed his party affiliation t</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>HMS Ajax ( 1880 ) = HMS Ajax was the name ship of her class of ironclad battleships built for the Royal Navy during the 1870s . Completed in 1883 , she was immediately placed in reserve until 1885 when the ship was commissioned for the first time . Later that year , Ajax was assigned as a coast guard ship in Scotland and remained there for the next six years . She was reduced to reserve again in 1891 and was taken out of service a decade later . The ship was sold for scrap in 1904 and subsequently broken up . = = Design and description = = The Ajax class was designed as a shallow-draught version of the preceding Inflexible that was also smaller and cheaper ; unfortunately the need , imposed by budgetary constraints , to produce a smaller ship produced a vessel with all of the shortcomings of Inflexible but with none of her virtues . The ships had a length between perpendiculars of 280 feet ( 85.3 m ) and were 300 feet 9 inches ( 91.7 m ) long overall , some 44 feet ( 13.4 m ) shorter t</t>
+          <t>Michael Dokeianos = Michael Dokeianos ( Greek : Μιχαήλ Δοκειανός ) , erroneously called Doukeianos by some modern writers , was a Byzantine nobleman and military leader , who married into the Komnenos family . He was active in Sicily under George Maniakes before going to Southern Italy as Catepan of Italy in 1040 – 41 . He was recalled after being twice defeated in battle during the Lombard-Norman revolt of 1041 , a decisive moment in the eventual Norman conquest of southern Italy . He is next recorded in 1050 , fighting against a Pecheneg raid in Thrace . He was captured during battle but managed to maim the Pecheneg leader , after which he was put to death and mutilated . = = Biography = = The family name of Dokeianos is considered to derive from Dok [ e ] ia in the Armeniac Theme . The family only came into prominence in the mid-11th century , with Michael one of the first to be mentioned . He is generally considered as the Dokeianos who married an unnamed daughter of Manuel Erotiko</t>
         </is>
       </c>
     </row>
@@ -1281,32 +1281,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>text notes book bach sunday published setting edition movements describes publication bass read author magazine stories poem note books printed works tone editor ensemble instrumental instruments aria piece strings introduction orchestra melody painting die voices closing poet composed scholar narrative stanza accompanied edited jesus reading repeated movement soprano details conclusion editions format hymn recordings poetry structured praise tenor page writes comments issues god verse focus readers solo volume gospel chapters issue informed occasion leipzig themes violins verses und chorus publishing alto readings sung beginning dramatic contrast composer depiction luke tune argues choral publisher aspects symbol translation content poems pages adventures</t>
+          <t>['text', 'notes', 'book', 'bach', 'sunday', 'published', 'setting', 'edition', 'movements', 'describes', 'publication', 'bass', 'read', 'author', 'magazine']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Por Debajo de la Mesa = " Por Debajo de la Mesa " ( " Underneath the Table " ) is a song written by Armando Manzanero and performed by Mexican recording artist Luis Miguel . Arranged by Bebu Silvetti , it was one of the two original compositions written for Miguel 's fifteenth studio album Romances . It was released as the lead single from the album on 15 July 1997 and it became his thirteenth number-one single on the Billboard Hot Latin Songs chart in the United States . The music video features Miguel performing at a fine-dining restaurant in New York City . The track received a negative reaction from Achy Obejas of the Chicago Tribune who called it " lame " . It was nominated Pop Song of the Year at the 10th Annual Lo Nuestro Awards and Manzanero was awarded a Broadcast Music , Inc . ( BMI ) Latin Award for writing the song . Manzanero performed the record as a duet with several artists such as Tania Libertad and Susana Zabaleta . = = Background = = In 1991 Miguel released Romance ,</t>
+          <t>Islamic geometric patterns = Islamic decoration , which tends to avoid using figurative images , makes frequent use of geometric patterns which have developed over the centuries . The geometric designs in Islamic art are often built on combinations of repeated squares and circles , which may be overlapped and interlaced , as can arabesques ( with which they are often combined ) , to form intricate and complex patterns , including a wide variety of tessellations . These may constitute the entire decoration , may form a framework for floral or calligraphic embellishments , or may retreat into the background around other motifs . The complexity and variety of patterns used evolved from simple stars and lozenges in the ninth century , through a variety of 6- to 13-point patterns by the 13th century , and finally to include also 14- and 16-point stars in the sixteenth century . Geometric patterns occur in a variety of forms in Islamic art and architecture including kilim carpets , Persian g</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Denial ( Sugababes song ) = " Denial " is a song by English girl group the Sugababes from their fifth studio album , Change ( 2007 ) . Coinciding with the commencement of the group 's 2008 Change Tour , it was released on 10 March 2007 as the album 's fourth and final single . V V Brown wrote " Denial " for the band while she was on London Underground 's Victoria line , and attempted to " get into their mindsets " in the process . The Sugababes and the song 's producers , Flex Turner and Elliot Malloy , co-wrote it . Composed of staccato verses , a harmonious chorus and a solo middle eight , " Denial " is a Europop and soft rock song that samples " Standing in the Way of Control " by The Gossip . The song received mixed reviews from critics , who were ambivalent towards its composition , but became a commercial success throughout Europe , where it peaked at number one on the Czech Singles Chart , number four on the Austrian Singles Chart , and within the top twenty on the charts in Ger</t>
+          <t>Captain Future ( magazine ) = Captain Future was a science fiction pulp magazine launched in 1940 by Better Publications , and edited initially by Mort Weisinger . It featured the adventures of Captain Future , a super-scientist whose real name was Curt Newton , in every issue . All but two of the novels in the magazine were written by Edmond Hamilton ; the other two were by Joseph Samachson . The magazine also published other stories that had nothing to do with the title character , including Fredric Brown 's first science fiction sale , " Not Yet the End " . Captain Future published unabashed space opera , and was , in the words of science fiction historian Mike Ashley , " perhaps the most juvenile " of the science fiction pulps to appear in the early years of World War II . Wartime paper shortages eventually led to the magazine 's cancellation : the last issue was dated Spring 1944 . = = Publication history and contents = = Although science fiction ( sf ) had been published before t</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Black Widows of Liverpool = Catherine Flannagan ( 1829 – 3 March 1884 ) and Margaret Higgins ( 1843 – 3 March 1884 ) were Irish sisters who were convicted of poisoning and murdering one person in Liverpool , Lancashire , England and suspected of more deaths . The women collected a burial society payout , a type of life insurance , on each death , and it was eventually found that they had been committing murders using arsenic to obtain the insurance money . Though Catherine Flannagan evaded police for a time , both sisters were eventually caught and convicted of one of the murders ; they were both hanged on the same day at Kirkdale Prison . Modern investigation of the crime has raised the possibility that Flannagan and Higgins were known or believed by investigators to be only part of a larger conspiracy of murder-for-profit — a network of " black widows " — but no convictions were ever obtained for any of the alleged conspiracy members other than the two sisters . = = Deaths = = In the</t>
+          <t>And Still I Rise = And Still I Rise is author Maya Angelou 's third volume of poetry , published by Random House in 1978 . It was published during one of the most productive periods in Angelou 's career ; she had written three autobiographies and published two other volumes of poetry up to that point . Angelou considered herself a poet and a playwright , but was best known for her seven autobiographies , especially her first , I Know Why the Caged Bird Sings , although her poetry has also been successful . She began , early in her writing career , alternating the publication of an autobiography and a volume of poetry . Although her poetry collections have been best-sellers , they have not received serious critical attention . And Still I Rise is made up of 32 short poems , divided into three parts . The poems ' themes focus on a hopeful determination to rise above difficulty and discouragement , and on many of the same topics as Angelou 's autobiographies and previous volumes of poetry</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ambler 's Texaco Gas Station = Ambler 's Texaco Gas Station , also known as Becker 's Marathon Gas Station , is a historic filling station located at the intersection of Old U.S. Route 66 and Illinois Route 17 in the village of Dwight , Illinois , United States . The station has been identified as the longest operating gas station along Route 66 ; it dispensed fuel for 66 continuous years until 1999 . The station is a good example of a domestic style gas station and derives its most common names from ownership stints by two different men . North of the station is an extant outbuilding that once operated as a commercial icehouse . Ambler 's was the subject of major restoration work from 2005 – 2007 , and reopened as a Route 66 visitor 's center in May 2007 . It was added to the U.S. National Register of Historic Places in 2001 . = = History = = Located at the intersection of U.S. Route 66 and Illinois Route 17 in Dwight , Illinois , United States , Ambler 's Texaco Station was built in </t>
+          <t>Johannes Rebmann = Johannes Rebmann ( January 16 , 1820 – October 4 , 1876 ) was a German missionary and explorer credited with feats including being the first European , along with his colleague Johann Ludwig Krapf , to enter Africa from the Indian Ocean coast . In addition , he was the first European to find Kilimanjaro . News of Rebmann 's discovery was published in the Church Missionary Intelligencer in May 1849 , but disregarded as mere fantasy for the next twelve years . The Geographical Society of London held that snow could not possibly occur let alone persist in such latitudes and considered the report to be the hallucination of a malaria-stricken missionary . It was only in 1861 that researchers began their efforts to measure Kilimanjaro . Expeditions to Tanzania between 1861 and 1865 , led by the German Baron Karl Klaus von der Decken , confirmed Rebmann ’ s report . Together with his colleague Johann Ludwig Krapf he also discovered Mt . Kenya . Their work there is also thou</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Halt im Gedächtnis Jesum Christ , BWV 67 = Halt im Gedächtnis Jesum Christ ( Keep Jesus Christ in mind ) , BWV 67 , is a church cantata by Johann Sebastian Bach . He composed it in Leipzig for Quasimodogeniti , the first Sunday after Easter , and first performed it on 16 April 1724 . Based on the prescribed gospel of the appearance of Jesus to the Disciples , first without then with Thomas , an unknown poet compares the situation of the doubtful Thomas to the Christian in general . He places Nikolaus Herman 's Easter hymn " Erschienen ist der herrlich Tag " in the centre of the cantata , repeats the line " Friede sei mit euch " ( Peace be with you ) several times , and ends with the first stanza from Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " ( Thou Prince of Peace , Lord Jesus Christ ) . Bach structured the work in seven movements , arranged in symmetry around the central chorale , and scored it for three solo voices , a four-part choir and a Baroque instrumental ensemb</t>
+          <t>Requiem for a Species = Requiem for a Species : Why We Resist the Truth about Climate Change is a 2010 non-fiction book by Australian academic Clive Hamilton which explores climate change denial and its implications . It argues that climate change will bring about large-scale , harmful consequences for habitability for life on Earth including humans , which it is too late to prevent . Hamilton explores why politicians , corporations and the public deny or refuse to act on this reality . He invokes a variety of explanations , including wishful thinking , ideology , consumer culture and active lobbying by the fossil fuel industry . The book builds on the author 's fifteen-year prior history of writing about these subjects , with previous books including Growth Fetish and Scorcher : The Dirty Politics of Climate Change . Requiem for a Species has been reviewed in Resurgence magazine , Socialist Review , Sydney Morning Herald , The Age , The Common Review , and Times Higher Education , whi</t>
         </is>
       </c>
     </row>
@@ -1316,32 +1316,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>raaf flying wing combat unit training operational pilot officer aircraft flight pilots disbanded commanding squadron air fighter deployed awarded royal_australian_air_force promoted commander responsible missions prototype rank staff aviation flew squadrons bomber fighters weight posted bombing equipment fuselage enemy engine operations headquarters crashed operating mission deployment testing victoria powerplant nuclear nos retired aerial responsibility tactical maintenance bomb instructor bombs duty trained employed chief wingspan conducted flown newly headquartered graduated activated radar senior honor united_states_army air_force cockpit bombers fuel trainers task airmen technical specifications royal_air_force delivered lockheed reconnaissance assistant civilian new_south_wales nose cancelled targets melbourne wartime operated ace disbanding weapon korean piloted</t>
+          <t>['raaf', 'flying', 'wing', 'combat', 'unit', 'training', 'operational', 'pilot', 'officer', 'aircraft', 'flight', 'pilots', 'disbanded', 'commanding', 'squadron']</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barzillai J. Chambers = Barzillai Jefferson Chambers ( December 5 , 1817 – September 16 , 1895 ) was an American surveyor , lawyer , and politician of the Gilded Age . Born in Kentucky , he moved to Texas to join that state 's war for independence against Mexico . Chambers stayed in Texas after its independence and annexation by the United States , earning a living as a surveyor and farmer in Johnson County . In the American Civil War , he served briefly in the Confederate army , then returned to his farming and business interests , becoming part-owner of a bank in his hometown of Cleburne . In the 1870s , Chambers became concerned with farming and monetary issues in politics , eventually joining the nascent Greenback Party in 1877 . He ran unsuccessfully for Vice President on the Greenback ticket with presidential nominee James B. Weaver of Iowa in 1880 . The Greenback nominees finished in a distant third place , receiving only 3.3 % of the popular vote and no electoral votes . After </t>
+          <t>Chocolatier ( video game ) = Chocolatier is a casual strategy video game with action game elements , developed by Big Splash Games and published by PlayFirst . The game was released as a download on May 1 , 2007 and was followed by CD-ROM release on September 27 , 2007 . Players assume the role of a young Chocolatier , who must navigate 14 cities around the globe while buying ingredients , manufacturing chocolates , and selling them to chocolate shops . Two modes of play are available : in story mode the player must rebuild an almost bankrupt chocolate empire and acquire 64 chocolate recipes from around the world ; in free mode players start out with scant resources and must become successful chocolatiers . Chocolatier was the first game developed by Big Splash Games , a trio of experienced video game designers , who remained employees whilst developing a prototype game in their spare time . This prototype was rejected by publishers , but after coming up with the premise of Chocolatier</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lavochkin La-7 = The Lavochkin La-7 ( Russian : Лавочкин Ла-7 ) was a piston-engined Soviet fighter developed during World War II by the Lavochkin Design Bureau ( OKB ) . It was a development and refinement of the Lavochkin La-5 , and the last in a family of aircraft that had begun with the LaGG-1 in 1938 . Its first flight was in early 1944 and it entered service with the Soviet Air Forces later in the year . A small batch of La-7s was given to the Czechoslovak Air Force the following year , but it was otherwise not exported . Armed with two or three 20 mm ( 0.79 in ) cannon , it had a top speed of 661 kilometers per hour ( 411 mph ) . The La-7 was felt by its pilots to be at least the equal of any German piston-engined fighter and even shot down a Messerschmitt Me 262 jet fighter . It was phased out in 1947 by the Soviet Air Force , but served until 1950 with the Czechoslovak Air Force . = = Design and development = = By 1943 , the La-5 had become a mainstay of the Soviet Air Forces </t>
+          <t xml:space="preserve">Amina Bokhary controversy = The Amina Bokhary controversy occurred in Hong Kong in 2010 involving the assault conviction of a wealthy woman from a well-connected political family . Amina Mariam Bokhary , 32 , received a non-custodial sentence and a one-year driving ban following an incident in the aftermath of a road traffic accident when she struck several police officers . As she had committed similar offences in 2001 and 2008 , her resulting probation was seen by some commentators as too lenient . The perceived leniency in her sentence provoked an uproar in Hong Kong for alleged preferential treatment . In particular , the presiding judge caused outrage when he said in his judgment that Bokhary had an " unblemished background and was born into a good family with caring parents [ and ] an outstanding academic record " . The comment highlighted the public perception of widening inequality and increasing disparities in the balance of political power between different social classes in </t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rose Catherine Pinkney = Rose Catherine Pinkney ( born 1964 ) is an American television development executive . She was hired as the VP Development and Original Programming for TV Land in 2012 . Pinkney has previously served as Director of Programming at Twentieth Century Fox Television , Senior Vice President of Comedy Development at Paramount Pictures Television and executive vice president of programming and production at TV One . She most recently served as the head of the television arm of Laurence Fishburne 's production company , Cinema Gypsy . Among Pinkney 's accolades are Network Journal 's 25 Most Influential Black Women in Business , Cable World 's Top 50 Women in Cable and Black Enterprise 's Top 50 Entertainment Executives . = = Early life and academic career = = Pinkney was born and raised in Prince George 's County , Maryland , the youngest child and only daughter of Joseph and Maud Pinkney . She points to her parents ' marriage , which as of 2008 had lasted 56 years , </t>
+          <t xml:space="preserve">Will Middlebrooks = William " Will " Scott Middlebrooks ( born September 9 , 1988 ) is an American professional baseball third baseman for the Milwaukee Brewers of Major League Baseball ( MLB ) . He made his MLB debut with the Boston Red Sox on May 2 , 2012 and played with them through 2014 . He also played for the San Diego Padres . A fifth round draft pick in the 2007 MLB draft out of Liberty-Eylau High School in Texarkana , Texas , Middlebrooks signed with the Red Sox for $ 925,000 , bypassing his commitment to Texas A &amp; M University . Middlebrooks was originally a shortstop , but the Red Sox converted him into a third baseman in the minor leagues . He represented the United States in the 2011 All-Star Futures Game . Following Middlebrooks ' emergence as the Red Sox ' starting third baseman in 2012 , the organization traded former All-Star Kevin Youkilis . After struggles in the 2013 and 2014 seasons , the Red Sox traded Middlebrooks to the San Diego Padres . = = Amateur career = = </t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Boeing Chinook ( UK variants ) = The Boeing Chinook is a tandem rotor helicopter operated by the Royal Air Force ( RAF ) . A series of variants based on the United States Army 's Boeing CH-47 Chinook , the RAF Chinook fleet is the largest outside the United States . RAF Chinooks have seen extensive service including fighting in the Falklands War , peace-keeping commitments in the Balkans , and action in the Iraq and Afghanistan wars . The Chinook aircraft , normally based at RAF Odiham , provides heavy-lift support and transport across all branches of the British armed forces , and is supported by the smaller , medium-lift helicopters such as the AgustaWestland Merlin HC.3 of the Royal Navy 's Commando Helicopter Force and the RAF 's Westland Puma HC.2 , based at RNAS Yeovilton and RAF Benson . = = Design and development = = = = = Chinook HC Mk1 = = = In March 1967 an order was placed for fifteen Chinook HC Mk1s , standing for Helicopter , Cargo Mark 1 , for the Royal Air Force to repl</t>
+          <t>Mir EO-19 = Mir EO-19 ( Russian : Мир ЭО-19 , also known as Principal Expedition 19 ) was the nineteenth manned expedition to the space station Mir , lasting from June to September 1995 . The crew , consisting of Russian cosmonauts Anatoly Solovyev and Nikolai Budarin , launched on June 27 , 1995 aboard the Space Shuttle Atlantis on the STS-71 mission . After remaining aboard Mir for approximately 75 days , Solovyev and Budarin returned aboard the Soyuz TM-21 spacecraft on September 11 , 1995 . EO-19 lasted just under three months and was the only complete all-Russian crewed expedition to Mir in 1995 and was the first Mir expedition launched on an American Space Shuttle . The mission that launched EO-19 , STS-71 , was the first Space Shuttle docking to Mir . = = Crew = = Antatoly Solovyev served as a crew member on three spaceflights prior to EO-19 : Mir EP-2 , Soyuz TM-9 , and Soyuz TM-15 . This flight was his first aboard a Space Shuttle , with his three previous flights being on the</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Humpty Dumpty = Humpty Dumpty is a character in an English nursery rhyme , probably originally a riddle and one of the best known in the English-speaking world . He is typically portrayed as an anthropomorphic egg , though he is not explicitly described so . The first recorded versions of the rhyme date from late eighteenth-century England and the tune from 1870 in James William Elliott 's National Nursery Rhymes and Nursery Songs . Its origins are obscure and several theories have been advanced to suggest original meanings . The character of Humpty Dumpty was popularised in the United States by actor George L. Fox ( 1825 – 77 ) . As a character and literary allusion , he has appeared or been referred to in a large number of works of literature and popular culture , particularly Lewis Carroll 's Through the Looking-Glass ( 1872 ) . The rhyme is listed in the Roud Folk Song Index as No. 13026 . = = Lyrics and melody = = The rhyme is one of the best known and most popular in the English </t>
+          <t>15th Sustainment Brigade = The 15th Sustainment Brigade was a sustainment brigade of the United States Army based at Fort Bliss , Texas . It provided logistics support to other units of the United States Army , and was subordinate to the 13th Sustainment Command ( Expeditionary ) . It previously had provided support to the 1st Cavalry Division , but now did so for the 1st Armored Division until 12 May 2015 when the 15th Sustainment Brigade became part of the 1st Armored Division and was renamed 1st Armored Division Sustainment Brigade . The brigade 's lineage dates back to 1919 , and it had a long and decorated history when designated as the supply command of the 1st Cavalry Division . Having seen service in every major conflict of the 20th century in support of its parent division , the unit was not designated as the 15th Sustainment Brigade permanently until 2005 . In February 2008 , the brigade was reassigned to the 13th Sustainment Command , ending almost a century of association w</t>
         </is>
       </c>
     </row>
@@ -1351,32 +1351,32 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>took second played runs team tour england australia playing class run came score match taking day scored batsman bat series cricket ended victory won play somerset seven win bowling career total highest bowler season batsmen unbeaten despite india dismissed average cricketer captain wicket bowled opening debut final miller partnership balls reached harvey duck overs having draw test boycott south_africa west_indies best scoring leg international tests scores hit australian players ashes saw leading centuries yorkshire new_zealand half maiden captained tourists fourth fell went ball touring barnes making lost drawn century returned successful keeper hosts reply south_australia victoria trinidad minutes spin club</t>
+          <t>['took', 'second', 'played', 'runs', 'team', 'tour', 'england', 'australia', 'playing', 'class', 'run', 'came', 'score', 'match', 'taking']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ontario Highway 35 = King 's Highway 35 , also known as Highway 35 , is a provincial highway in the Canadian province of Ontario , linking Highway 401 with Peterborough , Kawartha Lakes , and Algonquin Park . The highway travels from west of Newcastle , through Lindsay and the Kawarthas and into Haliburton before terminating at Highway 60 to the west of Algonquin Park , the province 's largest . The winding course of the highway , combined with the picturesque views offered along its length , have led some to declare it the most scenic highway in Ontario . Most of the highway , including a portion of today 's Highway 60 , was assumed by the Department of Highways by 1940 . In 1961 , Highway 115 was signed concurrently with Highway 35 for 19 kilometres ( 12 mi ) . This was widened to a divided expressway in the late eighties . In the mid-1950s , several bypasses were constructed to divert Highway 35 away from town centres such as Lindsay , Fenelon Falls and Minden . Highway 35 is patrol</t>
+          <t>Connie Talbot 's Holiday Magic = Connie Talbot 's Holiday Magic is the third album by British child singer Connie Talbot . Released 13 October 2009 by AAO Music , it features rerecordings of songs from Talbot 's previous album , Connie Talbot 's Christmas Album , as well as new tracks . The album was released after Talbot was named child ambassador for the Toys for Tots Campaign , and some of the proceeds from the album were given to the organisation . The album was marketed with a tour of the United States , a cross-marketing campaign with Boscov 's , and a television special produced by WVIA , a DVD of which was later released for sale . Reviews of the album were mixed ; while Talbot was called " sweet " and her range was praised , other reviewers considered the album to be " cloying " and " little more than a novelty act " . = = Production = = In September 2009 , it was announced that Talbot had been named child ambassador of the Marine Corps Toys for Tots Campaign , a charitable pr</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Headlines ( Friendship Never Ends ) = " Headlines ( Friendship Never Ends ) " is a song performed by British girl group Spice Girls for their greatest hits album Greatest Hits . It was written by the Spice Girls , Richard Stannard and Matt Rowe , whilst produced by the latter two . It was released as the only single from the album on 5 November 2007 , by Virgin Records . The song was the first commercial single release to feature the group 's original lineup since Geri Halliwell left in 1998 . It was also the official Children in Need single of 2007 . As of 2016 , it is the final release from the group . " Headlines ( Friendship Never Ends ) " is a midtempo ballad song , which lyrically talks about the group reuniting , and about their friendship throughout two decades together . The song received generally mixed reviews from music critics , with some calling it a " classic " from the group , while others felt it was not good enough . " Headlines ( Friendship Never Ends ) " was a moder</t>
+          <t>Bob Willis = Robert George Dylan Willis MBE ( born Robert George Willis on 30 May 1949 ) , known as Bob Willis , is an English former cricketer who played for Surrey , Warwickshire , Northern Transvaal and England . A right-handed and aggressive fast bowler with a notably long run-up , Willis spearheaded several England bowling attacks between 1971 and 1984 , across 90 Test matches in which he took 325 wickets at 25.20 runs per wicket , at the time second only to Dennis Lillee . He is currently England 's fourth leading wicket taker , behind James Anderson , Ian Botham , and Stuart Broad . Willis took 899 first-class wickets overall , although from 1975 onwards he bowled with constant pain , having had surgery on both knees . He nevertheless continued to find success , taking a Test career best eight wickets for 43 runs in the 1981 Ashes series against Australia , one of the all-time best Test bowling performances . He was Wisden Cricketer of the Year for 1978 . In addition to the Test</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Toyota Aurion ( XV40 ) = The Toyota Aurion ( XV40 ) / ˈɔːriən / is the original series of the Toyota Aurion , a mid-size car produced by Toyota in Australia and parts of Asia . Designated " XV40 " , Toyota manufactured the first generation Aurion between 2006 and 2012 until it was fully replaced by the XV50 series . While Asian production of the XV50 series began in late-2011 , Toyota 's Australian operations did not take on production of the new model until 2012 . Although marketed as a separate model , the XV40 series Aurion is essentially a Toyota Camry ( XV40 ) with revised front- and rear-end treatment , along with changes to the interior . In lieu of the " Aurion " nameplate , the majority of East and Southeast Asian markets received the Camry-based Aurion under the name Toyota Camry . However , in Australasia and the Middle East , Toyota sold the original version of the Camry alongside the Aurion . In these markets , the Aurion replaced the Avalon ( XX10 ) model , which could tr</t>
+          <t>Empedocles ( The X-Files ) = " Empedocles " is the seventeenth episode of the eighth season of the American science fiction television series The X-Files . It premiered on the Fox network on April 22 , 2001 . The episode was written by Greg Walker and directed by Barry K. Thomas . " Empedocles " is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . The episode received a Nielsen rating of 7.3 and was viewed by 7.46 million households and over 12.46 million viewers . Overall , the episode received mixed reviews from critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) , Dana Scully ( Gillian Anderson ) and John Doggett ( Robert Patrick ) , who work on cases linked to the paranormal , called X-Files . In this episode , Monica Reyes ( Annabeth Gish ) enlists Mulder ’ s help investigating a killer ’ s connection to the unsolved murder of Doggett ’ s son , but Mulder soon finds himself clashing with Doggett . " Empedocles " was named af</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">British Library = The British Library is the national library of the United Kingdom and the largest library in the world by number of items catalogued . A Grade I listed building , the library is a major research library , holding around 170 million items from many countries , in many languages and in many formats , both print and digital : books , manuscripts , journals , newspapers , magazines , sound and music recordings , videos , play-scripts , patents , databases , maps , stamps , prints , drawings . The Library 's collections include around 14 million books , along with substantial holdings of manuscripts and historical items dating back as far as 2000 BC . As a legal deposit library , the British Library receives copies of all books produced in the United Kingdom and Ireland , including a significant proportion of overseas titles distributed in the UK . It also has a programme for content acquisitions . The British Library adds some three million items every year occupying 9.6 </t>
+          <t>SMS Wittelsbach = SMS Wittelsbach ( " His Majesty 's Ship Wittelsbach " ) was the lead ship of the Wittelsbach class of pre-dreadnought battleships of the Kaiserliche Marine . Wittelsbach was built at Wilhelmshaven Navy Dockyard . She was laid down in 1899 and completed in October 1902 , at the cost of 22,740,000 marks . Wittelsbach was the first capital ship built under the Navy Law of 1898 , brought about by Admiral Alfred von Tirpitz . The ship served in the I Squadron of the German fleet for the majority of her career . Wittelsbach was rapidly superseded by new " all-big-gun " warships , and as a result served for less than eight years before being decommissioned on 20 September 1910 . After the start of World War I in August 1914 , Wittelsbach was brought back to active duty in the IV Battle Squadron . The ship saw limited duty in the Baltic Sea against Russian forces , though the threat from British submarines forced the ship to withdraw by 1916 . The ship then saw service in a n</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Norman Yardley = Norman Walter Dransfield Yardley ( 19 March 1915 – 3 October 1989 ) was an English cricketer who played for Cambridge University , Yorkshire County Cricket Club and England , as a right-handed batsman and occasional bowler . An amateur , he captained Yorkshire from 1948 to 1955 and England on fourteen occasions between 1947 and 1950 , winning four Tests , losing seven and drawing three . Yardley was named Wisden Cricketer of the Year in 1948 and in his obituary in Wisden Cricketers ' Almanack , he was described as Yorkshire 's finest amateur since Stanley Jackson . Yardley played schoolboy cricket at St Peter 's , York . A highly talented all-round sportsman , he went to St John 's College , Cambridge , and won Blues at cricket , squash , rugby fives and field hockey . In the university matches , he scored 90 in his second year , 101 in his third and was captain for his final year . He made his Yorkshire debut in 1936 and played for the county until 1955 , when he reti</t>
+          <t>Christine Chapel = Christine Chapel is a fictional character who appears in all three seasons of the American science fiction television series Star Trek : The Original Series , as well as Star Trek : The Animated Series and the films Star Trek : The Motion Picture and Star Trek IV : The Voyage Home . Portrayed by Majel Barrett , she was the ship 's nurse on board the Starfleet starship USS Enterprise . Barrett had previously been cast under her real name as Number One in the first pilot for the series , " The Cage " , due in part to her romantic relationship with the series creator Gene Roddenberry . But following feedback from the Network executives , she was not in the cast for the second pilot . The character made her first appearance in " The Naked Time " following a re-write of the script by Roddenberry . He had been inspired after Barrett read a proposal for the episode " What Are Little Girls Made Of ? " and bleached her hair blonde to better fit a role in that episode . The ch</t>
         </is>
       </c>
     </row>
@@ -1386,32 +1386,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>highway north road east route lane south intersection west continues interchange designated completed state passes divided southern freeway portion access turns street northern crosses extended terminus heads northeast past intersects near eastern crossing bus designation lanes segment residential follow exit enters downtown alignment meets comes begins passing concurrent entire business heading follows section southeast end cross concurrency southbound avenue northwest border rural northbound roadway rerouted town continuing bypass highways cloverleaf mile undivided traffic concurrently areas intersections routes constructed routing baltimore old western eastbound commercial delaware splits ends corridor existing widened roads interstate maryland ramp description remainder expressway construction junction expanded</t>
+          <t>['highway', 'north', 'road', 'east', 'route', 'lane', 'south', 'intersection', 'west', 'continues', 'interchange', 'designated', 'completed', 'state', 'passes']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Siege of Güns = The Siege of Güns or Siege of Kőszeg ( Turkish : Güns Kuşatması ) was a siege of Kőszeg ( German : Güns ) in the Kingdom of Hungary within the Habsburg Empire , that took place in 1532 . In the siege , the defending forces of the Austrian Habsburg Monarchy under the leadership of Croatian Captain Nikola Jurišić ( Hungarian : Miklós Jurisics ) , defended the small border fort of Kőszeg with only 700 – 800 Croatian soldiers , with no cannons and few guns . The defenders prevented the advance of the Ottoman army of 120,000 – 200,000 toward Vienna , under the leadership of Sultan Suleiman the Magnificent ( Ottoman Turkish : سليمان Süleymān ) and Pargalı Ibrahim Pasha . The exact outcome is unknown , since it has two versions which differ depending on the source . In the first version Nikola Jurišić rejected the offer to surrender on favourable terms , and in the second version , the city was offered terms for a nominal surrender . Suleiman , having been delayed nearly four </t>
+          <t>Business routes of U.S. Route 10 in Michigan = There are three business routes of US Highway 10 in the state of Michigan . They serve as connections from the main highway into Reed City , Clare and Midland . Additionally , there were another two business routes that connected US Highway 10 ( US 10 ) to the downtowns of Flint and Pontiac . All of these business routes are , or were , former sections of US 10 that were marked Business US Highway 10 ( Bus . US 10 ) after the main highway was realigned to bypass the downtowns of the cities . The Reed City Bus . US 10 was created by 1960 to follow Chestnut and Church streets into the community 's central business district and through adjacent residential areas . In 1975 when US 10 was rerouted to follow the freeways around Clare , the former routing through downtown on McEwan and Fifth streets was redesignated as a business loop ; it was also signed to provide connections between US 10 and what is now US 127 because of an incomplete interch</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Mississippi Highway 465 = Mississippi Highway 465 ( MS 465 ) is a highway in the southern region of the Mississippi Delta . The highway starts at U.S. Route 61 ( US 61 ) near Redwood . It travels westward towards the Mississippi River , and then northwards to the village of Eagle Bend . The highway then traverses on the Mississippi River levee on a one-lane road . Later , MS 465 leaves the levee , continues northward , and soon ends at MS 1 . The highway was built around 1956 , as a gravel road from US 61 in Vicksburg , to MS 1 in Fitler . The southern terminus was moved in 1960 to near Redwood , and the highway was completely paved by 1984 . = = Route description = = MS 465 is located in Warren and Issaquena counties . The route is legally defined in Mississippi Code § 65-3-3 , and is maintained by the Mississippi Department of Transportation . The section from US 61 to the Warren – Issaquena county line was designated " William W. " Bill " Ramsey Memorial Highway " in 2009 . The high</t>
+          <t>St Ceidio 's Church , Rhodogeidio = St Ceidio 's Church , Rhodogeidio is a rural 19th-century church near Llannerch-y-medd , in Anglesey , north Wales . It was built using materials from the 14th-century church that previously stood on the site , which has been used for Christian worship since some time in the 7th century . The present building , which contains an east window dating from the 14th century and a 15th-century font , is no longer used for services , but has been looked after by local people . It is a Grade II listed building , a national designation given to " buildings of special interest , which warrant every effort being made to preserve them " , in particular because it is " unusual in being built closely to the form and detail of its Medieval predecessor . " Two 19th-century writers thought that the church was in a " dreary spot " , but a 2006 guide to Anglesey churches describes it as being in a pleasant location with good views . = = History and location = = The chu</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>M-53 ( Michigan highway ) = M-53 is a state trunkline highway in the US state of Michigan that connects Detroit to The Thumb region . The highway starts in Detroit at a connection with M-3 and ends in Port Austin , Michigan at M-25 . In between , the trunkline passes through the northern suburbs of Metro Detroit , connects to freeways like Interstate 69 ( I-69 ) and provides access to rural farmland . In Macomb County , M-53 follows the Christopher Columbus Freeway , while the remainder of the highway is known as Van Dyke Avenue in the metro area or Van Dyke Road elsewhere . The highway has also been named the Earle Memorial Highway for one of the pioneers of the Good Roads Movement and Michigan 's highway system . When the first state highways were signed in the field in 1919 , M-53 was one of them , running from Detroit to Elkton . In the 1920s , the highway was extended northward to connect with Port Austin . Later improvements through 1940 realigned a section of the roadway near Im</t>
+          <t>M-30 ( Michigan highway ) = M-30 is a state trunkline highway in the U.S. state of Michigan that runs in a north – south direction from the Midland area to West Branch . The highway runs through rural parts of three counties in the Lower Peninsula . The southern end runs along the Michigan Meridian and parallel to the Tittabawassee River . Prior to 1962 , M-30 's southern terminus ended at a junction with M-46 in Merrill . Since then , the segment south of US Highway 10 ( US 10 ) was returned to local control and decommissioned . In May 2009 , M-30 was extended southerly from US 10 to M-20 , restoring some of the highway decommissioned in the 1960s to M-30 . = = Route description = = M-30 is a rural , two-lane highway . M-30 follows Meridian Road starting at an intersection with M-20 ( Isabella Road ) outside of Midland . From this intersection , the highway runs north along the Michigan Meridian through forest lands to a crossing of the Tittabawassee River near Sanford . M-30 passes t</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>The Video Collection 93 : 99 = The Video Collection 93 : 99 is the second music video compilation by American singer-songwriter Madonna . Released by Warner Music Vision , Warner Reprise Video and Warner Bros. Records on November 2 , 1999 , it contained the music video of Madonna 's singles released between 1993 to 1999 . Originally , the collection was titled The Video Collection 92 – 99 , and had included the 1992 hit " Erotica " , but was omitted due to the explicit sexual content in the video ; instead the 1998 song " The Power of Good-Bye " was added . The videos in the collection were selected personally by Madonna , who felt the 14 videos to be her best work . After its release , the collection was critically appreciated , with one group of reviewers noting the artistic capabilities of Madonna while the others noting her ability to re-invent her image from one video to another . It reached a peak of eight on Billboard 's Top Music Video sales chart . In 2008 , was certified plat</t>
+          <t>Marasmius funalis = Marasmius funalis is a species of Marasmiaceae fungus known only from Japan . The species produces small mushrooms with reddish-brown caps up to 6 millimetres ( 0.24 in ) in diameter and dark-brown , threadlike stems of up to 50 millimetres ( 2.0 in ) in length . The species has a number of distinctive microscopic features , including very long cystidia on the stem , visible as bristles . Described in 2002 by Haruki Takahashi , the species grows on dead wood . The closest relative of M. funalis is M. liquidambari , known from Mexico and Papua New Guinea , and it is also similar in appearance to M. hudonii and Setulipes funaliformis , the latter of which was named after M. funalis . = = Taxonomy = = Marasmius funalis was first described and named in a 2002 article in Mycoscience by Haruki Takahashi , based on specimens collected in 2000 . The specific name , funalis , is Latin for " rope-like " , and is in reference to the shape and character of the stem . Within the</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>U.S. Route 40 Scenic = U.S. Route 40 Scenic ( US 40 Scenic ) is a scenic route of US 40 in the U.S. state of Maryland . US 40 Scenic , which is known for most of its route as National Pike , is the old alignment of US 40 over Town Hill in eastern Allegany County and Sideling Hill in far western Washington County . The highway was originally constructed as part of a turnpike connecting Baltimore with the eastern end of the National Road at Cumberland in the early 19th century . The highway was paved as a modern road in the mid-1910s and designated US 40 in the late 1920s . US 40 was relocated over Sideling Hill in the early 1950s and over Town Hill in the mid-1960s . The US 40 Scenic designation was first applied to the old highway over Town Hill in 1965 . Following the completion of Interstate 68 ( I-68 ) at Sideling Hill , US 40 Scenic was extended east along old US 40 's crossing of the mountain in the late 1980s . US 40 Scenic is the only scenic route in the U.S. Highway System ; fo</t>
+          <t xml:space="preserve">Maryland Route 346 = Maryland Route 346 ( MD 346 ) is a state highway in the U.S. state of Maryland . The state highway runs 23.72 miles ( 38.17 km ) from U.S. Route 50 Business ( US 50 Business ) in Salisbury east to US 50 in Berlin . MD 346 is the old alignment of US 50 between Salisbury and Berlin , connecting those cities with Parsonsburg , Pittsville , and Willards in eastern Wicomico County and Whaleyville in northern Worcester County . Much of what is now MD 346 was built as the original state road between Salisbury and Ocean City in the mid-1910s . The highway was designated US 213 in 1927 and changed to US 50 in 1949 . MD 346 was first applied to Church Street in Salisbury in the 1940s ; this designation was removed in 1954 . MD 346 was reassigned in the mid-1960s to the old alignments of US 50 left behind after US 50 's bypass of Berlin opened in the late 1950s and the US 50 divided highway was completed between Salisbury and Berlin in the mid-1960s . = = Route description = </t>
         </is>
       </c>
     </row>
@@ -1421,32 +1421,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>game team play season second defense kick led lead week half record end football field named line year touchdowns players total yards ranked score completed fourth point goal drive quarterback big points head coach teams running remaining nfl punt conference defensive rushing halftime receiver player pass interception returned time offense attempt school loss offensive espn win regular quarter victory coaches plays coordinator national tackles alabama recovered tackle touchdown selected bowl linebacker yard tech passing michigan coaching sec turnover following notre dame played wide ncaa gain ball incomplete senior tennessee possession final passes preseason freshman nationally responded intercepted rushed ohio_state history</t>
+          <t>['game', 'team', 'play', 'season', 'second', 'defense', 'kick', 'led', 'lead', 'week', 'half', 'record', 'end', 'football', 'field']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hellenic Nomarchy = Hellenic Nomarchy ( Greek : Ελληνική Νομαρχία The Greek rule of law ) was a pamphlet written by " Anonymous the Greek " published and printed in Italy in 1806 . It advocated the ideals of freedom , social justice and equality as the main principles of a well-governed society , making it the most important theoretical monument of Greek republicanism . Its author , arguing for both social autonomy and national sovereignty , supported the Greek struggle for national liberation and turned to the moral greatness of ancient Greece in order to stimulate collective pride . Although this work was widely read by Greeks before the outbreak of the Greek War of Independence in 1821 , from its first appearance it was received with discomfort by contemporary scholars , and generated debates on the identity of its author . = = Background = = The origins of modern Greek republican thought can be traced in the works of Iosipos Moisiodax , a major representative of the modern Greek En</t>
+          <t xml:space="preserve">George S. Armstrong = George Seale Armstrong ( May 16 , 1867 – June 9 , 1947 ) was a Canadian businessman and politician . He served on the Edmonton City Council from 1907 to 1910 and as Mayor of Edmonton from 1910 to 1912 . Armstrong was born in what would soon become the province of Ontario in 1867 . After briefly teaching school , he entered the business industry , as a druggist . After initially gaining experience in politics on the council of Eastnor Township , he relocated west to the city of Edmonton , Alberta . In Edmonton , he established his pharmaceutical business once again and worked briefly with his brother on real estate and construction projects . In 1907 , he ran for election to the Edmonton City Council and was elected to a two-year term . In 1910 , he decided to run for the mayoralty in the municipal election ; uncontested as the only nominated candidate on election day , Armstrong was acclaimed to the mayor 's chair for the upcoming year . During his term , several </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>South Park ( season 1 ) = The first season of animated television series South Park ran for 13 episodes from August 13 , 1997 to February 25 , 1998 on the American network Comedy Central . The creators Trey Parker and Matt Stone wrote most of the season 's episodes ; Dan Sterling , Philip Stark and David Goodman were credited with writing five episodes . The narrative revolves around four children — Stan Marsh , Kyle Broflovski , Eric Cartman and Kenny McCormick — and their unusual experiences in the titular mountain town . South Park originated from Parker and Stone 's 1992 animated short , Jesus vs. Frosty . The low-budget , crudely made film featured prototypes of South Park 's main characters and was followed in 1995 by another short film , Jesus vs. Santa . The latter became popular and was widely shared over the Internet , which led to talks for a series with representatives from Fox Network and Comedy Central . It debuted on the latter with an initial run of six episodes ; due t</t>
+          <t>Field hockey pitch = A hockey pitch is the playing surface for the game of field hockey . Historically , the game was played on natural turf ( grass ) but nowadays is predominantly played on an artificial turf . The transition onto artificial pitches came during the 1970s and was made mandatory for major competitions in 1976 . All the lines , markings and goal specifications are outlined by the International Hockey Federation in " The Rules of Hockey " . All line markings on the pitch form part of the area which they define . For example , a ball on the side line is still in the field of play ; a ball on the line of the penalty circle is in the penalty circle ; a foul committed over the 23-metre ( 25-yard ) line has occurred in the 23-metre area . A ball must completely cross a boundary line to be out of play , and a ball must wholly cross the goal line before a goal is scored . Due to the original formulation of the rules in England , the standard dimensions of a hockey pitch were ori</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Kevin Youkilis = Kevin Edmund Youkilis ( / ˈjuːkəlɪs / ; born March 15 , 1979 ) , also known as " Youk " / ˈjuːk / , is an American former professional baseball first baseman and third baseman . A native of Cincinnati , Ohio , he was drafted by the Boston Red Sox in 2001 , after playing college baseball at the University of Cincinnati . He played in Major League Baseball ( MLB ) for the Red Sox , the Chicago White Sox , and the New York Yankees . He is currently a special assistant to the Chicago Cubs and former Red Sox GM Theo Epstein . Known for his ability to get on base , while he was still a minor leaguer , Youkilis was nicknamed Euclis : The Greek God of Walks in the best-selling book , Moneyball : The Art of Winning an Unfair Game . A Gold Glove Award-winning first baseman , he once held baseball 's record for most consecutive errorless games at first base ( later broken by Casey Kotchman ) . He is also a three-time MLB All-Star , two-time World Series Champion , and winner of t</t>
+          <t xml:space="preserve">1986 Peach Bowl = The 1986 Peach Bowl was a post-season American college football bowl game at Fulton County Stadium in Atlanta , Georgia between the Virginia Tech Hokies and the North Carolina State Wolfpack from on December 31 , 1986 . The game was the final contest of the 1986 NCAA Division I-A football season for both teams , and ended in a 25 – 24 victory for Virginia Tech , the first bowl victory in school history . Virginia Tech came into the game with a 9 – 1 – 1 record that included an unusual win over the Temple Owls , who were forced to forfeit a victory to Virginia Tech after using an ineligible player . Facing the Hokies in the Peach Bowl were the 18th-ranked Wolfpack from North Carolina State University . N.C. State was led by head coach Dick Sheridan and had a regular-season record of 8 – 2 – 1 that included five wins over Atlantic Coast Conference teams . The 1986 Peach Bowl kicked off five years minus one day since Virginia Tech had last played in Atlanta — during the </t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Fountain of the Great Lakes = Fountain of the Great Lakes or Spirit of the Great Lakes Fountain is an allegorical sculpture by Lorado Taft in the Art Institute of Chicago South Stanley McCormick Memorial Court south of the Art Institute of Chicago Building in the Loop community area of Chicago in Cook County , Illinois , United States . It is a bronze work of art created between 1907-1913 . The fountain depicts five women arranged so that the water flows through them in the same way water passes through the Great Lakes . Note that the Great Lakes waterflow starts in Lake Superior at 600 feet ( 180 m ) above sea level and continues eastward through each lake until it reaches Lake Ontario and then passes into the St. Lawrence River . The Fountain is one of Taft 's best known works . The fountain was originally installed facing south where it remained until 1963 when it was moved next to the Morton Wing addition facing west where it sits today . In its original location it was visible fro</t>
+          <t xml:space="preserve">Curley Byrd = Harry Clifton " Curley " Byrd ( February 12 , 1889 – October 2 , 1970 ) was an American university administrator , educator , athlete , coach , and politician . Byrd began a long association with the University of Maryland as an undergraduate in 1905 , and eventually rose to the position of university president from 1936 to 1954 . In the interim , he had also served as the university 's athletic director and head coach for the football and baseball teams . Byrd amassed a 119 – 82 – 15 record in football from 1911 to 1934 and 88 – 73 – 4 record in baseball from 1913 to 1923 . Byrd Stadium , the university 's current football field , and its predecessor were both named in his honor . In graduate school at Georgetown University , he became one of football 's early users of the newly legalized forward pass , and he had a brief baseball career including one season as pitcher for the San Francisco Seals . Byrd resigned as university president in order to enter politics in 1954 </t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Key Sounds Label = Key Sounds Label is a Japanese independent record label formed in 2001 as a brand of the publishing company VisualArt 's . Key Sounds Label was formed to catalog and release music related to visual novels produced by the brand Key , also under VisualArt 's , known for developing such titles as Kanon and Air . Excluding two albums and one single that were released by Key and VisualArt 's before the label 's formation , the majority of releases on the label all have a basis from one of Key 's titles . There are other albums and singles on the label not directly related to the visual novels , such as two singles by Lia and one album by Riya . Unlike typical record labels , Key Sounds Label does not license any of the artists featured on albums and singles released on the label . When Key Sounds Label formed , Jun Maeda , Shinji Orito , and Magome Togoshi were Key 's signature composers and have continued to produce the majority of the music on the label , though Togoshi</t>
+          <t>Jan Karol Chodkiewicz = Jan Karol Chodkiewicz ( c . 1560 – 24 September 1621 ; Belarusian : Ян Караль Хадкевіч , Jan Karal Chadkievič , Lithuanian : Jonas Karolis Chodkevičius ) was a military commander of the Polish – Lithuanian Commonwealth army who was from 1601 Field Hetman of Lithuania , and from 1605 Grand Hetman of Lithuania , and was one of the most prominent noblemen and military commanders of the Polish – Lithuanian Commonwealth of his era . His coat of arms was Chodkiewicz , as was his family name . He played a major role , often as the top commander of the Commonwealth forces , in the Wallachian campaign of 1599 – 1600 , the Polish – Swedish War of 1600 – 11 , the Polish – Muscovite War of 1605 – 18 , and the Polish – Ottoman War of 1620 – 21 . His most famous victory was the Battle of Kircholm in 1605 , in which he dealt a major defeat to a Swedish army three time the size of his own . He died on the front lines during the battle of Chocim , in the besieged Khotyn Fortress</t>
         </is>
       </c>
     </row>
@@ -1456,32 +1456,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>second place position race track car lead fifth fourth sixth pole passed championship ferrari stop grid qualifying practice points drivers prix williams start finished seventh standings held pit teammate ahead started driver positions session seconds tyre flag tyres grand caution laps leading maintained podium saturday stewart finish nascar racing gearbox spun tenth quickest pitted restart fastest button lap going stops chassis conditions able win grip collided moved problems ninth eighth penalty turn team overtake gap races cars retired retire overtaking followed corner engine failed faster meant overtook time final safety collision sessions finishers set reclaimed lotus chevrolet came failure winner</t>
+          <t>['second', 'place', 'position', 'race', 'track', 'car', 'lead', 'fifth', 'fourth', 'sixth', 'pole', 'passed', 'championship', 'ferrari', 'stop']</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Hey Daddy ( Daddy 's Home ) = " Hey Daddy ( Daddy 's Home ) " is a song by American R &amp; B singer , Usher . The song is the first single in the United States from Usher 's sixth studio album Raymond v. Raymond , following the buzz single " Papers " . The song was written by longtime Usher collaborator Rico Love , Usher , Plies and The Runners and it was also produced by the Love and The Runners . The remix version of the song , featuring Plies was released to radio stations on December 8 , 2009 , and subsequently available for digital download on December 15 , 2009 . The song received positive reviews with critics praising Usher 's return to the style of music in 2004 's Confessions , as also with " Papers " . The song has peaked at number twenty-four on the Billboard Hot 100 , and at number two on the Hot R &amp; B / Hip-Hop Songs , giving Usher his third consecutive U.S. R &amp; B top five hit . = = Background and composition = = The song was leaked onto the internet in later October 2009 wit</t>
+          <t>Grenade ( song ) = " Grenade " is a song by American singer and songwriter Bruno Mars from his debut studio album , Doo-Wops &amp; Hooligans ( 2010 ) . A pop and R &amp; B ballad , " Grenade " was written and produced by The Smeezingtons ( Mars , Phillip Lawrence , Ari Levine ) with additional songwriting by Brody Brown , Claude Kelly , and Andrew Wyatt . The song was developed from an unreleased track with similar lyrical themes played by record producer Benny Blanco to Mars . " Grenade " was completely rearranged and re ‑ recorded two days before the album 's release . The song 's lyrics carry a message of unrequited love and how Mars ' heart was broken , despite his best efforts to show her his love . Initially released as a promotional single on September 28 , 2010 , it was later announced as the album 's second single , released by Atlantic and Elektra Records . " Grenade " was well received by critics , praising the vocals and emotional lyrics of the song and also considered it as one of</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Fearful Symmetry ( The X-Files ) = " Fearful Symmetry " is the eighteenth episode of the second season of the American science fiction television series The X-Files . It premiered on the Fox network on February 24 , 1995 . It was written by Steve De Jarnatt and directed by James Whitmore , Jr . The episode is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . " Fearful Symmetry " received a Nielsen rating of 10.1 and was watched by 9.6 million households . The episode received mixed reviews from critics but later won an EMA Award . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Mulder and Scully investigate the death of a federal construction worker and the destruction of various property that can only be tied to an</t>
+          <t>Labyrinth : The Computer Game = Labyrinth : The Computer Game is a 1986 graphic adventure game developed by Lucasfilm Games and published by Activision . Based on the fantasy film Labyrinth , it tasks the player with navigating a maze while solving puzzles and evading dangers . The player 's goal is to find and defeat the main antagonist , Jareth , within 13 real-time hours . Unlike other adventure games of the period , Labyrinth does not feature a command-line interface . Instead , the player uses two scrolling " word wheel " menus on the screen to construct basic sentences . Labyrinth was the first adventure game created by Lucasfilm . The project was led by designer David Fox , who invented its word wheels to avoid the text parsers and syntax guessing typical of text-based adventure games . Early in development , the team collaborated with author Douglas Adams in a week-long series of brainstorming sessions , which inspired much of the final product . Labyrinth received positive rev</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Europa Point Lighthouse = The Europa Point Lighthouse , also referred to as the Trinity Lighthouse at Europa Point and the Victoria Tower or La Farola in Llanito , is a lighthouse at Europa Point , on the southeastern tip of the British Overseas Territory of Gibraltar , on the southern end of the Iberian Peninsula , at the entrance to the Mediterranean Sea . Europa Lighthouse was inaugurated on 1 August 1841 in a brief ceremony witnessed by about 10,000 people . The first upgrade of the lighthouse occurred in 1864 , when the single-wick lamp was replaced with a Chance Brothers four-wick burner , with further changes in 1875 and in 1894 when the amount of light emitted was increased . A three incandescent mantle burner was added in 1905 . Following further modernisation in the 20th century , the lighthouse was fully automated in 1994 . Europa Point Lighthouse is operated by Trinity House . The cylindrical tower is painted white , with a wide red horizontal band in the middle . The light</t>
+          <t>Virgin Islands at the 2008 Summer Olympics = The United States Virgin Islands competed in the 2008 Summer Olympics , which were held in Beijing , the People 's Republic of China from August 8 to August 24 , 2008 . The appearance of its 23-person delegation marked its fifteenth appearance at the Olympic games , and its tenth appearance at the Summer Olympic games . In total , seven athletes participated on behalf of the Virgin Islands ( Tabarie Henry and LaVerne Jones-Ferrette in track and field , John and Julius Jackson in boxing , Thomas Barrows III in sailing , Ned Gerard in shooting , and Josh Laban in swimming ) in Beijing . Of those , John Jackson and Tabarie Henry progressed to a post-preliminary event , and Henry reached semifinals in his own . There were no Virgin Islander medalists at the Beijing Olympics . = = Background = = Between its beginning and the Beijing Olympics , the United States Virgin Islands have participated in fifteen Olympics games , including five Winter Oly</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Tiber Oil Field = The Tiber Oil Field is a deepwater offshore oil field located in the Keathley Canyon block 102 of the United States sector of the Gulf of Mexico . The deepwater field ( defined as water depth 1,300 to 5,000 feet ( 400 to 1,520 m ) , ) was discovered in September 2009 and it is operated by BP . Described as a " giant " find , it is estimated to contain 4 to 6 billion barrels ( 640 × 10 ^ 6 to 950 × 10 ^ 6 m3 ) of oil in place . Although BP states it is too early to be sure of the size – a " huge " field is usually considered to contain 250 million barrels ( 40 × 10 ^ 6 m3 ) . It required the drilling of a 10,685 m ( 35,056 ft ) deep well under 1,260 m ( 4,130 ft ) of water , making it one of the deepest wells ever drilled at the time of discovery . = = Description = = Tiber comprises multiple Lower Tertiary petroleum reservoirs located in Keathley Canyon block 102 about 250 mi ( 400 km ) southeast of Houston and 300 mi ( 480 km ) south west of New Orleans . Tiber is on</t>
+          <t>2009 Checker Auto Parts 500 = The 2009 Checker O 'Reilly Auto Parts 500 was the thirty-fifth and penultimate stock car race of the 2009 NASCAR Sprint Cup Series and the ninth in the ten-race season-ending Chase for the Sprint Cup . It was held on November 15 , 2009 at Phoenix International Raceway , in Avondale , Arizona before a crowd of 90,000 . The 312-lap race was won by Jimmie Johnson of the Hendrick Motorsports team after starting from third position . Jeff Burton finished second and Denny Hamlin came in third . Martin Truex , Jr. won the pole position , although he was passed by Kurt Busch by the end of the first lap . Fifty-six laps later , Johnson became the leader of the race . Many Chase for the Sprint Cup participants , including Jeff Gordon and Mark Martin ran in the top ten for most of the race . Johnson maintained the first position to lead the most laps of 238 , and to win his seventh race of the season . There were four cautions and nine lead changes among four differe</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Fantastic Light = Fantastic Light ( foaled February 13 , 1996 ) is a retired Thoroughbred racehorse and active sire . He was foaled in the United States but was trained in England and Dubai during his racing career , which ran from August 1998 to his retirement following the Breeders ' Cup Turf on October 2001 . He raced in six countries , winning Group One / Grade I races in five of them and was a dual winner of the Emirates World Series Racing Championship . He was named United States Champion Male Turf Horse , European Horse of the Year and European Champion Older Horse in 2001 . He was also well known for his two races against the 2001 Epsom Derby winner Galileo . In August 2012 it was announced that he had been pensioned from stallion duty while in Japan and would return to Dalham Hall in England to live out his days as a pensioner . In his early racing career , when trained by Michael Stoute , he won the Sandown Classic Trial , the Great Voltigeur Stakes , the Arc Trial and the D</t>
+          <t xml:space="preserve">Nokota horse = The Nokota horse is a feral and semi-feral horse breed located in the badlands of southwestern North Dakota in the United States . The breed developed in the 19th century from foundation bloodstock consisting of ranch-bred horses produced from the horses of local Native Americans mixed with Spanish horses , Thoroughbreds , harness horses and related breeds . The Nokota was almost wiped out during the early 20th century when ranchers , in cooperation with state and federal agencies , worked together to reduce competition for livestock grazing . However , when Theodore Roosevelt National Park was created in the 1940s , a few bands were inadvertently trapped inside , and thus were preserved . In 1986 , the park sold off a large number of horses , including herd stallions , and released several stallions with outside bloodlines into the herds . At this point , brothers Leo and Frank Kuntz began purchasing the horses with the aim of preserving the breed , and in 1999 started </t>
         </is>
       </c>
     </row>
@@ -1491,32 +1491,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>episode viewers glee club watched relationship finn rating rachel character tells kurt storyline share demographic television ratings broadcast plot creator aired guest enjoyed reception viewership quinn sue south_park praised vanderwerff storylines gave emma deemed felt think cast received tries nielsen cory_monteith commented kyle liz brittany fun rendition appearance know airing neighbours asks leave reviewers good lea_michele want ign episodes musical said nbc gets going help decides performances attracted scene tina moments houston_chronicle premiere recurring finale canning entertainment_weekly getting job wants previous mash lynch nice funny originally gives comedy cheerleader returns didn james_poniewozik logan perform characters producer reveals friends emotional mike</t>
+          <t>['episode', 'viewers', 'glee', 'club', 'watched', 'relationship', 'finn', 'rating', 'rachel', 'character', 'tells', 'kurt', 'storyline', 'share', 'demographic']</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Henry Adams Thompson = Henry Adams Thompson ( March 23 , 1837 – July 8 , 1920 ) was an American prohibitionist and professor who was the vice-presidential nominee of the Prohibition Party in 1880 . Thompson was a native of Pennsylvania , but spent much of his career in Ohio . He became a member of the United Brethren church and taught mathematics at several United Brethren colleges in the Midwest . Thompson served as president of Otterbein University from 1872 to 1886 . Much of his time as college president was devoted to improving the financial standing of the school during the economic depression that followed the Panic of 1873 . Initially a Republican , he became an early member of the Prohibition Party . His attempt at election to the vice presidency in 1880 , running on a ticket with Neal Dow of Maine , was the party 's best showing to date , but they still placed a distant fourth to the eventual winners , James A. Garfield and Chester A. Arthur . He ran for office under the Prohi</t>
+          <t xml:space="preserve">Into the Crevasse = " Into the Crevasse " is the second episode of the fourth season of the American television comedy series 30 Rock , and the 60th overall episode of the series . The episode was written by co-showrunner and executive producer Robert Carlock and directed by Beth McCarthy-Miller . It originally aired on the National Broadcasting Company ( NBC ) network in the United States on October 22 , 2009 . Guest stars in " Into the Crevasse " include Will Arnett , Caitlin Fowler , Shawn Gianella , Jon Glaser , and Savanna Samson . The episode largely revolves around repercussions from a sketch " Dealbreakers " that Liz Lemon ( Tina Fey ) had written for the fictional sketch comedy show The Girlie Show with Tracy Jordan ( TGS ) . Meanwhile , Jack Donaghy ( Alec Baldwin ) travels to Washington D.C. for a hearing on microwaves and Kenneth Parcell ( Jack McBrayer ) volunteers at an animal shelter . " Into the Crevasse " received generally positive reception from television critics . </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>I Am Unicorn = " I Am Unicorn " is the second episode of the third season of the American musical television series Glee , and the forty-sixth overall . The episode was written by series co-creator Ryan Murphy , directed by series co-creator Brad Falchuk , and first aired on September 27 , 2011 on Fox in the United States . It features the return of Shelby Corcoran ( Idina Menzel ) to the show to direct a rival glee club at William McKinley High even while New Directions , the current club , is having trouble recruiting members . Shelby also wants Quinn ( Dianna Agron ) and Puck ( Mark Salling ) , the biological parents of her adopted daughter Beth , to be a part of Beth 's life . The director of New Directions , Will Schuester ( Matthew Morrison ) sets up a " booty camp " for the less capable dancers in the club , and auditions for the school musical , West Side Story , begin . The episode received mostly positive reviews , which ranged from okay to fabulous , with approval being give</t>
+          <t>Raglan Castle = Raglan Castle ( Welsh : Castell Rhaglan ) is a late medieval castle located just north of the village of Raglan in the county of Monmouthshire in south east Wales . The modern castle dates from between the 15th and early 17th-centuries , when the successive ruling families of the Herberts and the Somersets created a luxurious , fortified castle , complete with a large hexagonal keep , known as the Great Tower or the Yellow Tower of Gwent . Surrounded by parkland , water gardens and terraces , the castle was considered by contemporaries to be the equal of any other in England or Wales . During the English Civil War the castle was held on behalf of Charles I and was taken by Parliamentary forces in 1646 . In the aftermath , the castle was slighted , or deliberately put beyond military use ; after the restoration of Charles II , the Somersets declined to restore the castle . Raglan Castle became first a source of local building materials , then a romantic ruin , and is now</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hellcats = Hellcats is an American cheerleading comedy-drama television series that originally aired on The CW in the United States from September 8 , 2010 , to May 17 , 2011 . Based on the book Cheer : Inside the Secret World of College Cheerleaders by journalist Kate Torgovnick , the series focuses in the lives of college cheerleaders , mainly Marti Perkins ( Aly Michalka ) , a pre-law college student who has to join the cheerleading team , the Hellcats , in order to get the athletic scholarship she needs . The main cast also includes Ashley Tisdale , Robbie Jones , Heather Hemmens , Matt Barr , Gail O 'Grady , and Sharon Leal . In May 2010 , Hellcats had been picked by The CW for the fall 2010 – 11 season . Initially with a 13-episode order , The CW aired the series after America 's Next Top Model on Wednesday nights . The pilot episode aired on September 8 , 2010 , and became the first premiere to ever match or build on an America 's Next Top Model lead-in since The CW began in 200</t>
+          <t>Washington Park Court District = The Washington Park Court District is a Grand Boulevard community area neighborhood on the South Side of Chicago , Illinois . It was designated a Chicago Landmark on October 2 , 1991 . Despite its name , it is not located within either the Washington Park community area or the Washington Park park , but is one block north of both . The district was named for the Park . The district includes row houses built between 1895 and 1905 , with addresses of 4900 – 4959 South Washington Park Court and 417 – 439 East 50th Street . Many of the houses share architectural features . The neighborhood was part of the early twentieth century segregationist racial covenant wave that swept Chicago following the Great Migration . The community area has continued to be almost exclusively African American since the 1930s . = = Architecture = = Washington Park Court , which runs one-way northbound from East 50th Street to East 49th Street , is a one-city block-long street loc</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Something Borrowed ( Torchwood ) = " Something Borrowed " is the ninth episode of the second series of British science fiction television series Torchwood . It was first broadcast by BBC Three on 5 March 2008 and repeated on BBC Two one week later . The episode was written by Phil Ford , directed by Ashley Way and produced by Richard Stokes . The episode featured the five initial series regulars John Barrowman , Eve Myles , Burn Gorman , Naoko Mori and Gareth David Lloyd plus recurring actor Kai Owen in a central role . The episode centers on the marriage of Torchwood employee Gwen Cooper ( Eve Myles ) to her long-term partner Rhys Williams ( Kai Owen ) . The wedding is complicated by Gwen 's sudden impregnation by a shape-shifting alien Nostrovite . Although she resolves to see her wedding through , her nuptials are interrupted by an attack from the biological mother of the alien fetus ( played successively by Collette Brown , Nerys Hughes and John Barrowman ) . With the help of Rhys </t>
+          <t>Beautiful ( MercyMe song ) = " Beautiful " is a song by contemporary Christian music band MercyMe . Written and composed by MercyMe , Dan Muckala , and Brown Bannister , the song was written for the daughters of the band 's members . The song 's lyrics revolve around self-worth and the love of God . " Beautiful " was released on September 17 , 2010 as the second single from MercyMe 's 2010 album The Generous Mr. Lovewell . " Beautiful " received generally mixed to positive reviews from critics and attained success on Christian radio , peaking at the top spot on Billboard magazine 's Christian Songs , Christian AC Indicator , Christian AC Monitored , and Soft AC / Inspo charts . " Beautiful " ranked at number 7 on the 2011 year-end Christian Songs chart , as well as at number 10 on the 2011 year-end Hot Christian AC chart . = = Background and composition = = " Beautiful " was written and composed by the members of MercyMe , Dan Muckala , and Brown Bannister . " Beautiful " was written f</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>The Other Woman ( Mad Men ) = " The Other Woman " is the eleventh episode of the fifth season of the American television drama series Mad Men and the 63rd episode of the series overall . It is co-written by Semi Chellas and Matthew Weiner , and directed by Phil Abraham . It aired on AMC in the United States on May 27 , 2012 . The episode takes place in January 1967 . Pete asks Joan to make a personal and moral sacrifice to ensure the company lands the Jaguar account . Meanwhile , the creatives work long nights to come up with the perfect pitch for the presentation . Don becomes furious after learning of the impact Megan 's new profession will have on their life . Feeling unappreciated , Peggy has lunch with Freddy Rumsen , who encourages her to make a move . Later , Peggy meets with Ted Chaough , from rival firm CGC , and accepts an offer for chief copywriter at CGC . " The Other Woman " was critically acclaimed , with some critics calling it one of the best episodes of the series . Jo</t>
+          <t xml:space="preserve">Black and Blue ( Homicide : Life on the Street ) = " Black and Blue " is the third episode of the second season of the American police drama television series Homicide : Life on the Street , and the twelfth overall episode of the series . It originally aired on NBC in the United States on January 20 , 1994 . In the episode , Pembleton aggressively investigates what he believes to be a police-related shooting . Amid pressure from Gee to pursue civilian suspects , Pembleton elicits a successful confession from an innocent man , leaving Gee feeling conflicted . Directed by Chris Menaul , the episode 's teleplay was written by James Yoshimura based on a story by series executive producer Tom Fontana . Yoshimura considered " Black and Blue " the favorite script he wrote for Homicide . Pembleton 's investigation was based on a real-life investigation into a suspicious shooting featured in David Simon 's non-fiction book Homicide : A Year on the Killing Streets , on which the Homicide series </t>
         </is>
       </c>
     </row>
@@ -1526,32 +1526,32 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>time year world won games record team years title season final second player win best set open game played career players defeated singles round lost gold sets tournament medal murray said events july olympic history later olympics championships april winning play including reached seed summer march times major following met chess series nba semifinals tournaments tennis august straight november chamberlain event american finals men titles place championship semifinal february june january records doubles slam received silver medals points playing match champion beat bolt high meter fischer masters fight losing clay madrid french relay defeating despite ranked began end freestyle reach</t>
+          <t>['time', 'year', 'world', 'won', 'games', 'record', 'team', 'years', 'title', 'season', 'final', 'second', 'player', 'win', 'best']</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Maryland Route 222 = Maryland Route 222 ( MD 222 ) is a state highway in the U.S. state of Maryland . The state highway runs 11.36 miles ( 18.28 km ) from MD 7 in Perryville north to U.S. Route 1 ( US 1 ) near Conowingo . MD 222 parallels the Susquehanna River in western Cecil County , connecting Perryville and Conowingo with Port Deposit . Due to limitations in the highway in Port Deposit , including a steep hill and a low railroad bridge , the state highway has a truck bypass that uses MD 275 , MD 276 , and US 1 through Woodlawn and Rising Sun to connect Interstate 95 ( I-95 ) with US 222 in Conowingo . MD 222 was originally constructed as MD 268 , a number presently assigned to North Street in Elkton . The state highway was paved from Perryville to Port Deposit in the late 1910s and early 1920s . MD 268 was extended north to Conowingo in the early 1930s . In 1938 , MD 268 was superseded when US 222 was extended south from US 1 in Conowingo to US 40 in Perryville . The only significa</t>
+          <t xml:space="preserve">The Distrest Poet = The Distrest Poet is an oil painting produced sometime around 1736 by the British artist William Hogarth . Reproduced as an etching and engraving , it was published in 1741 from a third state plate produced in 1740 . The scene was probably inspired by Alexander Pope 's satirical poem The Dunciad . It depicts a scene in a small , dingy attic room where a poet sits at his desk in the dormer and , scratching his head , stares at the papers on the desk before him , evidently looking for inspiration to complete the poem he is writing . Near him sits his wife darning clothes , surprised by the entrance of a milkmaid , who impatiently demands payment of debts . = = Background = = The engraving of The Distrest Poet in its third state was issued on 15 December 1741 as a companion piece to The Enraged Musician , a comic scene of a violinist driven to distraction by the noise from the street outside his practice room . The initial plate for The Distrest Poet was produced soon </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Emanuel Lasker = Emanuel Lasker ( December 24 , 1868 – January 11 , 1941 ) was a German chess player , mathematician , and philosopher who was World Chess Champion for 27 years ( from 1894 to 1921 ) . In his prime Lasker was one of the most dominant champions , and he is still generally regarded as one of the strongest players ever . His contemporaries used to say that Lasker used a " psychological " approach to the game , and even that he sometimes deliberately played inferior moves to confuse opponents . Recent analysis , however , indicates that he was ahead of his time and used a more flexible approach than his contemporaries , which mystified many of them . Lasker knew contemporary analyses of openings well but disagreed with many of them . He published chess magazines and five chess books , but later players and commentators found it difficult to draw lessons from his methods . Lasker made contributions to the development of other games . He was a first-class contract bridge play</t>
+          <t xml:space="preserve">Hurricane Celeste ( 1972 ) = Hurricane Celeste of August 1972 was the first known tropical cyclone to strike Johnston Atoll as a hurricane . Forming from a disturbance in the East Pacific on August 6 , the storm began a general westward movement it would take throughout most of its life . The storm intensified steadily , becoming a Category 1 hurricane on August 10 . It kept steady at this intensity until it reached the Central Pacific . Upon entering the Central Pacific , intensification began anew , and by August 14 , the hurricane reached a peak intensity of 135 mph ( 217 km / h ) . After maintaining this intensity for twelve hours , the hurricane began to weaken while passing south of Hawaii . The weakening phase was similar to its intensification in that the storm lost intensity slowly . Celeste then made a turn to the northwest and dropped below hurricane intensity on August 21 . The storm then entered an area of vertical wind shear , causing it to dissipate soon after . Celeste </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Nicola Zagame = Nicola Maree " Ziggy " Zagame ( born 11 August 1990 in Sydney ) is an Australian water polo centre back / driver . She attended Kirrawee High School in New South Wales . One of her hobbies is art , and some of it was displayed as part of an exhibit at the Hazelworth Regional Gallery and Arts Centre in 2008 . She became a water polo player after being recruited from surf lifesaving when she was thirteen . She has had a water polo scholarship with the New South Wales Institute of Sport . She plays for the Cronulla Sharks in the National Water Polo League where she has twice set single season scoring records . She has represented her country as a member of Australia women 's national water polo team on both the junior and senior levels , and was part of the silver winning team at the 2010 FINA Women 's Water Polo World Cup . She represented Australia at the 2012 Summer Olympics . = = Personal = = Zagame , nicknamed Ziggy and Nicky , was born on 11 August 1990 in Sydney and</t>
+          <t>Tommy Thompson presidential campaign , 2008 = The Tommy Thompson presidential campaign of 2008 began when the former Wisconsin Governor and Secretary of Health and Human Services Tommy Thompson announced his candidacy for the Republican nomination for president of the United States on April 1 , 2007 . Thompson centered his campaign in Iowa , focusing primarily on the issues of health care reform and the War in Iraq . He dropped out of the race on August 12 , 2007 following a sixth-place finish in the Ames straw poll and went on to endorse Rudy Giuliani for president and then John McCain following Giuliani 's withdrawal . Had he been elected , Thompson would have become the second Roman Catholic president ( after John F. Kennedy ) and the first Wisconsin-born president . He was the first former Secretary of Health and Human Services to seek the presidency . = = Background = = Tommy Thompson 's political career began in 1966 upon his election to the Wisconsin State Assembly after graduat</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Grammy Award for Best Concept Music Video = The Grammy Award for Best Concept Music Video was an award that was presented to recording artists at the 30th Grammy Awards in 1988 , and the 31st Grammy Awards in 1989 , for quality , concept music videos . The Grammy Awards ( Grammys ) is an annual ceremony that was established in 1958 and was originally called the Gramophone Awards ; awards are presented by the National Academy of Recording Arts and Sciences of the United States to " honor artistic achievement , technical proficiency and overall excellence in the recording industry , without regard to album sales or chart position " . Beginning in 1982 , the Academy began to honor quality music videos with the Video of the Year category , which was discontinued with the establishment of the MTV Video Music Awards in 1984 and was replaced with two awards ; Best Video , Short Form and Best Video Album . Criteria changes for the 1988 and 1989 ceremonies resulted in the Best Concept Music Vid</t>
+          <t>Polikarpov VIT-1 = The Polikarpov VIT-1 ( Russian : Vozdooshny Istrebitel ' Tahnkov — Flying Tank Destroyer ) was a Soviet twin-engined multi-purpose aircraft developed before World War II . One prototype was built in 1937 , with an extremely heavy armament for ground attack duties . That was the only example built as it was decided to revise the design with more powerful engines as the VIT-2 . = = Development = = The Polikarpov design bureau ( OKB ) was ordered , in 1936 , to begin development of a fast twin-engined aircraft that could be used for ground attack duties and as a heavy fighter . It delivered the ground attack version the following year for evaluation , although it could be modified as necessary for other roles . The VIT-1 was reasonably successful , but it was decided to give it more powerful engines and modify its structure . The improved aircraft was designated as the VIT-2 . The VIT-1 was a low-winged , twin-engined aircraft with a mixed structure . The monocoque fuse</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>The X-Files = The X-Files is an American science fiction horror drama television series created by Chris Carter . The program originally aired from September 10 , 1993 , to May 19 , 2002 , on Fox , spanning nine seasons , with 202 episodes and a feature film of the same name , before returning with a second film in 2008 and a six-episode tenth season in 2016 . The series revolves around FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who investigate X-Files : marginalized , unsolved cases involving paranormal phenomena . Mulder believes in the existence of aliens and the paranormal while Scully , a medical doctor and a skeptic , is assigned to make scientific analyses of Mulder 's discoveries to debunk his work and thus return him to mainstream cases . Early in the series , both agents become pawns in a larger conflict and come to trust only each other and a very few select people . They develop a close relationship which begins as a platonic frien</t>
+          <t xml:space="preserve">Jacques Le Gris = Sir Jacques Le Gris ( c . 1330s – 27 December 1386 ) was a squire and knight in fourteenth century France who gained fame and infamy when he engaged in the last judicial duel permitted by the Parlement of Paris after he was accused of rape by the wife of his neighbour and rival Sir Jean de Carrouges . Carrouges brought legal proceedings against Le Gris before King Charles VI who after hearing the evidence , authorised a trial by combat to determine the question . The duel attracted thousands of spectators and has been discussed by many notable French writers , from the contemporary Jean Froissart to Voltaire . Described as a large and physically imposing character with a reputation for womanising , Le Gris was a liege man ( feudal retainer ) of Count Pierre d 'Alençon and a favourite at his court , governing a large swathe of his liege lord 's territory in addition to his own ancestral holdings . Le Gris ' insistence on defending his case by chivalric trial by combat </t>
         </is>
       </c>
     </row>
@@ -1561,32 +1561,32 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>game player mario mega gameplay graphics praised enemies players ign controls gaming sonic arcade console levels development gamespot mode nintendo screen nes adventure features reviewers version games gamepro scrolling developers super boy gamecube multiplayer rare sega ups robot crash graphical bosses items wii gamespy eurogamer reception weapon nintendo_power reviewer difficulty available visuals japan virtual weapons informer lack puzzles metacritic level ported shooter gamers feature collect xbox gamerankings gamesradar handheld north_america enemy puzzle characters allows modes obstacles stages developed criticized sequel creatures gamer abilities predecessor sprites lauded nintendo_entertainment_system hidden ability consoles evil addictive takes playable stating developer online shoot genre cartridge</t>
+          <t>['game', 'player', 'mario', 'mega', 'gameplay', 'graphics', 'praised', 'enemies', 'players', 'ign', 'controls', 'gaming', 'sonic', 'arcade', 'console']</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mikengreg = Mikengreg is an independent video game development team of Mike Boxleiter and Greg Wohlwend . Their games include Solipskier , Gasketball , and TouchTone . The two met in a game development class at Iowa State University and later began to collaborate on the Adobe Flash game Dinowaurs . When the project was funded , they founded Intuition Games with other college friends in Ames , Iowa , where they worked on small Flash games such as Gray , Lifecraft , and Fig . 8 for Flash game sites such as Kongregate . Dinowaurs was one of the first games signed for the Kongregate platform . Their other games involved controlling the weather , influencing individuals in a riot , and riding a bicycle . Boxleiter and Wohlwend worked on several additional games that were put on hiatus . They later became Mikengreg in 2010 and released Solipskier in August for both Flash and iOS later that year . Its success let them take a more experimental approach towards their next game , the free-to-pla</t>
+          <t>Grey Matters ( Fringe ) = " Grey Matters " is the 10th episode of the second season of the American science fiction drama television series Fringe . The episode was written by Ashley Edward Miller and Zack Stentz , and directed by Jeannot Szwarc . It centered on three mental patients who mysteriously became sane again after shapeshifters from the parallel universe removed a piece of foreign tissue from each of their brains ; this tissue is later revealed to have been taken from the brain of Walter Bishop years before . The fringe team of Olivia Dunham , Peter Bishop , and Walter investigate and face a new enemy , Thomas Jerome Newton ( guest actor Sebastian Roché ) , whose purpose is to decipher the missing parts of Walter 's brain and find out how to move between universes . The episode features the first scene between Walter and his old colleague William Bell ( played by guest actor Leonard Nimoy ) . At the time , it fulfilled Nimoy 's commitment to the show , though he later returne</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>The Lord of the Rings : The Return of the King ( video game ) = The Lord of the Rings : The Return of the King is a 2003 action / hack and slash video game developed by EA Redwood Shores for the PlayStation 2 and Windows . It was ported to the GameCube and Xbox by Hypnos Entertainment , to the Game Boy Advance by Griptonite Games , to mobile by JAMDAT , and to OS X by Beenox . The game was published by Electronic Arts . It is a sequel to the 2002 game The Lord of the Rings : The Two Towers . The game is an adaptation of Peter Jackson 's 2002 film The Lord of the Rings : The Two Towers and his 2003 film The Lord of the Rings : The Return of the King , which was released shortly after the game . As it is not an adaptation of J. R. R. Tolkien 's 1954 novel , The Return of the King , the third volume in his Lord of the Rings trilogy , anything from the novel not specifically mentioned or depicted in the films could not be represented in the game . This is because , at the time , Vivendi Un</t>
+          <t>Snake Rattle ' n ' Roll = Snake Rattle ' n ' Roll is a platforming video game developed by Rare . It was published by Nintendo and released for the Nintendo Entertainment System in North America in July 1990 and in Europe on March 27 , 1991 . It was ported to the Mega Drive and released by Sega in June 1993 . The game features two snakes , Rattle and Roll , as they make their way through eleven 3D isometric levels . The object is to navigate the obstacles in each level and eat enough " Nibbley Pibbleys " to ring a weigh-in bell located in the level , which will allow the snakes to exit . The game can be played by a single player or by two players simultaneously . Snake Rattle ' n ' Roll was developed by Rare members Tim Stamper and Mark Betteridge , with music composed by David Wise , which featured music inspired by " Shake , Rattle and Roll " , as well as other 1950s-era oldies . It was well received by various video gaming magazines , and praises include well-designed 3D environment</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>The Black Island = The Black Island ( French : L 'Île noire ) is the seventh volume of The Adventures of Tintin , the comics series by Belgian cartoonist Hergé . Commissioned by the conservative Belgian newspaper Le Vingtième Siècle for its children 's supplement Le Petit Vingtième , it was serialised weekly from April to November 1937 . The story tells of young Belgian reporter Tintin and his dog Snowy , who travel to England in pursuit of a gang of counterfeiters . Framed for theft and hunted by detectives Thomson and Thompson , Tintin follows the criminals to Scotland , discovering their lair on the Black Island . The Black Island was a commercial success and was published in book form by Casterman shortly after its conclusion . Hergé continued The Adventures of Tintin with King Ottokar 's Sceptre , while the series itself became a defining part of the Franco-Belgian comics tradition . In 1943 , The Black Island was coloured and re-drawn in Hergé 's distinctive ligne-claire style fo</t>
+          <t>The Last Remnant = The Last Remnant ( ラストレムナント , Rasuto Remunanto ) is a role-playing video game developed and published by Square Enix for the Xbox 360 . The game had a worldwide release on November 20 , 2008 , and was also released for Microsoft Windows in March 2009 , and received an international release through digital retailer Steam in April 2009 . A PlayStation 3 version was originally announced , but was never released . The game is set in a fictional world divided into multiple city-states inhabited by four different species and whose past includes conflicts over " Remnants , " magical artifacts of varying forms . The player takes the role of Rush Sykes , a young man searching for his sister that becomes entangled in a secret war . It features a unique battle system in which the player command multiple groups , or " unions " , of characters rather than individual units . The game was directed by Hiroshi Takai and was the first game developed by Square Enix to use the Unreal En</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Silent Hill : Origins = Silent Hill : Origins , known as Silent Hill : Zero ( Japanese : サイレントヒル ゼロ , Hepburn : Sairentohiru Zero ) in Japan , is a survival horror video game for the PlayStation Portable developed by Climax Studios . It was published by Konami Digital Entertainment worldwide in late 2007 , beginning in early November with the United Kingdom . A port for the PlayStation 2 was released worldwide in early 2008 , beginning in March with North America , and it is available on the PlayStation Network in Europe . The fifth installment in the Silent Hill series , Origins is a prequel to the first game ( 1999 ) . Set in the series ' eponymous , fictional American town , Origins follows trucker Travis Grady as he searches for information about a girl whom he rescued from a fire . Along the way , he unlocks his repressed childhood memories . Gameplay uses a third-person perspective , and emphasizes combat , exploration , and puzzle-solving , similar to the previous installments .</t>
+          <t>Cold War ( Doctor Who ) = " Cold War " is the eighth episode of the seventh series of the British science-fiction television drama Doctor Who . It first aired on BBC One on 13 April 2013 , and was written by Mark Gatiss and directed by Douglas Mackinnon . In the episode , alien time traveller the Doctor ( Matt Smith ) and his companion Clara Oswald ( Jenna-Louise Coleman ) land on a Soviet submarine in 1983 during the Cold War , where the Ice Warrior Grand Marshal Skaldak breaks loose and plots revenge against humanity . " Cold War " reintroduces the Ice Warriors , who were last seen in the Third Doctor serial The Monster of Peladon ( 1974 ) . Bringing back the monsters was Gatiss ' idea , and he convinced executive producer Steven Moffat by coming up with new things to do with them . The Ice Warriors ' costume was improved but not significantly redesigned , as the production team felt they were not well known enough . The episode was filmed in June 2012 on a submarine set , as the sto</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>ToeJam &amp; Earl in Panic on Funkotron = ToeJam &amp; Earl in Panic on Funkotron is a platform video game developed by Johnson Voorsanger Productions and published by Sega in 1993 for the Sega Genesis . The game is the sequel to cult video game ToeJam &amp; Earl , released in 1991 . The game concerns two alien protagonists , ToeJam and Earl , both of whom have escaped from Earth , where they had crash landed . After returning to their home planet of Funkotron , the duo discover a number of antagonistic Earthlings have stowed away on the spacecraft and are wreaking havoc across the planet . The player must hunt down these Earthlings and imprison them in jars before sending them back to Earth . The game 's platform format was a departure from the original ToeJam &amp; Earl , a treasure hunt game with randomly generated levels , inspired by the game Rogue . Creators Greg Johnson and Mark Voorsanger originally began designing a game built on the concepts of the original , but changed to a more generic ty</t>
+          <t>SimTower = SimTower : The Vertical Empire ( known as The Tower ( ザ ・ タワー , Za Tawā ) in Japan ) is a construction and management simulation video game developed by OpenBook Co . , Ltd. and published by Maxis for the Microsoft Windows and Macintosh System 7 operating systems in November 1994 . In Japan , it was published by OpenBook that same year and was later released for the Sega Saturn and Sony PlayStation in 1996 . The game allows players to build and manage a tower and decide what facilities to place in it , in order to ultimately build a five-star tower . Random events take place during play , such as terrorist acts that the player must respond to immediately . Critical reception towards the game was generally positive . Reviews praised the game 's formula , including its open-ended nature and its ability to immerse the player into the game . Criticism targeted the game 's lack of documentation , which some reviewers found made it harder to learn how to play the game . The in-gam</t>
         </is>
       </c>
     </row>
@@ -1596,32 +1596,32 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>series character television season episodes episode characters story cast dvd aired doctor viewers producer seasons awards broadcast voice producers finale ratings star writing trek original bbc fans relationship enterprise writer comic simpsons anime south_park role writers nominated drama clark homer manga created appeared pilot premiere production gwen voiced animated wanted felt actors animation award emmy nickelodeon voyager executive recurring lisa released airing audience script comedy produced best outstanding shows arc idea portrayed written adventures scripts primetime davies featured spin filmed showrunner scenes adam kenny plot sitcom programme tardis comics main friends life angel volumes fringe fan described actor crew originally</t>
+          <t>['series', 'character', 'television', 'season', 'episodes', 'episode', 'characters', 'story', 'cast', 'dvd', 'aired', 'doctor', 'viewers', 'producer', 'seasons']</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Skyfall = Skyfall is the 23rd James Bond film produced by Eon Productions and released in 2012 . It features Daniel Craig in his third performance as James Bond , and Javier Bardem as Raoul Silva , the film 's villain . It was directed by Sam Mendes and written by Neal Purvis , Robert Wade and John Logan , and features an Academy Award-winning theme , sung by Adele . It was distributed by Metro-Goldwyn-Mayer ( MGM ) and Columbia Pictures . The story centres on Bond investigating an attack on MI6 ; the attack is part of a plot by former MI6 agent Raoul Silva to humiliate , discredit and kill M as revenge against her for betraying him . The film sees the return of two recurring characters to the series after an absence of two films : Q , played by Ben Whishaw , and Moneypenny , played by Naomie Harris . Skyfall is the last film of the series for Judi Dench , who played M , a role that she had played in the previous six films . The position is subsequently filled by Ralph Fiennes ' charac</t>
+          <t>Let 's Kill Hitler = " Let 's Kill Hitler " is the eighth episode of the sixth series of the British science fiction television series Doctor Who , and was first broadcast on BBC One , Space and BBC America on 27 August 2011 . " Let 's Kill Hitler " was written by Steven Moffat and directed by Richard Senior . In the episode , alien time traveller the Doctor ( Matt Smith ) and his companions Amy Pond ( Karen Gillan ) and her husband Rory Williams ( Arthur Darvill ) crash land in 1938 Berlin when the TARDIS is hijacked by Amy and Rory 's childhood friend , Mels ( Nina Toussaint-White ) . They accidentally save Adolf Hitler ( Albert Welling ) who was scheduled for torture by the Teselecta , a time-travelling justice department . When shot by Hitler , Mels unexpectedly regenerates into River Song , the grown version of Amy and Rory 's child who had been taken away from them . As River is a criminal herself due to her future execution of the Doctor , the Teselecta pursue her instead , whil</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Bad Words ( film ) = Bad Words is a 2013 American black comedy film directed by Jason Bateman and written by Andrew Dodge . Marking Bateman 's directorial debut , the film stars Bateman as a middle-aged eighth grade dropout who enters the National Golden Quill Spelling Bee through a loophole . It also stars Kathryn Hahn , Rohan Chand , Ben Falcone , Philip Baker Hall , and Allison Janney . Dodge 's screenplay for Bad Words was featured on the 2011 Black List and was shortly thereafter picked up by Bateman . In the original script , the story was set at the Scripps National Spelling Bee , but the name was changed to a fictional bee since the filmmakers did not expect Scripps to allow the use of their name in the film . After two other actors declined to play the main character , Bateman decided to take on the role himself , and cast the other roles by a combination of contacting friends and open casting calls . Filming took place in Los Angeles at the end of 2012 . The film premiered at</t>
+          <t>The Big Bang ( Doctor Who ) = " The Big Bang " is the thirteenth and final episode in the fifth series of British science fiction television programme Doctor Who , broadcast on 26 June 2010 on BBC One . It is the second part of the two-part series finale started with " The Pandorica Opens " , written by Steven Moffat and directed by Toby Haynes . Following the end of the previous episode , alien time traveller the Doctor ( Matt Smith ) is trapped in a prison from which escape is impossible , the TARDIS has blown up with River Song ( Alex Kingston ) inside , and the Doctor 's companion Amy Pond ( Karen Gillan ) has been shot and killed by an Auton replica of her fiancé Rory Williams ( Arthur Darvill ) . As the universe is collapsing , the Doctor uses time travel to solve these problems and ultimately reboot the universe . The episode sees the climax of Amy 's character arc and the story arc of the series regarding the cracks in the universe , though Moffat chose to leave a few things un</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Nausicaä of the Valley of the Wind ( film ) = Nausicaä of the Valley of the Wind ( Japanese : 風の谷のナウシカ , Hepburn : Kaze no Tani no Naushika ) is a 1984 Japanese animated epic science fantasy adventure film written and directed by Hayao Miyazaki , based on his own 1982 manga of the same name . Isao Takahata produced the film for Tokuma Shoten and Hakuhodo , with Topcraft animating . Joe Hisaishi , in his first collaboration with Miyazaki , composed the film 's musical score . The film stars the voices of Sumi Shimamoto , Goro Naya , Yoji Matsuda , Yoshiko Sakakibara and Iemasa Kayumi . Taking place in a post-apocalyptic world in the far future , the film tells the story of Nausicaä ( Shimamoto ) , the young princess of the Valley of the Wind . She becomes embroiled in a struggle with Tolmekia , a kingdom that tries to use an ancient weapon to eradicate a jungle of mutant giant insects , and attempts to stop the Tolmekians from enraging these creatures . The film was released in Japan on</t>
+          <t xml:space="preserve">7 Khoon Maaf = 7 Khoon Maaf , pronounced Saat Khoon Maaf , released internationally as Seven Sins Forgiven , is a 2011 Indian romantic crime thriller film directed , co-written and co-produced by Vishal Bhardwaj . The film stars Priyanka Chopra in the lead role , with Naseeruddin Shah , Irrfan Khan , Annu Kapoor , Neil Nitin Mukesh , John Abraham , Aleksandr Dyachenko , Vivaan Shah and Usha Uthup in supporting roles . The film tells the story of a femme fatale , Susanna Anna-Marie Johannes , an Anglo-Indian woman who murders her seven husbands in an unending quest for love . 7 Khoon Maaf is an adaptation of the short story Susanna 's Seven Husbands by Ruskin Bond . After Bhardwaj saw the possibility of a script in the short story , he requested Bond to develop the story for a film adaptation . Bond expanded his four-page short story into an 80-page novella , and later co-wrote the script with Bhardwaj . The film 's musical score was composed by Bhardwaj , and Gulzar wrote the lyrics . </t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Stan Marsh = Stanley " Stan " Marsh is a main character in the animated television series South Park . He is voiced by and loosely based on series co-creator Trey Parker . Stan is one of the show 's four central characters , along with his friends Kyle Broflovski , Kenny McCormick and Eric Cartman . He debuted on television when South Park first aired on August 13 , 1997 , after having first appeared in The Spirit of Christmas shorts created by Parker and long-time collaborator Matt Stone in 1992 ( Jesus vs. Frosty ) and 1995 ( Jesus vs. Santa ) . Stan is a third , then fourth-grade student who commonly has extraordinary experiences not typical of conventional small-town life in his fictional hometown of South Park , Colorado . Stan is generally depicted as friendly , knowledgeable , helpful , and relaxed . He often shares with his best friend Kyle a leadership role as the protagonist of the show . Stan is unreserved in expressing his distinct lack of esteem for adults and their influe</t>
+          <t>Mobile Suit Gundam SEED = Mobile Suit Gundam SEED ( Japanese : 機動戦士ガンダムSEED ( シード ) , Hepburn : Kidō Senshi Gandamu Shīdo ) is an anime series developed by Sunrise and directed by Mitsuo Fukuda . The ninth installment in the Gundam franchise , Gundam SEED takes place in a future calendar era , in this case the Cosmic Era , the first to do so . In this era , mankind has developed into two subspecies : Naturals , who reside on Earth , and Coordinators , genetically enhanced humans capable of amazing feats of intellect who emigrate to man-made orbital colonies to escape persecution by natural humans . The story revolves around a young Coordinator Kira Yamato who becomes involved in the war between the two races after a third , neutral faction 's space colony is invaded by the Coordinators . The television series was broadcast in Japan between 2002 and 2003 , on the Tokyo Broadcasting System and Mainichi Broadcasting System networks , beginning a broadcast partnership with the Gundam franc</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>The Diamond Smugglers = The Diamond Smugglers is a non-fiction work by Ian Fleming that was first published in 1957 in the United Kingdom and in 1958 in the United States . The book is based on two weeks of interviews Fleming undertook with John Collard , a member of the International Diamond Security Organisation ( IDSO ) , which was headed by Sir Percy Sillitoe , the ex-chief of MI5 who worked exclusively for the diamond company De Beers . The IDSO was formed by Sillitoe to combat the smuggling of diamonds from Africa , where , it was estimated , £ 10 million ( £ 217,431,365 in 2016 pounds ) worth of gems were being smuggled out of South Africa alone every year . The book expands upon articles Fleming wrote for The Sunday Times in 1957 . Fleming was better known as the author of a series of books about his super-spy creation , James Bond ; The Diamond Smugglers is one of two non-fiction books he wrote . It was broadly well-received , although some reviewers commented on the stories n</t>
+          <t>Jalen Brunson = Jalen Brunson ( born August 31 , 1996 ) is an American basketball player who plays for the Villanova Wildcats men 's basketball where he has completed his freshman season for the 2015 – 16 team . He completed his senior season for Stevenson High School in Lincolnshire , Illinois in the 2014 – 15 academic year . According to ESPN , he ended his junior year of high school as the number one point guard in the country and prior to his senior year he was rated number one by Scout.com. He was selected as the 2014 Illinois Boys Basketball Gatorade Player of the Year . He was selected to participate in the 2015 McDonald 's All-American Boys Game as well as the 2015 Jordan Brand Classic and to represent the Team USA in the Nike Hoop Summit . As a senior he repeated as the 2015 Illinois Gatorade Player of the Year and earned a third Associated Press All-state recognition ( 2nd first team ) . That year , he led Stevenson to the Illinois High School Association ( IHSA ) Class 4A ch</t>
         </is>
       </c>
     </row>
@@ -1631,32 +1631,32 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>campaign said announced stated saying support election media party political criticized government president leader presidential republican nomination polls campaigning debate bush january interview primary candidacy candidate issues poll senator democratic policy reagan stating nixon asked people conservative nominee vote percent mccarthy kennedy democrats run obama candidates hillary_clinton running state press barack_obama march november cuts issue public voters iraq brown labour told endorsement endorsed general campaigned supported member contest liberal conservatives votes police polling vice harper opposition february white_house gravel cnn budget allegations leadership ballot ronald_reagan senate minister clinton announcement incumbent news showed investigation politics gore received republican_party controversial spending members</t>
+          <t>['campaign', 'said', 'announced', 'stated', 'saying', 'support', 'election', 'media', 'party', 'political', 'criticized', 'government', 'president', 'leader', 'presidential']</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Alexei Kosygin = Alexei Nikolayevich Kosygin ( Russian : Алексе ́ й Никола ́ евич Косы ́ гин , tr . Aleksej Nikolajevič Kosygin ; IPA : [ ɐlʲɪˈksʲej nʲɪkɐˈlajɪvʲɪtɕ kɐˈsɨɡʲɪn ] ; 21 February [ O.S. 5 March ] 1904 – 18 December 1980 ) was a Soviet-Russian statesman during the Cold War . Kosygin was born in the city of St. Petersburg in 1904 to a Russian working-class family . He was conscripted into the labour army during the Russian Civil War , and after the Red Army 's demobilisation in 1921 , he worked in Siberia as an industrial manager . Kosygin returned to Leningrad in the early 1930s and worked his way up the Soviet hierarchy . During the Great Patriotic War ( World War II ) , Kosygin was a member of the State Defence Committee and was tasked with moving Soviet industry out of territories soon to be overrun by the German Army . He served as Minister of Finance for a year before becoming Minister of Light Industry and later , the Minister of Light and Food Industry . Stalin remove</t>
+          <t>The Collection ( 30 Rock ) = " The Collection " is the third episode of NBC 's second season of 30 Rock , and the twenty-fourth episode overall . It was written by producer Matt Hubbard and directed by producer Don Scardino , and first aired on October 18 , 2007 in the United States . In the episode , Jack Donaghy ( Alec Baldwin ) hires a private detective , Len ( Steve Buscemi ) , to investigate his past ; Angie Jordan ( Sherri Shepherd ) asks Liz Lemon ( Tina Fey ) to help her watch Tracy Jordan ( Tracy Morgan ) ; and Kenneth Parcell ( Jack McBrayer ) attempts to help Jenna Maroney ( Jane Krakowski ) gain weight by insulting her . The episode features a reference to Studio 60 on the Sunset Strip , which was compared to 30 Rock because of their similar premise . This is a recurring element in the series , as well as references to other aspects of popular culture . " The Collection " received generally positive reviews , however several critics expressed their concern over the misuse o</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Édifice Price = The Édifice Price ( English : Price Building ) is an 18-floor ( originally 16 ) skyscraper in Quebec City , Canada . Built in 1930-1931 amid controversy for Price Brothers ltd . , it is the tallest building in the Old Quebec historical district , and one of the oldest skyscrapers in Canada . The building is the property of the Quebec City municipal administration , but is leased to and used by the Caisse de dépôt et placement du Québec . A memorial is attached to the building . In 2001 , it became the location of an official residence for the Premier of Quebec , which occupies two of the upper floors . = = History = = In 1927 , John Herbert and Arthur Clifford Price , having inherited the prosperous Price Brothers Limited after the 1924 death of their father , Sir William Price III , decided to build a new headquarters for the company in Quebec City . They did not find anything to their liking on Saint-Pierre street , at the time Quebec 's main financial district , so d</t>
+          <t>Bootleg recording = A bootleg recording is an audio or video recording of a performance that was not officially released by the artist or under other legal authority . The process of making and distributing such recordings is known as bootlegging . Recordings may be copied and traded among fans of the artist without financial exchange , but some bootleggers have sold recordings for profit , sometimes by adding professional-quality sound engineering and packaging to the raw material . Bootlegs usually consist of either unreleased studio recordings or live performances , with an unpredictable level of quality . The concept of releasing unauthorised performances had been established before the 20th century , but reached new levels of popularity with Bob Dylan 's Great White Wonder , a compilation of studio outtakes and demos released in 1969 using low-priority pressing plants . The following year , the Rolling Stones ' Live 'r Than You 'll Ever Be , an audience recording of a late 1969 sh</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Pieter Nuyts = Pieter Nuyts or Nuijts ( 1598 – 11 December 1655 ) was a Dutch explorer , diplomat , and politician . He was part of a landmark expedition of the Dutch East India Company in 1626 – 27 which mapped the southern coast of Australia . He became the Dutch ambassador to Japan in 1627 , and he was appointed Governor of Formosa in the same year . Later he became a controversial figure because of his disastrous handling of official duties , coupled with rumours about private indiscretions . He was disgraced , fined and imprisoned , before being made a scapegoat to ease strained Dutch relations with the Japanese . He returned to the Dutch Republic in 1637 , where he became the mayor of Hulster Ambacht and of Hulst . He is chiefly remembered today in the place names of various points along the southern Australian coast , named for him after his voyage of 1626 – 27 . During the early 20th century , he was vilified in Japanese school textbooks in Taiwan as an example of a " typical a</t>
+          <t>Marty Hogan = Martin Francis Hogan ( October 25 , 1869 – August 15 , 1923 ) , nicknamed " The Indianapolis Ringer " , was an Anglo-American right fielder in Major League Baseball who played for the Cincinnati Reds ( 1894 ) and St. Louis Browns ( 1894 – 1895 ) . After leaving the National League , Hogan moved on to the minor league Indianapolis Hoosiers . Some sources suggest he set a national baserunning record in the 1890s . When his playing career ended , he worked as a minor league baseball manager in Ohio , Pennsylvania , and Wisconsin . As a manager , Hogan groomed several pitchers who excelled in the major leagues . He signed future stars Stan Coveleski and Sam Jones to their first professional contracts and helped launch the career of Roy Castleton , the first native of Utah to play in the major leagues . In 1912 , Hogan was among a select group of veteran managers invited to participate in the United States Baseball League , which was treated by the baseball establishment as an</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Klemens von Metternich = Prince Klemens Wenzel von Metternich ( German : Klemens Wenzel Nepomuk Lothar , Fürst von Metternich-Winneburg zu Beilstein , Anglicized as Clement Wenceslaus Lothair , Prince of Metternich-Winneburg-Beilstein ; 15 May 1773 – 11 June 1859 ) was a politician and statesman of Rhenish extraction and one of the most important diplomats of his era , serving as the Austrian Empire 's Foreign Minister from 1809 and Chancellor from 1821 until the liberal revolutions of 1848 forced his resignation . One of his first tasks was to engineer a détente with France that included the marriage of Napoleon to the Austrian archduchess Marie Louise . Soon after , he engineered Austria 's entry into the War of the Sixth Coalition on the Allied side , signed the Treaty of Fontainebleau that sent Napoleon into exile , and led the Austrian delegation at the Congress of Vienna that divided post-Napoleonic Europe amongst the major powers . For his service to the Austrian Empire he was g</t>
+          <t>Langit Makin Mendung = " Langit Makin Mendung " ( " The Sky is Increasingly Cloudy " ) is a controversial Indonesian short story . Published in Sastra magazine under the pen name Kipandjikusmin in August 1968 , it tells the story of Muhammad descending to Earth with the angel Gabriel to investigate the decreasing number of Muslims entering heaven , only to find that Muslims in Indonesia have begun fornicating , drinking alcohol , waging war on Muslims , and otherwise going against the tenets of Islam because of nasakom , a government policy during Sukarno 's administration that combined nationalism , religion , and communism . Unable to do anything to stop the rampant sinning , Muhammad and Gabriel watch the political maneuvering , crime , and famine in Jakarta in the form of eagles . Upon publication , " Langit Makin Mendung " drew heavy criticism for its depictions of Allah , Muhammad , and Gabriel . Sastra was banned in North Sumatra , and the magazine 's offices in Jakarta were att</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t xml:space="preserve">WAVES = The United States Naval Reserve ( Women 's Reserve ) , better known under the acronym WAVES for Women Accepted for Volunteer Emergency Service , was the World War II women 's branch of the United States Naval Reserve . It was established on 21 July 1942 by the U.S. Congress and signed into law by the president on 30 July 1942 . This authorized the U.S. Navy to accept women into the Naval Reserve as commissioned officers and at the enlisted level , effective for the duration of the war plus six months . The purpose of the law was to release officers and men for sea duty and replace them with women in shore activities . Mildred H. McAfee became the first director of the WAVES . She was commissioned a lieutenant commander in the Navy on 3 August 1942 , and was the first woman commissioned as an officer in the U.S. Naval Reserve ( she was later promoted to commander and then to captain ) . McAfee , on leave as President of Wellesley College , was an experienced educator and highly </t>
+          <t>OutRun Online Arcade = OutRun Online Arcade is a racing video game and the most recent release in the OutRun series . It was developed by Sumo Digital and published by Sega . The game was released on April 15 , 2009 on Xbox Live Arcade . It was also released exclusively in Europe for the PlayStation 3 on April 16 , 2009 via the PlayStation Network . Gameplay involves players racing their choice of Ferrari through a selection of fifteen stages in the shortest time possible . The game was fairly well received by critics , with aggregate scores averaging 78 % for both platforms at GameRankings . Reviewers generally felt that the game was a faithful adaptation of the OutRun 2 series of games . The upgraded high definition graphics were also lauded . Critics felt that the game was worth the price , however , some felt that the amount of available content was lacking considering the cars and stages available in the series ' other titles . On October 13 , 2010 , Sega announced that OutRun Onl</t>
         </is>
       </c>
     </row>
@@ -1666,32 +1666,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>member served elected governor committee serving worked election appointed kentucky married resigned attended born fellow legislature term opposed president massachusetts politics died secretary commission virginia admitted serve chairman votes tenure professor graduated candidate politician education buried attorney retirement helped honor seat degree chosen judge republican vote assistant wife senate democratic prominent union political studied legacy lived practice bill mayor rank board lieutenant deputy lawyer estate majority efforts senator honorary taught retired survived resign vice congress health administration post legislation appointment session delegate west_virginia voted sought refused jones opposition representing candidates daughter reform enrolled democrat master interred graduating establishing parsons attending</t>
+          <t>['member', 'served', 'elected', 'governor', 'committee', 'serving', 'worked', 'election', 'appointed', 'kentucky', 'married', 'resigned', 'attended', 'born', 'fellow']</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Copano Bay = Copano Bay is a northwestern extension of Aransas Bay , west of Rockport , Texas in Refugio and Aransas counties . It is supplied with seawater from the Gulf of Mexico via Aransas Bay , and fed freshwater from the Aransas River , Mission River and Copano Creek . As an estuary , the bay is home to a diverse ecosystem consisting of various birds including the endangered whooping crane , and numerous finfish including the redfish as well as shellfish such as oysters . It is classified as a nursery for shrimp , which prohibits production from the bay . Copano Bay is also a historic location for human usage and settlement that dates back to the 18th century , beginning with the historic port of El Copano and the 19th century settlements of St. Mary 's of Aransas and Copano . The present-day towns of Bayside , Copano Village and Holiday Beach were all founded in the 20th century . Oil and natural gas are pumped from below the bay 's surface , and contribute to the livelihood of </t>
+          <t xml:space="preserve">Kim Davis ( county clerk ) = Kimberly Jean Davis ( née Bailey ; born September 17 , 1965 ) is the county clerk for Rowan County , Kentucky who gained international attention in August 2015 when she defied a U.S. federal court order to issue marriage licenses to same-sex couples , following the June 26 , 2015 , U.S. Supreme Court decision in Obergefell v. Hodges . Kim Davis reacted to the decision by denying marriage licenses to all couples , saying she was acting " under God 's authority " . Her defiance led to her jail sentence , while both supporters and detractors hotly debated her stance in the national media . Marriage licenses in Rowan County are now being issued to all citizens as required by law . Davis was born in Jackson , Kentucky . By 1991 , Davis was serving as chief deputy clerk of Rowan County , reporting to her mother , the Rowan County clerk . Davis ' first three marriages ended in divorce in 1994 , 2006 , and 2008 ; she then remarried her second husband in 2009 . She </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bahadur Shah I = Bahadur Shah ( Urdu : بہادر شاه اول — Bahādur Shāh Awwal ) ( 14 October 1643 – 27 February 1712 ) , the seventh Mughal emperor of India , ruled from 1707 until his death in 1712 . Born Mu 'azzam , Shah was the third son of Aurangzeb with his Muslim Rajput wife Nawab Bai and the grandson of Shah Jahan . In his youth , he conspired to overthrow his father and ascend to the throne a number of times . Shah 's plans were intercepted by the emperor , who imprisoned him several times . From 1696 to 1707 , he was governor of Akbarabad ( later known as Agra ) , Kabul and Lahore . After Aurangzeb 's death Shah 's brother , Muhammad Azam Shah , declared himself successor before his defeat in the Battle of Jajau . During his reign , Shah bloodlessly annexed the Rajput states of Jodhpur and Amber and sparked controversy in the khutba by inserting the declaration of Ali as wali . His reign was also disturbed by the Sikh leader Banda Singh Bahadur , who led a rebellion against him . </t>
+          <t>Robert Winchelsey = Robert Winchelsey ( or Winchelsea ; c . 1245 – 1313 ) was an English Christian theologian and Archbishop of Canterbury . He studied at the universities of Paris and Oxford , and later taught at both . Influenced by Thomas Aquinas , he was a scholastic theologian . Winchelsey held various benefices in England , and was the Chancellor of Oxford University before being elected to Canterbury in early 1293 . Although he initially had the support of Edward I , Winchelsey later became a forceful opponent of the king . The archbishop was encouraged by the papacy to resist Edward 's attempts to tax the clergy . Winchelsey was also an opponent of the king 's treasurer Walter Langton as well as other clergy . On one occasion he rebuked an abbot so sternly that the abbot suffered a fatal heart attack . Following the election of a former royal clerk as Pope Clement V in 1305 , the king was able to secure the archbishop 's exile that same year . Upon the succession of Edward 's s</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Mzoli 's = Mzoli 's ( also known as Mzoli 's Place , Mzoli 's Meat , or Mzoli 's Butchery ) is a butchery in Gugulethu , a township on the outskirts of Cape Town , South Africa . Since Mzoli 's opened in early 2003 , the restaurant has become a popular gathering spot for Cape Town residents and a tourist attraction . Amongst Gugulethu 's residents , Mzoli 's Place has a reputation for public drunkenness and disrespect for the local community . Mzoli 's is named after the founder and owner , Mzoli Ngcawuzele . = = History = = The establishment opened in early 2003 . Owner Mzoli Ngcawuzele obtained start-up funding from the Development Bank of South Africa , which supports black-owned businesses . In October 2006 , an economic study said that Mzoli had " moved , from selling meat informally from a garage , to owning one of the most popular hangouts in Cape Town " . In November 2006 , more than 30 restaurant patrons , including a group of tourists and Democratic Alliance councillor Masizo</t>
+          <t>Peter Bynoe = Peter Charles Bernard Bynoe ( born March 20 , 1951 ) is a Chicago attorney and businessman , formerly the only African-American equity partner in the Chicago office of DLA Piper . In 1989 , he and his business partner Bertram Lee were the first African-Americans to buy a controlling interest in a National Basketball Association ( NBA ) team , when they purchased a 37.5 % share of the Denver Nuggets basketball team , and he is among the most influential minority figures in sports law and management . Bynoe kept the Chicago White Sox from leaving Chicago by developing a New Comiskey Park ( now known as U.S. Cellular Field ) . He has become a negotiator for professional sports teams ' venues . In addition , he was involved in the development of the 1996 and 2012 Summer Olympics . Bynoe serves on several boards of directors . = = Personal Background = = Born in Boston , Massachusetts , Bynoe came from a well-respected family . His father Victor C. Bynoe , had emigrated from h</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>James Sloan Kuykendall = James Sloan Kuykendall ( December 9 , 1878 – February 28 , 1928 ) was an American farmer , lawyer , and Democratic politician in the U.S. state of West Virginia . Kuykendall was twice elected as a member of the West Virginia House of Delegates representing Hampshire County ( 1907 – 1908 and 1919 – 1920 ) . Kuykendall also served three terms as the mayor of Romney and later fulfilled the position of city attorney . Kuykendall was born in 1878 in Hampshire County , West Virginia , into one of the oldest families in the county , which was of Dutch descent . He was raised on his family 's farm , where he engaged in agricultural pursuits . Kuykendall was educated in Hampshire County 's rural public schools and subsequently completed his post-secondary education at Hampden – Sydney College and Washington and Lee University . In 1901 , he graduated from the Cumberland School of Law , then completed a course in jurisprudence at the University of North Carolina School o</t>
+          <t>Multilateral Investment Guarantee Agency = The Multilateral Investment Guarantee Agency ( MIGA ) is an international financial institution which offers political risk insurance and credit enhancement guarantees . Such guarantees help investors protect foreign direct investments against political and non-commercial risks in developing countries . MIGA is a member of the World Bank Group and is headquartered in Washington , D.C. , United States . It was established in 1988 as an investment insurance facility to encourage confident investment in developing countries . MIGA 's stated mission is " to promote foreign direct investment into developing countries to support economic growth , reduce poverty , and improve people 's lives " . It targets projects that endeavor to create new jobs , develop infrastructure , generate new tax revenues , and take advantage of natural resources through sustainable policies and programs . MIGA is owned and governed by its member states , but has its own e</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Asplenium bradleyi = Asplenium bradleyi , commonly known as Bradley 's spleenwort or cliff spleenwort , is a rare epipetric fern of east-central North America . Named after Professor Frank Howe Bradley , who first collected it in Tennessee , it may be found infrequently throughout much of the Appalachian Mountains , the Ozarks , and the Ouachita Mountains , growing in small crevices on exposed sandstone cliffs . The species originated as a hybrid between mountain spleenwort ( Asplenium montanum ) and ebony spleenwort ( Asplenium platyneuron ) ; A. bradleyi originated when that sterile diploid hybrid underwent chromosome doubling to become a fertile tetraploid , a phenomenon known as allopolyploidy . Studies indicate that the present population of Bradley 's spleenwort arose from several independent doublings of sterile diploid hybrids . A. bradleyi can also form sterile hybrids with several other spleenworts . While A. bradleyi is easily outcompeted by other plants in more fertile habi</t>
+          <t>Goin ' Home ( Archie Shepp and Horace Parlan album ) = Goin ' Home is a studio album by American saxophonist Archie Shepp and pianist Horace Parlan . After their respective work in the avant-garde jazz movement of the 1960s , Shepp and Parlan both faced career challenges as the jazz scene diverged stylistically . They left the United States for Europe during the 1970s and met each other in Denmark before recording the album on April 25 , 1977 , at Sweet Silence Studio in Copenhagen . A jazz and gospel album , Goin ' Home features Shepp and Parlan 's interpretations of African-American folk melodies and spirituals . Its title is an allusion to Shepp 's return to his African cultural roots . Shepp had never recorded spirituals before and was overcome with emotion during the album 's recording because of the historical and cultural context of the songs . Although it surprised jazz listeners upon its release in 1977 , Goin ' Home was praised by music critics for its reverent tone and styli</t>
         </is>
       </c>
     </row>
@@ -1701,32 +1701,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>daily trunkline roadway national_highway_system travels designated surveys entire paved intersections designation traveling terminus rural mdot existed crosses intersection aadt continuing mobility turns calculated segment renumbering connecting routing michigan_department_of_transportation continues description connects vehicles annual intersects highways 1930s economy extended concurrency passes turning junction entirely farmland truncated alignment spur racially concurrent concurrently shortened flamboyant responsibilities heading traveled courted terminates buddy continuation calculation meets 1940s mile subtitles enters shifted limits route defied replacing rerouted rampant profanity highway entertained unchanged conducts academically portion statistical ferry lowest undivided oppressed frantic psychologically stretch altogether interstate entering counts bitterness connect reliant heads sacrificing ethnicity realigned exit apocalyptic</t>
+          <t>['daily', 'trunkline', 'roadway', 'national_highway_system', 'travels', 'designated', 'surveys', 'entire', 'paved', 'intersections', 'designation', 'traveling', 'terminus', 'rural', 'mdot']</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>M-294 ( Michigan highway ) = M-294 is a state trunkline highway in Calhoun County in the US state of Michigan . It is one of a handful of highways that was established or realigned as a result of a rationalization process initiated in 1998 during the tenure of Governor John Engler . M-294 is approximately two miles ( 3.2 km ) east of Interstate 194 ( I-194 ) and connects M-96 with I-94 southeast of Battle Creek . = = Route description = = M-294 runs northward along Beadle Lake Road from I-94 at exit 100 north through a commercial area . Past these businesses , the adjoining land is not developed for a short distance , and the roadway runs through some woodlands . North of the intersection with Golden Avenue , the highway passes through a residential neighborhood before terminating at M-96 ( Columbia Avenue ) . The highway lies entirely within Emmett Township just southeast of Battle Creek . The trunkline carries an average annual daily traffic of 6,078 vehicles south , and 5,728 vehicl</t>
+          <t>Delaware Route 16 = Delaware Route 16 ( DE 16 ) is an east-west state highway in Delaware , mainly across northern Sussex County , with a small portion near the Maryland border in extreme southwestern Kent County . It runs from Maryland Route 16 ( MD 16 ) at the Maryland border in Hickman to the Delaware Bay at Broadkill Beach . The route runs through rural areas , passing through the towns of Greenwood , Ellendale , and Milton . DE 16 intersects U.S. Route 13 ( US 13 ) and DE 36 in Greenwood , US 113 in Ellendale , DE 30 and DE 5 in the Milton area , and DE 1 between Milton and Broadkill Beach . West of DE 1 , the route serves as part of a connection between the Baltimore-Washington Metropolitan Area and the Delaware Beaches . DE 16 was built as a state highway during the 1920s and 1930s . By 1936 , the route was designated onto its current alignment . = = Route description = = DE 16 begins at the Maryland border in Hickman , Kent County , where the road continues west into that state</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Hurricane Lester ( 1998 ) = Hurricane Lester was the fifteenth tropical cyclone , twelfth named storm and eighth hurricane of the 1998 Pacific hurricane season . Lester originated from a tropical wave that emerged off the coast of Africa on September 29 . Under favorable conditions , the storm was classified as a tropical depression on October 15 . The depression was upgraded to a tropical storm later that day and a hurricane on October 16 . After undergoing fluctuations in intensity , Lester reached peak winds of 115 mph ( 185 km / h ) , a Category 3 hurricane on the Saffir-Simpson Hurricane Scale . After several days , it degenerated into a tropical storm on October 26 , and dissipated shortly after . The hurricane made its closest approach to land on October 18 , producing moderate winds and heavy rainfall . A mudslide triggered by the precipitation killed two children , although damage is unknown . = = Meteorological history = = A tropical wave moved off the coast of Africa on Sept</t>
+          <t xml:space="preserve">Ohio State Route 372 = State Route 372 ( SR 372 ) is a very short , two-lane east – west state highway in the southern part of the U.S. state of Ohio . The western terminus of this spur route is at a T-intersection with the concurrency of U.S. Route 23 ( US 23 ) and SR 104 about six and a half miles ( 10.5 km ) north of Waverly . Its eastern terminus is just 0.68 miles ( 1.09 km ) to the east of that point at the boundary of Scioto Trail State Forest . Continuing east of that point is Stoney Creek Road , which traverses through the state forest in the direction of the Scioto River . From its inception in the middle of the 1930s , the primary function of SR 372 has been to provide access to the state forest from the state highway system . = = Route description = = The entirety of SR 372 is located within Franklin Township in rural southern Ross County . Beginning at a T-intersection with the US 23 / SR 104 concurrency , SR 372 travels easterly into a series of curves in the shape of an </t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rachel Henderson = Rachel Henderson ( born 8 September 1992 ) is an Australian goalball player and is classified as a B2 competitor . While only starting playing the game in 2010 , she made the national team in 2011 and competed in the 2011 IBSA Goalball World Cup and 2011 African-Oceania regional Paralympic qualifying competition . She was selected to represent Australia at the 2012 Summer Paralympics in goalball . = = Personal life = = Henderson was born in Nuriootpa , South Australia , on 8 September 1992 . She has the visual disability of retinitis pigmentosa , a heredity disease she was diagnosed with when she was four years old . As a child , Henderson was involved in javelin , and only stopped competing in 2010 following taking up goalball . She was also involved in swimming , representing South Australia in a few national competitions , before leaving the sport at the same time she quit athletics . She graduated from Nuriootpa High School in 2010 . As of 2012 , she is studying </t>
+          <t>M-88 ( Michigan highway ) = M-88 is a state trunkline highway in the U.S. state of Michigan . It runs between US Highway 31 ( US 31 ) and US 131 / M-66 in the Lower Peninsula . Running from Mancelona to Eastport , M-88 also goes through the communities of Bellaire and Central Lake . The highway is completely within Antrim County and is known by the street name of " Scenic Highway " outside of the various communities along its routing . M-88 is an original trunkline dating back to the 1919 signing of the state system . An extension in the 1920s and paving in the late 1930s created the highway as it exists today . The highway was not listed on the National Highway System , nor is it included in the Lake Michigan Circle Tour . = = Route description = = M-88 starts in the community of Eastport at an intersection four blocks east of the Grand Traverse Bay of Lake Michigan next to Barnes County Park . From its start , it runs east along the northern end of Torch Lake . M-88 zig-zags south an</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Covered Bridges Today = Covered Bridges Today is a non-fiction book on the architecture of covered bridges in the United States . The book was written by Brenda Krekeler and published by Daring Books in 1989 . Covered Bridges Today is a frequently cited source on the topic of covered bridges and serves as a record of numerous covered bridges that have since been dismantled or demolished since the book 's publication . Krekeler 's text includes 412 covered bridges in fourteen states with a complete record of all 142 covered bridges in Ohio during its writing in 1986 and 1987 . The work has been utilized in numerous citations by later publications including Historic American Engineering Record surveys and New England 's Covered Bridges : A Complete Guide , Indiana Covered Bridges and Covered Bridges in Virginia . = = Background = = Covered bridges are timber-truss bridges with a roof and siding which , in most covered bridges , create an almost complete enclosure . The purpose of the cov</t>
+          <t>Benton City – Kiona Bridge = The Benton City – Kiona Bridge is a steel box girder and cable-stayed bridge carrying two lanes of Washington State Route 225 over the Yakima River in Benton City , Benton County , Washington . The current span was opened to traffic on July 4 , 1957 and measures 400-foot-long ( 121.9 m ) by 26-foot ( 7.8 m ) wide . Two bridges had previously connected the cities of Benton City and Kiona before and were located 300 feet ( 91 m ) downstream . The first bridge was open by 1901 , and the immediate predecessor bridge was closed and torn down in 1964 . The bridge is owned and maintained by the Washington State Department of Transportation , and was added to the Washington Heritage Register on January 25 , 2002 . = = Description = = The Benton City – Kiona Bridge is located about 150 feet ( 46 m ) from the southern terminus of Washington State Route 225 ( SR 225 ) in Benton City , just south of downtown . The unincorporated community of Kiona is just south of conc</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Herbert Hope Risley = Sir Herbert Hope Risley KCIE CSI ( 4 January 1851 – 30 September 1911 ) was a British ethnographer and colonial administrator , a member of the Indian Civil Service who conducted extensive studies on the tribes and castes of the Bengal Presidency . He is notable for the formal application of the caste system to the entire Hindu population of British India in the 1901 census , of which he was in charge . As an exponent of race science , he used the ratio of the width of a nose to its height to divide Indians into Aryan and Dravidian races , as well as seven castes . Risley was born in Buckinghamshire , England , in 1851 and attended New College , Oxford University prior to joining the Indian Civil Service ( ICS ) . He was initially posted to Bengal , where his professional duties engaged him in statistical and ethnographic research , and he soon developed an interest in anthropology . His decision to indulge these interests curtailed his initial rapid advancement t</t>
+          <t>Whitefish Bay National Forest Scenic Byway = The Whitefish Bay National Forest Scenic Byway is a National Forest Scenic Byway that runs along Whitefish Bay in the Hiawatha National Forest in the U.S. state of Michigan . The byway mostly follows Federal Forest Highway 42 ( FFH 42 ) through Chippewa County in the Upper Peninsula . As a forest highway , it is maintained jointly by the Chippewa County Road Commission ( CCRC ) and the U.S. Forest Service ( USFS ) . The route of the byway first existed as an earth road by the 1930s ; it was improved into a gravel road in the 1940s and paved between the 1950s and the 1980s . The byway designation was created in 1989 . = = Route description = = The byway starts at an intersection with M-123 south of Paradise in the Hiawatha National Forest where it runs eastward along Lake Superior Shoreline Road through birch forests . The roadway runs parallel to the North Country Trail , a hiking trail that spans several northern U.S. states ; the trail cro</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1736,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>song video number single chart performed peaked weeks carey debuted rihanna hot background week girl performance charts pop madonna swift chorus love billboard dance singer lyrics commented live singles vocals wearing united_kingdom beats ballad tempo digital jackson composition don music credits dancing track usher remix vocal accompanying directed mtv critics certified singing dancers compared entered spears artist mtv_news certifications ending formats listings progression scenes version mariah sings reception chord know downloads radio belgium verse charted videos shown premiered peak dress lyrically platinum beat dressed airplay feel peaking perry australian_recording_industry_association boyfriend songwriting hook written critical begins wore awards idolator filmed songwriter</t>
+          <t>['song', 'video', 'number', 'single', 'chart', 'performed', 'peaked', 'weeks', 'carey', 'debuted', 'rihanna', 'hot', 'background', 'week', 'girl']</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Rabiosa ( song ) = " Rabiosa " ( English : " Rabid " ) is a song by Colombian singer-songwriter Shakira , taken from her ninth studio album Sale el Sol . It was written by Armando Pérez , Edward Bello , and Shakira , and released by Epic Records as the third single from the album , on 8 April 2011 . Two versions of the song exist ; the English-language version , which features American rapper Pitbull , and the Spanish-language version , which features Dominican rapper El Cata . It is heavily influenced by merengue and dance music . Shakira and El Cata , or Pitbull , sing about each other 's sex appeal in the song . Upon its release , " Rabiosa " received generally favourable reviews from music critics , some of whom deemed it as one of the strongest tracks on Sale el Sol . Commercially , the English version of the song became a worldwide success , peaking atop record charts of countries like Portugal and Spain , and reaching the top ten in Belgium , France , Italy , and Switzerland . I</t>
+          <t>Antes de las Seis = " Antes de las Seis " ( English : " Before Six O 'Clock " ) is a song recorded by Colombian singer-songwriter Shakira for her ninth studio album Sale el Sol ( 2010 ) . Written and produced by the singer and her frequent collaborator Lester Mendez , " Antes de las Seis " is one of the " romantic " songs from the album and is musically a Latin pop ballad . It features a simple piano and acoustic guitar-supplemented beat over which Shakira delivers sad and emotional vocals . Epic Records released the song as the fourth single from Sale el Sol on 21 October 2011 . Critics gave positive reviews to " Antes de las Seis " , complimenting its lyrical content . The song performed poorly on singles charts , but was moderately successful on airplay charts . It reached number 1 on the Spanish Airplay Chart and peaked at number 14 on the Monitor Latino chart in Mexico . In the United States , it peaked at numbers 21 and 4 on the Billboard Hot Latin Songs and Latin Pop Airplay cha</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Move ( MercyMe song ) = " Move " is a song by Christian rock band MercyMe . Written by MercyMe and Dan Muckala , " Move " is a dance-rock song with a sound similar to that of pop rock band Maroon 5 . The theme of the song 's lyrics is perseverance through adversity . Released on May 23 , 2011 as the third single from MercyMe 's 2010 album The Generous Mr. Lovewell , " Move " was received with positive critical reviews , especially for the arrangement of the song . " Move " attained success as a single , peaking atop Billboard magazine 's Christian Songs , Hot Christian AC , and Christian AC Indicator charts , as well as at No. 6 on the Billboard Christian CHR chart and No. 20 on the Billboard Bubbling Under Hot 100 Singles chart . = = Background and composition = = " Move " was written by MercyMe and Dan Muckala . It was produced by Brown Bannister and Muckala , and was recorded by F. Reid Shippen at Sonic Ranch in El Paso , Texas . Overdubs were recorded by Muckala , Bannister , and B</t>
+          <t>The Story of Sigurd the Volsung and the Fall of the Niblungs = The Story of Sigurd the Volsung and the Fall of the Niblungs ( 1876 ) is an epic poem of over 10,000 lines by William Morris that tells the tragic story , drawn from the Volsunga Saga and the Elder Edda , of the Norse hero Sigmund , his son Sigurd ( the equivalent of Siegfried in the Nibelungenlied and Wagner 's Ring of the Nibelung ) and Sigurd 's wife Gudrun . It sprang from a fascination with the Volsung legend that extended back twenty years to the author 's youth , and had already resulted in several other literary and scholarly treatments of the story . It was Morris 's own favorite of his poems , and was enthusiastically praised both by contemporary critics and by such figures as T. E. Lawrence and George Bernard Shaw . In recent years it has been rated very highly by many William Morris scholars , but has never succeeded in finding a wide readership on account of its great length and archaic diction . It has been se</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Sunday Morning ( No Doubt song ) = " Sunday Morning " is a song recorded by American rock band No Doubt . It was released as the sixth single from their third studio album Tragic Kingdom ( 1995 ) . The single was made available as a CD single , cassette single , and VHS single on May 27 , 1997 through Interscope . Lyrically , the song is about Gwen Stefani 's relationship with Tony Kanal , and their breakup that followed . The track was written by band members Kanal , Gwen Stefani , and Eric Stefani , while production was handled by Matthew Wilder . The single was well received by many music critics , with one of them calling it a " standout track " . It also performed well commercially , peaking in the top 50 in several countries , including the UK , Canada , and Australia ; the song was certified gold in the latter country for sales of over 35,000 copies . Musically , " Sunday Morning " is a ska punk and reggae rock song . A music video for the single was released in 1996 and directe</t>
+          <t xml:space="preserve">Señorita ( Justin Timberlake song ) = " Señorita " is a song recorded by American singer-songwriter Justin Timberlake for his debut studio album , Justified ( 2002 ) . It was released on July 8 , 2003 by Jive Records as the fourth single from the album . The song was co-written by Timberlake , and The Neptunes ' Pharrell Williams and Chad Hugo . It was also produced by the Neptunes . According to Timberlake , the song was influenced by Stevie Wonder . Musically " Señorita " is an R &amp; B , Pop , Jazz up-tempo ballad , featuring an electric piano strut , cowbell in beat of the song , and a rhythm section . The song has been described as a Spanish " number " with a " Latin flavored " cut beat . In the track , Timberlake sings about a woman , whose attention he is trying to capture . " Señorita " received positive reviews from music critics , who commented on the track 's general sound and lyrics . The song peaked at number five on Billboard 's Top 40 Mainstream chart . It also appeared on </t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>William F. Dean = William Frishe Dean , Sr. ( August 1 , 1899 – August 24 , 1981 ) was a United States Army major general during World War II and the Korean War . He received the Medal of Honor for his actions on July 20 and 21 , 1950 , during the Battle of Taejon in South Korea . Dean was also the highest ranking American officer captured by the North Koreans during the Korean War . Born in Illinois , Dean attended the University of California at Berkeley before graduating with a commission in the US Army through the Reserve Officer 's Training Corps ( ROTC ) in 1921 . Slowly rising up the ranks in the inter-war years , Dean worked a desk job in Washington D.C. for much of World War II before being transferred to the 44th Infantry Division which he later commanded during the final days of the war , and was awarded a Distinguished Service Cross . Dean is known for commanding the 24th Infantry Division at the outbreak of the Korean War . Dean led the division for several weeks in unsucc</t>
+          <t>Undertale = Undertale is a role-playing video game created by indie developer Toby Fox . In the game , players control a human child who has fallen into the Underground , a large , secluded region underneath the surface of the Earth , separated by a magic barrier . The player meets various monsters during a quest to return to the surface , mainly through the combat system ; the player navigates through mini-bullet hell attacks by the opponent cyclically , and can opt to spare monsters instead of attacking and killing them . These choices affect the game , with the dialogue , characters , and story changing based on outcomes . Fox developed the entirety of the game independently , including writing and composing the score , with only additional art created by other artists . The game was inspired by the Mother and Mario &amp; Luigi role-playing series , the bullet hell shooter series Touhou Project , and the British comedy show Mr. Bean . Undertale was initially meant to be two hours in len</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Butterfly ( Mariah Carey song ) = " Butterfly " is a song by American singer-songwriter Mariah Carey from her sixth studio album of the same name . It was released as the second single from the album on December 1 , 1997 by Columbia Records . The song was written by Carey and Walter Afanasieff ; both of them producing and arranging the song as well . " Butterfly " is a ballad combining elements of pop and gospel genres . Carey had originally conceived it as a house record with David Morales titled " Fly Away ( Butterfly Reprise ) " . After realizing how personal the lyrics were and how they could be applied to Butterfly , she wrote the album 's title track with Afanasieff . On the song 's lyrics , Carey sings to someone , telling them to spread their wings and release into the world on their own , like a butterfly . The song 's music video depicts Carey in an abandoned house , trapped in a desolate life . As the video progresses , she leaves , apparently for the first time in years , a</t>
+          <t>Lady in the Lake trial = The Lady in the Lake trial was a 2005 murder case in which Gordon Park ( 25 January 1944 – 25 January 2010 ) a retired teacher from Leece , near Barrow-in-Furness , Cumbria , England , was jailed for life for the murder of his first wife , Carol Ann Park , in 1976 . Carol Park went missing on 17 July 1976 , and was never seen alive again by her family . In 1997 , her body was discovered by divers in Coniston Water and Gordon was arrested on suspicion of murder . The charges were subsequently dropped but in 2004 Gordon was arrested again and found guilty of his wife 's murder . The trial judge sentenced him to life imprisonment and recommended that he should serve a minimum of 15 years before being considered for parole . He was held at Garth prison , Leyland , Preston . In December 2007 he lodged an appeal against his conviction which was dismissed in November 2008 . On 25 January 2010 , he was found hanged in his cell , and pronounced dead at the scene . The d</t>
         </is>
       </c>
     </row>
@@ -1771,32 +1771,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>war following german april training japanese division attack march assigned transferred november december command commander 2nd august battalion remained 1st personnel october heavy february service awarded fighting officer september june support july killed men machine raised honours 5th days 6th australian unit combat formed january offensive units germans officers staff formation commanding advance operation 7th positions action battalions moved reserve operations period patrols brigade infantry rest middle_east divisions casualties subsequently world overseas new_zealand returned relieved disbanded squadron 3rd headquarters forces strength elements australia undertook 4th divisional general new_guinea north_africa duties served involved germany lieutenant korean wounded artillery fire gallipoli advancing</t>
+          <t>['war', 'following', 'german', 'april', 'training', 'japanese', 'division', 'attack', 'march', 'assigned', 'transferred', 'november', 'december', 'command', 'commander']</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>No. 1 Basic Flying Training School RAAF = No. 1 Basic Flying Training School ( No. 1 BFTS ) was a flying training school of the Royal Australian Air Force ( RAAF ) . Along with No. 1 Initial Flying Training School ( No. 1 IFTS ) , it was formed in response to increased demand for aircrew during the Korean War and Malayan Emergency . No. 1 BFTS was established in December 1951 at RAAF Base Uranquinty , New South Wales , where it operated de Havilland Tiger Moths and CAC Wirraways . The school absorbed the activities of No. 1 IFTS in January 1955 , as aircrew training requirements had ased following the end of the Korean War . No. 1 BFTS moved to RAAF Base Point Cook , Victoria , in May 1958 , by which time it was exclusively flying CAC Winjeels . Its training program expanded in the mid-1960s owing to Australia 's commitments in the Vietnam War . No. 1 BFTS was re-formed as No. 1 Flying Training School at Point Cook in January 1969 . = = History = = Prior to World War II , all pilot tra</t>
+          <t>Harajuku Lovers Tour = The Harajuku Lovers Tour was the first solo concert tour of American recording artist Gwen Stefani . The tour began through October to November 2005 , to support of her debut studio album Love . Angel . Music . Baby . ( 2004 ) . Although Stefani embarked on multiple tours with her band No Doubt , she initially opted not to participate in a tour to promote her album , an attitude that the singer eventually abandoned due to the commercial success of Love . Angel . Music . Baby . The Harajuku Lovers Tour consisted of only one leg , which encompassed a three-month-long series of performances that visited cities throughout the United States and Canada . Stefani recruited hip hop group The Black Eyed Peas , rapper M.I.A. , and singer Ciara to accompany her as opening acts for her endeavors . The tour produced varying responses from contemporary critics , who despite praising Stefani 's vocals , were critical of other aspects of the show such as its musical material . A</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>SMS Stettin = SMS Stettin ( " His Majesty 's Ship Stettin " ) was a Königsberg-class light cruiser of the Kaiserliche Marine . She had three sister ships : Königsberg , Nürnberg , and Stuttgart . Laid down at AG Vulcan Stettin shipyard in 1906 , Stettin was launched in March 1907 and commissioned into the High Seas Fleet seven months later in October . Like her sisters , Stettin was armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and a pair of 45 cm ( 18 in ) torpedo tubes , and was capable of a top speed in excess of 25 knots ( 46 km / h ; 29 mph ) . In 1912 , Stettin joined the battlecruiser Moltke and cruiser Bremen for a goodwill visit to the United States . After the outbreak of World War I , Stettin served in the reconnaissance forces of the German fleet . She saw heavy service for the first three years of the war , including at the Battle of Heligoland Bight in August 1914 and the Battle of Jutland in May – June 1916 , along with other smaller operations in the North an</t>
+          <t>Yes / No ( Glee ) = " Yes / No " is the tenth episode of the third season of the American musical television series Glee , and the fifty-fourth overall . Written by Brad Falchuk and directed by Eric Stoltz , the episode aired on Fox in the United States on January 17 , 2012 . It contains the revelation of an elopement , and two marriage proposals , including the proposal by Will Schuester ( Matthew Morrison ) to Emma Pillsbury ( Jayma Mays ) . Reviews were mixed for the episode . While Will 's actual proposal to Emma was received with more favor than not , the scene where Will asks Finn ( Cory Monteith ) to be his best man was roundly condemned : the notion that Will had no adult friends and would ask one of his students was inconceivable to many . There was acclaim for the subplot featuring Becky 's ( Lauren Potter ) pursuit of Artie ( Kevin McHale ) , and her mental voiceovers by Helen Mirren . The musical performances from the episode were greeted more positively than the episode as</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Russian battleship Ekaterina II = Ekaterina II ( Russian : Екатерина II Catherine II of Russia ) was the lead ship of the Ekaterina II-class pre-dreadnought battleships built for the Imperial Russian Navy in the 1880s . Her crew was considered unreliable when the crew of the battleship Potemkin mutinied in June 1905 and her engines were decoupled from the propellers to prevent her from joining Potemkin . She was turned over to the Sevastopol port authorities before being stricken on 14 August 1907 . She was re-designated as Stricken Vessel Nr. 3 on 22 April 1912 before being sunk as a torpedo target for the Black Sea Fleet . = = Design and description = = Ekaterina II was 331 feet 8.5 inches ( 101.1 m ) long at the waterline and 339 feet 3 inches ( 103.40 m ) long overall . She had a beam of 68 feet 11 inches ( 21.0 m ) and a draft of 27 feet 11 inches ( 8.5 m ) , 24 inches ( 610 mm ) more than designed . Her displacement was 11,050 long tons ( 11,230 t ) at load , almost 900 long tons</t>
+          <t>St Symphorien Military Cemetery = The St Symphorien Military Cemetery is a First World War Commonwealth War Graves Commission burial ground in Saint-Symphorien , Belgium . It contains the graves of 284 German and 229 Commonwealth soldiers , principally those killed during the Battle of Mons . The cemetery was established by the German Army on land donated by Jean Houzeau de Lehaie . It was initially designed as a woodland cemetery before being redesigned by William Harrison Cowlishaw after the Imperial War Graves Commission took over maintenance of the cemetery after the war . Notable Commonwealth burials in the cemetery include John Parr and George Lawrence Price , traditionally believed to be the first and last Commonwealth soldiers killed in action during the First World War , and Maurice Dease , the first posthumous recipient of the Victoria Cross of World War I. Notable German burials include Oskar Niemeyer , the first Iron Cross recipient of World War I. = = History = = = = = Bat</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve">German cruiser Admiral Scheer = Admiral Scheer was a Deutschland-class heavy cruiser ( often termed a pocket battleship ) which served with the Kriegsmarine of Nazi Germany during World War II . The vessel was named after Admiral Reinhard Scheer , German commander in the Battle of Jutland . She was laid down at the Reichsmarinewerft shipyard in Wilhelmshaven in June 1931 and completed by November 1934 . Originally classified as an armored ship ( Panzerschiff ) by the Reichsmarine , in February 1940 the Germans reclassified the remaining two ships of this class as heavy cruisers . The ship was nominally under the 10,000 long tons ( 10,000 t ) limitation on warship size imposed by the Treaty of Versailles , though with a full load displacement of 15,180 long tons ( 15,420 t ) , she significantly exceeded it . Armed with six 28 cm ( 11 in ) guns in two triple gun turrets , Admiral Scheer and her sisters were designed to outgun any cruiser fast enough to catch them . Their top speed of 28 </t>
+          <t>United States Institute of Peace Headquarters = The United States Institute of Peace Headquarters houses staff offices and other facilities for the government-funded think tank focused on peacemaking and conflict avoidance . The building is the first permanent home for the United States Institute of Peace ( USIP ) , established in 1984 . The headquarters is sited on a prominent location near the National Mall and Potomac River in the Foggy Bottom neighborhood of Washington , D.C. The environmentally friendly building , noted for its unique roof , was designed by architect Moshe Safdie and completed in 2011 . Critics ' reviews of the building 's design have been mixed . = = History = = In the 1980s , Democratic Senator Jennings Randolph of West Virginia led a group of lawmakers calling for a federal peace institute . USIP was established by Congress in 1984 and for many years rented office space in various buildings in downtown Washington , the last being 1200 17th Street NW . In 1996 ,</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>373rd ( Croatian ) Infantry Division ( Wehrmacht ) = The 373rd ( Croatian ) Infantry Division ( German : 373 . ( Kroatische ) Infanterie-Division , Croatian : 373 . ( hrvatska ) pješačka divizija ) was a division of the German Army during World War II . It was formed in June 1943 using a brigade from the Home Guard of the Independent State of Croatia ( Croatian : Nezavisna Država Hrvatska , NDH ) with the addition of a German cadre . The division was commanded by Germans down to battalion and even company level in nearly all cases , and was commonly referred to as a " legionnaire division " . Originally formed with the intention of service on the Eastern Front , it was used instead for anti-Partisan operations in the territory of the NDH until the end of the war . It fought mainly in the western areas of the NDH , and was involved in the attempt to kill or capture the leader of the Partisans , Josip Broz Tito , in May 1944 . Severely depleted by desertion , the division withdrew toward</t>
+          <t xml:space="preserve">Glenwood Generating Station = Glenwood Generating Station is a power station in Glenwood Landing , New York owned by National Grid plc . It is mainly known for being the former site of an architecturally significant 1920s brick power station . That building and an adjacent 1950s station were demolished over the course of 2013 to 2015 , due to their obsolescence as well as the excessive cost of safely retaining the building given its poor condition . Two smaller generators constructed in 2002 remain in operation . = = Architecture = = Station 2 was constructed in the 1920s and considered significant as a rare surviving example of early 20th-century industrial architecture . It was designed in an industrial Beaux-Arts style , with large arched windows and stringcourse intended to prevent it from becoming an eyesore given its proximity to affluent communities . It was constructed with Flemish bond brickwork and decorative limestone elements . It was also constructed to minimize noise and </t>
         </is>
       </c>
     </row>
@@ -1806,32 +1806,32 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>rainfall meteorological preparations watch florida flooding damage winds hurricane issued reported rain landfall mexico usd rains warnings sustained caused wave homes category storm national_hurricane_center flooded flash affected mbar heavy louisiana tides waves hours causing occurred inland gulf_of_mexico evacuated washed shelters warning nhc caribbean_sea saffir offshore eye mph gusts gale estimated remnants watches crops coast destroyed intensity attained ashore downed totaled minimal advised beach coastline reports southeastern strong status portions hundreds tracked surge inhg weakened disaster utc simpson atlantic_ocean impact rapidly rough gradually damaged extratropical coastal drowned hpa bahamas worst wind bermuda evacuation seas peak strongest circulation moderate resulting dropped northwestward</t>
+          <t>['rainfall', 'meteorological', 'preparations', 'watch', 'florida', 'flooding', 'damage', 'winds', 'hurricane', 'issued', 'reported', 'rain', 'landfall', 'mexico', 'usd']</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Tropical Storm Beryl ( 2012 ) = Tropical Storm Beryl was the strongest off-season Atlantic tropical cyclone on record to make landfall in the United States . The second tropical cyclone of the 2012 Atlantic hurricane season , Beryl developed on May 26 from a low-pressure system offshore North Carolina . Initially subtropical , the storm slowly acquired tropical characteristics as it tracked across warmer sea surface temperatures and within an environment of decreasing vertical wind shear . Late on May 27 , Beryl transitioned into a tropical cyclone less than 120 miles ( 190 km ) from North Florida . Early the following day , the storm moved ashore near Jacksonville Beach , Florida , with peak winds of 65 mph ( 100 km / h ) . It quickly weakened to a tropical depression , dropping heavy rainfall while moving slowly across the southeastern United States . A cold front turned Beryl to the northeast , and the storm became extratropical on May 30 . The precursor to Beryl produced heavy rain</t>
+          <t>Hurricane Baker ( 1950 ) = Hurricane Baker was a major hurricane that affected the Leeward Islands , Greater Antilles , and the Gulf Coast of the United States . The tropical cyclone was the second intense hurricane , second hurricane , and second tropical storm of the 1950 Atlantic hurricane season . Hurricane Baker attained peak winds of 120 mph ( 195 km / h ) near the Leeward Islands , traversed Antigua , and weakened to a tropical depression southwest of Puerto Rico . It re-intensified south of Cuba , strengthened to a strong Category 2 hurricane in the Gulf of Mexico , and hit the United States near Gulf Shores , Alabama , with winds of 85 mph ( 140 km / h ) . Hurricane Baker produced extensive damage in the Lesser Antilles and Cuba , but impacts were minimal in the United States . = = Meteorological history = = On the morning of August 20 , a strong tropical storm developed about 446 miles ( 718 km ) east of Basse-Terre , Guadeloupe . The tropical storm deepened to hurricane inte</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1993 – 94 South-West Indian Ocean cyclone season = The 1993 – 94 South-West Indian Ocean cyclone season was the most active since the start of reliable satellite coverage in 1967 , with 15 named storms including one named tropical depression . Activity lasted from mid-November , when Moderate Tropical Storm Alexina formed , until mid-April , when Tropical Cyclone Odille became extratropical . Four tropical cyclones – Daisy , Geralda , Litanne , and Nadia – struck eastern Madagascar , of which Geralda was the costliest and deadliest . With gusts as strong as 350 km / h ( 220 mph ) accompanied by heavy rainfall , the cyclone destroyed more than 40,000 homes and left 356,000 people homeless . Geralda killed 231 people and left more than $ 10 million in damage . Cyclone Nadia was the second deadliest cyclone , having killed 12 people in northern Madagascar and later severely damaging portions of northeastern Mozambique , killing about 240 people and leaving $ 20 million in damage in the la</t>
+          <t>Hurricane Ophelia ( 2005 ) = Hurricane Ophelia was the fifteenth named tropical cyclone and the eighth hurricane of the 2005 Atlantic hurricane season . It was a long-lived storm that was most remembered for its very erratic and extremely slow track off the East Coast of the United States , alternating several times between tropical storm and hurricane intensity . Ophelia caused some damage and beach erosion along the United States coastline from Florida to North Carolina , with its closest approach occurring on September 14 and 15 with its western eyewall crossing land and the eye remaining just offshore . Minimal damage and erosion was also reported in Atlantic Canada when Ophelia hit as a tropical storm in extratropical transition on September 17 and 18 . = = Meteorological history = = On September 6 a non-tropical low over the northern Bahamas became more organized and formed into Tropical Depression Sixteen between Andros and Grand Bahama . Shortly after forming the depression mov</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1948 Atlantic hurricane season = The 1948 Atlantic hurricane season featured the first tropical cyclone before the month of June since 1940 . The season officially began on June 15 , 1948 , and lasted until November 15 , 1948 . These dates conventionally delimit the period of each year when most tropical cyclones form in the Atlantic basin . There were 10 tropical cyclones ; six storms attained hurricane status , and four storms intensified into major hurricanes , which are Category 3 or higher on the modern-day Saffir – Simpson hurricane wind scale . Operationally , it was believed that a weak tropical disturbance formed over the southeast Bahamas in May and moved northwest into the Georgia coast near Savannah . This system was later excluded from HURDAT . The seventh tropical cyclone was not operationally considered a tropical cyclone , but was later added to HURDAT . The sixth and eighth systems , designated as Dog and Easy by the Air Weather Service in real time , respectively , we</t>
+          <t>Hurricane Kenneth ( 2005 ) = Hurricane Kenneth was the strongest and longest-tracked hurricane of the 2005 Pacific hurricane season . The eleventh named storm and fifth hurricane of the season , Kenneth developed from a disturbance in the Intertropical Convergence Zone to the southwest of Mexico on September 14 . It quickly attained peak winds of 135 mph ( 215 km / h ) on September 18 , before weakening due to increased wind shear and turning to a southwest drift . After weakening to tropical storm status , Kenneth attained a steady west-northwest motion and encountered favorable enough conditions for it to gain power and attain hurricane status on September 25 . The cyclone again weakened as its motion halted , and on September 30 Kenneth dissipated a short distance off the Big Island of Hawaii . The remnants of Kenneth produced one of the highest rainfall totals in Hawaii , reaching up to 12 inches ( 305 mm ) on Oahu . The rainfall caused flooding , though no major damage was reporte</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Hurricane Bob ( 1979 ) = Hurricane Bob was the first Atlantic tropical cyclone to be officially designated using a masculine name after the discontinuation of Joint Army / Navy Phonetic Alphabet names . Bob brought moderate damage to portions of the United States Gulf Coast and areas farther inland in July 1979 . The storm was the first hurricane in the Gulf of Mexico to form in the month of July since 1959 , and was the fifth tropical cyclone to form during the annual hurricane season . Though the origin of Bob can be traced back to a tropical wave near the western coast of Africa in late June , Bob formed from a tropical depression in the southwestern Gulf of Mexico on July 9 . Tracking in a general northward direction , favorable conditions allowed for quick strengthening . Less than a day after formation , the system reached tropical storm intensity , followed by hurricane intensity on July 11 . Shortly after strengthening into a hurricane , Bob reached its peak intensity with maxi</t>
+          <t>M-86 ( Michigan highway ) = M-86 is an east – west state trunkline highway in the US state of Michigan in the southern portion of the Lower Peninsula . The highway starts at Business US Highway 131 ( Bus . US 131 ) and M-60 in Three Rivers and ends at US Highway 12 ( US 12 ) near Coldwater . In between , it crosses farm country and runs along a section of the Prairie River . Following a highway originally numbered M-7 , the roadway was renumbered M-86 in 1940 . It has been a part of the state highway system at least since 1927 . Two other roadways carried the M-86 designation in the 1920s . Two bridges along the road are eligible for inclusion on the National Register of Historic Places ( NHRP ) . = = Route description = = M-86 begins in Three Rivers at a junction with Bus . US 131 and M-60 . From there the road travels south out of town on Main Street and across the St. Joseph River . After crossing the river , the highway runs through a residential area of town and turns eastward int</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t xml:space="preserve">1973 Pacific hurricane season = The 1973 Pacific hurricane season was an event in tropical cyclone meteorology . The most important system this year was Hurricane Ava , which was the most intense Pacific hurricane known at the time . Several other much weaker tropical cyclones came close to , or made landfall on , the Pacific coast of Mexico . The most serious of these was Hurricane Irah , which downed power and communication lines in parts of the Baja California Peninsula ; the other landfalling storms caused rain and some flooding . No tropical cyclone this season caused any deaths . This season had a quick start but a slow end . Overall activity was below average , with twelve named systems in total . Of these , five were tropical storms , seven were hurricanes , of which three were major ( Category 3 or higher on the Saffir-Simpson hurricane scale ) . Just one storm formed in August , one of the least active Augusts ever in the east Pacific . The season officially started May 15 , </t>
+          <t>Tropical Storm Debby ( 1994 ) = Tropical Storm Debby was a weak but costly tropical cyclone that affected the Lesser Antilles in September 1994 . It was the fourth named tropical storm of the 1994 Atlantic hurricane season ; it developed on September 9 east of Barbados . Debby made landfall on Saint Lucia early on September 10 , producing heavy rainfall and tropical storm-force wind gusts . The rains caused flooding and landslides , damaging about half of the island 's banana plantations . Several villages were isolated after roads and bridges were damaged . Damage totaled about $ 103 million ( 1994 USD ) . On nearby Dominica , Debby damaged crops and fisheries . While Debby was crossing Saint Lucia , its strongest thunderstorms were located north and east of the center due to wind shear . A station in Martinique reported hurricane-force winds , and about 20,000 people on the island lost power . After entering the eastern Caribbean Sea , Debby attained peak winds of 70 mph ( 110 km / h</t>
         </is>
       </c>
     </row>
@@ -1841,32 +1841,32 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>rating office jim dwight episode aired nbc watching nielsen michael pam share rated viewed ratings andy directed broadcast mulder viewers noting guest references files demographic scully agents olds plot tells tries enjoyed television liz households ages employees ign david_duchovny angela rainn_wilson scranton gets fictional dana_scully steve_carell john_krasinski funny comedy lives watched reviews dunder mifflin fbi paranormal credit fox_mulder ultimately trying gillian_anderson jenna deleted camera jenna_fischer documentary says stars talking x-files getting realizes mifflin_paper_company moments finds job michael_scott linked ed_helms calling everyday jim_halpert guide saturday reference aged entry asks depicts favorite cbs dwight_schrute ryan calls decides adults creator alan_sepinwall jan oscar</t>
+          <t>['rating', 'office', 'jim', 'dwight', 'episode', 'aired', 'nbc', 'watching', 'nielsen', 'michael', 'pam', 'share', 'rated', 'viewed', 'ratings']</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Music of Chrono Cross = The Chrono series is a video game franchise developed and published by Square Enix ( formerly Square ) . It began in 1995 with the time travel role-playing video game Chrono Trigger , which spawned two continuations , Radical Dreamers and Chrono Cross . The music of Chrono Cross was composed by Yasunori Mitsuda , the main composer of Chrono Trigger and Radical Dreamers . Chrono Cross has sparked a soundtrack album , released in 1999 by DigiCube and re-released in 2005 by Square Enix , and a greatest hits mini-album , published in 2000 by Square along with the North American release of the game . Radical Dreamers , the music of which heavily inspired the soundtrack of Chrono Cross , has not sparked any albums , though some songs from its soundtrack were reused in Chrono Cross . An album of arrangements of Chrono Cross songs was first announced by Mitsuda in 2005 , and later intended to be released to coincide with the tenth anniversary of the game in 2009 ; its r</t>
+          <t>Valentine 's Day ( The Office ) = " Valentine 's Day " is the sixteenth episode of the second season of the American comedy television series The Office , and the show 's twenty-second episode overall . Written by Michael Schur and directed by Greg Daniels , the episode first aired in the United States on February 9 , 2006 on NBC . The episode guest stars Craig Anton , Andy Buckley , Charles Esten , and Conan O 'Brien as himself . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In this episode , Michael Scott ( Steve Carell ) travels to New York City to give a presentation , but accidentally tells everyone that he " hooked up " with Jan Levinson ( Melora Hardin ) . Meanwhile , the rest of the office is jealous when Phyllis Lapin 's ( Phyllis Smith ) boyfriend Bob Vance gives her several gifts . Also , Angela Martin ( Angela Kinsey ) gives Dwight Schrute ( Rainn Wilson ) a bobblehead model of</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>The Convict = " The Convict " is the ninth episode of the third season of the American comedy television series The Office , and the show 's 37th overall . It first aired on November 30 , 2006 in the United States on NBC . The episode was the series ' only original script written by Ricky Gervais and Stephen Merchant , who are the creators of the original British comedy series of the same name . It was directed by Jeffrey Blitz , his first such credit of the series . The series depicts the everyday lives of office employees in the Scranton and Stamford branches of the fictional Dunder Mifflin Paper Company . In this episode , Michael Scott ( Steve Carell ) discovers that an employee named Martin Nash ( Wayne Wilderson ) , who came with the branches ' recent merger , was previously in prison . Michael becomes frustrated when Martin 's stories of prison sound better than working in the office . Meanwhile , Jim Halpert ( John Krasinski ) plays a prank on Pam Beesly ( Jenna Fischer ) by gi</t>
+          <t>Norodom Chakrapong = Norodom Chakrapong ( born 21 October 1945 ) is a Cambodian prince , politician , military commander and businessman . He is the fourth son of Norodom Sihanouk of Cambodia and also a half-brother of the current king , Norodom Sihamoni . Chakrapong started his career as a military pilot in 1963 . After Sihanouk was overthrown in 1970 , Chakrapong spent time under house arrest and living overseas before he joined the Funcinpec Party in 1981 . In 1991 , Chakrapong left Funcinpec to join the Cambodian People 's Party ( CPP ) and served as the Deputy Prime Minister of Cambodia between 1992 and 1993 . When the CPP lost the 1993 general elections , Chakrapong led a secession attempt in 1993 and another coup attempt in 1994 which led him to be sent into exile . After Chakrapong was pardoned in 1998 , he founded a private airline company , Royal Phnom Penh Airways . The airlines later went bankrupt in early 2006 . In 2002 , Chakrapong established a royalist party , the Khmer</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Karthi = Karthik Sivakumar ( born 25 May 1977 ) , better known by his stage name Karthi , is an Indian film actor who works in the Tamil and Telugu film industries . The younger son of actor Sivakumar , Karthi holds a Bachelor 's degree in Mechanical Engineering and master of business administration in Industrial Engineering . Since he had always wanted to become a film director , he returned to India and joined Mani Ratnam as an assistant director . He was offered acting roles and made his acting debut in Paruthiveeran in 2007 as the title character , a careless village ruffian , winning critical acclaim and several accolades including the Filmfare Award for Best Actor and a Tamil Nadu State Film Award . His next role was that of a coolie in Aayirathil Oruvan ( 2010 ) , an adventure film directed by Selvaraghavan . He achieved consecutive commercial successes with his subsequent releases – Paiyaa ( 2010 ) , Naan Mahaan Alla ( 2010 ) and Siruthai ( 2011 ) . After appearing in a series </t>
+          <t>Hurricane Brenda ( 1973 ) = Hurricane Brenda of August 1973 was the first tropical cyclone on record to make landfall in the Mexican Province of Campeche . The tropical wave that spawned Brenda moved off the west coast of Africa on August 9 , and uneventfully traversed the Atlantic . By August 18 , an associated area of low pressure developed sufficient convective activity to be declared a tropical depression . Later that day , the system intensified into a tropical storm before moving inland over the Yucatan Peninsula . Brenda had moved back over water by August 21 and began to quickly intensify , with an eye forming later that day . The storm peaked as an upper-end Category 1 hurricane with winds of 90 mph ( 140 km / h ) before making landfall in Campeche . The hurricane rapidly weakened after moving over land and dissipated the following day . Brenda made two landfalls in Mexico : first in the Yucatan and later in Campeche . Little damage resulted from the storm throughout the Yucat</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Palanga Amber Museum = The Palanga Amber Museum ( Lithuanian : Palangos gintaro muziejus ) , near the Baltic Sea in Palanga , Lithuania , is a branch of the Lithuanian Art Museum . It is housed in the restored 19th-century Tiškevičiai Palace and is surrounded by the Palanga Botanical Garden . The museum 's collection of amber comprises about 28,000 pieces , of which about 15,000 contain inclusions of insects , spiders , or plants . About 4,500 pieces of amber are exhibited ; many of these are items of artwork and jewelry . = = History and background = = The Baltic Sea coast has been a source of Eurasian amber trade since prehistoric times ( see Amber Road ) . Neolithic artifacts made of amber were discovered in nearby Juodkrantė in the 19th century - these artifacts unfortunately disappeared during the 20th century . Lithuanian mythology , folklore , and art have long associations with amber ; the legend of Jūratė and Kastytis imagines an undersea palace of amber under the Baltic , whi</t>
+          <t xml:space="preserve">Guthy-Renker = Guthy-Renker ( pronounced : Guh-thee Ren-ker ) is a Santa Monica , California , based direct-response marketing company that sells products directly to consumers through infomercials , television ads , direct mail , telemarketing , e-mail marketing , and the Internet . As of 2014 , it has 8 different product groups , with an emphasis on celebrity-endorsed beauty products . Guthy-Renker was founded in 1988 by Bill Guthy and Greg Renker . In 1995 , it began distributing the acne treatment Proactiv , which became responsible for more than half its revenues by 2005 . The company also created seven subsidiaries in the late 1990s for different products and advertising channels . It founded an infomercial channel , GRTV , which was sold to TVN Entertainment Corporation in 1999 . Guthy-Renker 's revenues grew from $ 400 million in 2001 to $ 1.5 billion by 2009 . = = History = = Guthy-Renker was founded in November 1988 by Bill Guthy and Greg Renker , who met at the Indian Wells </t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Herbert Charles Wilson = Herbert Charles Wilson ( December 7 , 1859 – December 17 , 1909 ) was a Canadian politician and physician . He served as mayor of the Town of Edmonton and Speaker of the Legislative Assembly of the North-West Territories . Wilson was born in 1859 in what would become the province of Ontario . The son of a manufacturer , Wilson 's family had extensive business interests in the area of Picton , Ontario . Wilson studied medicine and moved to Edmonton in 1882 , one of the first physicians to settle there . He was appointed to official medical positions and , for several years , owned a drugstore in town . He served as a consultant to First Nations reserves near Edmonton and also became a director of many local corporations . He was elected to the Territorial council in 1885 , and soon became its speaker . During his speakership , he helped to change the council 's rules and procedures . He left territorial politics after six years , citing health reasons . He maint</t>
+          <t>Verna ( 30 Rock ) = " Verna " is the twelfth episode of the fourth season of the American television comedy series 30 Rock , and the 70th overall episode of the series . The episode was written by co-executive producer Ron Weiner and directed by series producer Don Scardino . It originally aired on the National Broadcasting Company ( NBC ) network in the United States on February 4 , 2010 . Jan Hooks guest stars as the title character of this episode and was her last acting role before dying on October 9 , 2014 . In the episode , Jenna Maroney 's ( Jane Krakowski ) mother Verna ( Hooks ) comes to visit her , and Jenna turns to Jack Donaghy ( Alec Baldwin ) for help . At the same time , Frank Rossitano ( Judah Friedlander ) moves in with Liz Lemon ( Tina Fey ) temporarily , and they both decide to make a pact to give up their bad habits . " Verna " has received generally positive reception from television critics . According to the Nielsen ratings , the episode was watched by 5.93 milli</t>
         </is>
       </c>
     </row>
@@ -1876,32 +1876,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>species small female large male found larger size long shark dorsal head adult waters body range eyes sharks females males fins fin mainly upper feeding caught eggs adults prey black predators length lower genus populations tail habitat pectoral shallow fisheries reef bird fishes juveniles individuals marine birds water teeth sea food likely fish common skin taxonomy highly concern nest spots tip fishing mouth egg feeds reproductive snout ray assessed mating smaller jaw occurs bony animals sexual feed caudal aggressive juvenile predator pairs threatened reproduction threat tooth relatively description embryos ventral mature jaws animal subspecies usually observed anal yolk habitats catch</t>
+          <t>['species', 'small', 'female', 'large', 'male', 'found', 'larger', 'size', 'long', 'shark', 'dorsal', 'head', 'adult', 'waters', 'body']</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">M-32 ( Michigan highway ) = M-32 is a state trunkline highway in the Lower Peninsula of the U.S. state of Michigan . It is an east – west route running just over 100 miles ( 160.9 km ) from M-66 in East Jordan to US Highway 23 ( US 23 ) in Alpena . It runs via Gaylord and Atlanta through forested terrain . There is one business spur for the highway that currently exists . The highway has been extended a few times during its history , once reaching both lakes Michigan and Huron . Although it is no longer a true " cross-peninsular " highway , it is close , and there are efforts being made to extend the road back to US 31 , restoring the cross-peninsular status lost in 1974 when it was shortened away from Charlevoix . = = Route description = = M-32 starts at the corner of Lake and Water streets in East Jordan . From there it follows Water , Bridge , Mill and State streets through town . It finally turns south on Maple Street leaving town . The trunkline turns east on Rogers Road south of </t>
+          <t>Stephen Fry 's Podgrams = Stephen Fry 's Podgrams is a series of podcasts performed and recorded by British comedian and author Stephen Fry . First made downloadable on 20 February 2008 , the series of podgrams is a collection of Fry 's writings , speeches and collective thoughts . The podgrams vary in length and are not released at any set date . The podgrams are one of the most downloaded podcast series on the internet , and have appeared in the top five most downloaded podcasts from iTunes . Critical reception has been positive , as reviewers have found the podgrams interesting and engaging . = = Content = = The subject of Stephen Fry 's Podgrams differs from episode to episode . Normally , each podgram begins with an update from Fry about what he has been doing recently , his activities since the last podgram , and any housekeeping that he needs to do concerning his website , www.stephenfry.com. Fry then continues to discuss his recent activities ; although in other editions the in</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Eurasian bittern = The Eurasian bittern or great bittern ( Botaurus stellaris ) is a wading bird in the bittern subfamily ( Botaurinae ) of the heron family Ardeidae . There are two subspecies , the northern race ( B. s. stellaris ) breeding in parts of Europe and Asia , as well as on the northern coast of Africa , while the southern race ( B. s. capensis ) is endemic to parts of southern Africa . It is a secretive bird , seldom seen in the open as it prefers to skulk in reed beds and thick vegetation near water bodies . Its presence is apparent in the spring , when the booming call of the male during the breeding season can be heard . It feeds on fish , small mammals , fledgling birds , amphibians , crustaceans and insects . The nest is usually built among reeds at the edge of bodies of water . The female incubates the clutch of eggs and feeds the young chicks , which leave the nest when about two weeks old . She continues to care for them until they are fully fledged some six weeks l</t>
+          <t>Hanlon Expressway = The Hanlon Expressway or Hanlon Parkway is a high-capacity at-grade suburban limited-access road connecting Highway 401 with the city of Guelph in the Canadian province of Ontario . The 17 km ( 11 mi ) route travels in a generally north-south direction in the city 's west end . It is signed as Highway 6 for its entire length ; from Wellington Street to Woodlawn Road it is concurrent with Highway 7 . The speed limit alternates between 70 and 80 km / h ( 45 and 50 mph ) . Though the road was originally designed to be a freeway , budget limitations precluded the construction of overpasses ; apart from the interchanges with Highway 401 , Laird Road , and Wellington Street West ( Highway 7 and former Highway 24 ) , all junctions are at-grade intersections . There are also two railway crossings near the northern terminus , though both are for spur lines . The Hanlon is graded and landscaped similarly to a freeway , with broad flat shoulders and an open median . It was ini</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Black catbird = The black catbird ( Melanoptila glabrirostris ) is a songbird species in the monotypic genus Melanoptila , part of the family Mimidae . At 19 – 20.5 cm ( 7.5 – 8 in ) in length and 31.6 – 42 g ( 1.1 – 1.5 oz ) in mass , it is the smallest of the mimids . Sexes appear similar , with glossy black plumage , black legs and bill , and dark reddish eyes . The species is endemic to the Yucatán Peninsula , and is found as far south as Campeche , northern Guatemala and northern Belize . Although there are historical records from Honduras and the US state of Texas , the species is not now known to occur in either location . It is found at low elevations in semi-arid to humid habitats ranging from shrubland and abandoned farmland to woodland with thick understory , and is primarily sedentary . Although it is a mimid , the black catbird is not known to imitate any other species . Its song is a mix of harsh notes and clear flute-like whistles , with the phrases repeated . It builds </t>
+          <t>Johngarthia lagostoma = Johngarthia lagostoma is a species of terrestrial crab that lives on Ascension Island and three other islands in the South Atlantic . It grows to a carapace width of 110 mm ( 4.3 in ) on Ascension Island , where it is the largest native land animal . It exists in two distinct colour morphs , one yellow and one purple , with few intermediates . The yellow morph dominates on Ascension Island , while the purple morph is more frequent on Atol das Rocas . The species differs from other Johngarthia species by the form of the third maxilliped . Johngarthia lagostoma lives in burrows among vegetation , at altitudes of up to 400 m ( 1,300 ft ) , emerging at night to feed on plant matter and occasionally on animals . From January to March there is an annual migration to the sea to release the planktonic larvae . The species was first described ( as Gecarcinus lagostoma ) by Henri Milne-Edwards in 1837 from material sent to him by the naturalists Jean René Constant Quoy an</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lesser yellow-headed vulture = The lesser yellow-headed vulture ( Cathartes burrovianus ) also known as the savannah vulture , is a species of bird in the New World vulture family Cathartidae . It was considered to be the same species as the greater yellow-headed vulture until they were split in 1964 . It is found in Mexico , Central America , and South America in seasonally wet or flooded lowland grassland , swamps , and heavily degraded former forest . It is a large bird , with a wingspan of 150 – 165 centimetres ( 59 – 65 in ) . The body plumage is black , and the head and neck , which are featherless , are pale orange with red or blue areas . It lacks a syrinx , so therefore its vocalizations are limited to grunts or low hisses . The lesser yellow-headed vulture feeds on carrion and locates carcasses by sight and by smell , an ability which is rare in birds . It is dependent on larger vultures , such as the king vulture , to open the hides of larger animal carcasses as its bill is </t>
+          <t>Chroogomphus vinicolor = Chroogomphus vinicolor , commonly known as the wine-cap Chroogomphus or the pine spike , is a species of mushroom in the family Gomphidiaceae . Found in North America and the Dominican Republic , mushrooms grow on the ground under pine trees . Fruit bodies have reddish-brown , shiny caps up to 7.5 cm ( 3.0 in ) wide atop tapered stems up to 7.5 cm ( 3.0 in ) long . The gills are thick , initially pale orange before turning blackish , and extend a short way down the length of the stem . Although the mushroom is edible , and sold in local markets in Mexico , it is not highly rated . Distinguishing this species from some other similar Chroogomphus species is difficult , as their morphology is similar , and cap coloration is too variable to be a reliable characteristic . C. vinicolor is differentiated from the European C. rutilus and the North American C. ochraceus by the thickness of its cystidial walls . = = Taxonomy = = The species was first described as Gomphid</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t xml:space="preserve">St Margaret 's Church , Ifield = St Margaret 's Church is an Anglican church in the Ifield neighbourhood of Crawley , a town and borough in West Sussex , England . It is the ancient parish church of the village of Ifield ; the medieval settlement was expanded to form one of the New Town of Crawley 's 13 neighbourhoods , and the church 's modern parish now serves several other neighbourhoods as well . The present building incorporates the chancel from a 13th-century church which may have replaced a wooden building of two or three centuries earlier . Additions in the 14th century included stone effigies representing a knight and his wife , considered to be excellent examples of such sculptures . More structural changes took place at regular intervals , and a major Victorian restoration by architect Somers Clarke included an extension to the nave and a new tower . English Heritage has listed the church at Grade I because of its architectural and historical importance . The churchyard has </t>
+          <t xml:space="preserve">Shadows ( The X-Files ) = " Shadows " is the sixth episode of the first season of the American science fiction television series The X-Files . It premièred on the Fox network on October 22 , 1993 . It was written by Glen Morgan and James Wong , directed by Michael Lange , and featured guest appearances by Barry Primus and Lisa Waltz . The episode is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . " Shadows " earned a Nielsen household rating of 5.9 , being watched by 5.6 million households in its initial broadcast . The episode was not well received by the production staff , and received mixed reviews from critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . In this episode , Mulder and Scully investigate the death of two muggers and encounter an office worker who may be haunted by the spirit of her dead boss , who is using her to </t>
         </is>
       </c>
     </row>
@@ -1911,32 +1911,32 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ride train coaster roller riders station steel trains lift operate hour brake drop themed officially cars passengers roll opened passenger foot operated attraction chain oslo norwegian services hill guests locomotive owned market rides locomotives plans height build tall flags amusement nok railway platform shoulder manufactured longest operating adventure car supports park planning travel layout tallest tunnel experience pier coasters queue bought ticket cedar poll seating attractions capacity vertical operates stock delivered announcement platforms purchase acquired norway facilities railways brand approximately opening installation drops attendance loop purchased products restraints installed freight seats allow reopened manufacturer store banked stations venue express axle</t>
+          <t>['ride', 'train', 'coaster', 'roller', 'riders', 'station', 'steel', 'trains', 'lift', 'operate', 'hour', 'brake', 'drop', 'themed', 'officially']</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Delhi Metro = The Delhi Metro is a metro system serving Delhi and its satellite cities of Faridabad , Gurgaon , Noida and Ghaziabad in National Capital Region in India . Delhi Metro is the world 's 12th largest metro system in terms of both length and number of stations . , the network consists of five colour-coded regular lines and the faster Airport Express line , with a total length of 213 kilometres ( 132 mi ) serving 160 stations ( including 6 on Airport Express line ) . The system has a mix of underground , at-grade , and elevated stations using both broad-gauge and standard-gauge . The metro has an average daily ridership of 2.4 million passengers , and , as of August 2010 , had already carried over 1.25 billion passengers since its inception.DMRC named second best metro in world Delhi Metro Rail Corporation Limited ( DMRC ) , a state-owned company with equal equity participation from Government of India and Government of Delhi , built and operates the Delhi Metro . The Delhi Me</t>
+          <t xml:space="preserve">Hamilton Disston = Hamilton Disston ( August 23 , 1844 – April 30 , 1896 ) , was an industrialist and real-estate developer who purchased four million acres ( 16,000 km ² ) of Florida land in 1881 , an area larger than the state of Connecticut , and reportedly the most land ever purchased by a single person in world history . Disston was the son of Pennsylvania-based industrialist Henry Disston who formed Disston &amp; Sons Saw Works , which Hamilton later ran and which was one of the largest saw manufacturing companies in the world . Hamilton Disston 's investment in the infrastructure of Florida spurred growth throughout the state . His related efforts to drain the Everglades triggered the state 's first land boom with numerous towns and cities established through the area . Disston 's land purchase and investments were directly responsible for creating or fostering the towns of Kissimmee , St. Cloud , Gulfport , Tarpon Springs , and indirectly aided the rapid growth of St. Petersburg , </t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Zennor Head = Zennor Head / ˈzɛnʊər hɛd / is a 750-metre ( 2,460 ft ) long promontory on the Cornish coast of England , between Pendour Cove and Porthzennor Cove . Facing the Atlantic Ocean , it lies 1 kilometre north-west of the village of Zennor and 1.6 kilometres east of the next promontory , Gurnard 's Head . The granite ( Killas ) cliffs rise over 200 feet ( 60 m ) from the sea and the highest point of the headland is 314 feet ( 96 m ) above sea level , with an Ordnance Survey triangulation station . Zennor Head is on the South West Coast Path , which follows the cliff edge closely , skirting the entire perimeter of the headland . The promontory is part of the Penwith Heritage Coast , and is the largest coastal feature in the United Kingdom that begins with the letter " Z " . It gets its name from a local saint , Senara . Zennor Head was mined for copper and tin in the Victorian Era . There is no longer any residential or commercial occupancy on the headland , but it is occupied b</t>
+          <t>WhiteWater World = WhiteWater World is a water park situated in the suburb of Coomera on the Gold Coast , Australia . It is owned and operated by Ardent Leisure . After years of planning and a year of construction , WhiteWater World opened to the public on 8 December 2006 . The ten Australian beach culture themed attractions cost approximately A $ 56 million . These included The Green Room , Super Tubes Hydrocoaster , The Rip , The BRO , Temple of Huey , Cave of Waves , Wiggle Bay , and Pipeline Plunge . Since then , four additional water slides : two called Little Rippers , one called The Wedgie and one called the Triple Vortex , have been added . WhiteWater World was designed to be very efficient in its water use . Since opening , the quantity of visitors has consistently been above expectations . Ardent Leisure has submitted a development application for the expansion of the water park and plans to add five new attractions . = = History = = = = = Development = = = In 2004 , Macquari</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Saverne Tunnel = The Saverne Tunnel ( French : Tunnel de Saverne ) , also known as the Ernolsheim-lès-Saverne Tunnel ( French : Tunnel d 'Ernolsheim-lès-Saverne ) , is a twin-bore , high-speed rail tunnel in western Bas-Rhin , France . It carries the LGV Est line of France 's TGV high-speed rail network through the narrowest part of the Vosges mountain range , beneath Mont Saint-Michel and adjacent to the Saverne Pass . The tunnel consists of two bores , containing one railroad track each , that are connected by passageways every 500 metres ( 1,600 ft ) . The LGV Est crosses the 270 m ( 890 ft ) Haspelbaechel viaduct near the western end of the tunnel . The tunnel was excavated by a tunnel boring machine between November 2011 and February 2013 . Civil engineering work on the tunnel ended in April 2014 and it will open with the rest of the second phase of the LGV Est in July 2016 . The total cost of the tunnel was approximately € 200 million . = = Background = = The Saverne Tunnel was c</t>
+          <t xml:space="preserve">Oslo Metro rolling stock = The rolling stock of Oslo Metro , Norway has consisted of three classes : T1000 / T1300 , T2000 and MX3000 . The T1000 was built as 162 single cars from 1964 to 1978 . From 1979 to 1985 , 33 new T1300 trains were built , followed by the conversion of 16 T1000s . Six two-car T2000 units were delivered in 1994 . Since 2005 , the first 83 three-car MX3000 units have been replacing the older stock , and the last T1000 was retired in 2007 . From 2010 , only MX3000-trains are in use . The T1000 / T1300 and T2000 were built by Strømmens Værksted , with motors from Norsk Elektrisk &amp; Brown Boveri ( NEBB ) and AEG , respectively , and the MX3000 were built by Siemens . All trains receive 750 V DC from a third rail shoe , while the T1300 and T2000 also have pantographs . This allows the latter to also operate on the suburban lines of the Oslo Tramway , which the western part of the current metro was part of until 1995 . All trains feature automatic train protection and </t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Nest of Angels = " Nest of Angels " is the second episode of the second series of the British espionage television series Spooks , and the eighth episode overall . It was originally broadcast on BBC Three on 2 June 2003 , and repeated on frontline channel BBC One on 9 June . The episode was written by Howard Brenton , and directed by Bharat Nalluri . The episode centres on MI5 's actions in stopping Muhammed Rachid ( Qarie Marshall ) , a radicalised mullah in a mosque and community centre in Birmingham , who they believe is recruiting young suicide bombers . After their previous asset is discovered and brutally expelled , the team turn to Muhammed Ibhn Khaldun ( Alexander Siddig ) , an Algerian agent who left his country to work with the British . Brenton came up with the idea to show an episode dealing with a Muslim hero set out to stop a group of Islamic terrorists . Brenton and the producers researched elements of Islam in order to provide a balanced view towards the religion , as w</t>
+          <t>New Don Pedro Dam = New Don Pedro Dam , often known simply as Don Pedro Dam , is an earthen embankment dam across the Tuolumne River , about 2 miles ( 3.2 km ) northeast of La Grange , in Tuolumne County , California . The dam was completed in 1971 , after four years of construction , to replace the 1924 concrete-arch Don Pedro Dam . The dam serves mainly for irrigation water storage , flood control and hydroelectricity production , and impounds Don Pedro Reservoir in the foothills of the Sierra Nevada . The New Don Pedro Dam is owned and operated by the Modesto Irrigation District ( MID ) and Turlock Irrigation District ( TID ) . At 585 feet ( 178 m ) tall , the dam is the tenth highest in the U.S. and its reservoir is the sixth largest artificial lake in California . The original dam was named for the old mining town of Don Pedros Bar on the Tuolumne River , which in turn takes its name from prospector Pierre " Don Pedro " Sainsevain . = = Background = = Shortly after their formation</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>The Northern Celestial Masters = The Northern Celestial Masters type of the Way of the Celestial Master ( simplified Chinese : 天师道 ; traditional Chinese : 天師道 ; pinyin : Tiān Shī Dào ) Daoist movement existed in the north of China during the Southern and Northern Dynasties . The Northern Celestial Masters were a continuation of the Way of the Celestial Masters as it had been practiced in Sichuan province by Zhang Lu and his followers . After the community was forced to relocate in 215 CE , a group of Celestial Masters established themselves in Northern China . Kou Qianzhi , from a family who followed the Celestial Master , brought a new version of Celestial Master Daoism to the Northern Wei . The Northern Wei government embraced his form of Daoism and established it as the state religion , thereby creating a new Daoist theocracy that lasted until 450 CE . The arrival of Buddhism had great influence on the Northern Celestial Masters , bringing monasticism and influencing the diet of pra</t>
+          <t>2008 Georgia sugar refinery explosion = The 2008 Georgia sugar refinery explosion was an industrial disaster that occurred on February 7 , 2008 in Port Wentworth , Georgia , United States . 14 people were killed and 40 injured when a dust explosion occurred at a sugar refinery owned by Imperial Sugar . Dust explosions had been an issue of concern among United States authorities since three fatal accidents in 2003 , with efforts made to improve safety and reduce the risk of recurrence . The refinery was large and old , featuring outdated construction methods , and these factors are believed to have contributed to the fire 's severity . The origin of the explosion has been narrowed down to the center of the factory . It was believed to have occurred in a basement beneath storage silos . Investigations conducted by the Department of Justice ruled out deliberate criminal activity in 2013 . As a result of the disaster , new safety legislation was proposed . The local economy declined becaus</t>
         </is>
       </c>
     </row>
@@ -1946,32 +1946,32 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>building church stone wall built site listed roof windows century walls buildings tower 19th restoration corner chapel entrance interior structure memorial architect parish window constructed location house hall architecture floor grade temple decorated architectural nave designed surrounding monument chancel rebuilt remains exterior dedicated towers bell demolished sir room 16th brick 18th door castle arches erected masonry facing cathedral rooms carved stands style pier medieval date glass statue rector houses restored mosque surrounded oldest centuries originally cross foundation centre rectangular arch nearby metres square occupied dating block storey 17th stained topped marble altar structures housed architects porch installed slate font depicting</t>
+          <t>['building', 'church', 'stone', 'wall', 'built', 'site', 'listed', 'roof', 'windows', 'century', 'walls', 'buildings', 'tower', '19th', 'restoration']</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Oh Mother = " Oh Mother " is a song recorded by American singer Christina Aguilera for her fifth studio album , Back to Basics ( 2006 ) . The song was released on November 23 , 2007 by RCA Records as the fourth and final single from the album in European territories , while " Slow Down Baby " was serviced as the final single in Oceania . It was written by Aguilera , Derryck Thornton , Mark Rankin , Liz Thornton , Christophe Barratier , Bruno Coulais and Kara DioGuardi . Production was done by Big Tank and Q , with L Boggie credited as co-producer and Aguilera serviced as additional producer . " Oh Mother " is a downtempo piano ballad that talks about Aguilera 's abusive childhood . It incorporates various musical instruments , from strings to keyboards . It contains a sample from " Vois Sur Ton Chemin " , written by Bruno Coluais and Christopher Barratler . Upon its release , the song was met with mainly positive reviews from contemporary music critics . It also managed to enter charts</t>
+          <t>Jennifer Blow = Jennifer Blow ( born 10 January 1991 ) is an Australian goalball player and is classified as a B3 competitor . Having only started playing the sport in 2009 , she has several goalball scholarships . She plays for the New South Wales women 's goalball team in the Australian national championships , where she has won three silver medals . As a member of the national team , she has competed in the 2010 World Championships , 2011 IBSA Goalball World Cup and the 2011 African-Oceania regional Paralympic qualifying competition . She was selected to represent Australia at the 2012 Summer Paralympics in goalball . = = Personal life = = Nicknamed " Awesome " by her goalball teammates , Blow was born in Narraweena , New South Wales , on 10 January 1992 . She has the visual disability of oculocutaneous albinism , a congenital vision impairment , and is 165 centimetres ( 65 in ) . As of 2012 , Blow is attending the University of Sydney and double majoring in Arts and Education , whi</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Sky Scrapper = Sky Scrapper ( also known as Starry Sky Ripper ) is a flying roller coaster at World Joyland in Wujin , Changzhou , Jiangsu , China . Sky Scrapper was one of World Joyland 's opening day attractions , officially opening on April 30 , 2011 . The 2,805.1-foot-long ( 855.0 m ) ride stands 131.3 feet ( 40.0 m ) tall , and features a top speed of 54.7 mph ( 88.0 km / h ) . Designed by Swiss firm Bolliger &amp; Mabillard , Sky Scrapper restrains riders in the prone position and features five inversions . = = History = = World Joyland officially opened to the public on April 4 , 2011 . The park opened with the custom-designed Sky Scrapper , a Flying Coaster model from Bolliger &amp; Mabillard . The ride is located in the Universe of Starship area of the park . The park is derived from the World of Warcraft and Starcraft franchises . = = Characteristics = = The roller coaster 's steel track is approximately 2,805 feet ( 855 m ) in length and the height of the lift is 131.3 feet ( 40.0 m</t>
+          <t>Bristol Customshouse and Post Office = Bristol Customshouse and Post Office is a historic two-story rectangular Italian palazzo style brick building that was used as a post office and customshouse in Bristol , Rhode Island , United States . The land for the site was acquired for $ 4,400 . The building was designed by Ammi B. Young and completed in 1858 for a cost of $ 22,135.75 . The building roughly measures 46 feet ( 14 m ) by 32 feet ( 9.8 m ) and is constructed of deep red brick and has three arched openings on each of its sides and stories that are lined with sandstone moldings . The archways protrude from the side of the building and the center archway serves as the first floor with the adjacent archways housing large windows that are barred with iron . As it typical of the style , the second floor is more elaborate with a shallow balcony of iron supported by iron brackets and the paneling of the upper facade 's surmounting entablature is elaborately decorative . The sides and re</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Woodstock Mural = Woodstock Mural is a mural designed by artist Mike Lawrence , painted on the west side of the New Seasons Market store in the Woodstock neighborhood of Portland , Oregon , in the United States . The painting has three sections , each representing a theme : commerce , education , and the outdoors . It depicts figures adorned with symbolism related to characters in Greek mythology , including Hermes , Athena , and Demeter , along with local businesses and local landmarks such as the neighborhood farmers ' market , Grand Central Bakery , Portland Fish Market , Woodstock Park , and the Woodstock Library . The Woodstock Neighborhood Association ( WNA ) originally made plans for a mural on the exterior wall of Lutz Tavern . Following an outreach effort to identify an artist , Lawrence and WNA met for a brainstorming session , during which they agreed on theme 's for the proposed public artwork . Even after some funding was secured , efforts stalled . The association later p</t>
+          <t>Aboriginal Memorial = The Aboriginal Memorial is a work of contemporary Indigenous Australian art from the late 1980s , and comprises 200 decorated hollow log coffins . It was conceived by Djon ( John ) Mundine in 1987 – 88 and realised by 43 artists from Ramingining and neighbouring communities of Central Arnhem Land , in the Northern Territory . Artists who participated in its creation included David Malangi and George Milpurrurru . The work was created to coincide with the Australian Bicentenary and commemorates those Indigenous Australians who died as a result of European settlement . It was acquired by the National Gallery of Australia , where it is on permanent display . Its first exhibition was at the Sydney Biennale in 1988 , and it was the centrepiece of an exhibition of Indigenous art at Russia 's Hermitage Museum in 2000 . As of 2014 it stands at the entry to the National Gallery 's new wing that opened in September 2010 . = = Creation = = In 1988 , Australia marked 200 year</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Caught Up ( Usher song ) = " Caught Up " is a song by American R &amp; B singer Usher . It was written by Ryan Toby , Andre Harris , Vidal Davis and Jason Boyd , and produced by Dre &amp; Vidal for Usher 's 2004 album Confessions . The song was released as the fifth and final single from the album on November 30 , 2004 . The single peaked at number eight in the United States , the only single released from Confessions without topping the Billboard Hot 100 , and generally below top ten on most charts worldwide . It received positive reviews from contemporary critics . = = Background and release = = Although Usher " didn 't look too far " when starting working on his fourth studio album Confessions and decided to " continue building " with previous producers , he branched out with several musical collaborators . Usher enlisted Philadelphia producers Andre " Dre " Harris and Vidal Davis of Dre &amp; Vidal , along with other musical collaborators . During the sessions , Usher asked them to create a " </t>
+          <t>Saluki = The Saluki or Persian Greyhound is a dog breed originating in the Fertile Crescent and Persia . The Saluki is classed as a sighthound and is typically deep-chested and long-legged . Salukis tend to be independent animals requiring patient training and are gentle and affectionate with their owners . = = Name = = The two ancient Sumerian words " Salu-ki " translate into " plunge-earth . " However there is no evidence the breed was referred to by the Sumerians with this name nor what " plunge to earth " might have meant in reference to the Saluki . The name of the breed first appeared in writing in pre-Islamic Arabic poetry and may have derived from " Saluqiyyah , " the Arabic form of Seleucia . However , this is disputed . British diplomat Sir Terence Clark wrote that the Arabic word " Saluqi " describes a person or thing from a place named Saluq . Arab tradition states that Saluq was an ancient town in Yemen not far from modern Ta 'izz , and the Arabs associate this town with t</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>The Boat ( The Office ) = " The Boat " is the sixth episode of the ninth season of the American comedy television series The Office and the 182nd episode overall . The episode originally aired on NBC on November 8 , 2012 . It guest stars Josh Groban as Andy 's brother Walter . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In the episode , Andy Bernard ( Ed Helms ) must help his family when his dad loses all of their money , Dwight Schrute ( Rainn Wilson ) is pranked into thinking he is a guest on a radio show , and Kevin Malone ( Brian Baumgartner ) learns of Oscar Martinez 's ( Oscar Nunez ) affair with Angela Martin 's husband . " The Boat " received positive reviews from television critics . The episode was also viewed by 4.83 million viewers and received a 2.4 / 6 percent rating among adults between the ages of 18 and 49 , ranking third in its timeslot , making it the highest rated epi</t>
+          <t>George Rogers Clark National Historical Park = George Rogers Clark National Historical Park , located in Vincennes , Indiana , on the banks of the Wabash River at what is believed to be the site of Fort Sackville , is a United States National Historical Park . President Calvin Coolidge authorized a classical memorial and President Franklin D. Roosevelt dedicated the completed structure in 1936 . In a celebrated campaign , Lieutenant Colonel George Rogers Clark , older brother of William Clark , and his frontiersmen captured Fort Sackville and British Lt. Governor Henry Hamilton on February 25 , 1779 . The heroic march of Clark 's men from Kaskaskia on the Mississippi River in mid-winter and the subsequent victory over the British remains one of the great feats of the American Revolution . In 1966 , Indiana transferred the site to the National Park Service . Adjacent to the memorial is a visitor center which presents interpretive programs and displays . The center is located on South 2n</t>
         </is>
       </c>
     </row>
@@ -1981,32 +1981,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>battle men army troops french command general british sent attack soldiers forces wounded killed commanded camp siege retreat captured advance garrison arrived aftermath retreated supplies expedition ordered casualties force fire cavalry capture americans fort losses militia colonel news arrival fought flank fleet advanced wars armies surrender action marched infantry continental_army commander captain orders withdrew artillery occupied reinforcements suffered howe companies new_york enemy led guard battles defeat engagement crossed washington persian frigate revolutionary austrians left assault sailed surrendered regiments raid marching rhine learned defenders retreating allies fight column invasion musket engaged eventually hms quebec surprise loyalist attempt taken frigates decided landed</t>
+          <t>['battle', 'men', 'army', 'troops', 'french', 'command', 'general', 'british', 'sent', 'attack', 'soldiers', 'forces', 'wounded', 'killed', 'commanded']</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">German cruiser Admiral Scheer = Admiral Scheer was a Deutschland-class heavy cruiser ( often termed a pocket battleship ) which served with the Kriegsmarine of Nazi Germany during World War II . The vessel was named after Admiral Reinhard Scheer , German commander in the Battle of Jutland . She was laid down at the Reichsmarinewerft shipyard in Wilhelmshaven in June 1931 and completed by November 1934 . Originally classified as an armored ship ( Panzerschiff ) by the Reichsmarine , in February 1940 the Germans reclassified the remaining two ships of this class as heavy cruisers . The ship was nominally under the 10,000 long tons ( 10,000 t ) limitation on warship size imposed by the Treaty of Versailles , though with a full load displacement of 15,180 long tons ( 15,420 t ) , she significantly exceeded it . Armed with six 28 cm ( 11 in ) guns in two triple gun turrets , Admiral Scheer and her sisters were designed to outgun any cruiser fast enough to catch them . Their top speed of 28 </t>
+          <t>Tom Weisner = Tom Weisner ( born c . 1949 ) is an American politician . He is the mayor of Aurora , Illinois , which is the second largest municipality in the state . He won re-election on April 9 , 2013 . Prior to his election he worked for over eighteen years in high-ranking positions in the city of Aurora and for five years as a volunteer in the Peace Corps . He has been involved in several interstate new stories . In 2007 , he was embroiled in an interstate advertising controversy when the Governor of Kentucky used video footage of the local casino taken on a visit to Aurora for his re-election campaign , which included a platform against gambling . In 2008 , his city-wide wifi installation initiative was halted due to change in business strategy by the installing company . His decision-making skills again made headlines outside of Illinois when a Planned Parenthood clinic 's permits became an issue . = = Background = = Weisner is a native of Batavia , Illinois , but moved to Auror</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>HMS Tabard ( P342 ) = HMS Tabard was a British submarine of the third group of the T class . She was built by Scotts , Greenock , and launched on 21 November 1945 . So far she has been the only boat of the Royal Navy to bear the name Tabard , after the item of clothing . Having been launched after the war , she was selected , along with a number of boats of her class , to try out new streamlining techniques based on the German Type XXIII submarine . In May 1963 , she was involved in a collision with HMAS Queenborough , and on 10 February 1964 she underwent exercises with HMAS Melbourne and HMAS Voyager in the hours before their collision . When she returned to the UK , she became the static training submarine at the shore establishment HMS Dolphin , until 1974 when she was sold and broken up . = = Design and description = = Tabard had been originally ordered from Vickers Armstrong , Barrow , but the orders were switched to Scotts Shipbuilding and Engineering Company , Greenock . Ordere</t>
+          <t>Hurricane Maria ( 2011 ) = Hurricane Maria was a Category 1 hurricane that made landfall on the island of Newfoundland during September 2011 . Originating from a tropical wave over the central Atlantic on September 6 , Maria moved toward the west and slowly strengthened . While approaching the northern Leeward Islands , however , the system entered a region of higher vertical wind shear and cooler sea surface temperatures , causing it to degenerate into a low-pressure area . It slowly curved toward the north and northeast around the western periphery of the subtropical ridge , and regained tropical storm status on September 10 . Maria further strengthened to attain hurricane status while making its closest approach to Bermuda . The cyclone attained peak winds of 80 mph ( 130 km / h ) on September 16 , but weakened thereafter because of an increase in wind shear and cooler sea surface temperatures . Maria made landfall on the southeastern coast of Newfoundland during the afternoon hours</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Army of the Danube = The Army of the Danube ( French : Armée du Danube ) was a field army of the French Directory in the 1799 southwestern campaign in the Upper Danube valley . It was formed on 2 March 1799 by the simple expedient of renaming the Army of Observation , which had been observing Austrian movements on the border between French First Republic and the Holy Roman Empire . It was commanded by General Jean-Baptiste Jourdan , 1st Comte Jourdan ( 1762 – 1833 ) . The formation of the army was part of the French Directory 's long term strategy to undermine Habsburg influence in the Holy Roman Empire , and , conversely , to strengthen French hegemony in central Europe after the wars of the First Coalition and the Treaty of Campo Formio in 1797 . Despite the Treaty , Austria and France remained suspicious of each other 's motives , and the purpose of the Army of the Observation was to watch for Austrian border transgressions . Understanding that the negotiations at the Congress of Ra</t>
+          <t>German Type IXA submarine = The German Type IXA submarine was a sub-class of the German Type IX submarine built for Nazi Germany 's Kriegsmarine between 1937 and 1938 . These U-boats were designed between 1935 and 1936 and were intended to be fairly large ocean-going submarines . The inspiration for the Type IXA submarine came from the German Type IA submarine , which had a similar diving depth and identical submerged horsepower . Two of the eight Type IXA submarines ( U-37 and U-38 ) would become the 6th and 10th most successful U-boats that saw service in World War II , sinking 53 and 35 ships respectively . All of the Type IXA submarines were sunk fairly early in the war except for U-37 and U-38 , which were scuttled in May 1945 to prevent them from falling into the hands of the Allies . = = Construction = = All Type IXA submarines were ordered by the Kriegsmarine between 29 July 1936 and 21 November 1936 as part of Plan Z and the overall German plan of re-armament in violation of t</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Battle of Long Island = The Battle of Long Island , also known as the Battle of Brooklyn and the Battle of Brooklyn Heights , fought on August 27 , 1776 , was the first major battle of the American Revolutionary War to take place after the United States declared its independence on July 4 , 1776 . It was a victory for the British Army and the beginning of a successful campaign that gave them control of the strategically important city of New York . In terms of troop deployment and fighting , it was the largest battle of the entire war . After defeating the British in the Siege of Boston on March 17 , 1776 , General George Washington , commander-in-chief , brought the Continental Army to defend the port city of New York , then limited to the southern end of Manhattan Island . Washington understood that the city 's harbor would provide an excellent base for the British Navy during the campaign . There he established defenses and waited for the British to attack . In July , the British , </t>
+          <t>Vojislav Lukačević = Vojislav Lukačević ( Serbian Cyrillic : Војислав Лукачевић ; 1908 – 14 August 1945 ) was a Serbian Chetnik commander in the Kingdom of Yugoslavia during World War II . At the outbreak of war , he held the rank of captain of the reserves in the Royal Yugoslav Army . When the Axis powers invaded Yugoslavia in April 1941 , Lukačević became a leader of Chetniks in the Sandžak region and joined the movement of Draža Mihailović . While the Chetniks were an anti-Axis movement in their long-range goals and did engage in marginal resistance activities for limited periods , they also pursued almost throughout the war a tactical or selective collaboration with the occupation authorities against the Yugoslav Partisans . They engaged in cooperation with the Axis powers to one degree or another by establishing modi vivendi or operating as auxiliary forces under Axis control . Lukačević himself collaborated extensively with the Italians and the Germans in actions against the Yugo</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Liudhard medalet = The Liudhard medalet is a gold Anglo-Saxon coin or small medal found some time before 1844 near St Martin 's Church in Canterbury , England . It was part of the Canterbury-St Martin 's hoard of six items . The coin , along with other items found with it , now resides in the World Museum Liverpool . Although some scholarly debate exists on whether or not all the items in the hoard were from the same grave , most historians who have studied the object conclude that they were buried together as a necklace in a 6th-century woman 's grave . The coin is set in a mount so that it could be worn as jewellery , and has an inscription on the obverse or front surrounding a robed figure . The inscription refers to Liudhard , a bishop who accompanied Bertha to England when she married Æthelberht the king of Kent . The reverse side of the coin has a double-barred cross , or patriarchal cross , with more lettering . The coin was probably struck at Canterbury in the late 6th century </t>
+          <t>Moses Hazen = Moses Hazen ( June 1 , 1733 – February 5 , 1803 ) was a Brigadier General in the Continental Army during the American Revolutionary War . Born in the Province of Massachusetts Bay , he saw action in the French and Indian War with Rogers ' Rangers . His service included particularly brutal raids during the Expulsion of the Acadians and the 1759 Siege of Quebec . He was formally commissioned into the British Army shortly before the war ended , and retired on half-pay outside Montreal , Canada , where he and Gabriel Christie , another British officer , made extensive land purchases in partnership . During his lifetime he acquired land in Quebec , New Hampshire , Vermont , and New York , but lost most of his Quebec land due to litigation with Christie and the effects of the revolution . In 1775 he became involved in the American invasion of Quebec early in the American Revolutionary War , and served with the Continental Army in the 1775 Battle of Quebec . He went on to lead h</t>
         </is>
       </c>
     </row>
@@ -2016,32 +2016,32 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>championship match title defeated event team face won night following kane attacked main wrestler win referee rope professional view pay heavyweight wrestlers champion survivor announced pinfall pin contest michaels interfered rematch cage ring retain pinned undertaker pinning wrestlemania shawn_michaels smackdown john_cena wrestled wrestling featured backstage wwf ecw randy_orton feud contender bout storyline summerslam teamed ringside elimination eliminated superstars faced fight heel began submission world_wrestling_entertainment involved ladder joe wwe disqualification stipulation nwa mat rumble signature retained feuds challenged versus defended lost intercontinental raw divas maneuver fan feuded hart promotion flair scripted royal_rumble world teaming attacking hold edge triple tag wrestle impact</t>
+          <t>['championship', 'match', 'title', 'defeated', 'event', 'team', 'face', 'won', 'night', 'following', 'kane', 'attacked', 'main', 'wrestler', 'win']</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">TouchWave = TouchWave , Inc . ( now WebCom ) , was a privately held Palo Alto , California IP-telephony network switch provider founded in 1997 . TouchWave developed a product line called WebSwitch that was designed to replace traditional private telephone exchange systems in small-to-medium-sized companies . WebSwitch was part of a phone system that incorporates communication features provided by the Internet . The rapid success of TouchWave was memorialized with awards and an acquisition by Ericsson Communications for $ 46M two years after TouchWave was founded . Ericsson continued the TouchWave product line under the name WebCom , but its efforts have been viewed as less than successful . = = History = = In 1997 , TouchWave was a privately held , venture-backed startup company in Palo Alto , California , with future entrepreneur Oliver Muoto as its marketing director . Co-founded by CEO Bo Larsson , Jeff Snider , David F. Wittenkamp , and Jesper Stroe , TouchWave released its first </t>
+          <t xml:space="preserve">Tom Johnson ( bareknuckle boxer ) = Tom Johnson ( born Tom Jackling ; c . 1750 – 21 January 1797 ) was a bare-knuckle fighter who was referred to as the Champion of England between 1784 and 1791 . His involvement in pugilistic prizefighting is generally seen to have coincided with a renewed interest in the sport . Although a strong man , his success was largely attributed to his technical abilities and his calm , analytical approach to despatching his opponents . But Johnson was less prudent outside the ring ; he was a gambler and considered by many of his acquaintances to be an easy mark . He is thought to have earned more money from the sport than any other fighter until nearly a century later , but much of it was squandered . Johnson 's first fight probably took place in June 1783 against Jack Jarvis , after he had unintentionally slighted the wagon driver and professional fighter . Jarvis challenged Johnson to fight him as a matter of honour , and was comprehensively beaten in the </t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Du Friedefürst , Herr Jesu Christ , BWV 116 = Du Friedefürst , Herr Jesu Christ ( You Prince of Peace , Lord Jesus Christ ) , BWV 116 , is a church cantata written by Johann Sebastian Bach in 1724 in Leipzig for the 25th Sunday after Trinity . He led the first performance it on 26 November 1724 , concluding the liturgical year of 1724 . The cantata is based upon Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " . It matches the Sunday 's prescribed gospel reading , the Tribulation from the Gospel of Matthew , in a general way . The hymn 's first and last stanza are used unchanged in both text and tune : the former is set as a chorale fantasia , the latter as a four-part closing chorale . An unknown librettist paraphrased the inner stanzas as alternating arias and recitatives . Bach scored the cantata for four vocal soloists ( soprano , alto , tenor , bass ) , a four-part choir and a Baroque instrumental ensemble of natural horn , enforcing the soprano in the hymn tune , two obo</t>
+          <t>Slammiversary ( 2005 ) = Slammiversary ( 2005 ) was a professional wrestling pay-per-view ( PPV ) event produced by the Total Nonstop Action Wrestling ( TNA ) promotion , which took place on June 19 , 2005 at the TNA Impact ! Zone in Orlando , Florida . It was the first event under the Slammiversary chronology and the sixth event in the 2005 TNA PPV schedule . Nine professional wrestling matches , three of which featured championships , and one pre-show match were featured on the event 's card . The event commemorated TNA 's third-year anniversary , after forming on June 19 , 2002 . The main event was the 2005 King of the Mountain match for the NWA World Heavyweight Championship , in which then-champion A.J. Styles defended the title against Abyss , Monty Brown , Sean Waltman , and Raven . Raven won the match and the NWA World Heavyweight Championship . The TNA X Division Championship was defended in a Three Way Elimination match by Christopher Daniels against Chris Sabin and Michael S</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Jermain Taylor = Jermain Taylor ( born August 11 , 1978 ) is an American former professional boxer . He remains the last undisputed middleweight champion , having unified the WBA , WBC , IBF , WBO , The Ring magazine and lineal titles in 2005 by beating Bernard Hopkins . This made Taylor the first boxer to ever claim each title from all four major boxing sanctioning organizations . He is also a two-time former IBF middleweight champion , having won the title for a second time in 2014 . Taylor made his professional debut in 2001 and won his first 25 bouts , which included victories over former champions Raúl Márquez and William Joppy . Taylor , who began boxing officially at age 13 , earned numerous accolades throughout his amateur career , starting with his achievement of the 1996 Under-19 Championship . He went on to win a pair of Police Athletic League ( PAL ) Championships and National Golden Gloves titles and he finished second and third at the 1997 and 1998 United States Champions</t>
+          <t>Don 't Judge Me = " Don 't Judge Me " is a song by American recording artist Chris Brown on his fifth studio album , Fortune ( 2012 ) . It was written by Brown , Adam Messinger , Nasri Atweh and Mark Pellizzer , and produced by The Messengers . The song was sent to urban contemporary radio stations in the United States on August 14 , 2012 as the fifth and final single from the album . " Don 't Judge Me " is a midtempo ballad , with lyrics in which Brown asks his lover to forgive him " for his past indiscretions " and " move on with the future . " The lyrics reportedly referred to Brown 's former relationships with aspiring American model and fashion designer Karrueche Tran and Barbadian recording artist Rihanna . " Don 't Judge Me " received positive reviews from music critics ; some complimented the song and considered it a highlight on Fortune , while others criticized its production . In the United States , " Don 't Judge Me " reached number 10 on the R &amp; B Songs chart , number 18 o</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Maria Kanellis = Maria Louise Kanellis-Bennett ( born February 25 , 1982 ) is an American professional wrestler , valet , actress and singer currently signed to Total Nonstop Action Wrestling ( TNA ) under the ring name Maria ( Kanellis-Bennett ) . She is best known for her time with World Wrestling Entertainment ( WWE ) , and Ring of Honor ( ROH ) as the valet of her real-life husband Michael Bennett . Kanellis 's career began as a contestant on the reality show Outback Jack in 2004 . In the same year , she placed fifth in the Raw Diva Search , but was later hired by WWE as a backstage interviewer . Kanellis began competing in the ring as a wrestler in 2005 . She also posed for the April 2008 cover of Playboy magazine , which was incorporated into a storyline on Raw . She released her debut album Sevin Sins on April 13 , 2010 on iTunes . = = Early life = = Kanellis was born in Ottawa , Illinois . She has two younger siblings ; a brother and sister named Bill and Janny , respectively .</t>
+          <t>Suillus collinitus = Suillus collinitus is a pored mushroom of the genus Suillus in the family Suillaceae . It is an edible mushroom found in European pine forests . The mushroom has a reddish to chestnut-brown cap that reaches up to 11 cm ( 4.3 in ) in diameter , and a yellow stem measuring up to 7 cm ( 2.8 in ) tall by 1 to 2 cm ( 0.4 to 0.8 in ) thick . On the underside of the cap are small angular pores , initially bright yellow before turning greenish-brown with age . A characteristic feature that helps to distinguish it from similar Suillus species , such as S. granulatus , is the pinkish mycelia at the base of the stem . Molecular analysis has shown the species to be related to other typical Mediterranean Suillus species such as S. bellinii , S. luteus , and S. mediterraneensis . S. collinitus is a mycorrhizal species , and forms associations with several species of pine , most notably the Aleppo pine . This tree species is commonly used in reforestation schemes and soil conserv</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Augustus E. Willson = Augustus Everett Willson ( October 13 , 1846 – August 24 , 1931 ) was the 36th Governor of Kentucky . Orphaned at the age of twelve , Willson went to live with relatives in New England . This move exposed him to such literary masters as Ralph Waldo Emerson , Henry Wadsworth Longfellow , Oliver Wendell Holmes , and James Russell Lowell , who were associates of his older brother , poet Forceythe Willson . He was also afforded the opportunity to attend Harvard University , where he earned an A.B. in 1869 and an A.M. in 1872 . After graduation , he secured a position at the law firm of future Supreme Court justice John Marshall Harlan . Willson and Harlan became lifelong friends , and Willson 's association with Harlan deepened his support of the Republican Party . A Republican in a primarily Democratic state , Willson suffered several defeats for public office , but was elected governor of Kentucky on his second attempt . Due to his handling of the Black Patch Tobacc</t>
+          <t>Jillian Hall = Jillian Faye Hall ( née Fletcher ; September 6 , 1980 ) is an American retired professional wrestler and singer best known for her time in World Wrestling Entertainment ( WWE ) as a WWE Diva under the ring name Jillian ( Hall ) . She also worked as a trainer in WWE 's developmental territory Florida Championship Wrestling . After debuting in 1998 , Hall worked on the independent circuit under the name Macaela Mercedes . She won numerous championships , before beginning to work for Ohio Valley Wrestling in 2003 under her real name . She debuted on WWE 's SmackDown brand as the " fixer " for the MNM faction . After leaving MNM , she became John " Bradshaw " Layfield 's " image consultant " , and managed him to the WWE United States Championship at WrestleMania 22 . In February 2007 , Hall developed an in-ring persona as a tone-deaf singer . In June 2007 , she was drafted to Raw , where she participated in numerous tag team matches after allying with Melina . In October 200</t>
         </is>
       </c>
     </row>
@@ -2051,32 +2051,32 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>entertain entertained buddy profanity flamboyant racially courted rampant subtitles bishop psychologically app oppressed horrific bother sacrificing unconventional bitterness pencil backgrounds academically format infamous predecessor dos manipulate ethnicity preparation longstanding oppressive physique fortunes balloons defied revamped denominations passport onscreen monstrous odyssey proficient apocalyptic dump laborers surpass misunderstood masks frantic promoting reliant headline economies packages dictated virtually slump professed massively dialog exchanges fascinated revolutions adapting variations solidified awakened prepared challenging stirred injustice healed opt verbally reconsider apologized dealt irresponsible replicated exams endorsing despised portrayals manage promoter hugely multinational repercussions reviewed eyewitness lifestyles inherently adversary famously certificates irregularities hoc frequented improves instalment resorted</t>
+          <t>['entertain', 'entertained', 'buddy', 'profanity', 'flamboyant', 'racially', 'courted', 'rampant', 'subtitles', 'bishop', 'psychologically', 'app', 'oppressed', 'horrific', 'bother']</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Oregon ( Awake ) = " Oregon " is the fifth episode of the American police procedural drama television series Awake . The episode first premiered on March 29 , 2012 in the United States on NBC , was simultaneously broadcast on Global in Canada , and was subsequently aired on Sky Atlantic in the United Kingdom on June 1 , 2012 . It was written by consulting producer Lisa Zwerling , and directed by Aaron Lipstadt . " Oregon " was well received by television critics , who praised its storylines . Commentators noted that the script was well-written and that the episode was the " strongest outing " since " Pilot " broadcast on March 1 , 2012 . Upon airing , the episode garnered 3.18 million viewers in the United States and a 1.0 / 3 rating-share in the 18 – 49 demographic , according to Nielsen ratings . It ranked second in its timeslot , behind The Mentalist on CBS . The show centers on Michael Britten ( Jason Isaacs ) , a police detective living in two separate realities after a car accide</t>
+          <t>Luke Cain = Luke Cain ( born 3 February 1980 ) is an SH2-classified Australian shooter who became a paraplegic after an accident while playing Australian rules football . He started competing in 2007 , as the sport suited his disability , and has been a Victorian Institute of Sport scholarship holder since 2008 . He first represented Australia internationally in 2009 at a World Cup event in South Korea.He has been selected to represent Australia at the 2016 Rio Paralympics . These will be his second Games . = = Personal = = Cain was born on 3 February 1980 in Rosebud , Victoria . He started playing Australian rules football when he was seven years old for the Rye Football Club . He played senior football for Rosebud Football Club as a full-forward . In August 1999 , at the age of nineteen , he was playing for Rosebud in a game against Hastings Football Club when he broke his neck after being sandwiched between a teammate and an opposing player . He is a paraplegic , and requires use of</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Percy Cherry = Percy Herbert Cherry , VC , MC ( 4 June 1895 – 27 March 1917 ) was an Australian recipient of the Victoria Cross , the highest decoration for gallantry " in the face of the enemy " that can be awarded to members of the British and Commonwealth armed forces . The award was granted posthumously for Cherry 's actions during an attack on the French village of Lagnicourt which was strongly defended by German forces . Born in the Australian state of Victoria , Cherry moved to Tasmania at the age of seven when his family took up an apple orchard . Becoming an expert apple packer , he was also a skilled rifle shot and member of the Franklin rowing club . In 1913 , he was commissioned as a second lieutenant in the 93rd Infantry Regiment , Citizens Military Force , and served as a drill instructor at the outbreak of war . Enlisting in the Australian Imperial Force in March 1915 , he served at Gallipoli before transferring to the Western Front . In early March 1917 , Cherry was dec</t>
+          <t>William de Blois ( bishop of Lincoln ) = William de Blois ( or William of Blois ; died 1206 ) was a medieval Bishop of Lincoln . He first served in the household of Hugh du Puiset , the Bishop of Durham , then later served the household of Hugh of Avalon , Bishop of Lincoln . After Hugh 's death and a two-year vacancy in the see , or bishopric , Blois was elected to succeed Hugh in 1203 . Little is known about his episcopate , although 86 of his documents survive from that time period . He died in 1206 and was buried in his cathedral . = = Early life = = Possibly related to Hugh de Puiset the bishop of Durham , who he went on to serve later in life , Blois probably came from Blois in France . His relationship with Puiset reinforces the likelihood of his origins being in Blois , as Puiset was a nephew of King Stephen of England and Stephen 's brother Henry of Blois , the Bishop of Winchester , both of whom came from Blois . Nothing else is known of Blois ' origins . He was titled magist</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Andrew Fisher = Andrew Fisher ( 29 August 1862 – 22 October 1928 ) was an Australian politician who served as Prime Minister of Australia on three separate occasions between 1908 and 1915 . Fisher 's second government between 1910 and 1913 completed a vast legislative programme which made him , along with Protectionist Alfred Deakin , the founder of the statutory structure of the new nation . The Fisher government legacy of reforms and national development lasted beyond the divisions that would later occur with World War I and Billy Hughes ' conscription push . Fisher 's second Prime Ministership resulting from the 1910 federal election represented a number of firsts : it was Australia 's first elected federal majority government , Australia 's first elected Senate majority and the world 's first Labour Party majority government at a national level . After the minority governments of 1904 Chris Watson and his own in 1908-1909 it was the world 's third Labour Party government at a natio</t>
+          <t>Applesauce cake = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as primary ingredients . Various spices are typically used , and it tends to be a moist cake . Applesauce cake prepared with chunky-style apple sauce may be less moist . Several additional ingredients may also be used in its preparation , and it is sometimes prepared and served as a coffee cake . The cake dates back to early colonial times in the United States . National Applesauce Cake Day occurs annually on June 6 in the U.S. = = History = = The preparation of applesauce cake dates back to early colonial times in the New England Colonies of the northeastern United States . From 1900 to the 1950s , recipes for applesauce cake frequently appeared in American cookbooks . In the United States , National Applesauce Cake Day occurs annually on June 6 . = = Ingredients and preparation = = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as main ingredients . Store-b</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Richard Minifie = Richard Pearman Minifie , DSC &amp; Two Bars ( 2 February 1898 – 31 March 1969 ) was an Australian fighter pilot and flying ace of the First World War . Born in Victoria , he attended Melbourne Church of England Grammar School . Travelling to the United Kingdom , he enlisted in the Royal Naval Air Service in June 1916 . Accepted for flight training , he completed his instruction in December and joined No. 1 ( Naval ) Squadron RNAS on the Western Front in January 1917 , flying Sopwith Triplanes . He went on to score seventeen aerial victories on this type of machine throughout the year , becoming both the youngest Australian flying ace of the First World War and No. 1 ( Naval ) Squadron 's highest-scoring ace on the Triplane . The unit re-equipped with the Sopwith Camel late in 1917 , with Minifie going on to achieve a further four victories on the aircraft , raising his final tally to a score of twenty-one aircraft shot down . Minifie crash landed in German-held territory</t>
+          <t>Footprints in the Sand ( Leona Lewis song ) = " Footprints in the Sand " is a song recorded by British singer Leona Lewis for her debut studio album Spirit ( 2007 ) . It was written by Simon Cowell , David Kreuger , Per Magnusson , Richard Page , and produced by Steve Mac . The song was digitally released as Lewis 's third single on 9 March 2008 in the United Kingdom . Sony BMG and Syco Music launched it as a double A-side with " Better in Time " , and " You Bring Me Down " as the B-side . It is a R &amp; B and pop song composed with a tempo of sixty beats per minute . It was written in a period of one day at Page 's home in Malibu , California , with Cowell giving the idea to base it on the Christian poem " Footprints " . The single 's music video was filmed by British director Sophie Muller in Johannesburg , South Africa . The video describes social problems within the city , but ends with a message of hope . " Footprints in the Sand " became the official theme of the 2008 version of bie</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Final Fantasy Fables : Chocobo Tales = Final Fantasy Fables : Chocobo Tales , released in Japan as Chocobo to Mahō no Ehon ( チョコボと魔法の絵本 , lit . " Chocobo and the Magic Picture Book " ) is a Nintendo DS adventure game developed by h.a.n.d. and published by Square Enix . It was released in Japan on December 14 , 2006 , in North America on April 3 , 2007 , and in the PAL region in May 2007 . Final Fantasy Fables is a Final Fantasy spinoff starring a Chocobo in a setting which features common elements and creatures of the series . Music from the rest of the series is also reused . The game is composed of a number of minigames woven into a main adventure . The game was received positively by critics , who appreciated the originality and light-hearted nature of the title . A sequel , Chocobo to Mahō no Ehon : Majō to Shōjo to Gonin no Yūsha ( チョコボと魔法の絵本 魔女と少女と5人の勇者 , lit . " Chocobo and the Magic Picture Book : The Witch , the Girl , and the Five Heroes " ) was released in Japan on December </t>
+          <t xml:space="preserve">Washington State Route 117 = State Route 117 ( SR 117 ) is a short , 1.40-mile ( 2.25 km ) long state highway located entirely within Port Angeles , the county seat of Clallam County , in the U.S. state of Washington . The short roadway , named the Tumwater Truck Route , serves the waterfront of Port Angeles and intersects two streets and crosses under another street on a short bridge . Beginning at an interchange with U.S. Route 101 ( US 101 ) , the highway travels northeast to terminate at Marine Drive . SR 117 was first established in 1991 , but a road parallel to the current roadway had existed since 1966 . = = Route description = = SR 117 begins as the Tumwater Truck Road at an interchange with U.S. Route 101 ( US 101 ) in southwest Port Angeles . The interchange only serves traffic from US 101 eastbound driving onto SR 117 northbound and motorists driving from the route southbound onto US 101 westbound , however , left turns are allowed to serve the missing movements . Traveling </t>
         </is>
       </c>
     </row>
@@ -2086,32 +2086,32 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>production system crew mission use development based high million aircraft engine control announced new flight launch including spacecraft range program speed time nasa vehicle apollo missions sales fuel ground air lunar market low project moon performance twitter launched landing pilot developed car flights engines cost version available models orbit designed weapons level hours saturn technology vehicles toyota began capability june manned march service testing missile altitude module radar total united_states combat tested december earth produced capabilities company stage model thrust billion rocket systems cabin january missiles planned oxygen price equipment flew nuclear industry april stated design reported increased year software</t>
+          <t>['production', 'system', 'crew', 'mission', 'use', 'development', 'based', 'high', 'million', 'aircraft', 'engine', 'control', 'announced', 'new', 'flight']</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Afterburn ( roller coaster ) = Afterburn is a steel inverted roller coaster located at Carowinds amusement park . After more than two years of planning and construction , the roller coaster opened on March 20 , 1999 . The ride previously operated as Top Gun : The Jet Coaster , before it was renamed Afterburn following Cedar Fair 's purchase of the park in 2006 . Designed by Bolliger &amp; Mabillard , Afterburn stands 113 feet ( 34 m ) tall and reaches speeds of 62 miles per hour ( 100 km / h ) . It features a 2,956-foot-long ( 901 m ) track and a nearly three-minute-long ride time . Afterburn has generally been well received , having been featured several times as a top 50 roller coaster in Amusement Today 's Golden Ticket Awards . = = History = = In early 1997 , Paramount 's Carowinds began consultations with roller coaster manufacturer Bolliger &amp; Mabillard about adding a new ride to their park . During 18 months of discussions , several designs and themes for the ride were developed , in</t>
+          <t>Raëlism = Raëlism ( also known as Raëlianism or the Raëlian movement ) is a UFO religion that was founded in 1974 by Claude Vorilhon ( b . 1946 ) , now known as Raël . The Raëlian Movement teaches that life on Earth was scientifically created by a species of extraterrestrials , which they call the Elohim . Members of this species appeared human when having personal contacts with the descendants of the humans that they made . They purposefully misinformed early humanity that they were angels , cherubim , or gods . Raëlians believe that messengers , or prophets , of the Elohim include Buddha , Jesus , and others who informed humans of each era . The founder of Raëlism , members claim , received the final message of the Elohim and that its purpose is to inform the world about Elohim and that if humans become aware and peaceful enough , they wish to be welcomed by them . The Raëlian Church has a quasi-clerical structure of seven levels . Joining the movement requires an official apostasy f</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>No. 81 Wing RAAF = No. 81 Wing is the wing responsible for operating the McDonnell Douglas F / A-18 Hornet multi-role fighters of the Royal Australian Air Force ( RAAF ) . Headquartered at RAAF Base Williamtown , New South Wales , the wing comprises three combat units , Nos. 3 and 77 Squadrons based at Williamtown and No. 75 Squadron based at RAAF Base Tindal , Northern Territory , as well as an operational conversion unit at Williamtown . No. 81 Wing headquarters oversees squadron training in air-to-air combat , air-to-ground tactics , and support for the Australian Army and Royal Australian Navy . Tasked with offensive and defensive counter-air operations , the Hornets have been deployed to Diego Garcia in 2001 – 02 , when they provided local air defence , and to Iraq in 2003 , when they saw action flying fighter escort and close air support missions in concert with Coalition forces . They have also been employed to patrol high-profile events in Australia , including the Commonwealth</t>
+          <t>Oregon Theatre = The Oregon Theatre , or Oregon Theater , is an adult movie theater in the Richmond neighborhood of southeast Portland , Oregon . The theater was completed in 1925 and originally housed a Wurlitzer pipe organ and vaudeville stage . It would later screen Hollywood , art-house , and Spanish-language films . The building was acquired by the Maizels family in 1967 and became an adult cinema in the 1970s . It continues to operate as the city 's longest running pornographic cinema and remains owned by a member of the Maizels family . The cinema has been described as " less creepy than most of its kind " and " out of place " along the newly developed Southeast Division Street . It has also been called " the last holdout of an era " , referring to both the prominence of adult film screenings in the city during the 1970s and its status as the last property owned by the Maizels family . In 2004 , the building was identified as an " Investment and Identity Site " and commended for</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Number 1 to Infinity = # 1 to Infinity is the sixth compilation album by American singer and songwriter Mariah Carey . It was released by Sony Music Entertainment on May 15 , 2015 . It features Carey 's eighteen U.S. number-one singles on the Billboard Hot 100 . A new recording called " Infinity " was released as the only single on April 27 , 2015 . In January 2015 , the singer announced that she had signed a residency deal to perform at The Colosseum at the Caesars Palace hotel in Las Vegas in May and July 2015 , and would perform all of her number-ones . As a result , she decided to re-release her first compilation , # 1 's , from 1998 with an updated list of subsequent chart toppers . Carey promoted the album with her Mariah Carey # 1 's residency and with live performances at the Billboard Music Awards , Jimmy Kimmel Live ! and Live ! with Kelly and Michael . = = Background = = Following the release of Mariah Carey 's fourteenth studio album , Me . I Am Mariah … The Elusive Chanteu</t>
+          <t>Woodhull Sexual Freedom Alliance = The Woodhull Sexual Freedom Alliance ( WSFA ) , previously known as the Woodhull Freedom Foundation , is an American non-profit organization founded in 2003 that advocates for sexual freedom as a fundamental human right . The organization is based in Washington , D.C. , United States . Named after an influential member of the American woman 's suffrage movement , Victoria Woodhull , its focus includes analyzing groups and individuals that seek to perpetuate a culture of sexual repression . Sexual Freedom Day , officially recognized in 2011 in Washington , DC , celebrates the birthday of Victoria Woodhull . The WSFA has held the Sexual Freedom Summit annually since 2010 . Organization members have included LGBT activist Jeffrey Montgomery , former chairwoman of the United States Commission on Civil Rights Mary Frances Berry , writer Eric Rofes , lawyer Lawrence G. Walters , and activist Dan Massey . In the furtherance of activities relating to its goal</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Philadelphia transit strike of 1944 = The Philadelphia transit strike of 1944 was a sickout strike by white transit workers in Philadelphia that lasted from August 1 to August 6 , 1944 . The strike was triggered by the decision of the Philadelphia Transportation Company ( PTC ) , made under prolonged pressure from the federal government in view of significant labor shortages , to allow black employees of the PTC to hold non-menial jobs , such as motormen and conductors , that were previously reserved for white workers only . On August 1 , 1944 the eight black employees being trained as streetcar motormen were to make their first trial run ; that fact was used by the white PTC workers to start a massive sickout strike . The strike paralyzed the public transport system in Philadelphia for several days , bringing the city to a standstill and crippling its war production . Although the Transport Workers Union ( TWU ) was in favor of allowing promotions of black workers to any positions the</t>
+          <t>Roguelike = Roguelike is a subgenre of role-playing video games characterized by a dungeon crawl through procedurally generated game levels , turn-based gameplay , tile-based graphics , and permanent death of the player-character . Most roguelikes are based on a high fantasy narrative , reflecting their influence from tabletop role playing games such as Dungeons &amp; Dragons . Though the roguelikes Beneath Apple Manor and Sword of Fargoal predate it , the 1980 game Rogue is considered the forerunner and the namesake of the genre , with derivative games mirroring Rogue 's character- or sprite-based graphics . These games were popularized among college students and computer programmers of the 1980s and 1990s , leading to a large number of variants but adhering to these common gameplay elements , often titled the " Berlin Interpretation " . Some of the better-known variants include Hack , NetHack , Ancient Domains of Mystery , Moria , Angband , and Tales of Maj 'Eyal . The Japanese series of</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Maple Leaf Sports &amp; Entertainment = Maple Leaf Sports &amp; Entertainment Ltd . ( MLSE ) is a professional sports and commercial real estate company based in Toronto , Ontario , Canada . With assets that include franchises in three of the six major professional sports leagues in the United States and Canada , it is the largest sports and entertainment company in Canada , and one of the largest in North America . The primary holdings of the company are its major sports franchises , the Toronto Maple Leafs of the National Hockey League , Toronto Raptors of the National Basketball Association and Toronto FC of Major League Soccer , as well as their minor league farm teams , the Toronto Marlies of the American Hockey League ( AHL ) , Raptors 905 of the NBA D-League and Toronto FC II of the United Soccer League , respectively . In addition , it owns the Air Canada Centre , the home arena of the Maple Leafs and Raptors . MLSE also manages or has invested in several other sports facilities includ</t>
+          <t>Avro Canada VZ-9 Avrocar = The Avro Canada VZ-9 Avrocar was a VTOL aircraft developed by Avro Aircraft Ltd . ( Canada ) as part of a secret U.S. military project carried out in the early years of the Cold War . The Avrocar intended to exploit the Coandă effect to provide lift and thrust from a single " turborotor " blowing exhaust out the rim of the disk-shaped aircraft to provide anticipated VTOL-like performance . In the air , it would have resembled a flying saucer . Originally designed as a fighter-like aircraft capable of very high speeds and altitudes , the project was repeatedly scaled back over time and the U.S. Air Force eventually abandoned it . Development was then taken up by the U.S. Army for a tactical combat aircraft requirement , a sort of high-performance helicopter . In flight testing , the Avrocar proved to have unresolved thrust and stability problems that limited it to a degraded , low-performance flight envelope ; subsequently , the project was cancelled in Septem</t>
         </is>
       </c>
     </row>
@@ -2121,32 +2121,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>album songs number band release single music track copies released chart billboard tracks sound recording albums record week features reviews lyrics critics soundtrack studio debuted pop charts peaked vocals carey sold previous selling albums_chart contains certified producer performed singles cover platinum recorded felt listing song rock metacritic allmusic debut sales best label stars live hip sample hot hop rap shipments inspired promotion fans awards riaa promotional interview featuring drake grammy united_kingdom feel additional want jay-z written itunes assigns samples weeks bonus piano charting featured arranged writing arrangements sessions produced artist garbage recording_industry_association_of_america charted tour mixed wanted praised composed sounds rapper</t>
+          <t>['album', 'songs', 'number', 'band', 'release', 'single', 'music', 'track', 'copies', 'released', 'chart', 'billboard', 'tracks', 'sound', 'recording']</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Whatever ( Ayumi Hamasaki song ) = " Whatever " ( capitalized as " WHATEVER " ) is a song recorded by Japanese recording artist Ayumi Hamasaki for her second studio album , Loveppears ( 1999 ) . It was written by Hamasaki , while production was handled by Max Matsuura . The track is Hamasaki 's sixth single with Matsuura since her debut single in April 1998 , " Poker Face " . " Whatever " premiered on February 10 , 199 as the lead single from the album . It was re-released on February 28 , 2001 as a CD single . Musically , " Whatever " was described as a dance song , and is written in third person narrative . Upon its release , the track garnered mixed reviews from music critics . Critics praised Hamasaki 's move from pop rock to dance music , but criticized her vocal delivery and song writing . It also achieved success in Japan , peaking at number five on the Japanese Oricon Singles Chart . The re-released single peaked at number 28 on the same chart . As of March 2016 , " Whatever " </t>
+          <t>Marc Lépine = Marc Lépine ( French pronunciation : ​ [ maʁk lepin ] ; October 26 , 1964 – December 6 , 1989 ) was a 25-year-old Canadian man from Montreal , Quebec , who in 1989 murdered 14 women , and wounded 10 women and four men at the École Polytechnique , an engineering school affiliated with the Université de Montréal , in the École Polytechnique massacre , also known as the " Montreal Massacre " . Lépine was born in Montreal , the son of a Canadian nurse and an Algerian businessman . His father was abusive and contemptuous of women . After his parents separated when he was seven , his mother returned to nursing to support her children . Lépine and his younger sister lived with other families , seeing their mother on weekends . Lépine was considered bright but withdrawn and having difficulties with peer and family relationships . He changed his name to Marc Lépine at the age of 14 giving as the reason his hatred of his father . Lépine 's application to the Canadian Forces was rej</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Night of the Dead Living = " Night of the Dead Living " is the ninth episode and first season finale of the American police drama television series Homicide : Life on the Street . It originally aired on NBC in the United States on March 31 , 1993 . In the episode , the homicide squad works the night shift on a summer evening , but no calls come in , leaving the detectives to brood over their personal matters . The teleplay was written by Frank Pugliese based on a story he wrote along with executive producer Tom Fontana . It was directed by Michael Lehmann . " Night of the Dead Living " was originally intended to be the third episode of the season , but NBC programmers moved it to the end of the season because they felt its slow pace and lack of traditional action was inappropriate early in the series , when the show was trying to woo viewers . The broadcast schedule change led to some consistency and time-line errors , which Homicide producers addressed by adding the words " One hot ni</t>
+          <t>Kings and Queens ( Thirty Seconds to Mars song ) = " Kings and Queens " is a song by American rock band Thirty Seconds to Mars , featured on their third studio album This Is War ( 2009 ) . Written by lead vocalist Jared Leto across the United States and South Africa , the track was produced by Flood , Steve Lillywhite and Thirty Seconds to Mars . According to Leto , the lyrics of " Kings and Queens " explore the triumphant feeling of human possibilities . The melody of the song contains several qualities similar to that of 1980s adult contemporary musical works and is imbued with elements of progressive rock . The song was released as the lead single from This Is War on October 13 , 2009 . " Kings and Queens " received critical acclaim , with critics deeming it as an album highlight . Much of the praise went to the song 's lyrics and the musical production ; reviewers also complimented Leto 's vocals . The song became the band 's second number one single on the US Alternative Songs and</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Mario Ramírez Treviño = Mario Armando Ramírez Treviño ( born 5 March 1962 ) , commonly referred to by his aliases El Pelón and / or X-20 , is an alleged Mexican drug lord and former leader of the Gulf Cartel , a drug trafficking organization . In the early 2000s , Ramírez Treviño was a close associate of Jaime González Durán ( El Hummer ) , a founder and top leader of Los Zetas drug cartel . In 2008 , González Durán was arrested and sentenced to 35 years in prison ; by 2010 , Los Zetas , who were working as the armed wing of the Gulf Cartel , separated from the organization to operate independently . Both criminal organizations went to war with each other , but Ramírez Treviño remained in the Gulf Cartel . Under the tutelage of Samuel Flores Borrego ( El Metro 3 ) , he worked as the second-in-command for the criminal organization in Reynosa , Tamaulipas . In an apparent power struggle within the Gulf Cartel , however , El Metro 3 was killed , and he became the regional kingpin in Septe</t>
+          <t>A Different Kind of Love Song = " A Different Kind of Love Song " is a song by American recording artist Cher , taken from her 24th studio album , Living Proof ( 2002 ) . The song was written and produced by Sigurd Rosnes and Johan Aberg , with additional writing done by Michelle Lewis , and was co-produced by Anders Hansson . The dance-pop song alludes to themes of tragedy , heroism and brotherhood , and was released as a double A-side single with " The Music 's No Good Without You " in July 2002 through Warner Bros. Records and WEA . " A Different Kind of Love Song " received mostly positive reviews from music critics , who deemed it as one of the album 's highlights , although noting Cher 's heavily processed vocals due to the use of auto-tune . The song charted on a few Billboard components , such as Dance / Club Play Songs , where it reached number one , Hot Dance Music / Maxi-Singles Sales , peaking at number two , and on the Adult Contemporary chart . No accompanying music video</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve">What 's My Name ? ( Rihanna song ) = " What 's My Name ? " is a song recorded by Barbadian recording artist Rihanna , for her fifth studio album Loud ( 2010 ) . Featuring guest vocals from Canadian rapper Drake , the song was released as the second single from Loud on October 29 , 2010 through Def Jam Recordings . The electro-R &amp; B song was produced by the Norwegian production duo StarGate , and was written by the duo along with Ester Dean , Traci Hale , and Drake . Lyrically , it incorporates themes of sexual intercourse and romance . Music critics gave the song positive reviews , citing it some of Rihanna 's best vocal work to date ; there was a praise regarding its romantic nature , as well as its sexual tones . " What 's My Name ? " was a commercial success and topped the US Billboard Hot 100 chart , giving Rihanna her sixth number-one single in 2010 , as well as her eighth overall on the chart . The song also topped the charts in Hungary and the United Kingdom and reached the top </t>
+          <t>Lo Mejor de Mí ( song ) = " Lo Mejor de Mí " ( " All My Best " ) is a song written and produced by Rudy Pérez and first recorded by Spanish singer Juan Ramon for his second studio album Por Haberte Amado Tanto ( 1990 ) . In the song , the protagonist tells his lover how he gave his best despite not meeting his lover 's expectation . In 1997 , Mexican recording artist Cristian Castro covered the song for his fifth studio album Lo Mejor de Mí which Pérez also produced and arranged . Castro 's version peaked at number-one on the Billboard Hot Latin Songs and the Billboard Latin Pop Songs charts in the United States . The song received a Billboard Latin Music Awards and a Lo Nuestro nomination for Pop Song of the Year . Pérez earned the American Society of Composers , Authors and Publishers award in the Pop / Ballad field . = = Background = = In 1990 , Spanish recording artist Juan Ramon released his second studio album Por Haberte Amado Tanto which was arranged and produced by Cuban-Ameri</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Red Headed Stranger = Red Headed Stranger is a 1975 album by American outlaw country singer Willie Nelson . After the wide success of his recordings with Atlantic Records , coupled with the negotiating skills of his manager , Neil Reshen , Nelson signed a contract with Columbia Records , a label that gave him total creative control over his works . The concept for the album was inspired by the " Tale of the Red Headed Stranger " , a song that Nelson used to play as a disk jockey on his program in Fort Worth , Texas . After signing with Columbia he decided to record the song , and arranged the details during his return to Austin , Texas , from a trip to Colorado . It was recorded at low cost at Autumn Sound Studios in Garland , Texas . The songs featured sparse arrangements , largely limited to Nelson 's guitar , piano and drums . Nelson presented the finished material to Columbia executives , who were dubious about releasing an album that they at first thought was a demo . However , Ne</t>
+          <t>Mr.Mr. ( song ) = " Mr.Mr. " is a Korean song recorded by South Korean girl group Girls ' Generation for their fourth Korean titular extended play ( 2014 ) . The song was released on February 25 , 2014 , as a single from the EP . The song was composed by American production team The Underdogs , who had previously worked with Western artists including Britney Spears , Beyoncé , and Justin Timberlake . A music video for the song was initially planned to be released on February 19 but was postponed to February 28 due to the accidental deletion of some of the original files . " Mr.Mr. " was described as an electropop and pop-R &amp; B song that incorporates a hip hop beat and EDM-influenced buildups . The song received generally positive reviews from music critics , who praised its musical styles , which were deemed a departure from the group 's signature bubblegum pop sound . The single ranked number 18 on Billboard magazine 's list of 20 Best K-pop Songs of 2014 and was included on Time 's l</t>
         </is>
       </c>
     </row>
@@ -2156,32 +2156,32 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ship ships torpedo tons guns admiral cruiser fleet submarine sank laid sinking convoy german destroyer destroyers ordered boats damaged deck naval sunk knots escorted gun mounts repairs flagship torpedoes assigned stern shaft british flotilla vessels nautical escort transferred hms admiralty fire battleship aboard boilers cruisers beam hull convoys shipyard port malta april crew captain armament aft returning bow vessel horsepower sailed commissioned turbines french north_sea merchant royal_navy launched engagement submarines tubes range frigate escorting carried refit shipping inch displaced turrets kiel twin submerged engaged survivors warships wreck sms sea joined consisted battleships blockade departed fired maximum hipper thick sister returned</t>
+          <t>['ship', 'ships', 'torpedo', 'tons', 'guns', 'admiral', 'cruiser', 'fleet', 'submarine', 'sank', 'laid', 'sinking', 'convoy', 'german', 'destroyer']</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>Japanese cruiser Azuma = Azuma ( 吾妻 ) ( sometimes transliterated ( archaically ) as Adzuma ) was an armored cruiser built for the Imperial Japanese Navy ( IJN ) in the late 1890s . As Japan lacked the industrial capacity to build such warships herself , the ship was built in France . She participated in most of the naval battles of the Russo-Japanese War of 1904 – 05 and was lightly damaged during the Battle off Ulsan and the Battle of Tsushima . Azuma began the first of five training cruises in 1912 and saw no combat during World War I. She was never formally reclassified as a training ship although she exclusively served in that role from 1921 until she was disarmed and hulked in 1941 . Azuma was badly damaged in an American carrier raid in 1945 , and subsequently scrapped in 1946 . = = Background and design = = The 1896 Naval Expansion Plan was made after the First Sino-Japanese War , and included four armored cruisers in addition to four more battleships , all of which had to be or</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>C and D-class destroyer = The C and D class was a group of 14 destroyers built for the Royal Navy in the early 1930s . As in previous years , it was originally intended to order a complete flotilla comprising eight destroyers — plus a flotilla leader as the ninth unit — in each year . However , only four ships — plus a leader — were ordered under the 1929 – 30 Programme as the C class . The other four ships planned for the C class were never ordered as an economy measure and disarmament gesture by the Labour government of Ramsay Macdonald . A complete flotilla — the ' D ' class — was ordered under the 1930 – 31 Programme . The five ships of the C class were assigned to Home Fleet upon their completion , although they reinforced the Mediterranean Fleet during the Italian invasion of Abyssinia of 1935 – 36 and enforced the Non-Intervention Agreement during the Spanish Civil War of 1936 – 39 . They were transferred to the Royal Canadian Navy ( RCN ) in 1937 – 39 and spent most of their ti</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
           <t xml:space="preserve">SMS Gneisenau = SMS Gneisenau was an armored cruiser of the German navy , part of the two-ship Scharnhorst class . She was named after August von Gneisenau , a Prussian general of the Napoleonic Wars . The ship was laid down in 1904 at the AG Weser dockyard in Bremen , launched in June 1906 , and completed in March 1908 , at a cost of over 19 million goldmarks . She was armed with a main battery of eight 21-centimetre ( 8.3 in ) guns , had a top speed of 23.6 knots ( 43.7 km / h ; 27.2 mph ) , and displaced 12,985 metric tons ( 12,780 long tons ; 14,314 short tons ) at full combat load . Gneisenau was assigned to the German East Asia Squadron based in Tsingtao , China , along with Scharnhorst , in 1910 . They served as the core of Vice Admiral Maximilian von Spee 's fleet . After the outbreak of World War I in August 1914 , the two ships , accompanied by three light cruisers and several colliers , sailed across the Pacific ocean — in the process evading the various Allied naval forces </t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Italian cruiser San Giorgio = The Italian cruiser San Giorgio was the name ship of her class of two armored cruisers built for the Royal Italian Navy ( Regia Marina ) in the first decade of the 20th century . Commissioned in 1910 , the ship was badly damaged when she ran aground before the start of the Italo-Turkish War in 1911 , although she was repaired before its end . During World War I , San Giorgio 's activities were limited by the threat of Austro-Hungarian submarines , although the ship did participate in the bombardment of Durazzo , Albania , in late 1918 . She acted as a royal yacht for Crown Prince Umberto 's 1924 tour of South America and then deployed to the Indian Ocean to support operations in Italian Somaliland in 1925 – 26 . San Giorgio served as a training ship from 1930 to 1935 and was then rebuilt in 1937 – 38 to better serve in that role . As part of her reconstruction , she received a modern anti-aircraft suite that was augmented before she was transferred to bols</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>HMS Majestic ( 1895 ) = HMS Majestic was a Majestic-class pre-dreadnought battleship of the Royal Navy . Commissioned in 1895 , she was the largest predreadnought launched at the time . She served with the Channel Fleet until 1904 , following which she was assigned to the Atlantic Fleet . In 1907 , she was part of the Home Fleet , firstly assigned to the Nore Division and then with the Devonport Division . From 1912 , she was part of the 7th Battle Squadron . When World War I broke out Majestic , together with the rest of the squadron , was attached to the Channel Fleet during the early stages of the war before being detached for escort duties with Canadian troop convoys . She then had spells as a guard ship at the Nore and the Humber . In early 1915 , she was dispatched to the Mediterranean for service in the Dardanelles Campaign . She participated in bombardments of Turkish forts and supported the Allied landings at Gallipoli . On 27 May 1915 , she was torpedoed by a U-boat at Cape H</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Flat Bastion Road = Flat Bastion Road is a road in Gibraltar , the British Overseas Territory at the southern end of the Iberian Peninsula . The road runs north-south , providing views of the city and Bay of Gibraltar . Previously known in Spanish as Senda del Moro ( English : Path of the Moor ) , the traditional Llanito name for the road is Cuesta de Mr. Bourne . The road angles along the west side of the Rock of Gibraltar to the Flat Bastion , a fortification . Married quarters were built along the road . In the nineteenth century there were outbreaks of yellow fever in the 1820s and of diphtheria in the 1880s among the residents , apparently due to faulty sewers . Developments included , in the 1830s a school for poor children which remained in use as a school into the early twentieth century and a club where masked balls were held . In modern times the bastion 's magazine has been refurbished for civilian use , the barracks have been converted into affordable housing , and parking </t>
+          <t>HMS Jamaica ( 44 ) = HMS Jamaica , a Crown Colony-class cruiser of the Royal Navy , was named after the island of Jamaica , which was a British possession when she was built in the late 1930s . The light cruiser spent almost her entire wartime career on Arctic convoy duties , except for a deployment south for the landings in North Africa in November 1942 . She participated in the Battle of the Barents Sea in 1942 and the Battle of North Cape in 1943 . Jamaica escorted several aircraft carriers in 1944 as they flew off airstrikes that attacked the German battleship Tirpitz in northern Norway . Late in the year she had an extensive refit to prepare her for service with the British Pacific Fleet , but the war ended before she reached the Pacific . Jamaica spent the late 1940s in the Far East and on the North America and West Indies Station . When the Korean War began in 1950 she was ordered , in cooperation with the United States Navy , to bombard North Korean troops as they advanced down</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Königsberg-class cruiser ( 1915 ) = The Königsberg class of light cruisers was a group of four ships commissioned into Germany 's Imperial Navy shortly before the end of World War I. The class comprised Königsberg , Karlsruhe , Emden , and Nürnberg , all of which were named after light cruisers lost earlier in the war . The ships were an incremental improvement over the preceding Wiesbaden-class cruisers , and were armed with a main battery of eight 15 cm SK L / 45 guns and had a designed speed of 27.5 knots ( 50.9 km / h ; 31.6 mph ) . Königsberg and Nürnberg saw action at the Second Battle of Heligoland Bight , where Königsberg was hit by a shell from the battlecruiser Repulse . Three of the four ships were to participate in a climactic fleet operation to attack the British Grand Fleet in the final days of the war , but revolts in the fleet forced the cancellation of the plan . Karlsruhe , Emden , and Nürnberg were interned at Scapa Flow after the end of the war , and were scuttled o</t>
+          <t xml:space="preserve">French seaplane carrier Commandant Teste = Commandant Teste was a large seaplane tender of the French Navy ( French : Marine Nationale ) built before World War II . She was designed to be as large as possible without counting against the Washington Treaty limits . During the Spanish Civil War , she protected neutral merchant shipping and played a limited role during World War II as she spent the early part of the war in North African waters or acting as an aviation transport between France and North Africa . She was slightly damaged during the British bombardment of the French Fleet at Mers-el-Kébir in July 1940 . Commandant Teste was scuttled at Toulon when the Germans invaded Vichy France in November 1942 , but was refloated after the war and considered for conversion to an escort or training carrier . Neither proposal was accepted and she was sold for scrap in 1950 . = = Design = = After the completion of aircraft carrier Béarn , the Marine Nationale desired another aviation vessel </t>
         </is>
       </c>
     </row>
@@ -2191,32 +2191,32 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>government war military led political country party support polish foreign soviet revolution leader russian members alliance army influence forces russia france poland coup leaders german independence economic minister arab regime germany nationalist according established power people communist soviet_union reforms policies control european death western official ties conflict lithuanian diplomatic commonwealth relations leadership french general exile empire countries hitler peasants authorities local remained appointed uprising agreed faction moscow lithuania armed central anti new struggle nationalists sent troops supported syria emperor jewish national jews prime policy nationalism commander austria egypt armenian increasingly years international despite socialist revolt member ethnic china monarchy governments</t>
+          <t>['government', 'war', 'military', 'led', 'political', 'country', 'party', 'support', 'polish', 'foreign', 'soviet', 'revolution', 'leader', 'russian', 'members']</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pyrrhus ' invasion of the Peloponnese = Pyrrhus ' invasion of the Peloponnese in 272 BC was an invasion of south Greece by Pyrrhus , King of Epirus . He was opposed by Macedon and a coalition of Greek city-states ( poleis ) , most notably Sparta . The war ended in a joint victory by Macedonia and Sparta . After being defeated by the Roman Republic in the Pyrrhic War in 275 BC , Pyrrhus ( r . 297 – 272 BC ) decided to turn his attention to Greece . He declared war on Antigonus Gonatas ( r . 283 – 239 BC ) of Macedon and in a rapid campaign , managed to defeat him and make himself king of Macedon . In 272 BC , Pyrrhus agreed to assist the disgruntled Spartan prince , Cleonymus , who requested his assistance in securing the Spartan throne . Pyrrhus advanced with his army through central Greece and upon reaching the Peloponnese , he marched against Sparta . The city was sparsely defended at the time as the majority of its army had been taken to Crete by King Areus I ( r . 309 – 265 BC ) . </t>
+          <t>Tupelo Honey = Tupelo Honey is the fifth studio album by Northern Irish singer-songwriter Van Morrison . It was released in October 1971 by Warner Bros. Records . Morrison had written all of the songs on the album in Woodstock , New York , before his move to Marin County , California , except for " You 're My Woman " , which he wrote during the recording sessions . Recording began at the beginning of the second quarter of 1971 at the Wally Heider Studios , San Francisco . Morrison moved to the Columbia Studios in May 1971 to complete the album . The namesake for the album and its title track is a varietal honey produced from the flowers of the tupelo tree found in the Southeastern United States . The album features various musical genres , most prominently country , but also R &amp; B , soul , folk-rock and blue-eyed soul . The lyrics echo the domestic bliss portrayed on the album cover ; they largely describe and celebrate the rural surroundings of Woodstock and Morrison 's family life wi</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Robotron : 2084 = Robotron : 2084 ( also referred to as Robotron ) is an arcade video game developed by Eugene Jarvis and Larry DeMar of Vid Kidz and released by Williams Electronics ( part of WMS Industries ) in 1982 . It is a shoot ' em up with two-dimensional graphics . The game is set in the year 2084 in a fictional world where robots have turned against humans in a cybernetic revolt . The aim is to defeat endless waves of robots , rescue surviving humans , and earn as many points as possible . Robotron popularized the twin joystick control scheme , one that had previously been used in Taito 's Space Dungeon . Robotron : 2084 was critically and commercially successful . Praise among critics focused on the game 's intense action and control scheme . The game is frequently listed as one of Jarvis 's best contributions to the video game industry . Robotron : 2084 arcade cabinets have since become a sought-after collector 's item . It was ported to numerous platforms . = = Gameplay = =</t>
+          <t>New Guinea Volunteer Rifles = The New Guinea Volunteer Rifles ( NGVR ) was an infantry battalion of the Australian Army . It was initially raised as a unit of the Militia from white Australian and European expatriates in New Guinea upon the outbreak of the Second World War in 1939 , before being activated for full-time service following the Japanese landings in early 1942 . NGVR personnel then helped rescue survivors of Lark Force from Rabaul in February and March 1942 . Between March and May , the NGVR monitored the Japanese bases which had been established in the Huon Gulf region , being the only Allied force in the area until the arrival of Kanga Force at Wau in May . The battalion subsequently established observation posts overlooking the main approaches and reported on Japanese movements . Later , it inflicted significant casualties on the Japanese in a series of raids , and led them to believe that they faced a much larger opposing force . On 29 June , the NGVR and the newly arri</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Western Wall = The Western Wall , Wailing Wall or Kotel ( Hebrew : הַכֹּתֶל הַמַּעֲרָבִי , translit . : HaKotel HaMa 'aravi ; Ashkenazic pronunciation : Kosel ; Arabic : حائط البراق , translit . : Ḥā 'iṭ al-Burāq , translat . : the Buraq Wall , or al-Mabka : the Place of Weeping ) is an ancient limestone wall in the Old City of Jerusalem . It is a relatively small segment of a far longer ancient retaining wall , known also in its entirety as the " Western Wall " . The wall was originally erected as part of the expansion of the Second Jewish Temple by Herod the Great , which resulted in the encasement of the natural , steep hill known to Jews and Christians as the Temple Mount , in a large rectangular structure topped by a huge flat platform , thus creating more space for the Temple itself and its auxiliary buildings . The Western Wall is considered holy due to its connection to the Temple Mount . Because of the status quo policy , the Wall is the holiest place where Jews are permitted </t>
+          <t>Malagasy Uprising = The Malagasy Uprising ( French : Insurrection malgache ) was a Malagasy nationalist rebellion against French colonial rule in Madagascar , lasting from March 1947 to December 1948 . Starting in late 1945 , Madagascar 's first French National Assembly deputies , Joseph Raseta , Joseph Ravoahangy and Jacques Rabemananjara of the Mouvement démocratique de la rénovation malgache ( MDRM ) political party , led an effort to achieve independence for Madagascar through legal channels . The failure of this initiative and the harsh response it drew from the Socialist Ramadier administration radicalized elements of the Malagasy population , including leaders of several militant nationalist secret societies . On the evening of 29 March 1947 , coordinated surprise attacks were launched by Malagasy nationalists , armed mainly with spears , against military bases and French-owned plantations in the eastern part of the island concentrated around Moramanga and Manakara . The nationa</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Malcolm III of Scotland = Malcolm ( Gaelic : Máel Coluim ; c . 1031 – 13 November 1093 ) was King of Scots from 1058 to 1093 . He was later nicknamed Canmore ( ceann mòr ) in Scottish Gaelic , " Great Chief " . ( Ceann = leader , " head " [ of state ] . Mòr = pre-eminent , great , " big " . ) Malcolm 's long reign , lasting 35 years , preceded the beginning of the Scoto-Norman age . He is the historical equivalent of the character of the same name in Shakespeare 's Macbeth . Malcolm 's kingdom did not extend over the full territory of modern Scotland : the north and west of Scotland remained in Scandinavian , Norse-Gael and Gaelic control , and the areas under the control of the Kings of Scots did not advance much beyond the limits set by Malcolm II until the 12th century . Malcolm III fought a succession of wars against the Kingdom of England , which may have had as their goal the conquest of the English earldom of Northumbria . These wars did not result in any significant advances so</t>
+          <t>Campaign of Grodno = The Campaign of Grodno was a plan developed by Johann Patkul and Otto Arnold von Paykull during the Swedish invasion of the Polish – Lithuanian Commonwealth , a part of the Great Northern War . Its purpose was to crush Charles XII 's army with overwhelming force in a combined offensive of Russian and Saxon troops . The campaign , executed by Peter I of Russia and Augustus II of Saxony , began in July 1705 and lasted almost a year . In divided areas the allies would jointly strike the Swedish troops occupied in Poland , in order to neutralize the influence the Swedes had in the Polish politics . However , the Swedish forces under Charles XII successfully outmaneuvered the allies , installed a Polish king in favor of their own and finally won two decisive victories at Grodno and Fraustadt in 1706 . This resulted in the Treaty of Altranstädt ( 1706 ) in which Augustus renounced his claims to the Polish throne , broke off his alliance with Russia , and established peac</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Persecution of Zoroastrians = Persecution of Zoroastrians is the religious persecution inflicted upon the followers of the Zoroastrian faith . The persecution of Zoroastrians occurred throughout its history . The discrimination and harassment began in the form of sparse violence and forced conversions . Muslims are recorded to have destroyed fire temples . Zoroastrians living under Muslim rule were required to pay a tax called Jizya . Zoroastrian places of worship were desecrated , shrines were destroyed and mosques built in their place . Many libraries were burned and much cultural heritage was lost . Gradually there were increased number of laws regulating Zoroastrian behavior , limiting their ability to participate in society . Over time , persecution of Zoroastrians became more common and widespread , and the number of believers decreased significantly . Many converted , some superficially , to escape the systematic abuse and discrimination by the law of the land . Once a Zoroastri</t>
+          <t>Charlotte Lewis ( Lost ) = Dr. Charlotte Staples Lewis is a fictional character on the American Broadcasting Company ( ABC ) television series Lost , played by Rebecca Mader . Charlotte is introduced in the second episode of season four and is a cultural anthropologist on a mission to the island where Oceanic Flight 815 crashed . On the island she is initially held hostage by one of the plane crash survivors , John Locke ( Terry O 'Quinn ) , but is freed when another person from her team switches place with her . She helps prevent poison gas from being released over the island , and develops a relationship with Daniel Faraday ( Jeremy Davies ) . Charlotte dies in Daniel 's arms after the frequent time traveling causes her headaches to worsen into something unexplainable . Although conceived by the show 's creators to be American , Charlotte 's nationality was changed to British after the producers were impressed with English actress Rebecca Mader 's audition . She was supposed to featu</t>
         </is>
       </c>
     </row>

</xml_diff>